<commit_message>
Semainiers de cette semaine 2020-02-19 , Heures Jord-Alex
</commit_message>
<xml_diff>
--- a/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
+++ b/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alxbo\Source\Repos\mrjrdg\marque-sans-nom\Semainiers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Desktop/marque-sans-nom/Semainiers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289E67B7-38AB-41A3-A718-7F7AF83E414B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C231F6-63FA-AB4D-9755-55CA56435E74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
   <si>
     <t>UQÀM - Hiver 2020</t>
   </si>
@@ -264,16 +262,28 @@
   <si>
     <t>Rédiger le rapport de sprint 1</t>
   </si>
+  <si>
+    <t>Schema design pattern</t>
+  </si>
+  <si>
+    <t>Travail sur Controlleur : Account, admin,error,event</t>
+  </si>
+  <si>
+    <t>Diagrammes de comprehension au membres</t>
+  </si>
+  <si>
+    <t>Account management settings. Front end/ back, Asp Razor Pages implentation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_)_ ;_ * \(#,##0.00\)_ ;_ * &quot;-&quot;??_)_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="0\ %"/>
-    <numFmt numFmtId="165" formatCode="[$-C0C]dd/mmm"/>
-    <numFmt numFmtId="166" formatCode="\\;;;"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_)_ ;_ * \(#,##0.00\)_ ;_ * &quot;-&quot;??_)_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0\ %"/>
+    <numFmt numFmtId="166" formatCode="[$-C0C]dd/mmm"/>
+    <numFmt numFmtId="167" formatCode="\\;;;"/>
   </numFmts>
   <fonts count="26" x14ac:knownFonts="1">
     <font>
@@ -960,7 +970,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0"/>
-    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -972,7 +982,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="4" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="5" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="6" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -987,19 +997,19 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="11" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="11" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="13" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="13" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1018,19 +1028,19 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="11" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="11" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
@@ -1073,28 +1083,28 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="8" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="43" fontId="20" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="20" fillId="0" borderId="33" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="33" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="20" fillId="0" borderId="25" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="25" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="20" fillId="0" borderId="26" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="26" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="43" fontId="20" fillId="0" borderId="28" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="28" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="20" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1119,19 +1129,19 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="2" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="12" fillId="2" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="16" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="16" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1139,7 +1149,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="18" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="18" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1152,7 +1162,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="20" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="20" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1164,21 +1174,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="21" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="21" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="22" fillId="6" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="22" fillId="6" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="24" fillId="3" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="24" fillId="3" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="24" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="24" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1195,7 +1205,7 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="24" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="24" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1203,14 +1213,14 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="24" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="24" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="24" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="24" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1230,7 +1240,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="20" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="20" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1238,11 +1248,11 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="30" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="30" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="30" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="30" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1269,11 +1279,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1303,44 +1313,30 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="8" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="8" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="8" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="8" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="8" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="8" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="30" xfId="4" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="4" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="7" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1351,6 +1347,9 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1376,22 +1375,33 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="30" xfId="4" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="4" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
+    <cellStyle name="Comma" xfId="8" builtinId="3"/>
     <cellStyle name="Excel Built-in 60% - Accent4" xfId="6" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Excel Built-in Bad" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Excel Built-in Good" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Excel Built-in Good 1" xfId="7" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Excel Built-in Neutral" xfId="4" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Excel Built-in Normal" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Milliers" xfId="8" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
@@ -1555,7 +1565,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1856,69 +1866,69 @@
   </sheetPr>
   <dimension ref="A1:AMJ61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="64.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.77734375" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.109375" style="23" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.1640625" style="23" customWidth="1"/>
     <col min="6" max="6" width="7.6640625" style="23" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" style="32" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="32" customWidth="1"/>
     <col min="9" max="10" width="9.33203125" style="39" customWidth="1"/>
-    <col min="11" max="13" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="21" width="6.6640625" style="1" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="6.6640625" style="2" hidden="1" customWidth="1"/>
     <col min="23" max="25" width="6.6640625" style="1" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="6.6640625" style="2" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="20.77734375" style="25" customWidth="1"/>
-    <col min="28" max="28" width="22.77734375" style="1" customWidth="1"/>
+    <col min="27" max="27" width="20.83203125" style="25" customWidth="1"/>
+    <col min="28" max="28" width="22.83203125" style="1" customWidth="1"/>
     <col min="29" max="1024" width="10.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="130" t="s">
+    <row r="1" spans="1:1024" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="148" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="130"/>
-      <c r="D1" s="126" t="s">
+      <c r="B1" s="148"/>
+      <c r="D1" s="144" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="126"/>
-      <c r="L1" s="126"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="144"/>
+      <c r="G1" s="144"/>
+      <c r="H1" s="144"/>
+      <c r="I1" s="144"/>
+      <c r="J1" s="144"/>
+      <c r="K1" s="144"/>
+      <c r="L1" s="144"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1024" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="130" t="s">
+    <row r="2" spans="1:1024" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="148" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="130"/>
+      <c r="B2" s="148"/>
       <c r="D2" s="45"/>
       <c r="E2" s="45"/>
-      <c r="F2" s="132" t="s">
+      <c r="F2" s="149" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="132"/>
-      <c r="H2" s="132"/>
-      <c r="I2" s="132"/>
-      <c r="J2" s="132"/>
+      <c r="G2" s="149"/>
+      <c r="H2" s="149"/>
+      <c r="I2" s="149"/>
+      <c r="J2" s="149"/>
       <c r="K2" s="46"/>
       <c r="L2" s="46"/>
       <c r="P2" s="4"/>
@@ -1926,13 +1936,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1024" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1024" ht="16" x14ac:dyDescent="0.2">
       <c r="P3" s="5"/>
       <c r="Q3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:1024" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1024" ht="16" x14ac:dyDescent="0.2">
       <c r="N4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1941,7 +1951,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:1024" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1024" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="N5" s="7">
         <v>0.25</v>
       </c>
@@ -1957,73 +1967,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:1024" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K6" s="127" t="s">
+    <row r="6" spans="1:1024" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="145" t="s">
         <v>51</v>
       </c>
-      <c r="L6" s="128"/>
-      <c r="M6" s="128"/>
-      <c r="N6" s="128"/>
-      <c r="O6" s="128"/>
-      <c r="P6" s="128"/>
-      <c r="Q6" s="128"/>
-      <c r="R6" s="129"/>
+      <c r="L6" s="146"/>
+      <c r="M6" s="146"/>
+      <c r="N6" s="146"/>
+      <c r="O6" s="146"/>
+      <c r="P6" s="146"/>
+      <c r="Q6" s="146"/>
+      <c r="R6" s="147"/>
       <c r="V6" s="7"/>
       <c r="Z6" s="7"/>
     </row>
-    <row r="7" spans="1:1024" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="139" t="s">
+    <row r="7" spans="1:1024" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="140" t="s">
+      <c r="B7" s="137" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="141" t="s">
+      <c r="C7" s="138" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="141"/>
-      <c r="E7" s="141"/>
-      <c r="F7" s="141"/>
-      <c r="G7" s="142" t="s">
+      <c r="D7" s="138"/>
+      <c r="E7" s="138"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="139" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="143" t="s">
+      <c r="H7" s="140" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="144" t="s">
+      <c r="I7" s="141" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="144" t="s">
+      <c r="J7" s="141" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="146" t="s">
+      <c r="K7" s="143" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="146"/>
-      <c r="M7" s="146"/>
-      <c r="N7" s="146"/>
-      <c r="O7" s="146"/>
-      <c r="P7" s="146"/>
-      <c r="Q7" s="146"/>
-      <c r="R7" s="146"/>
-      <c r="S7" s="146"/>
-      <c r="T7" s="146"/>
-      <c r="U7" s="146"/>
-      <c r="V7" s="146"/>
-      <c r="W7" s="146"/>
-      <c r="X7" s="146"/>
-      <c r="Y7" s="146"/>
-      <c r="Z7" s="146"/>
-      <c r="AA7" s="135" t="s">
+      <c r="L7" s="143"/>
+      <c r="M7" s="143"/>
+      <c r="N7" s="143"/>
+      <c r="O7" s="143"/>
+      <c r="P7" s="143"/>
+      <c r="Q7" s="143"/>
+      <c r="R7" s="143"/>
+      <c r="S7" s="143"/>
+      <c r="T7" s="143"/>
+      <c r="U7" s="143"/>
+      <c r="V7" s="143"/>
+      <c r="W7" s="143"/>
+      <c r="X7" s="143"/>
+      <c r="Y7" s="143"/>
+      <c r="Z7" s="143"/>
+      <c r="AA7" s="131" t="s">
         <v>16</v>
       </c>
-      <c r="AB7" s="136" t="s">
+      <c r="AB7" s="132" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:1024" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="139"/>
-      <c r="B8" s="140"/>
+    <row r="8" spans="1:1024" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="136"/>
+      <c r="B8" s="137"/>
       <c r="C8" s="35" t="s">
         <v>18</v>
       </c>
@@ -2036,10 +2046,10 @@
       <c r="F8" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="142"/>
-      <c r="H8" s="143"/>
-      <c r="I8" s="145"/>
-      <c r="J8" s="145"/>
+      <c r="G8" s="139"/>
+      <c r="H8" s="140"/>
+      <c r="I8" s="142"/>
+      <c r="J8" s="142"/>
       <c r="K8" s="30">
         <v>43838</v>
       </c>
@@ -2103,10 +2113,10 @@
         <f t="shared" si="0"/>
         <v>43943</v>
       </c>
-      <c r="AA8" s="135"/>
-      <c r="AB8" s="137"/>
+      <c r="AA8" s="131"/>
+      <c r="AB8" s="133"/>
     </row>
-    <row r="9" spans="1:1024" ht="18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1024" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
       <c r="B9" s="10" t="s">
         <v>22</v>
@@ -2138,7 +2148,7 @@
       <c r="AA9" s="26"/>
       <c r="AB9" s="16"/>
     </row>
-    <row r="10" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="57">
         <v>1</v>
       </c>
@@ -3189,7 +3199,7 @@
       <c r="AMI10" s="68"/>
       <c r="AMJ10" s="68"/>
     </row>
-    <row r="11" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="57">
         <v>2</v>
       </c>
@@ -4240,7 +4250,7 @@
       <c r="AMI11" s="68"/>
       <c r="AMJ11" s="68"/>
     </row>
-    <row r="12" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="57">
         <v>3</v>
       </c>
@@ -5291,7 +5301,7 @@
       <c r="AMI12" s="68"/>
       <c r="AMJ12" s="68"/>
     </row>
-    <row r="13" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="57">
         <v>4</v>
       </c>
@@ -6342,7 +6352,7 @@
       <c r="AMI13" s="68"/>
       <c r="AMJ13" s="68"/>
     </row>
-    <row r="14" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="57">
         <v>5</v>
       </c>
@@ -7393,7 +7403,7 @@
       <c r="AMI14" s="68"/>
       <c r="AMJ14" s="68"/>
     </row>
-    <row r="15" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="57">
         <v>6</v>
       </c>
@@ -8444,7 +8454,7 @@
       <c r="AMI15" s="68"/>
       <c r="AMJ15" s="68"/>
     </row>
-    <row r="16" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="57">
         <v>7</v>
       </c>
@@ -9495,7 +9505,7 @@
       <c r="AMI16" s="68"/>
       <c r="AMJ16" s="68"/>
     </row>
-    <row r="17" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="57">
         <v>8</v>
       </c>
@@ -10546,7 +10556,7 @@
       <c r="AMI17" s="68"/>
       <c r="AMJ17" s="68"/>
     </row>
-    <row r="18" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="57">
         <v>9</v>
       </c>
@@ -11597,7 +11607,7 @@
       <c r="AMI18" s="68"/>
       <c r="AMJ18" s="68"/>
     </row>
-    <row r="19" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="57">
         <v>10</v>
       </c>
@@ -12648,7 +12658,7 @@
       <c r="AMI19" s="68"/>
       <c r="AMJ19" s="68"/>
     </row>
-    <row r="20" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="57">
         <v>11</v>
       </c>
@@ -13699,7 +13709,7 @@
       <c r="AMI20" s="68"/>
       <c r="AMJ20" s="68"/>
     </row>
-    <row r="21" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="57">
         <v>12</v>
       </c>
@@ -14748,7 +14758,7 @@
       <c r="AMI21" s="68"/>
       <c r="AMJ21" s="68"/>
     </row>
-    <row r="22" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="57">
         <v>13</v>
       </c>
@@ -15799,7 +15809,7 @@
       <c r="AMI22" s="68"/>
       <c r="AMJ22" s="68"/>
     </row>
-    <row r="23" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="57">
         <v>14</v>
       </c>
@@ -16850,7 +16860,7 @@
       <c r="AMI23" s="68"/>
       <c r="AMJ23" s="68"/>
     </row>
-    <row r="24" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="57">
         <v>15</v>
       </c>
@@ -17901,7 +17911,7 @@
       <c r="AMI24" s="68"/>
       <c r="AMJ24" s="68"/>
     </row>
-    <row r="25" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="57">
         <v>16</v>
       </c>
@@ -18952,7 +18962,7 @@
       <c r="AMI25" s="68"/>
       <c r="AMJ25" s="68"/>
     </row>
-    <row r="26" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="57">
         <v>17</v>
       </c>
@@ -20003,7 +20013,7 @@
       <c r="AMI26" s="68"/>
       <c r="AMJ26" s="68"/>
     </row>
-    <row r="27" spans="1:1024" s="110" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1024" s="110" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="57">
         <v>18</v>
       </c>
@@ -20024,10 +20034,10 @@
       </c>
       <c r="G27" s="60">
         <f>VLOOKUP(H27,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H27" s="107" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I27" s="108">
         <v>21</v>
@@ -21054,7 +21064,7 @@
       <c r="AMI27" s="109"/>
       <c r="AMJ27" s="109"/>
     </row>
-    <row r="28" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="57">
         <v>19</v>
       </c>
@@ -21075,10 +21085,10 @@
       </c>
       <c r="G28" s="60">
         <f>VLOOKUP(H28,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H28" s="61" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I28" s="62">
         <v>10</v>
@@ -22105,7 +22115,7 @@
       <c r="AMI28" s="68"/>
       <c r="AMJ28" s="68"/>
     </row>
-    <row r="29" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="57">
         <v>20</v>
       </c>
@@ -22126,10 +22136,10 @@
       </c>
       <c r="G29" s="60">
         <f>VLOOKUP(H29,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H29" s="61" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I29" s="62">
         <v>5</v>
@@ -23156,7 +23166,7 @@
       <c r="AMI29" s="68"/>
       <c r="AMJ29" s="68"/>
     </row>
-    <row r="30" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="57">
         <v>21</v>
       </c>
@@ -24207,7 +24217,7 @@
       <c r="AMI30" s="68"/>
       <c r="AMJ30" s="68"/>
     </row>
-    <row r="31" spans="1:1024" s="110" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1024" s="110" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="57">
         <v>22</v>
       </c>
@@ -24228,10 +24238,10 @@
       </c>
       <c r="G31" s="60">
         <f>VLOOKUP(H31,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H31" s="107" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I31" s="108">
         <v>12</v>
@@ -25258,7 +25268,7 @@
       <c r="AMI31" s="109"/>
       <c r="AMJ31" s="109"/>
     </row>
-    <row r="32" spans="1:1024" s="110" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1024" s="110" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="57">
         <v>23</v>
       </c>
@@ -26309,7 +26319,7 @@
       <c r="AMI32" s="109"/>
       <c r="AMJ32" s="109"/>
     </row>
-    <row r="33" spans="1:1024" s="69" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="57">
         <v>24</v>
       </c>
@@ -26347,8 +26357,8 @@
       <c r="M33" s="103"/>
       <c r="N33" s="104"/>
       <c r="O33" s="113"/>
-      <c r="P33" s="148"/>
-      <c r="Q33" s="149"/>
+      <c r="P33" s="127"/>
+      <c r="Q33" s="128"/>
       <c r="R33" s="120"/>
       <c r="S33" s="103"/>
       <c r="T33" s="103"/>
@@ -27360,7 +27370,7 @@
       <c r="AMI33" s="68"/>
       <c r="AMJ33" s="68"/>
     </row>
-    <row r="34" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="57">
         <v>25</v>
       </c>
@@ -27399,7 +27409,7 @@
       <c r="N34" s="75"/>
       <c r="O34" s="64"/>
       <c r="P34" s="64"/>
-      <c r="Q34" s="147"/>
+      <c r="Q34" s="126"/>
       <c r="R34" s="75"/>
       <c r="S34" s="101"/>
       <c r="T34" s="101"/>
@@ -28411,7 +28421,7 @@
       <c r="AMI34" s="68"/>
       <c r="AMJ34" s="68"/>
     </row>
-    <row r="35" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="57">
         <v>26</v>
       </c>
@@ -29460,11 +29470,13 @@
       <c r="AMI35" s="68"/>
       <c r="AMJ35" s="68"/>
     </row>
-    <row r="36" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="57">
         <v>27</v>
       </c>
-      <c r="B36" s="97"/>
+      <c r="B36" s="97" t="s">
+        <v>57</v>
+      </c>
       <c r="C36" s="59">
         <v>0</v>
       </c>
@@ -29475,19 +29487,19 @@
         <v>0</v>
       </c>
       <c r="F36" s="59">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G36" s="60">
         <f>VLOOKUP(H36,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="H36" s="61" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I36" s="62"/>
       <c r="J36" s="62">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K36" s="101"/>
       <c r="L36" s="101"/>
@@ -29495,7 +29507,7 @@
       <c r="N36" s="75"/>
       <c r="O36" s="101"/>
       <c r="P36" s="101"/>
-      <c r="Q36" s="64"/>
+      <c r="Q36" s="128"/>
       <c r="R36" s="75"/>
       <c r="S36" s="101"/>
       <c r="T36" s="101"/>
@@ -29507,7 +29519,7 @@
       <c r="Z36" s="75"/>
       <c r="AA36" s="66">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="AB36" s="71"/>
       <c r="AC36" s="68"/>
@@ -30507,13 +30519,15 @@
       <c r="AMI36" s="68"/>
       <c r="AMJ36" s="68"/>
     </row>
-    <row r="37" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="57">
         <v>28</v>
       </c>
-      <c r="B37" s="97"/>
+      <c r="B37" s="97" t="s">
+        <v>58</v>
+      </c>
       <c r="C37" s="59">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D37" s="59">
         <v>0</v>
@@ -30522,19 +30536,19 @@
         <v>0</v>
       </c>
       <c r="F37" s="59">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G37" s="60">
         <f>VLOOKUP(H37,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="H37" s="61" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I37" s="62"/>
       <c r="J37" s="62">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K37" s="101"/>
       <c r="L37" s="101"/>
@@ -30542,7 +30556,7 @@
       <c r="N37" s="75"/>
       <c r="O37" s="101"/>
       <c r="P37" s="101"/>
-      <c r="Q37" s="101"/>
+      <c r="Q37" s="128"/>
       <c r="R37" s="75"/>
       <c r="S37" s="101"/>
       <c r="T37" s="101"/>
@@ -30554,7 +30568,7 @@
       <c r="Z37" s="75"/>
       <c r="AA37" s="66">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="AB37" s="71"/>
       <c r="AC37" s="68"/>
@@ -31554,11 +31568,13 @@
       <c r="AMI37" s="68"/>
       <c r="AMJ37" s="68"/>
     </row>
-    <row r="38" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="57">
         <v>29</v>
       </c>
-      <c r="B38" s="97"/>
+      <c r="B38" s="97" t="s">
+        <v>59</v>
+      </c>
       <c r="C38" s="59">
         <v>0</v>
       </c>
@@ -31569,19 +31585,19 @@
         <v>0</v>
       </c>
       <c r="F38" s="59">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G38" s="60">
         <f>VLOOKUP(H38,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="H38" s="61" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I38" s="62"/>
       <c r="J38" s="62">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K38" s="101"/>
       <c r="L38" s="101"/>
@@ -31589,7 +31605,7 @@
       <c r="N38" s="75"/>
       <c r="O38" s="101"/>
       <c r="P38" s="101"/>
-      <c r="Q38" s="101"/>
+      <c r="Q38" s="128"/>
       <c r="R38" s="65"/>
       <c r="S38" s="101"/>
       <c r="T38" s="101"/>
@@ -31601,7 +31617,7 @@
       <c r="Z38" s="75"/>
       <c r="AA38" s="66">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="AB38" s="71"/>
       <c r="AC38" s="68"/>
@@ -32601,13 +32617,15 @@
       <c r="AMI38" s="68"/>
       <c r="AMJ38" s="68"/>
     </row>
-    <row r="39" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1024" s="69" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="57">
         <v>30</v>
       </c>
-      <c r="B39" s="97"/>
+      <c r="B39" s="97" t="s">
+        <v>60</v>
+      </c>
       <c r="C39" s="59">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D39" s="59">
         <v>0</v>
@@ -32620,15 +32638,15 @@
       </c>
       <c r="G39" s="60">
         <f>VLOOKUP(H39,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="H39" s="61" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I39" s="62"/>
       <c r="J39" s="62">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K39" s="101"/>
       <c r="L39" s="101"/>
@@ -32636,7 +32654,7 @@
       <c r="N39" s="75"/>
       <c r="O39" s="101"/>
       <c r="P39" s="101"/>
-      <c r="Q39" s="101"/>
+      <c r="Q39" s="128"/>
       <c r="R39" s="75"/>
       <c r="S39" s="64"/>
       <c r="T39" s="101"/>
@@ -32648,7 +32666,7 @@
       <c r="Z39" s="75"/>
       <c r="AA39" s="66">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="AB39" s="71"/>
       <c r="AC39" s="68"/>
@@ -33648,7 +33666,7 @@
       <c r="AMI39" s="68"/>
       <c r="AMJ39" s="68"/>
     </row>
-    <row r="40" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="57">
         <v>31</v>
       </c>
@@ -34695,7 +34713,7 @@
       <c r="AMI40" s="68"/>
       <c r="AMJ40" s="68"/>
     </row>
-    <row r="41" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="57">
         <v>32</v>
       </c>
@@ -35742,7 +35760,7 @@
       <c r="AMI41" s="68"/>
       <c r="AMJ41" s="68"/>
     </row>
-    <row r="42" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="57">
         <v>33</v>
       </c>
@@ -36789,7 +36807,7 @@
       <c r="AMI42" s="68"/>
       <c r="AMJ42" s="68"/>
     </row>
-    <row r="43" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="57">
         <v>34</v>
       </c>
@@ -37836,7 +37854,7 @@
       <c r="AMI43" s="68"/>
       <c r="AMJ43" s="68"/>
     </row>
-    <row r="44" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="57">
         <v>35</v>
       </c>
@@ -38883,7 +38901,7 @@
       <c r="AMI44" s="68"/>
       <c r="AMJ44" s="68"/>
     </row>
-    <row r="45" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="57">
         <v>36</v>
       </c>
@@ -39930,7 +39948,7 @@
       <c r="AMI45" s="68"/>
       <c r="AMJ45" s="68"/>
     </row>
-    <row r="46" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="57">
         <v>37</v>
       </c>
@@ -40977,7 +40995,7 @@
       <c r="AMI46" s="68"/>
       <c r="AMJ46" s="68"/>
     </row>
-    <row r="47" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="57">
         <v>38</v>
       </c>
@@ -42024,7 +42042,7 @@
       <c r="AMI47" s="68"/>
       <c r="AMJ47" s="68"/>
     </row>
-    <row r="48" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1024" s="69" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="57">
         <v>39</v>
       </c>
@@ -43071,7 +43089,7 @@
       <c r="AMI48" s="68"/>
       <c r="AMJ48" s="68"/>
     </row>
-    <row r="49" spans="1:1024" s="69" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1024" s="69" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="57">
         <v>40</v>
       </c>
@@ -44118,14 +44136,14 @@
       <c r="AMI49" s="68"/>
       <c r="AMJ49" s="68"/>
     </row>
-    <row r="50" spans="1:1024" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="138" t="s">
+    <row r="50" spans="1:1024" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="134" t="s">
         <v>39</v>
       </c>
-      <c r="B50" s="138"/>
+      <c r="B50" s="134"/>
       <c r="C50" s="47">
         <f>SUM(C10:C49)</f>
-        <v>58.5</v>
+        <v>65.5</v>
       </c>
       <c r="D50" s="47">
         <f>SUM(D10:D49)</f>
@@ -44137,14 +44155,14 @@
       </c>
       <c r="F50" s="47">
         <f>SUM(F10:F49)</f>
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="G50" s="48"/>
       <c r="H50" s="49"/>
       <c r="I50" s="50"/>
       <c r="J50" s="47">
         <f>SUM(C50:F50)</f>
-        <v>223.5</v>
+        <v>245.5</v>
       </c>
       <c r="K50" s="51"/>
       <c r="L50" s="51"/>
@@ -44164,18 +44182,18 @@
       <c r="Z50" s="51"/>
       <c r="AA50" s="47">
         <f>SUM(AA10:AA49)</f>
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="AB50" s="52"/>
     </row>
-    <row r="51" spans="1:1024" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="131" t="s">
+    <row r="51" spans="1:1024" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="135" t="s">
         <v>40</v>
       </c>
-      <c r="B51" s="131"/>
+      <c r="B51" s="135"/>
       <c r="C51" s="47">
         <f>135-C50</f>
-        <v>76.5</v>
+        <v>69.5</v>
       </c>
       <c r="D51" s="47">
         <f>135-D50</f>
@@ -44187,14 +44205,14 @@
       </c>
       <c r="F51" s="47">
         <f>135-F50</f>
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="G51" s="48"/>
       <c r="H51" s="47"/>
       <c r="I51" s="47"/>
       <c r="J51" s="47">
         <f>SUM(C51:F51)</f>
-        <v>316.5</v>
+        <v>294.5</v>
       </c>
       <c r="K51" s="51"/>
       <c r="L51" s="51"/>
@@ -44215,11 +44233,11 @@
       <c r="AA51" s="53"/>
       <c r="AB51" s="51"/>
     </row>
-    <row r="52" spans="1:1024" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="133" t="s">
+    <row r="52" spans="1:1024" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="129" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="133"/>
+      <c r="B52" s="129"/>
       <c r="C52" s="47"/>
       <c r="D52" s="47"/>
       <c r="E52" s="47"/>
@@ -44250,11 +44268,11 @@
       <c r="AA52" s="53"/>
       <c r="AB52" s="51"/>
     </row>
-    <row r="53" spans="1:1024" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="131" t="s">
+    <row r="53" spans="1:1024" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="135" t="s">
         <v>54</v>
       </c>
-      <c r="B53" s="131"/>
+      <c r="B53" s="135"/>
       <c r="C53" s="47"/>
       <c r="D53" s="47"/>
       <c r="E53" s="54"/>
@@ -44267,7 +44285,7 @@
       </c>
       <c r="J53" s="47">
         <f>SUM(J10:J49)</f>
-        <v>223.5</v>
+        <v>245.5</v>
       </c>
       <c r="K53" s="51"/>
       <c r="L53" s="51"/>
@@ -44288,7 +44306,7 @@
       <c r="AA53" s="53"/>
       <c r="AB53" s="51"/>
     </row>
-    <row r="54" spans="1:1024" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1024" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="17"/>
       <c r="B54" s="17"/>
       <c r="C54" s="56"/>
@@ -44318,11 +44336,11 @@
       <c r="AA54" s="53"/>
       <c r="AB54" s="51"/>
     </row>
-    <row r="55" spans="1:1024" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="133" t="s">
+    <row r="55" spans="1:1024" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="129" t="s">
         <v>55</v>
       </c>
-      <c r="B55" s="133"/>
+      <c r="B55" s="129"/>
       <c r="C55" s="47">
         <f>135*4</f>
         <v>540</v>
@@ -44353,14 +44371,14 @@
       <c r="AA55" s="53"/>
       <c r="AB55" s="51"/>
     </row>
-    <row r="56" spans="1:1024" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="134" t="s">
+    <row r="56" spans="1:1024" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="130" t="s">
         <v>53</v>
       </c>
-      <c r="B56" s="134"/>
+      <c r="B56" s="130"/>
       <c r="C56" s="47">
         <f>C55-J53</f>
-        <v>316.5</v>
+        <v>294.5</v>
       </c>
       <c r="D56" s="56"/>
       <c r="E56" s="56"/>
@@ -44388,7 +44406,7 @@
       <c r="AA56" s="53"/>
       <c r="AB56" s="51"/>
     </row>
-    <row r="57" spans="1:1024" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1024" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="18"/>
       <c r="B57" s="17"/>
       <c r="C57" s="37"/>
@@ -44401,12 +44419,12 @@
       <c r="J57" s="41"/>
       <c r="AA57" s="27"/>
     </row>
-    <row r="58" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="D58" s="38"/>
       <c r="E58" s="38"/>
       <c r="F58" s="38"/>
     </row>
-    <row r="59" spans="1:1024" s="19" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1024" s="19" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A59" s="20"/>
       <c r="C59" s="24"/>
       <c r="D59" s="24"/>
@@ -44421,7 +44439,7 @@
       <c r="Z59" s="21"/>
       <c r="AA59" s="28"/>
     </row>
-    <row r="60" spans="1:1024" s="19" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1024" s="19" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="C60" s="24"/>
       <c r="D60" s="24"/>
       <c r="E60" s="24"/>
@@ -44435,7 +44453,7 @@
       <c r="Z60" s="21"/>
       <c r="AA60" s="28"/>
     </row>
-    <row r="61" spans="1:1024" s="19" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1024" s="19" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="C61" s="24"/>
       <c r="D61" s="24"/>
       <c r="E61" s="24"/>
@@ -44451,6 +44469,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="F2:J2"/>
     <mergeCell ref="A55:B55"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="AA7:AA8"/>
@@ -44466,12 +44490,6 @@
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:Z7"/>
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="F2:J2"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
     <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="En cours">
@@ -44528,12 +44546,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1025" width="10.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>5</v>
       </c>
@@ -44541,7 +44559,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -44549,7 +44567,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -44569,7 +44587,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1025" width="10.6640625" style="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Added last week hours
</commit_message>
<xml_diff>
--- a/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
+++ b/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Desktop/marque-sans-nom/Semainiers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alxbo\Source\Repos\mrjrdg\marque-sans-nom\Semainiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EB1231-6A42-3B41-AE4C-8AC715159DA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6B2071-F165-4C73-B0A2-85C55E6E7FC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
   <si>
     <t>UQÀM - Hiver 2020</t>
   </si>
@@ -283,16 +285,19 @@
   <si>
     <t>Conceptualiser le schema relationnel de la Base de donnée</t>
   </si>
+  <si>
+    <t>Template user-view</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_ * #,##0.00_)_ ;_ * \(#,##0.00\)_ ;_ * &quot;-&quot;??_)_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="0\ %"/>
-    <numFmt numFmtId="166" formatCode="[$-C0C]dd/mmm"/>
-    <numFmt numFmtId="167" formatCode="\\;;;"/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_)_ ;_ * \(#,##0.00\)_ ;_ * &quot;-&quot;??_)_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="0\ %"/>
+    <numFmt numFmtId="165" formatCode="[$-C0C]dd/mmm"/>
+    <numFmt numFmtId="166" formatCode="\\;;;"/>
   </numFmts>
   <fonts count="26" x14ac:knownFonts="1">
     <font>
@@ -970,9 +975,9 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0"/>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
@@ -982,7 +987,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="4" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="5" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="6" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -997,19 +1002,19 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="11" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="11" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="13" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="13" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1028,19 +1033,19 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="11" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="11" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
@@ -1083,25 +1088,25 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="8" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="20" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="32" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="20" fillId="0" borderId="32" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="25" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="20" fillId="0" borderId="25" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="27" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="18" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="20" fillId="0" borderId="27" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="21" fillId="0" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="20" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1122,19 +1127,19 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="2" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="12" fillId="2" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="16" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="16" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1142,7 +1147,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="18" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="18" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1155,7 +1160,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="20" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="20" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1167,21 +1172,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="21" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="21" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="167" fontId="22" fillId="6" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="22" fillId="6" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="24" fillId="3" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="24" fillId="3" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="24" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1197,7 +1202,7 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="24" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1205,14 +1210,14 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="24" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="24" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1228,15 +1233,15 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="20" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="20" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="29" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="29" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="29" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="29" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1259,11 +1264,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1285,15 +1290,15 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="8" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="8" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="8" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="8" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="8" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="8" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1"/>
@@ -1302,11 +1307,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="7" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1317,9 +1343,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1345,33 +1368,18 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="4" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Comma" xfId="8" builtinId="3"/>
     <cellStyle name="Excel Built-in 60% - Accent4" xfId="6" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Excel Built-in Bad" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Excel Built-in Good" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Excel Built-in Good 1" xfId="7" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Excel Built-in Neutral" xfId="4" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Excel Built-in Normal" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Milliers" xfId="8" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
@@ -1535,7 +1543,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1836,69 +1844,69 @@
   </sheetPr>
   <dimension ref="A1:AMJ59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34:F35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="64.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="23" customWidth="1"/>
-    <col min="4" max="5" width="8.1640625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" style="23" customWidth="1"/>
+    <col min="4" max="5" width="8.109375" style="23" customWidth="1"/>
     <col min="6" max="6" width="7.6640625" style="23" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" style="32" customWidth="1"/>
+    <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" style="32" customWidth="1"/>
     <col min="9" max="10" width="9.33203125" style="39" customWidth="1"/>
-    <col min="11" max="13" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="21" width="6.6640625" style="1" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="6.6640625" style="2" hidden="1" customWidth="1"/>
     <col min="23" max="25" width="6.6640625" style="1" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="6.6640625" style="2" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="20.83203125" style="25" customWidth="1"/>
-    <col min="28" max="28" width="22.83203125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="20.77734375" style="25" customWidth="1"/>
+    <col min="28" max="28" width="22.77734375" style="1" customWidth="1"/>
     <col min="29" max="1024" width="10.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="140" t="s">
+    <row r="1" spans="1:1024" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="140"/>
-      <c r="D1" s="136" t="s">
+      <c r="B1" s="125"/>
+      <c r="D1" s="121" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
-      <c r="I1" s="136"/>
-      <c r="J1" s="136"/>
-      <c r="K1" s="136"/>
-      <c r="L1" s="136"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="121"/>
+      <c r="J1" s="121"/>
+      <c r="K1" s="121"/>
+      <c r="L1" s="121"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1024" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="140" t="s">
+    <row r="2" spans="1:1024" ht="21" x14ac:dyDescent="0.4">
+      <c r="A2" s="125" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="140"/>
+      <c r="B2" s="125"/>
       <c r="D2" s="45"/>
       <c r="E2" s="45"/>
-      <c r="F2" s="141" t="s">
+      <c r="F2" s="127" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="141"/>
-      <c r="H2" s="141"/>
-      <c r="I2" s="141"/>
-      <c r="J2" s="141"/>
+      <c r="G2" s="127"/>
+      <c r="H2" s="127"/>
+      <c r="I2" s="127"/>
+      <c r="J2" s="127"/>
       <c r="K2" s="46"/>
       <c r="L2" s="46"/>
       <c r="P2" s="4"/>
@@ -1906,13 +1914,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1024" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1024" ht="15.6" x14ac:dyDescent="0.3">
       <c r="P3" s="5"/>
       <c r="Q3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:1024" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1024" ht="15.6" x14ac:dyDescent="0.3">
       <c r="N4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1921,7 +1929,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:1024" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1024" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N5" s="7">
         <v>0.25</v>
       </c>
@@ -1937,73 +1945,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:1024" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K6" s="137" t="s">
+    <row r="6" spans="1:1024" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K6" s="122" t="s">
         <v>50</v>
       </c>
-      <c r="L6" s="138"/>
-      <c r="M6" s="138"/>
-      <c r="N6" s="138"/>
-      <c r="O6" s="138"/>
-      <c r="P6" s="138"/>
-      <c r="Q6" s="138"/>
-      <c r="R6" s="139"/>
+      <c r="L6" s="123"/>
+      <c r="M6" s="123"/>
+      <c r="N6" s="123"/>
+      <c r="O6" s="123"/>
+      <c r="P6" s="123"/>
+      <c r="Q6" s="123"/>
+      <c r="R6" s="124"/>
       <c r="V6" s="7"/>
       <c r="Z6" s="7"/>
     </row>
-    <row r="7" spans="1:1024" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="128" t="s">
+    <row r="7" spans="1:1024" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="134" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="129" t="s">
+      <c r="B7" s="135" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="130" t="s">
+      <c r="C7" s="136" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="130"/>
-      <c r="E7" s="130"/>
-      <c r="F7" s="130"/>
-      <c r="G7" s="131" t="s">
+      <c r="D7" s="136"/>
+      <c r="E7" s="136"/>
+      <c r="F7" s="136"/>
+      <c r="G7" s="137" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="132" t="s">
+      <c r="H7" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="133" t="s">
+      <c r="I7" s="139" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="133" t="s">
+      <c r="J7" s="139" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="135" t="s">
+      <c r="K7" s="141" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="135"/>
-      <c r="M7" s="135"/>
-      <c r="N7" s="135"/>
-      <c r="O7" s="135"/>
-      <c r="P7" s="135"/>
-      <c r="Q7" s="135"/>
-      <c r="R7" s="135"/>
-      <c r="S7" s="135"/>
-      <c r="T7" s="135"/>
-      <c r="U7" s="135"/>
-      <c r="V7" s="135"/>
-      <c r="W7" s="135"/>
-      <c r="X7" s="135"/>
-      <c r="Y7" s="135"/>
-      <c r="Z7" s="135"/>
-      <c r="AA7" s="123" t="s">
+      <c r="L7" s="141"/>
+      <c r="M7" s="141"/>
+      <c r="N7" s="141"/>
+      <c r="O7" s="141"/>
+      <c r="P7" s="141"/>
+      <c r="Q7" s="141"/>
+      <c r="R7" s="141"/>
+      <c r="S7" s="141"/>
+      <c r="T7" s="141"/>
+      <c r="U7" s="141"/>
+      <c r="V7" s="141"/>
+      <c r="W7" s="141"/>
+      <c r="X7" s="141"/>
+      <c r="Y7" s="141"/>
+      <c r="Z7" s="141"/>
+      <c r="AA7" s="130" t="s">
         <v>16</v>
       </c>
-      <c r="AB7" s="124" t="s">
+      <c r="AB7" s="131" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:1024" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="128"/>
-      <c r="B8" s="129"/>
+    <row r="8" spans="1:1024" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="134"/>
+      <c r="B8" s="135"/>
       <c r="C8" s="35" t="s">
         <v>18</v>
       </c>
@@ -2016,10 +2024,10 @@
       <c r="F8" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="131"/>
-      <c r="H8" s="132"/>
-      <c r="I8" s="134"/>
-      <c r="J8" s="134"/>
+      <c r="G8" s="137"/>
+      <c r="H8" s="138"/>
+      <c r="I8" s="140"/>
+      <c r="J8" s="140"/>
       <c r="K8" s="30">
         <v>43838</v>
       </c>
@@ -2083,10 +2091,10 @@
         <f t="shared" si="0"/>
         <v>43943</v>
       </c>
-      <c r="AA8" s="123"/>
-      <c r="AB8" s="125"/>
+      <c r="AA8" s="130"/>
+      <c r="AB8" s="132"/>
     </row>
-    <row r="9" spans="1:1024" ht="19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1024" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="10" t="s">
         <v>22</v>
@@ -2118,7 +2126,7 @@
       <c r="AA9" s="26"/>
       <c r="AB9" s="16"/>
     </row>
-    <row r="10" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="56">
         <v>1</v>
       </c>
@@ -3169,7 +3177,7 @@
       <c r="AMI10" s="66"/>
       <c r="AMJ10" s="66"/>
     </row>
-    <row r="11" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="56">
         <v>2</v>
       </c>
@@ -4220,7 +4228,7 @@
       <c r="AMI11" s="66"/>
       <c r="AMJ11" s="66"/>
     </row>
-    <row r="12" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="56">
         <v>3</v>
       </c>
@@ -5271,7 +5279,7 @@
       <c r="AMI12" s="66"/>
       <c r="AMJ12" s="66"/>
     </row>
-    <row r="13" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="56">
         <v>4</v>
       </c>
@@ -6322,7 +6330,7 @@
       <c r="AMI13" s="66"/>
       <c r="AMJ13" s="66"/>
     </row>
-    <row r="14" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="56">
         <v>5</v>
       </c>
@@ -7373,7 +7381,7 @@
       <c r="AMI14" s="66"/>
       <c r="AMJ14" s="66"/>
     </row>
-    <row r="15" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="56">
         <v>6</v>
       </c>
@@ -8424,7 +8432,7 @@
       <c r="AMI15" s="66"/>
       <c r="AMJ15" s="66"/>
     </row>
-    <row r="16" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="56">
         <v>7</v>
       </c>
@@ -9475,7 +9483,7 @@
       <c r="AMI16" s="66"/>
       <c r="AMJ16" s="66"/>
     </row>
-    <row r="17" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="56">
         <v>8</v>
       </c>
@@ -10526,7 +10534,7 @@
       <c r="AMI17" s="66"/>
       <c r="AMJ17" s="66"/>
     </row>
-    <row r="18" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="56">
         <v>9</v>
       </c>
@@ -11577,7 +11585,7 @@
       <c r="AMI18" s="66"/>
       <c r="AMJ18" s="66"/>
     </row>
-    <row r="19" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="56">
         <v>10</v>
       </c>
@@ -12628,7 +12636,7 @@
       <c r="AMI19" s="66"/>
       <c r="AMJ19" s="66"/>
     </row>
-    <row r="20" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="56">
         <v>11</v>
       </c>
@@ -13679,7 +13687,7 @@
       <c r="AMI20" s="66"/>
       <c r="AMJ20" s="66"/>
     </row>
-    <row r="21" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="56">
         <v>12</v>
       </c>
@@ -14728,7 +14736,7 @@
       <c r="AMI21" s="66"/>
       <c r="AMJ21" s="66"/>
     </row>
-    <row r="22" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="56">
         <v>13</v>
       </c>
@@ -15779,7 +15787,7 @@
       <c r="AMI22" s="66"/>
       <c r="AMJ22" s="66"/>
     </row>
-    <row r="23" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="56">
         <v>14</v>
       </c>
@@ -16830,7 +16838,7 @@
       <c r="AMI23" s="66"/>
       <c r="AMJ23" s="66"/>
     </row>
-    <row r="24" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1024" s="67" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="56">
         <v>15</v>
       </c>
@@ -16844,7 +16852,7 @@
         <v>10</v>
       </c>
       <c r="E24" s="58">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F24" s="58">
         <v>0</v>
@@ -16861,7 +16869,7 @@
       </c>
       <c r="J24" s="60">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K24" s="89"/>
       <c r="L24" s="81"/>
@@ -16869,7 +16877,7 @@
       <c r="N24" s="90"/>
       <c r="O24" s="90"/>
       <c r="P24" s="92"/>
-      <c r="Q24" s="91"/>
+      <c r="Q24" s="142"/>
       <c r="R24" s="77"/>
       <c r="S24" s="76"/>
       <c r="T24" s="76"/>
@@ -16881,7 +16889,7 @@
       <c r="Z24" s="63"/>
       <c r="AA24" s="64">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AB24" s="69"/>
       <c r="AC24" s="66"/>
@@ -17881,7 +17889,7 @@
       <c r="AMI24" s="66"/>
       <c r="AMJ24" s="66"/>
     </row>
-    <row r="25" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="56">
         <v>16</v>
       </c>
@@ -18932,7 +18940,7 @@
       <c r="AMI25" s="66"/>
       <c r="AMJ25" s="66"/>
     </row>
-    <row r="26" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1024" s="67" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="56">
         <v>17</v>
       </c>
@@ -19983,7 +19991,7 @@
       <c r="AMI26" s="66"/>
       <c r="AMJ26" s="66"/>
     </row>
-    <row r="27" spans="1:1024" s="104" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1024" s="104" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="56">
         <v>18</v>
       </c>
@@ -21034,7 +21042,7 @@
       <c r="AMI27" s="103"/>
       <c r="AMJ27" s="103"/>
     </row>
-    <row r="28" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1024" s="67" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="56">
         <v>19</v>
       </c>
@@ -22085,7 +22093,7 @@
       <c r="AMI28" s="66"/>
       <c r="AMJ28" s="66"/>
     </row>
-    <row r="29" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="56">
         <v>20</v>
       </c>
@@ -22095,10 +22103,10 @@
       <c r="C29" s="58">
         <v>6</v>
       </c>
-      <c r="D29" s="58">
+      <c r="D29" s="106">
         <v>0</v>
       </c>
-      <c r="E29" s="58">
+      <c r="E29" s="106">
         <v>0</v>
       </c>
       <c r="F29" s="58">
@@ -23136,7 +23144,7 @@
       <c r="AMI29" s="66"/>
       <c r="AMJ29" s="66"/>
     </row>
-    <row r="30" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1024" s="67" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="56">
         <v>21</v>
       </c>
@@ -24187,7 +24195,7 @@
       <c r="AMI30" s="66"/>
       <c r="AMJ30" s="66"/>
     </row>
-    <row r="31" spans="1:1024" s="104" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1024" s="104" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="56">
         <v>22</v>
       </c>
@@ -25238,7 +25246,7 @@
       <c r="AMI31" s="103"/>
       <c r="AMJ31" s="103"/>
     </row>
-    <row r="32" spans="1:1024" s="104" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1024" s="104" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="56">
         <v>23</v>
       </c>
@@ -26289,7 +26297,7 @@
       <c r="AMI32" s="103"/>
       <c r="AMJ32" s="103"/>
     </row>
-    <row r="33" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1024" s="67" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="56">
         <v>24</v>
       </c>
@@ -27340,7 +27348,7 @@
       <c r="AMI33" s="66"/>
       <c r="AMJ33" s="66"/>
     </row>
-    <row r="34" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="56">
         <v>25</v>
       </c>
@@ -28391,7 +28399,7 @@
       <c r="AMI34" s="66"/>
       <c r="AMJ34" s="66"/>
     </row>
-    <row r="35" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="56">
         <v>27</v>
       </c>
@@ -29440,7 +29448,7 @@
       <c r="AMI35" s="66"/>
       <c r="AMJ35" s="66"/>
     </row>
-    <row r="36" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="56">
         <v>28</v>
       </c>
@@ -30489,7 +30497,7 @@
       <c r="AMI36" s="66"/>
       <c r="AMJ36" s="66"/>
     </row>
-    <row r="37" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="56">
         <v>29</v>
       </c>
@@ -31538,7 +31546,7 @@
       <c r="AMI37" s="66"/>
       <c r="AMJ37" s="66"/>
     </row>
-    <row r="38" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1024" s="67" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="56">
         <v>30</v>
       </c>
@@ -32587,7 +32595,7 @@
       <c r="AMI38" s="66"/>
       <c r="AMJ38" s="66"/>
     </row>
-    <row r="39" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="56">
         <v>31</v>
       </c>
@@ -33636,7 +33644,7 @@
       <c r="AMI39" s="66"/>
       <c r="AMJ39" s="66"/>
     </row>
-    <row r="40" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="56">
         <v>33</v>
       </c>
@@ -34685,7 +34693,7 @@
       <c r="AMI40" s="66"/>
       <c r="AMJ40" s="66"/>
     </row>
-    <row r="41" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="56">
         <v>26</v>
       </c>
@@ -35734,7 +35742,7 @@
       <c r="AMI41" s="66"/>
       <c r="AMJ41" s="66"/>
     </row>
-    <row r="42" spans="1:1024" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="56">
         <v>35</v>
       </c>
@@ -36783,11 +36791,13 @@
       <c r="AMI42" s="66"/>
       <c r="AMJ42" s="66"/>
     </row>
-    <row r="43" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1024" s="67" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="56">
         <v>36</v>
       </c>
-      <c r="B43" s="94"/>
+      <c r="B43" s="94" t="s">
+        <v>64</v>
+      </c>
       <c r="C43" s="58">
         <v>0</v>
       </c>
@@ -36795,22 +36805,24 @@
         <v>0</v>
       </c>
       <c r="E43" s="58">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F43" s="58">
         <v>0</v>
       </c>
       <c r="G43" s="120">
         <f>VLOOKUP(H43,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="H43" s="102" t="s">
-        <v>5</v>
-      </c>
-      <c r="I43" s="60"/>
+        <v>3</v>
+      </c>
+      <c r="I43" s="60">
+        <v>4</v>
+      </c>
       <c r="J43" s="60">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K43" s="97"/>
       <c r="L43" s="97"/>
@@ -36818,7 +36830,7 @@
       <c r="N43" s="73"/>
       <c r="O43" s="97"/>
       <c r="P43" s="97"/>
-      <c r="Q43" s="97"/>
+      <c r="Q43" s="142"/>
       <c r="R43" s="73"/>
       <c r="S43" s="97"/>
       <c r="T43" s="97"/>
@@ -36830,7 +36842,7 @@
       <c r="Z43" s="73"/>
       <c r="AA43" s="64">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB43" s="69"/>
       <c r="AC43" s="66"/>
@@ -37830,7 +37842,7 @@
       <c r="AMI43" s="66"/>
       <c r="AMJ43" s="66"/>
     </row>
-    <row r="44" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="56">
         <v>37</v>
       </c>
@@ -38877,7 +38889,7 @@
       <c r="AMI44" s="66"/>
       <c r="AMJ44" s="66"/>
     </row>
-    <row r="45" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="56">
         <v>38</v>
       </c>
@@ -39924,7 +39936,7 @@
       <c r="AMI45" s="66"/>
       <c r="AMJ45" s="66"/>
     </row>
-    <row r="46" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1024" s="67" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="56">
         <v>39</v>
       </c>
@@ -40971,7 +40983,7 @@
       <c r="AMI46" s="66"/>
       <c r="AMJ46" s="66"/>
     </row>
-    <row r="47" spans="1:1024" s="67" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1024" s="67" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="56">
         <v>40</v>
       </c>
@@ -42018,11 +42030,11 @@
       <c r="AMI47" s="66"/>
       <c r="AMJ47" s="66"/>
     </row>
-    <row r="48" spans="1:1024" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="126" t="s">
+    <row r="48" spans="1:1024" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="133" t="s">
         <v>39</v>
       </c>
-      <c r="B48" s="126"/>
+      <c r="B48" s="133"/>
       <c r="C48" s="47">
         <f>SUM(C10:C47)</f>
         <v>67.5</v>
@@ -42033,7 +42045,7 @@
       </c>
       <c r="E48" s="47">
         <f>SUM(E10:E47)</f>
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F48" s="47">
         <f>SUM(F10:F47)</f>
@@ -42044,7 +42056,7 @@
       <c r="I48" s="49"/>
       <c r="J48" s="47">
         <f>SUM(C48:F48)</f>
-        <v>259.5</v>
+        <v>263.5</v>
       </c>
       <c r="K48" s="50"/>
       <c r="L48" s="50"/>
@@ -42068,11 +42080,11 @@
       </c>
       <c r="AB48" s="51"/>
     </row>
-    <row r="49" spans="1:28" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="127" t="s">
+    <row r="49" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="126" t="s">
         <v>40</v>
       </c>
-      <c r="B49" s="127"/>
+      <c r="B49" s="126"/>
       <c r="C49" s="47">
         <f>135-C48</f>
         <v>67.5</v>
@@ -42083,7 +42095,7 @@
       </c>
       <c r="E49" s="47">
         <f>135-E48</f>
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F49" s="47">
         <f>135-F48</f>
@@ -42094,7 +42106,7 @@
       <c r="I49" s="47"/>
       <c r="J49" s="47">
         <f>SUM(C49:F49)</f>
-        <v>280.5</v>
+        <v>276.5</v>
       </c>
       <c r="K49" s="50"/>
       <c r="L49" s="50"/>
@@ -42115,11 +42127,11 @@
       <c r="AA49" s="52"/>
       <c r="AB49" s="50"/>
     </row>
-    <row r="50" spans="1:28" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="121" t="s">
+    <row r="50" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="128" t="s">
         <v>41</v>
       </c>
-      <c r="B50" s="121"/>
+      <c r="B50" s="128"/>
       <c r="C50" s="47"/>
       <c r="D50" s="47"/>
       <c r="E50" s="47"/>
@@ -42150,11 +42162,11 @@
       <c r="AA50" s="52"/>
       <c r="AB50" s="50"/>
     </row>
-    <row r="51" spans="1:28" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="127" t="s">
+    <row r="51" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="126" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="127"/>
+      <c r="B51" s="126"/>
       <c r="C51" s="47"/>
       <c r="D51" s="47"/>
       <c r="E51" s="53"/>
@@ -42163,11 +42175,11 @@
       <c r="H51" s="47"/>
       <c r="I51" s="54">
         <f>SUM(I10:I47)</f>
-        <v>254.5</v>
+        <v>258.5</v>
       </c>
       <c r="J51" s="47">
         <f>SUM(J10:J47)</f>
-        <v>259.5</v>
+        <v>263.5</v>
       </c>
       <c r="K51" s="50"/>
       <c r="L51" s="50"/>
@@ -42188,7 +42200,7 @@
       <c r="AA51" s="52"/>
       <c r="AB51" s="50"/>
     </row>
-    <row r="52" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="17"/>
       <c r="B52" s="17"/>
       <c r="C52" s="55"/>
@@ -42218,11 +42230,11 @@
       <c r="AA52" s="52"/>
       <c r="AB52" s="50"/>
     </row>
-    <row r="53" spans="1:28" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="121" t="s">
+    <row r="53" spans="1:28" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="128" t="s">
         <v>54</v>
       </c>
-      <c r="B53" s="121"/>
+      <c r="B53" s="128"/>
       <c r="C53" s="47">
         <f>135*4</f>
         <v>540</v>
@@ -42253,14 +42265,14 @@
       <c r="AA53" s="52"/>
       <c r="AB53" s="50"/>
     </row>
-    <row r="54" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="122" t="s">
+    <row r="54" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="129" t="s">
         <v>52</v>
       </c>
-      <c r="B54" s="122"/>
+      <c r="B54" s="129"/>
       <c r="C54" s="47">
         <f>C53-J51</f>
-        <v>280.5</v>
+        <v>276.5</v>
       </c>
       <c r="D54" s="55"/>
       <c r="E54" s="55"/>
@@ -42288,7 +42300,7 @@
       <c r="AA54" s="52"/>
       <c r="AB54" s="50"/>
     </row>
-    <row r="55" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="18"/>
       <c r="B55" s="17"/>
       <c r="C55" s="37"/>
@@ -42301,12 +42313,12 @@
       <c r="J55" s="41"/>
       <c r="AA55" s="27"/>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D56" s="38"/>
       <c r="E56" s="38"/>
       <c r="F56" s="38"/>
     </row>
-    <row r="57" spans="1:28" s="19" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" s="19" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A57" s="20"/>
       <c r="C57" s="24"/>
       <c r="D57" s="24"/>
@@ -42321,7 +42333,7 @@
       <c r="Z57" s="21"/>
       <c r="AA57" s="28"/>
     </row>
-    <row r="58" spans="1:28" s="19" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" s="19" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="C58" s="24"/>
       <c r="D58" s="24"/>
       <c r="E58" s="24"/>
@@ -42335,7 +42347,7 @@
       <c r="Z58" s="21"/>
       <c r="AA58" s="28"/>
     </row>
-    <row r="59" spans="1:28" s="19" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" s="19" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="C59" s="24"/>
       <c r="D59" s="24"/>
       <c r="E59" s="24"/>
@@ -42351,12 +42363,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="F2:J2"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="AA7:AA8"/>
@@ -42372,6 +42378,12 @@
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:Z7"/>
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="F2:J2"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
     <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="En cours">
@@ -42428,12 +42440,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1025" width="10.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>5</v>
       </c>
@@ -42441,7 +42453,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -42449,7 +42461,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -42469,7 +42481,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1025" width="10.6640625" style="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Added my hours for today
</commit_message>
<xml_diff>
--- a/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
+++ b/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alxbo\Source\Repos\mrjrdg\marque-sans-nom\Semainiers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abourdeau\source\repos\mrjrdg\marque-sans-nom\Semainiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E3E1FD-6F4A-46A0-B83C-5938BA5B8DA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D6E32C-DDC7-4076-9D1C-16DB44D2D3E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1809,35 +1809,35 @@
   </sheetPr>
   <dimension ref="A1:AMK72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A33" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="66.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.77734375" style="2" customWidth="1"/>
-    <col min="4" max="5" width="8.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="66.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="2" customWidth="1"/>
+    <col min="4" max="5" width="8.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" style="3" customWidth="1"/>
-    <col min="9" max="10" width="9.33203125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" style="3" customWidth="1"/>
+    <col min="9" max="10" width="9.28515625" style="4" customWidth="1"/>
     <col min="11" max="13" width="8" style="1" customWidth="1"/>
     <col min="14" max="14" width="8" style="5" customWidth="1"/>
-    <col min="15" max="16" width="7.77734375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="9.77734375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="7.77734375" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="8.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.21875" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="7.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.21875" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.77734375" style="6" customWidth="1"/>
-    <col min="28" max="28" width="22.77734375" style="1" customWidth="1"/>
-    <col min="29" max="1025" width="10.6640625" style="1"/>
+    <col min="15" max="16" width="7.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.7109375" style="6" customWidth="1"/>
+    <col min="28" max="28" width="22.7109375" style="1" customWidth="1"/>
+    <col min="29" max="1025" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="8" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="8" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="124" t="s">
         <v>0</v>
       </c>
@@ -1864,7 +1864,7 @@
       <c r="Z1" s="3"/>
       <c r="AA1" s="10"/>
     </row>
-    <row r="2" spans="1:28" s="8" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" s="8" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="124" t="s">
         <v>3</v>
       </c>
@@ -1891,7 +1891,7 @@
       <c r="Z2" s="3"/>
       <c r="AA2" s="10"/>
     </row>
-    <row r="3" spans="1:28" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -1909,7 +1909,7 @@
       <c r="Z3" s="3"/>
       <c r="AA3" s="10"/>
     </row>
-    <row r="4" spans="1:28" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
@@ -1929,7 +1929,7 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="10"/>
     </row>
-    <row r="5" spans="1:28" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
@@ -1953,7 +1953,7 @@
       </c>
       <c r="AA5" s="10"/>
     </row>
-    <row r="6" spans="1:28" s="8" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" s="8" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
@@ -1975,7 +1975,7 @@
       <c r="Z6" s="17"/>
       <c r="AA6" s="10"/>
     </row>
-    <row r="7" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="127" t="s">
         <v>10</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="127"/>
       <c r="B8" s="128"/>
       <c r="C8" s="20" t="s">
@@ -2110,7 +2110,7 @@
       <c r="AA8" s="134"/>
       <c r="AB8" s="135"/>
     </row>
-    <row r="9" spans="1:28" ht="18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>24</v>
@@ -2142,7 +2142,7 @@
       <c r="AA9" s="33"/>
       <c r="AB9" s="34"/>
     </row>
-    <row r="10" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="35">
         <v>1</v>
       </c>
@@ -2197,7 +2197,7 @@
       </c>
       <c r="AB10" s="45"/>
     </row>
-    <row r="11" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="35">
         <v>2</v>
       </c>
@@ -2252,7 +2252,7 @@
       </c>
       <c r="AB11" s="48"/>
     </row>
-    <row r="12" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="35">
         <v>3</v>
       </c>
@@ -2306,7 +2306,7 @@
       </c>
       <c r="AB12" s="49"/>
     </row>
-    <row r="13" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="35">
         <v>4</v>
       </c>
@@ -2361,7 +2361,7 @@
       </c>
       <c r="AB13" s="48"/>
     </row>
-    <row r="14" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="35">
         <v>5</v>
       </c>
@@ -2416,7 +2416,7 @@
       </c>
       <c r="AB14" s="48"/>
     </row>
-    <row r="15" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35">
         <v>6</v>
       </c>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AB15" s="48"/>
     </row>
-    <row r="16" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="35">
         <v>7</v>
       </c>
@@ -2526,7 +2526,7 @@
       </c>
       <c r="AB16" s="48"/>
     </row>
-    <row r="17" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="35">
         <v>8</v>
       </c>
@@ -2581,7 +2581,7 @@
       </c>
       <c r="AB17" s="48"/>
     </row>
-    <row r="18" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="35">
         <v>9</v>
       </c>
@@ -2636,7 +2636,7 @@
       </c>
       <c r="AB18" s="48"/>
     </row>
-    <row r="19" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="35">
         <v>10</v>
       </c>
@@ -2691,7 +2691,7 @@
       </c>
       <c r="AB19" s="48"/>
     </row>
-    <row r="20" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="35">
         <v>11</v>
       </c>
@@ -2746,7 +2746,7 @@
       </c>
       <c r="AB20" s="48"/>
     </row>
-    <row r="21" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="35">
         <v>12</v>
       </c>
@@ -2801,7 +2801,7 @@
       </c>
       <c r="AB21" s="48"/>
     </row>
-    <row r="22" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="35">
         <v>13</v>
       </c>
@@ -2856,7 +2856,7 @@
       </c>
       <c r="AB22" s="48"/>
     </row>
-    <row r="23" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="35">
         <v>14</v>
       </c>
@@ -2911,7 +2911,7 @@
       </c>
       <c r="AB23" s="48"/>
     </row>
-    <row r="24" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="35">
         <v>15</v>
       </c>
@@ -2966,7 +2966,7 @@
       </c>
       <c r="AB24" s="48"/>
     </row>
-    <row r="25" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="35">
         <v>16</v>
       </c>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="AB25" s="48"/>
     </row>
-    <row r="26" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="35">
         <v>17</v>
       </c>
@@ -3076,7 +3076,7 @@
       </c>
       <c r="AB26" s="82"/>
     </row>
-    <row r="27" spans="1:28" s="85" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" s="85" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="35">
         <v>18</v>
       </c>
@@ -3131,7 +3131,7 @@
       </c>
       <c r="AB27" s="48"/>
     </row>
-    <row r="28" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="35">
         <v>19</v>
       </c>
@@ -3186,7 +3186,7 @@
       </c>
       <c r="AB28" s="48"/>
     </row>
-    <row r="29" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="35">
         <v>20</v>
       </c>
@@ -3241,7 +3241,7 @@
       </c>
       <c r="AB29" s="48"/>
     </row>
-    <row r="30" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="35">
         <v>21</v>
       </c>
@@ -3296,7 +3296,7 @@
       </c>
       <c r="AB30" s="48"/>
     </row>
-    <row r="31" spans="1:28" s="85" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" s="85" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="35">
         <v>22</v>
       </c>
@@ -3351,7 +3351,7 @@
       </c>
       <c r="AB31" s="48"/>
     </row>
-    <row r="32" spans="1:28" s="85" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" s="85" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="35">
         <v>23</v>
       </c>
@@ -3406,7 +3406,7 @@
       </c>
       <c r="AB32" s="48"/>
     </row>
-    <row r="33" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="35">
         <v>24</v>
       </c>
@@ -3461,7 +3461,7 @@
       </c>
       <c r="AB33" s="48"/>
     </row>
-    <row r="34" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="35">
         <v>25</v>
       </c>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="AB34" s="48"/>
     </row>
-    <row r="35" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="35">
         <v>27</v>
       </c>
@@ -3569,7 +3569,7 @@
       </c>
       <c r="AB35" s="48"/>
     </row>
-    <row r="36" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="35">
         <v>28</v>
       </c>
@@ -3622,7 +3622,7 @@
       </c>
       <c r="AB36" s="48"/>
     </row>
-    <row r="37" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="35">
         <v>29</v>
       </c>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="AB37" s="48"/>
     </row>
-    <row r="38" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:28" s="46" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="35">
         <v>30</v>
       </c>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="AB38" s="48"/>
     </row>
-    <row r="39" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="35">
         <v>31</v>
       </c>
@@ -3781,7 +3781,7 @@
       </c>
       <c r="AB39" s="48"/>
     </row>
-    <row r="40" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="35">
         <v>32</v>
       </c>
@@ -3834,7 +3834,7 @@
       </c>
       <c r="AB40" s="48"/>
     </row>
-    <row r="41" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="35">
         <v>33</v>
       </c>
@@ -3889,7 +3889,7 @@
       </c>
       <c r="AB41" s="48"/>
     </row>
-    <row r="42" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="35">
         <v>34</v>
       </c>
@@ -3942,7 +3942,7 @@
       </c>
       <c r="AB42" s="48"/>
     </row>
-    <row r="43" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="35">
         <v>35</v>
       </c>
@@ -3997,7 +3997,7 @@
       </c>
       <c r="AB43" s="48"/>
     </row>
-    <row r="44" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="35">
         <v>36</v>
       </c>
@@ -4052,7 +4052,7 @@
       </c>
       <c r="AB44" s="48"/>
     </row>
-    <row r="45" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="35">
         <v>37</v>
       </c>
@@ -4105,7 +4105,7 @@
       </c>
       <c r="AB45" s="48"/>
     </row>
-    <row r="46" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="35">
         <v>38</v>
       </c>
@@ -4119,7 +4119,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="37">
-        <v>3.5</v>
+        <v>6.5</v>
       </c>
       <c r="F46" s="37">
         <v>0</v>
@@ -4136,7 +4136,7 @@
       </c>
       <c r="J46" s="40">
         <f t="shared" si="1"/>
-        <v>3.5</v>
+        <v>6.5</v>
       </c>
       <c r="K46" s="79"/>
       <c r="L46" s="79"/>
@@ -4156,11 +4156,11 @@
       <c r="Z46" s="52"/>
       <c r="AA46" s="44">
         <f t="shared" si="2"/>
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
       <c r="AB46" s="48"/>
     </row>
-    <row r="47" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="35">
         <v>39</v>
       </c>
@@ -4212,7 +4212,7 @@
       <c r="AA47" s="121"/>
       <c r="AB47" s="82"/>
     </row>
-    <row r="48" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="35">
         <v>40</v>
       </c>
@@ -4247,7 +4247,7 @@
       <c r="AA48" s="121"/>
       <c r="AB48" s="82"/>
     </row>
-    <row r="49" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="35">
         <v>41</v>
       </c>
@@ -4282,7 +4282,7 @@
       <c r="AA49" s="121"/>
       <c r="AB49" s="82"/>
     </row>
-    <row r="50" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="35">
         <v>42</v>
       </c>
@@ -4317,7 +4317,7 @@
       <c r="AA50" s="121"/>
       <c r="AB50" s="82"/>
     </row>
-    <row r="51" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="35">
         <v>43</v>
       </c>
@@ -4352,7 +4352,7 @@
       <c r="AA51" s="121"/>
       <c r="AB51" s="82"/>
     </row>
-    <row r="52" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="35">
         <v>44</v>
       </c>
@@ -4387,7 +4387,7 @@
       <c r="AA52" s="121"/>
       <c r="AB52" s="82"/>
     </row>
-    <row r="53" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="35">
         <v>45</v>
       </c>
@@ -4422,7 +4422,7 @@
       <c r="AA53" s="121"/>
       <c r="AB53" s="82"/>
     </row>
-    <row r="54" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="35">
         <v>46</v>
       </c>
@@ -4457,7 +4457,7 @@
       <c r="AA54" s="121"/>
       <c r="AB54" s="82"/>
     </row>
-    <row r="55" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="35">
         <v>47</v>
       </c>
@@ -4492,7 +4492,7 @@
       <c r="AA55" s="121"/>
       <c r="AB55" s="82"/>
     </row>
-    <row r="56" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="35">
         <v>48</v>
       </c>
@@ -4527,7 +4527,7 @@
       <c r="AA56" s="121"/>
       <c r="AB56" s="82"/>
     </row>
-    <row r="57" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="35">
         <v>49</v>
       </c>
@@ -4562,7 +4562,7 @@
       <c r="AA57" s="121"/>
       <c r="AB57" s="82"/>
     </row>
-    <row r="58" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="35">
         <v>50</v>
       </c>
@@ -4597,7 +4597,7 @@
       <c r="AA58" s="121"/>
       <c r="AB58" s="82"/>
     </row>
-    <row r="59" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="35">
         <v>51</v>
       </c>
@@ -4632,7 +4632,7 @@
       <c r="AA59" s="121"/>
       <c r="AB59" s="82"/>
     </row>
-    <row r="60" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="35">
         <v>52</v>
       </c>
@@ -4670,7 +4670,7 @@
       </c>
       <c r="AB60" s="97"/>
     </row>
-    <row r="61" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="137" t="s">
         <v>61</v>
       </c>
@@ -4685,7 +4685,7 @@
       </c>
       <c r="E61" s="98">
         <f>SUM(E10:E60)</f>
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F61" s="98">
         <f>SUM(F10:F60)</f>
@@ -4696,7 +4696,7 @@
       <c r="I61" s="100"/>
       <c r="J61" s="98">
         <f t="shared" si="1"/>
-        <v>294.5</v>
+        <v>297.5</v>
       </c>
       <c r="K61" s="101"/>
       <c r="L61" s="101"/>
@@ -4716,11 +4716,11 @@
       <c r="Z61" s="101"/>
       <c r="AA61" s="98">
         <f>SUM(AA10:AA60)</f>
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AB61" s="102"/>
     </row>
-    <row r="62" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:28" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="138" t="s">
         <v>62</v>
       </c>
@@ -4735,7 +4735,7 @@
       </c>
       <c r="E62" s="98">
         <f>135-E61</f>
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F62" s="98">
         <f>135-F61</f>
@@ -4746,7 +4746,7 @@
       <c r="I62" s="98"/>
       <c r="J62" s="98">
         <f t="shared" si="1"/>
-        <v>245.5</v>
+        <v>242.5</v>
       </c>
       <c r="K62" s="101"/>
       <c r="L62" s="101"/>
@@ -4767,7 +4767,7 @@
       <c r="AA62" s="101"/>
       <c r="AB62" s="101"/>
     </row>
-    <row r="63" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:28" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="139" t="s">
         <v>63</v>
       </c>
@@ -4802,7 +4802,7 @@
       <c r="AA63" s="101"/>
       <c r="AB63" s="101"/>
     </row>
-    <row r="64" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:28" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="138" t="s">
         <v>64</v>
       </c>
@@ -4819,7 +4819,7 @@
       </c>
       <c r="J64" s="98">
         <f>SUM(J10:J60)</f>
-        <v>294.5</v>
+        <v>297.5</v>
       </c>
       <c r="K64" s="101"/>
       <c r="L64" s="101"/>
@@ -4840,7 +4840,7 @@
       <c r="AA64" s="101"/>
       <c r="AB64" s="101"/>
     </row>
-    <row r="65" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="105"/>
       <c r="B65" s="105"/>
       <c r="C65" s="106"/>
@@ -4870,7 +4870,7 @@
       <c r="AA65" s="101"/>
       <c r="AB65" s="101"/>
     </row>
-    <row r="66" spans="1:28" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:28" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="139" t="s">
         <v>65</v>
       </c>
@@ -4905,14 +4905,14 @@
       <c r="AA66" s="101"/>
       <c r="AB66" s="101"/>
     </row>
-    <row r="67" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="136" t="s">
         <v>66</v>
       </c>
       <c r="B67" s="136"/>
       <c r="C67" s="98">
         <f>C66-J64</f>
-        <v>245.5</v>
+        <v>242.5</v>
       </c>
       <c r="D67" s="106"/>
       <c r="E67" s="106"/>
@@ -4940,7 +4940,7 @@
       <c r="AA67" s="101"/>
       <c r="AB67" s="101"/>
     </row>
-    <row r="68" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="107"/>
       <c r="B68" s="105"/>
       <c r="C68" s="108"/>
@@ -4953,12 +4953,12 @@
       <c r="J68" s="110"/>
       <c r="AA68" s="101"/>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D69" s="111"/>
       <c r="E69" s="111"/>
       <c r="F69" s="111"/>
     </row>
-    <row r="70" spans="1:28" s="113" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:28" s="113" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="112"/>
       <c r="C70" s="114"/>
       <c r="D70" s="114"/>
@@ -4973,7 +4973,7 @@
       <c r="Z70" s="117"/>
       <c r="AA70" s="118"/>
     </row>
-    <row r="71" spans="1:28" s="113" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:28" s="113" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C71" s="114"/>
       <c r="D71" s="114"/>
       <c r="E71" s="114"/>
@@ -4987,7 +4987,7 @@
       <c r="Z71" s="117"/>
       <c r="AA71" s="118"/>
     </row>
-    <row r="72" spans="1:28" s="113" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:28" s="113" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C72" s="114"/>
       <c r="D72" s="114"/>
       <c r="E72" s="114"/>
@@ -5080,12 +5080,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="10.6640625" style="1"/>
+    <col min="1" max="1025" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="119" t="s">
         <v>6</v>
       </c>
@@ -5093,7 +5093,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -5101,7 +5101,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -5121,9 +5121,9 @@
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="10.6640625" style="1"/>
+    <col min="1" max="1025" width="10.7109375" style="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Added more hours for today
</commit_message>
<xml_diff>
--- a/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
+++ b/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abourdeau\source\repos\mrjrdg\marque-sans-nom\Semainiers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alxbo\Source\Repos\mrjrdg\marque-sans-nom\Semainiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D6E32C-DDC7-4076-9D1C-16DB44D2D3E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0BD590-7B98-4DA2-BD10-B26D60920ADF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1290,42 +1290,6 @@
     <xf numFmtId="166" fontId="20" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1335,6 +1299,42 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1809,51 +1809,51 @@
   </sheetPr>
   <dimension ref="A1:AMK72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A33" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="66.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="2" customWidth="1"/>
-    <col min="4" max="5" width="8.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="66.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="8.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" style="3" customWidth="1"/>
-    <col min="9" max="10" width="9.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" style="3" customWidth="1"/>
+    <col min="9" max="10" width="9.33203125" style="4" customWidth="1"/>
     <col min="11" max="13" width="8" style="1" customWidth="1"/>
     <col min="14" max="14" width="8" style="5" customWidth="1"/>
-    <col min="15" max="16" width="7.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.7109375" style="6" customWidth="1"/>
-    <col min="28" max="28" width="22.7109375" style="1" customWidth="1"/>
-    <col min="29" max="1025" width="10.7109375" style="1"/>
+    <col min="15" max="16" width="7.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="7.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.6640625" style="6" customWidth="1"/>
+    <col min="28" max="28" width="22.6640625" style="1" customWidth="1"/>
+    <col min="29" max="1025" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="8" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="124" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="124"/>
+    <row r="1" spans="1:28" s="8" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="137" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="137"/>
       <c r="C1" s="7"/>
-      <c r="D1" s="125" t="s">
+      <c r="D1" s="138" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="125"/>
-      <c r="I1" s="125"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
+      <c r="J1" s="138"/>
+      <c r="K1" s="138"/>
+      <c r="L1" s="138"/>
       <c r="N1" s="3"/>
       <c r="P1" s="9"/>
       <c r="Q1" s="8" t="s">
@@ -1864,21 +1864,21 @@
       <c r="Z1" s="3"/>
       <c r="AA1" s="10"/>
     </row>
-    <row r="2" spans="1:28" s="8" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="124" t="s">
+    <row r="2" spans="1:28" s="8" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="137" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="124"/>
+      <c r="B2" s="137"/>
       <c r="C2" s="7"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="124" t="s">
+      <c r="F2" s="137" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="124"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="124"/>
+      <c r="G2" s="137"/>
+      <c r="H2" s="137"/>
+      <c r="I2" s="137"/>
+      <c r="J2" s="137"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
       <c r="N2" s="3"/>
@@ -1891,7 +1891,7 @@
       <c r="Z2" s="3"/>
       <c r="AA2" s="10"/>
     </row>
-    <row r="3" spans="1:28" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -1909,7 +1909,7 @@
       <c r="Z3" s="3"/>
       <c r="AA3" s="10"/>
     </row>
-    <row r="4" spans="1:28" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
@@ -1929,7 +1929,7 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="10"/>
     </row>
-    <row r="5" spans="1:28" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
@@ -1953,7 +1953,7 @@
       </c>
       <c r="AA5" s="10"/>
     </row>
-    <row r="6" spans="1:28" s="8" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" s="8" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
@@ -1961,73 +1961,73 @@
       <c r="H6" s="3"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="126" t="s">
+      <c r="K6" s="139" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="126"/>
-      <c r="M6" s="126"/>
-      <c r="N6" s="126"/>
-      <c r="O6" s="126"/>
-      <c r="P6" s="126"/>
-      <c r="Q6" s="126"/>
-      <c r="R6" s="126"/>
+      <c r="L6" s="139"/>
+      <c r="M6" s="139"/>
+      <c r="N6" s="139"/>
+      <c r="O6" s="139"/>
+      <c r="P6" s="139"/>
+      <c r="Q6" s="139"/>
+      <c r="R6" s="139"/>
       <c r="V6" s="17"/>
       <c r="Z6" s="17"/>
       <c r="AA6" s="10"/>
     </row>
-    <row r="7" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="127" t="s">
+    <row r="7" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="128" t="s">
+      <c r="B7" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="129" t="s">
+      <c r="C7" s="134" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="129"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="129"/>
-      <c r="G7" s="130" t="s">
+      <c r="D7" s="134"/>
+      <c r="E7" s="134"/>
+      <c r="F7" s="134"/>
+      <c r="G7" s="135" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="131" t="s">
+      <c r="H7" s="136" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="132" t="s">
+      <c r="I7" s="128" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="132" t="s">
+      <c r="J7" s="128" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="133" t="s">
+      <c r="K7" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="133"/>
-      <c r="M7" s="133"/>
-      <c r="N7" s="133"/>
-      <c r="O7" s="133"/>
-      <c r="P7" s="133"/>
-      <c r="Q7" s="133"/>
-      <c r="R7" s="133"/>
-      <c r="S7" s="133"/>
-      <c r="T7" s="133"/>
-      <c r="U7" s="133"/>
-      <c r="V7" s="133"/>
-      <c r="W7" s="133"/>
-      <c r="X7" s="133"/>
-      <c r="Y7" s="133"/>
-      <c r="Z7" s="133"/>
-      <c r="AA7" s="134" t="s">
+      <c r="L7" s="129"/>
+      <c r="M7" s="129"/>
+      <c r="N7" s="129"/>
+      <c r="O7" s="129"/>
+      <c r="P7" s="129"/>
+      <c r="Q7" s="129"/>
+      <c r="R7" s="129"/>
+      <c r="S7" s="129"/>
+      <c r="T7" s="129"/>
+      <c r="U7" s="129"/>
+      <c r="V7" s="129"/>
+      <c r="W7" s="129"/>
+      <c r="X7" s="129"/>
+      <c r="Y7" s="129"/>
+      <c r="Z7" s="129"/>
+      <c r="AA7" s="130" t="s">
         <v>18</v>
       </c>
-      <c r="AB7" s="135" t="s">
+      <c r="AB7" s="131" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="127"/>
-      <c r="B8" s="128"/>
+    <row r="8" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="132"/>
+      <c r="B8" s="133"/>
       <c r="C8" s="20" t="s">
         <v>20</v>
       </c>
@@ -2040,10 +2040,10 @@
       <c r="F8" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="130"/>
-      <c r="H8" s="131"/>
-      <c r="I8" s="132"/>
-      <c r="J8" s="132"/>
+      <c r="G8" s="135"/>
+      <c r="H8" s="136"/>
+      <c r="I8" s="128"/>
+      <c r="J8" s="128"/>
       <c r="K8" s="21">
         <v>43838</v>
       </c>
@@ -2107,10 +2107,10 @@
         <f t="shared" si="0"/>
         <v>43943</v>
       </c>
-      <c r="AA8" s="134"/>
-      <c r="AB8" s="135"/>
-    </row>
-    <row r="9" spans="1:28" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="AA8" s="130"/>
+      <c r="AB8" s="131"/>
+    </row>
+    <row r="9" spans="1:28" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>24</v>
@@ -2142,7 +2142,7 @@
       <c r="AA9" s="33"/>
       <c r="AB9" s="34"/>
     </row>
-    <row r="10" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="35">
         <v>1</v>
       </c>
@@ -2197,7 +2197,7 @@
       </c>
       <c r="AB10" s="45"/>
     </row>
-    <row r="11" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="35">
         <v>2</v>
       </c>
@@ -2252,7 +2252,7 @@
       </c>
       <c r="AB11" s="48"/>
     </row>
-    <row r="12" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="35">
         <v>3</v>
       </c>
@@ -2306,7 +2306,7 @@
       </c>
       <c r="AB12" s="49"/>
     </row>
-    <row r="13" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="35">
         <v>4</v>
       </c>
@@ -2361,7 +2361,7 @@
       </c>
       <c r="AB13" s="48"/>
     </row>
-    <row r="14" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="35">
         <v>5</v>
       </c>
@@ -2416,7 +2416,7 @@
       </c>
       <c r="AB14" s="48"/>
     </row>
-    <row r="15" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="35">
         <v>6</v>
       </c>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AB15" s="48"/>
     </row>
-    <row r="16" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="35">
         <v>7</v>
       </c>
@@ -2526,7 +2526,7 @@
       </c>
       <c r="AB16" s="48"/>
     </row>
-    <row r="17" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="35">
         <v>8</v>
       </c>
@@ -2581,7 +2581,7 @@
       </c>
       <c r="AB17" s="48"/>
     </row>
-    <row r="18" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="35">
         <v>9</v>
       </c>
@@ -2636,7 +2636,7 @@
       </c>
       <c r="AB18" s="48"/>
     </row>
-    <row r="19" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="35">
         <v>10</v>
       </c>
@@ -2691,7 +2691,7 @@
       </c>
       <c r="AB19" s="48"/>
     </row>
-    <row r="20" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="35">
         <v>11</v>
       </c>
@@ -2746,7 +2746,7 @@
       </c>
       <c r="AB20" s="48"/>
     </row>
-    <row r="21" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="35">
         <v>12</v>
       </c>
@@ -2801,7 +2801,7 @@
       </c>
       <c r="AB21" s="48"/>
     </row>
-    <row r="22" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="35">
         <v>13</v>
       </c>
@@ -2856,7 +2856,7 @@
       </c>
       <c r="AB22" s="48"/>
     </row>
-    <row r="23" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="35">
         <v>14</v>
       </c>
@@ -2911,7 +2911,7 @@
       </c>
       <c r="AB23" s="48"/>
     </row>
-    <row r="24" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="35">
         <v>15</v>
       </c>
@@ -2966,7 +2966,7 @@
       </c>
       <c r="AB24" s="48"/>
     </row>
-    <row r="25" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="35">
         <v>16</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>10</v>
       </c>
       <c r="E25" s="37">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="F25" s="37">
         <v>15</v>
@@ -2997,7 +2997,7 @@
       </c>
       <c r="J25" s="40">
         <f t="shared" si="1"/>
-        <v>37</v>
+        <v>38.5</v>
       </c>
       <c r="K25" s="68"/>
       <c r="L25" s="60"/>
@@ -3017,11 +3017,11 @@
       <c r="Z25" s="43"/>
       <c r="AA25" s="44">
         <f t="shared" si="2"/>
-        <v>-7</v>
+        <v>-8.5</v>
       </c>
       <c r="AB25" s="48"/>
     </row>
-    <row r="26" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="35">
         <v>17</v>
       </c>
@@ -3076,7 +3076,7 @@
       </c>
       <c r="AB26" s="82"/>
     </row>
-    <row r="27" spans="1:28" s="85" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" s="85" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="35">
         <v>18</v>
       </c>
@@ -3131,7 +3131,7 @@
       </c>
       <c r="AB27" s="48"/>
     </row>
-    <row r="28" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="35">
         <v>19</v>
       </c>
@@ -3186,7 +3186,7 @@
       </c>
       <c r="AB28" s="48"/>
     </row>
-    <row r="29" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="35">
         <v>20</v>
       </c>
@@ -3241,7 +3241,7 @@
       </c>
       <c r="AB29" s="48"/>
     </row>
-    <row r="30" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="35">
         <v>21</v>
       </c>
@@ -3296,7 +3296,7 @@
       </c>
       <c r="AB30" s="48"/>
     </row>
-    <row r="31" spans="1:28" s="85" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" s="85" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="35">
         <v>22</v>
       </c>
@@ -3351,7 +3351,7 @@
       </c>
       <c r="AB31" s="48"/>
     </row>
-    <row r="32" spans="1:28" s="85" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" s="85" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="35">
         <v>23</v>
       </c>
@@ -3406,7 +3406,7 @@
       </c>
       <c r="AB32" s="48"/>
     </row>
-    <row r="33" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="35">
         <v>24</v>
       </c>
@@ -3461,7 +3461,7 @@
       </c>
       <c r="AB33" s="48"/>
     </row>
-    <row r="34" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="35">
         <v>25</v>
       </c>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="AB34" s="48"/>
     </row>
-    <row r="35" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="35">
         <v>27</v>
       </c>
@@ -3569,7 +3569,7 @@
       </c>
       <c r="AB35" s="48"/>
     </row>
-    <row r="36" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="35">
         <v>28</v>
       </c>
@@ -3622,7 +3622,7 @@
       </c>
       <c r="AB36" s="48"/>
     </row>
-    <row r="37" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="35">
         <v>29</v>
       </c>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="AB37" s="48"/>
     </row>
-    <row r="38" spans="1:28" s="46" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="35">
         <v>30</v>
       </c>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="AB38" s="48"/>
     </row>
-    <row r="39" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="35">
         <v>31</v>
       </c>
@@ -3781,7 +3781,7 @@
       </c>
       <c r="AB39" s="48"/>
     </row>
-    <row r="40" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="35">
         <v>32</v>
       </c>
@@ -3834,7 +3834,7 @@
       </c>
       <c r="AB40" s="48"/>
     </row>
-    <row r="41" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="35">
         <v>33</v>
       </c>
@@ -3889,7 +3889,7 @@
       </c>
       <c r="AB41" s="48"/>
     </row>
-    <row r="42" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="35">
         <v>34</v>
       </c>
@@ -3942,7 +3942,7 @@
       </c>
       <c r="AB42" s="48"/>
     </row>
-    <row r="43" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="35">
         <v>35</v>
       </c>
@@ -3997,7 +3997,7 @@
       </c>
       <c r="AB43" s="48"/>
     </row>
-    <row r="44" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="35">
         <v>36</v>
       </c>
@@ -4052,7 +4052,7 @@
       </c>
       <c r="AB44" s="48"/>
     </row>
-    <row r="45" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="35">
         <v>37</v>
       </c>
@@ -4105,7 +4105,7 @@
       </c>
       <c r="AB45" s="48"/>
     </row>
-    <row r="46" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="35">
         <v>38</v>
       </c>
@@ -4160,7 +4160,7 @@
       </c>
       <c r="AB46" s="48"/>
     </row>
-    <row r="47" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="35">
         <v>39</v>
       </c>
@@ -4212,7 +4212,7 @@
       <c r="AA47" s="121"/>
       <c r="AB47" s="82"/>
     </row>
-    <row r="48" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="35">
         <v>40</v>
       </c>
@@ -4247,7 +4247,7 @@
       <c r="AA48" s="121"/>
       <c r="AB48" s="82"/>
     </row>
-    <row r="49" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="35">
         <v>41</v>
       </c>
@@ -4282,7 +4282,7 @@
       <c r="AA49" s="121"/>
       <c r="AB49" s="82"/>
     </row>
-    <row r="50" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="35">
         <v>42</v>
       </c>
@@ -4317,7 +4317,7 @@
       <c r="AA50" s="121"/>
       <c r="AB50" s="82"/>
     </row>
-    <row r="51" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="35">
         <v>43</v>
       </c>
@@ -4352,7 +4352,7 @@
       <c r="AA51" s="121"/>
       <c r="AB51" s="82"/>
     </row>
-    <row r="52" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="35">
         <v>44</v>
       </c>
@@ -4387,7 +4387,7 @@
       <c r="AA52" s="121"/>
       <c r="AB52" s="82"/>
     </row>
-    <row r="53" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="35">
         <v>45</v>
       </c>
@@ -4422,7 +4422,7 @@
       <c r="AA53" s="121"/>
       <c r="AB53" s="82"/>
     </row>
-    <row r="54" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="35">
         <v>46</v>
       </c>
@@ -4457,7 +4457,7 @@
       <c r="AA54" s="121"/>
       <c r="AB54" s="82"/>
     </row>
-    <row r="55" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="35">
         <v>47</v>
       </c>
@@ -4492,7 +4492,7 @@
       <c r="AA55" s="121"/>
       <c r="AB55" s="82"/>
     </row>
-    <row r="56" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="35">
         <v>48</v>
       </c>
@@ -4527,7 +4527,7 @@
       <c r="AA56" s="121"/>
       <c r="AB56" s="82"/>
     </row>
-    <row r="57" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="35">
         <v>49</v>
       </c>
@@ -4562,7 +4562,7 @@
       <c r="AA57" s="121"/>
       <c r="AB57" s="82"/>
     </row>
-    <row r="58" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="35">
         <v>50</v>
       </c>
@@ -4597,7 +4597,7 @@
       <c r="AA58" s="121"/>
       <c r="AB58" s="82"/>
     </row>
-    <row r="59" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="35">
         <v>51</v>
       </c>
@@ -4632,7 +4632,7 @@
       <c r="AA59" s="121"/>
       <c r="AB59" s="82"/>
     </row>
-    <row r="60" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="35">
         <v>52</v>
       </c>
@@ -4670,11 +4670,11 @@
       </c>
       <c r="AB60" s="97"/>
     </row>
-    <row r="61" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="137" t="s">
+    <row r="61" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="125" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="137"/>
+      <c r="B61" s="125"/>
       <c r="C61" s="98">
         <f>SUM(C10:C60)</f>
         <v>74.5</v>
@@ -4685,7 +4685,7 @@
       </c>
       <c r="E61" s="98">
         <f>SUM(E10:E60)</f>
-        <v>68</v>
+        <v>69.5</v>
       </c>
       <c r="F61" s="98">
         <f>SUM(F10:F60)</f>
@@ -4696,7 +4696,7 @@
       <c r="I61" s="100"/>
       <c r="J61" s="98">
         <f t="shared" si="1"/>
-        <v>297.5</v>
+        <v>299</v>
       </c>
       <c r="K61" s="101"/>
       <c r="L61" s="101"/>
@@ -4716,15 +4716,15 @@
       <c r="Z61" s="101"/>
       <c r="AA61" s="98">
         <f>SUM(AA10:AA60)</f>
-        <v>17</v>
+        <v>15.5</v>
       </c>
       <c r="AB61" s="102"/>
     </row>
-    <row r="62" spans="1:28" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="138" t="s">
+    <row r="62" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="126" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="138"/>
+      <c r="B62" s="126"/>
       <c r="C62" s="98">
         <f>135-C61</f>
         <v>60.5</v>
@@ -4735,7 +4735,7 @@
       </c>
       <c r="E62" s="98">
         <f>135-E61</f>
-        <v>67</v>
+        <v>65.5</v>
       </c>
       <c r="F62" s="98">
         <f>135-F61</f>
@@ -4746,7 +4746,7 @@
       <c r="I62" s="98"/>
       <c r="J62" s="98">
         <f t="shared" si="1"/>
-        <v>242.5</v>
+        <v>241</v>
       </c>
       <c r="K62" s="101"/>
       <c r="L62" s="101"/>
@@ -4767,11 +4767,11 @@
       <c r="AA62" s="101"/>
       <c r="AB62" s="101"/>
     </row>
-    <row r="63" spans="1:28" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="139" t="s">
+    <row r="63" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="127" t="s">
         <v>63</v>
       </c>
-      <c r="B63" s="139"/>
+      <c r="B63" s="127"/>
       <c r="C63" s="98"/>
       <c r="D63" s="98"/>
       <c r="E63" s="98"/>
@@ -4802,11 +4802,11 @@
       <c r="AA63" s="101"/>
       <c r="AB63" s="101"/>
     </row>
-    <row r="64" spans="1:28" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="138" t="s">
+    <row r="64" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="126" t="s">
         <v>64</v>
       </c>
-      <c r="B64" s="138"/>
+      <c r="B64" s="126"/>
       <c r="C64" s="98"/>
       <c r="D64" s="98"/>
       <c r="E64" s="103"/>
@@ -4819,7 +4819,7 @@
       </c>
       <c r="J64" s="98">
         <f>SUM(J10:J60)</f>
-        <v>297.5</v>
+        <v>299</v>
       </c>
       <c r="K64" s="101"/>
       <c r="L64" s="101"/>
@@ -4840,7 +4840,7 @@
       <c r="AA64" s="101"/>
       <c r="AB64" s="101"/>
     </row>
-    <row r="65" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="105"/>
       <c r="B65" s="105"/>
       <c r="C65" s="106"/>
@@ -4870,11 +4870,11 @@
       <c r="AA65" s="101"/>
       <c r="AB65" s="101"/>
     </row>
-    <row r="66" spans="1:28" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="139" t="s">
+    <row r="66" spans="1:28" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="127" t="s">
         <v>65</v>
       </c>
-      <c r="B66" s="139"/>
+      <c r="B66" s="127"/>
       <c r="C66" s="98">
         <f>135*4</f>
         <v>540</v>
@@ -4905,14 +4905,14 @@
       <c r="AA66" s="101"/>
       <c r="AB66" s="101"/>
     </row>
-    <row r="67" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="136" t="s">
+    <row r="67" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="124" t="s">
         <v>66</v>
       </c>
-      <c r="B67" s="136"/>
+      <c r="B67" s="124"/>
       <c r="C67" s="98">
         <f>C66-J64</f>
-        <v>242.5</v>
+        <v>241</v>
       </c>
       <c r="D67" s="106"/>
       <c r="E67" s="106"/>
@@ -4940,7 +4940,7 @@
       <c r="AA67" s="101"/>
       <c r="AB67" s="101"/>
     </row>
-    <row r="68" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="107"/>
       <c r="B68" s="105"/>
       <c r="C68" s="108"/>
@@ -4953,12 +4953,12 @@
       <c r="J68" s="110"/>
       <c r="AA68" s="101"/>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D69" s="111"/>
       <c r="E69" s="111"/>
       <c r="F69" s="111"/>
     </row>
-    <row r="70" spans="1:28" s="113" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:28" s="113" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A70" s="112"/>
       <c r="C70" s="114"/>
       <c r="D70" s="114"/>
@@ -4973,7 +4973,7 @@
       <c r="Z70" s="117"/>
       <c r="AA70" s="118"/>
     </row>
-    <row r="71" spans="1:28" s="113" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:28" s="113" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="C71" s="114"/>
       <c r="D71" s="114"/>
       <c r="E71" s="114"/>
@@ -4987,7 +4987,7 @@
       <c r="Z71" s="117"/>
       <c r="AA71" s="118"/>
     </row>
-    <row r="72" spans="1:28" s="113" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:28" s="113" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="C72" s="114"/>
       <c r="D72" s="114"/>
       <c r="E72" s="114"/>
@@ -5003,27 +5003,27 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:Z7"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
     <mergeCell ref="A67:B67"/>
     <mergeCell ref="A61:B61"/>
     <mergeCell ref="A62:B62"/>
     <mergeCell ref="A63:B63"/>
     <mergeCell ref="A64:B64"/>
     <mergeCell ref="A66:B66"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:Z7"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K6:R6"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
     <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="En cours">
@@ -5080,12 +5080,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1025" width="10.7109375" style="1"/>
+    <col min="1" max="1025" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="119" t="s">
         <v>6</v>
       </c>
@@ -5093,7 +5093,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -5101,7 +5101,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -5121,9 +5121,9 @@
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1025" width="10.7109375" style="1"/>
+    <col min="1" max="1025" width="10.6640625" style="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
ajout des heures Alex.d
</commit_message>
<xml_diff>
--- a/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
+++ b/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abourdeau\source\repos\mrjrdg\marque-sans-nom\Semainiers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Desktop/marque-sans-nom/Semainiers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F0580F-F029-4162-B85E-A9F0D0B1B540}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4D3CC7-15B0-B442-93A0-DE1E3A7477A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="76">
   <si>
     <t>UQÀM - Hiver 2020</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>Commentaires</t>
-  </si>
-  <si>
-    <t>Alex</t>
   </si>
   <si>
     <t>Philippe</t>
@@ -305,6 +302,30 @@
   </si>
   <si>
     <t>Réunion 2019-02-24</t>
+  </si>
+  <si>
+    <t>DEUXIEME SPRINT</t>
+  </si>
+  <si>
+    <t>Pages administration et gestion par GUI</t>
+  </si>
+  <si>
+    <t>Pages gestion d'entreprises (Create,Edit)</t>
+  </si>
+  <si>
+    <t>Pages gestion d'evenement (Create,Edit,Delete)</t>
+  </si>
+  <si>
+    <t>Messageries entre utilisateur</t>
+  </si>
+  <si>
+    <t>Babillards de commentaires</t>
+  </si>
+  <si>
+    <t>Alex . D</t>
+  </si>
+  <si>
+    <t>Page Contact</t>
   </si>
 </sst>
 </file>
@@ -515,7 +536,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -914,6 +935,17 @@
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -928,7 +960,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1136,17 +1168,6 @@
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="3" borderId="16" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="4" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="167" fontId="15" fillId="0" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -1209,13 +1230,7 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="7" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="8" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="7" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="167" fontId="14" fillId="0" borderId="8" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
@@ -1276,9 +1291,6 @@
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="5" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1286,42 +1298,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="166" fontId="20" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
@@ -1334,19 +1310,281 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="5" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="5" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="5" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="7" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Excel Built-in 60% - Accent4" xfId="7" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Excel Built-in Bad" xfId="6" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Excel Built-in Good" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Excel Built-in Good 1" xfId="8" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Excel Built-in Neutral" xfId="5" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Excel Built-in Normal" xfId="3" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Milliers" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="29">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1506,7 +1744,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1807,51 +2045,51 @@
   </sheetPr>
   <dimension ref="A1:AMK72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="66.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="2" customWidth="1"/>
-    <col min="4" max="5" width="8.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="66.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="8.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" style="3" customWidth="1"/>
-    <col min="9" max="10" width="9.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="3" customWidth="1"/>
+    <col min="9" max="10" width="9.33203125" style="4" customWidth="1"/>
     <col min="11" max="13" width="8" style="1" customWidth="1"/>
     <col min="14" max="14" width="8" style="5" customWidth="1"/>
-    <col min="15" max="16" width="7.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.7109375" style="6" customWidth="1"/>
-    <col min="28" max="28" width="22.7109375" style="1" customWidth="1"/>
-    <col min="29" max="1025" width="10.7109375" style="1"/>
+    <col min="15" max="16" width="7.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="7.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.6640625" style="6" customWidth="1"/>
+    <col min="28" max="28" width="22.6640625" style="1" customWidth="1"/>
+    <col min="29" max="1025" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="8" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="124" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="124"/>
+    <row r="1" spans="1:28" s="8" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="131" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="131"/>
       <c r="C1" s="7"/>
-      <c r="D1" s="125" t="s">
+      <c r="D1" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="125"/>
-      <c r="I1" s="125"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
+      <c r="H1" s="132"/>
+      <c r="I1" s="132"/>
+      <c r="J1" s="132"/>
+      <c r="K1" s="132"/>
+      <c r="L1" s="132"/>
       <c r="N1" s="3"/>
       <c r="P1" s="9"/>
       <c r="Q1" s="8" t="s">
@@ -1862,21 +2100,21 @@
       <c r="Z1" s="3"/>
       <c r="AA1" s="10"/>
     </row>
-    <row r="2" spans="1:28" s="8" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="124" t="s">
+    <row r="2" spans="1:28" s="8" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="124"/>
+      <c r="B2" s="131"/>
       <c r="C2" s="7"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="124" t="s">
+      <c r="F2" s="131" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="124"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="124"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="131"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
       <c r="N2" s="3"/>
@@ -1889,7 +2127,7 @@
       <c r="Z2" s="3"/>
       <c r="AA2" s="10"/>
     </row>
-    <row r="3" spans="1:28" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -1907,7 +2145,7 @@
       <c r="Z3" s="3"/>
       <c r="AA3" s="10"/>
     </row>
-    <row r="4" spans="1:28" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
@@ -1927,7 +2165,7 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="10"/>
     </row>
-    <row r="5" spans="1:28" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
@@ -1951,7 +2189,7 @@
       </c>
       <c r="AA5" s="10"/>
     </row>
-    <row r="6" spans="1:28" s="8" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" s="8" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
@@ -1959,89 +2197,89 @@
       <c r="H6" s="3"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="126" t="s">
+      <c r="K6" s="133" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="126"/>
-      <c r="M6" s="126"/>
-      <c r="N6" s="126"/>
-      <c r="O6" s="126"/>
-      <c r="P6" s="126"/>
-      <c r="Q6" s="126"/>
-      <c r="R6" s="126"/>
+      <c r="L6" s="133"/>
+      <c r="M6" s="133"/>
+      <c r="N6" s="133"/>
+      <c r="O6" s="133"/>
+      <c r="P6" s="133"/>
+      <c r="Q6" s="133"/>
+      <c r="R6" s="133"/>
       <c r="V6" s="17"/>
       <c r="Z6" s="17"/>
       <c r="AA6" s="10"/>
     </row>
-    <row r="7" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="127" t="s">
+    <row r="7" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="128" t="s">
+      <c r="B7" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="129" t="s">
+      <c r="C7" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="129"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="129"/>
-      <c r="G7" s="130" t="s">
+      <c r="D7" s="128"/>
+      <c r="E7" s="128"/>
+      <c r="F7" s="128"/>
+      <c r="G7" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="131" t="s">
+      <c r="H7" s="130" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="132" t="s">
+      <c r="I7" s="122" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="132" t="s">
+      <c r="J7" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="133" t="s">
+      <c r="K7" s="123" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="133"/>
-      <c r="M7" s="133"/>
-      <c r="N7" s="133"/>
-      <c r="O7" s="133"/>
-      <c r="P7" s="133"/>
-      <c r="Q7" s="133"/>
-      <c r="R7" s="133"/>
-      <c r="S7" s="133"/>
-      <c r="T7" s="133"/>
-      <c r="U7" s="133"/>
-      <c r="V7" s="133"/>
-      <c r="W7" s="133"/>
-      <c r="X7" s="133"/>
-      <c r="Y7" s="133"/>
-      <c r="Z7" s="133"/>
-      <c r="AA7" s="134" t="s">
+      <c r="L7" s="123"/>
+      <c r="M7" s="123"/>
+      <c r="N7" s="123"/>
+      <c r="O7" s="123"/>
+      <c r="P7" s="123"/>
+      <c r="Q7" s="123"/>
+      <c r="R7" s="123"/>
+      <c r="S7" s="123"/>
+      <c r="T7" s="123"/>
+      <c r="U7" s="123"/>
+      <c r="V7" s="123"/>
+      <c r="W7" s="123"/>
+      <c r="X7" s="123"/>
+      <c r="Y7" s="123"/>
+      <c r="Z7" s="123"/>
+      <c r="AA7" s="124" t="s">
         <v>18</v>
       </c>
-      <c r="AB7" s="135" t="s">
+      <c r="AB7" s="125" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="127"/>
-      <c r="B8" s="128"/>
+    <row r="8" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="126"/>
+      <c r="B8" s="127"/>
       <c r="C8" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="E8" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="F8" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="130"/>
-      <c r="H8" s="131"/>
-      <c r="I8" s="132"/>
-      <c r="J8" s="132"/>
+      <c r="G8" s="129"/>
+      <c r="H8" s="130"/>
+      <c r="I8" s="122"/>
+      <c r="J8" s="122"/>
       <c r="K8" s="21">
         <v>43838</v>
       </c>
@@ -2069,49 +2307,49 @@
         <f t="shared" si="0"/>
         <v>43880</v>
       </c>
-      <c r="R8" s="123">
+      <c r="R8" s="117">
         <f t="shared" si="0"/>
         <v>43887</v>
       </c>
-      <c r="S8" s="123">
+      <c r="S8" s="117">
         <f t="shared" si="0"/>
         <v>43894</v>
       </c>
-      <c r="T8" s="123">
+      <c r="T8" s="117">
         <f t="shared" si="0"/>
         <v>43901</v>
       </c>
-      <c r="U8" s="123">
+      <c r="U8" s="117">
         <f t="shared" si="0"/>
         <v>43908</v>
       </c>
-      <c r="V8" s="123">
+      <c r="V8" s="117">
         <f t="shared" si="0"/>
         <v>43915</v>
       </c>
-      <c r="W8" s="123">
+      <c r="W8" s="117">
         <f t="shared" si="0"/>
         <v>43922</v>
       </c>
-      <c r="X8" s="123">
+      <c r="X8" s="117">
         <f t="shared" si="0"/>
         <v>43929</v>
       </c>
-      <c r="Y8" s="123">
+      <c r="Y8" s="117">
         <f t="shared" si="0"/>
         <v>43936</v>
       </c>
-      <c r="Z8" s="123">
+      <c r="Z8" s="117">
         <f t="shared" si="0"/>
         <v>43943</v>
       </c>
-      <c r="AA8" s="134"/>
-      <c r="AB8" s="135"/>
-    </row>
-    <row r="9" spans="1:28" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="AA8" s="124"/>
+      <c r="AB8" s="125"/>
+    </row>
+    <row r="9" spans="1:28" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="25"/>
@@ -2140,12 +2378,12 @@
       <c r="AA9" s="33"/>
       <c r="AB9" s="34"/>
     </row>
-    <row r="10" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="35">
         <v>1</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="37">
         <v>1.5</v>
@@ -2195,12 +2433,12 @@
       </c>
       <c r="AB10" s="45"/>
     </row>
-    <row r="11" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="35">
         <v>2</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="37">
         <v>1.5</v>
@@ -2250,12 +2488,12 @@
       </c>
       <c r="AB11" s="48"/>
     </row>
-    <row r="12" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="35">
         <v>3</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="37">
         <v>3</v>
@@ -2304,12 +2542,12 @@
       </c>
       <c r="AB12" s="49"/>
     </row>
-    <row r="13" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="35">
         <v>4</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="37">
         <v>2</v>
@@ -2359,12 +2597,12 @@
       </c>
       <c r="AB13" s="48"/>
     </row>
-    <row r="14" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="35">
         <v>5</v>
       </c>
       <c r="B14" s="50" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="37">
         <v>3</v>
@@ -2414,12 +2652,12 @@
       </c>
       <c r="AB14" s="48"/>
     </row>
-    <row r="15" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="35">
         <v>6</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="37">
         <v>2</v>
@@ -2469,12 +2707,12 @@
       </c>
       <c r="AB15" s="48"/>
     </row>
-    <row r="16" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="35">
         <v>7</v>
       </c>
       <c r="B16" s="50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="37">
         <v>2</v>
@@ -2524,12 +2762,12 @@
       </c>
       <c r="AB16" s="48"/>
     </row>
-    <row r="17" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="35">
         <v>8</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="37">
         <v>2</v>
@@ -2579,12 +2817,12 @@
       </c>
       <c r="AB17" s="48"/>
     </row>
-    <row r="18" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="35">
         <v>9</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="37">
         <v>2</v>
@@ -2634,12 +2872,12 @@
       </c>
       <c r="AB18" s="48"/>
     </row>
-    <row r="19" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="35">
         <v>10</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="37">
         <v>1.5</v>
@@ -2689,12 +2927,12 @@
       </c>
       <c r="AB19" s="48"/>
     </row>
-    <row r="20" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="35">
         <v>11</v>
       </c>
       <c r="B20" s="50" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="37">
         <v>0</v>
@@ -2744,12 +2982,12 @@
       </c>
       <c r="AB20" s="48"/>
     </row>
-    <row r="21" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="35">
         <v>12</v>
       </c>
       <c r="B21" s="50" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="37">
         <v>3</v>
@@ -2799,12 +3037,12 @@
       </c>
       <c r="AB21" s="48"/>
     </row>
-    <row r="22" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="35">
         <v>13</v>
       </c>
       <c r="B22" s="67" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="37">
         <v>3</v>
@@ -2854,12 +3092,12 @@
       </c>
       <c r="AB22" s="48"/>
     </row>
-    <row r="23" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="35">
         <v>14</v>
       </c>
       <c r="B23" s="67" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="37">
         <v>0</v>
@@ -2875,10 +3113,10 @@
       </c>
       <c r="G23" s="38">
         <f>VLOOKUP(H23,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H23" s="39" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I23" s="40">
         <v>20</v>
@@ -2889,12 +3127,12 @@
       </c>
       <c r="K23" s="68"/>
       <c r="L23" s="60"/>
-      <c r="M23" s="70"/>
-      <c r="N23" s="71"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="41"/>
       <c r="O23" s="68"/>
       <c r="P23" s="68"/>
       <c r="Q23" s="69"/>
-      <c r="R23" s="65"/>
+      <c r="R23" s="56"/>
       <c r="S23" s="66"/>
       <c r="T23" s="66"/>
       <c r="U23" s="57"/>
@@ -2909,12 +3147,12 @@
       </c>
       <c r="AB23" s="48"/>
     </row>
-    <row r="24" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="35">
         <v>15</v>
       </c>
       <c r="B24" s="67" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C24" s="37">
         <v>1</v>
@@ -2944,12 +3182,12 @@
       </c>
       <c r="K24" s="68"/>
       <c r="L24" s="60"/>
-      <c r="M24" s="70"/>
-      <c r="N24" s="71"/>
-      <c r="O24" s="71"/>
-      <c r="P24" s="72"/>
-      <c r="Q24" s="71"/>
-      <c r="R24" s="73"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
+      <c r="O24" s="41"/>
+      <c r="P24" s="41"/>
+      <c r="Q24" s="41"/>
+      <c r="R24" s="70"/>
       <c r="S24" s="55"/>
       <c r="T24" s="55"/>
       <c r="U24" s="57"/>
@@ -2964,12 +3202,12 @@
       </c>
       <c r="AB24" s="48"/>
     </row>
-    <row r="25" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="35">
         <v>16</v>
       </c>
       <c r="B25" s="67" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" s="37">
         <v>10</v>
@@ -2999,12 +3237,12 @@
       </c>
       <c r="K25" s="68"/>
       <c r="L25" s="60"/>
-      <c r="M25" s="70"/>
-      <c r="N25" s="71"/>
-      <c r="O25" s="71"/>
-      <c r="P25" s="74"/>
-      <c r="Q25" s="71"/>
-      <c r="R25" s="71"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="41"/>
+      <c r="P25" s="71"/>
+      <c r="Q25" s="41"/>
+      <c r="R25" s="134"/>
       <c r="S25" s="55"/>
       <c r="T25" s="55"/>
       <c r="U25" s="57"/>
@@ -3019,67 +3257,67 @@
       </c>
       <c r="AB25" s="48"/>
     </row>
-    <row r="26" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="35">
         <v>17</v>
       </c>
-      <c r="B26" s="75" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="76">
-        <v>2</v>
-      </c>
-      <c r="D26" s="76">
-        <v>2</v>
-      </c>
-      <c r="E26" s="76">
-        <v>2</v>
-      </c>
-      <c r="F26" s="76">
-        <v>2</v>
-      </c>
-      <c r="G26" s="77">
+      <c r="B26" s="72" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="73">
+        <v>2</v>
+      </c>
+      <c r="D26" s="73">
+        <v>2</v>
+      </c>
+      <c r="E26" s="73">
+        <v>2</v>
+      </c>
+      <c r="F26" s="73">
+        <v>2</v>
+      </c>
+      <c r="G26" s="74">
         <f>VLOOKUP(H26,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
       <c r="H26" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="I26" s="78">
+      <c r="I26" s="75">
         <v>8</v>
       </c>
       <c r="J26" s="40">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="K26" s="79"/>
-      <c r="L26" s="79"/>
-      <c r="M26" s="79"/>
+      <c r="K26" s="76"/>
+      <c r="L26" s="76"/>
+      <c r="M26" s="76"/>
       <c r="N26" s="52"/>
-      <c r="O26" s="73"/>
+      <c r="O26" s="70"/>
       <c r="P26" s="42"/>
       <c r="Q26" s="42"/>
-      <c r="R26" s="80"/>
-      <c r="S26" s="81"/>
-      <c r="T26" s="81"/>
-      <c r="U26" s="79"/>
+      <c r="R26" s="77"/>
+      <c r="S26" s="78"/>
+      <c r="T26" s="78"/>
+      <c r="U26" s="76"/>
       <c r="V26" s="52"/>
-      <c r="W26" s="79"/>
-      <c r="X26" s="79"/>
-      <c r="Y26" s="79"/>
+      <c r="W26" s="76"/>
+      <c r="X26" s="76"/>
+      <c r="Y26" s="76"/>
       <c r="Z26" s="52"/>
       <c r="AA26" s="44">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB26" s="82"/>
-    </row>
-    <row r="27" spans="1:28" s="85" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AB26" s="79"/>
+    </row>
+    <row r="27" spans="1:28" s="82" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="35">
         <v>18</v>
       </c>
-      <c r="B27" s="83" t="s">
-        <v>42</v>
+      <c r="B27" s="80" t="s">
+        <v>41</v>
       </c>
       <c r="C27" s="37">
         <v>3</v>
@@ -3093,14 +3331,14 @@
       <c r="F27" s="37">
         <v>0</v>
       </c>
-      <c r="G27" s="77">
+      <c r="G27" s="74">
         <f>VLOOKUP(H27,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
       <c r="H27" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="I27" s="84">
+      <c r="I27" s="81">
         <v>21</v>
       </c>
       <c r="J27" s="40">
@@ -3111,7 +3349,7 @@
       <c r="L27" s="42"/>
       <c r="M27" s="42"/>
       <c r="N27" s="43"/>
-      <c r="O27" s="73"/>
+      <c r="O27" s="70"/>
       <c r="P27" s="42"/>
       <c r="Q27" s="42"/>
       <c r="R27" s="43"/>
@@ -3129,26 +3367,26 @@
       </c>
       <c r="AB27" s="48"/>
     </row>
-    <row r="28" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="35">
         <v>19</v>
       </c>
-      <c r="B28" s="86" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="87">
-        <v>2</v>
-      </c>
-      <c r="D28" s="87">
-        <v>0</v>
-      </c>
-      <c r="E28" s="87">
-        <v>0</v>
-      </c>
-      <c r="F28" s="87">
+      <c r="B28" s="83" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="84">
+        <v>2</v>
+      </c>
+      <c r="D28" s="84">
+        <v>0</v>
+      </c>
+      <c r="E28" s="84">
+        <v>0</v>
+      </c>
+      <c r="F28" s="84">
         <v>4</v>
       </c>
-      <c r="G28" s="77">
+      <c r="G28" s="74">
         <f>VLOOKUP(H28,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -3162,34 +3400,34 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="K28" s="88"/>
-      <c r="L28" s="88"/>
-      <c r="M28" s="88"/>
-      <c r="N28" s="89"/>
+      <c r="K28" s="85"/>
+      <c r="L28" s="85"/>
+      <c r="M28" s="85"/>
+      <c r="N28" s="86"/>
       <c r="O28" s="42"/>
-      <c r="P28" s="73"/>
+      <c r="P28" s="70"/>
       <c r="Q28" s="42"/>
-      <c r="R28" s="89"/>
-      <c r="S28" s="88"/>
-      <c r="T28" s="88"/>
-      <c r="U28" s="88"/>
-      <c r="V28" s="89"/>
-      <c r="W28" s="88"/>
-      <c r="X28" s="88"/>
-      <c r="Y28" s="88"/>
-      <c r="Z28" s="89"/>
+      <c r="R28" s="86"/>
+      <c r="S28" s="85"/>
+      <c r="T28" s="85"/>
+      <c r="U28" s="85"/>
+      <c r="V28" s="86"/>
+      <c r="W28" s="85"/>
+      <c r="X28" s="85"/>
+      <c r="Y28" s="85"/>
+      <c r="Z28" s="86"/>
       <c r="AA28" s="44">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="AB28" s="48"/>
     </row>
-    <row r="29" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="35">
         <v>20</v>
       </c>
       <c r="B29" s="67" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C29" s="37">
         <v>6</v>
@@ -3203,12 +3441,12 @@
       <c r="F29" s="37">
         <v>10</v>
       </c>
-      <c r="G29" s="77">
+      <c r="G29" s="74">
         <f>VLOOKUP(H29,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H29" s="39" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I29" s="40">
         <v>5</v>
@@ -3222,7 +3460,7 @@
       <c r="M29" s="42"/>
       <c r="N29" s="43"/>
       <c r="O29" s="42"/>
-      <c r="P29" s="71"/>
+      <c r="P29" s="41"/>
       <c r="Q29" s="42"/>
       <c r="R29" s="43"/>
       <c r="S29" s="42"/>
@@ -3239,54 +3477,54 @@
       </c>
       <c r="AB29" s="48"/>
     </row>
-    <row r="30" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="35">
         <v>21</v>
       </c>
-      <c r="B30" s="75" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="76">
-        <v>0</v>
-      </c>
-      <c r="D30" s="76">
+      <c r="B30" s="72" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="73">
+        <v>0</v>
+      </c>
+      <c r="D30" s="73">
         <v>9</v>
       </c>
-      <c r="E30" s="76">
+      <c r="E30" s="73">
         <v>18.5</v>
       </c>
-      <c r="F30" s="76">
-        <v>0</v>
-      </c>
-      <c r="G30" s="77">
+      <c r="F30" s="73">
+        <v>0</v>
+      </c>
+      <c r="G30" s="74">
         <f>VLOOKUP(H30,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
       <c r="H30" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="I30" s="78">
+      <c r="I30" s="75">
         <v>25</v>
       </c>
       <c r="J30" s="40">
         <f t="shared" si="1"/>
         <v>27.5</v>
       </c>
-      <c r="K30" s="79"/>
-      <c r="L30" s="79"/>
-      <c r="M30" s="79"/>
+      <c r="K30" s="76"/>
+      <c r="L30" s="76"/>
+      <c r="M30" s="76"/>
       <c r="N30" s="52"/>
       <c r="O30" s="42"/>
-      <c r="P30" s="73"/>
+      <c r="P30" s="70"/>
       <c r="Q30" s="42"/>
       <c r="R30" s="61"/>
-      <c r="S30" s="79"/>
-      <c r="T30" s="79"/>
-      <c r="U30" s="79"/>
+      <c r="S30" s="76"/>
+      <c r="T30" s="76"/>
+      <c r="U30" s="76"/>
       <c r="V30" s="52"/>
-      <c r="W30" s="79"/>
-      <c r="X30" s="79"/>
-      <c r="Y30" s="79"/>
+      <c r="W30" s="76"/>
+      <c r="X30" s="76"/>
+      <c r="Y30" s="76"/>
       <c r="Z30" s="52"/>
       <c r="AA30" s="44">
         <f t="shared" si="2"/>
@@ -3294,12 +3532,12 @@
       </c>
       <c r="AB30" s="48"/>
     </row>
-    <row r="31" spans="1:28" s="85" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" s="82" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="35">
         <v>22</v>
       </c>
-      <c r="B31" s="83" t="s">
-        <v>46</v>
+      <c r="B31" s="80" t="s">
+        <v>45</v>
       </c>
       <c r="C31" s="37">
         <v>5</v>
@@ -3313,14 +3551,14 @@
       <c r="F31" s="37">
         <v>0</v>
       </c>
-      <c r="G31" s="77">
+      <c r="G31" s="74">
         <f>VLOOKUP(H31,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
       <c r="H31" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="I31" s="84">
+      <c r="I31" s="81">
         <v>12</v>
       </c>
       <c r="J31" s="40">
@@ -3332,7 +3570,7 @@
       <c r="M31" s="42"/>
       <c r="N31" s="43"/>
       <c r="O31" s="42"/>
-      <c r="P31" s="73"/>
+      <c r="P31" s="70"/>
       <c r="Q31" s="42"/>
       <c r="R31" s="43"/>
       <c r="S31" s="42"/>
@@ -3349,12 +3587,12 @@
       </c>
       <c r="AB31" s="48"/>
     </row>
-    <row r="32" spans="1:28" s="85" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" s="82" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="35">
         <v>23</v>
       </c>
-      <c r="B32" s="83" t="s">
-        <v>47</v>
+      <c r="B32" s="80" t="s">
+        <v>46</v>
       </c>
       <c r="C32" s="37">
         <v>3</v>
@@ -3368,17 +3606,17 @@
       <c r="F32" s="37">
         <v>3</v>
       </c>
-      <c r="G32" s="77">
+      <c r="G32" s="74">
         <f>VLOOKUP(H32,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
       <c r="H32" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="I32" s="84">
+      <c r="I32" s="81">
         <v>12</v>
       </c>
-      <c r="J32" s="84">
+      <c r="J32" s="81">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
@@ -3387,7 +3625,7 @@
       <c r="M32" s="42"/>
       <c r="N32" s="43"/>
       <c r="O32" s="42"/>
-      <c r="P32" s="73"/>
+      <c r="P32" s="70"/>
       <c r="Q32" s="42"/>
       <c r="R32" s="43"/>
       <c r="S32" s="42"/>
@@ -3404,26 +3642,26 @@
       </c>
       <c r="AB32" s="48"/>
     </row>
-    <row r="33" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="35">
         <v>24</v>
       </c>
-      <c r="B33" s="90" t="s">
-        <v>48</v>
-      </c>
-      <c r="C33" s="87">
-        <v>0</v>
-      </c>
-      <c r="D33" s="87">
-        <v>0</v>
-      </c>
-      <c r="E33" s="87">
+      <c r="B33" s="87" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="84">
+        <v>0</v>
+      </c>
+      <c r="D33" s="84">
+        <v>0</v>
+      </c>
+      <c r="E33" s="84">
         <v>10</v>
       </c>
-      <c r="F33" s="87">
-        <v>0</v>
-      </c>
-      <c r="G33" s="77">
+      <c r="F33" s="84">
+        <v>0</v>
+      </c>
+      <c r="G33" s="74">
         <f>VLOOKUP(H33,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -3437,34 +3675,34 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="K33" s="81"/>
-      <c r="L33" s="81"/>
-      <c r="M33" s="81"/>
-      <c r="N33" s="80"/>
+      <c r="K33" s="78"/>
+      <c r="L33" s="78"/>
+      <c r="M33" s="78"/>
+      <c r="N33" s="77"/>
       <c r="O33" s="42"/>
-      <c r="P33" s="73"/>
-      <c r="Q33" s="73"/>
-      <c r="R33" s="91"/>
-      <c r="S33" s="81"/>
-      <c r="T33" s="81"/>
-      <c r="U33" s="81"/>
-      <c r="V33" s="80"/>
-      <c r="W33" s="81"/>
-      <c r="X33" s="81"/>
-      <c r="Y33" s="81"/>
-      <c r="Z33" s="80"/>
+      <c r="P33" s="70"/>
+      <c r="Q33" s="70"/>
+      <c r="R33" s="70"/>
+      <c r="S33" s="78"/>
+      <c r="T33" s="78"/>
+      <c r="U33" s="78"/>
+      <c r="V33" s="77"/>
+      <c r="W33" s="78"/>
+      <c r="X33" s="78"/>
+      <c r="Y33" s="78"/>
+      <c r="Z33" s="77"/>
       <c r="AA33" s="44">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB33" s="48"/>
     </row>
-    <row r="34" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="35">
         <v>25</v>
       </c>
-      <c r="B34" s="75" t="s">
-        <v>49</v>
+      <c r="B34" s="72" t="s">
+        <v>48</v>
       </c>
       <c r="C34" s="37">
         <v>0</v>
@@ -3478,7 +3716,7 @@
       <c r="F34" s="37">
         <v>0</v>
       </c>
-      <c r="G34" s="77">
+      <c r="G34" s="74">
         <f>VLOOKUP(H34,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -3492,21 +3730,21 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="K34" s="79"/>
-      <c r="L34" s="79"/>
-      <c r="M34" s="79"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="76"/>
+      <c r="M34" s="76"/>
       <c r="N34" s="52"/>
       <c r="O34" s="42"/>
       <c r="P34" s="42"/>
-      <c r="Q34" s="92"/>
+      <c r="Q34" s="88"/>
       <c r="R34" s="52"/>
-      <c r="S34" s="79"/>
-      <c r="T34" s="79"/>
-      <c r="U34" s="79"/>
+      <c r="S34" s="76"/>
+      <c r="T34" s="76"/>
+      <c r="U34" s="76"/>
       <c r="V34" s="52"/>
-      <c r="W34" s="79"/>
-      <c r="X34" s="79"/>
-      <c r="Y34" s="79"/>
+      <c r="W34" s="76"/>
+      <c r="X34" s="76"/>
+      <c r="Y34" s="76"/>
       <c r="Z34" s="52"/>
       <c r="AA34" s="44">
         <f t="shared" si="2"/>
@@ -3514,12 +3752,12 @@
       </c>
       <c r="AB34" s="48"/>
     </row>
-    <row r="35" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="35">
         <v>27</v>
       </c>
-      <c r="B35" s="75" t="s">
-        <v>50</v>
+      <c r="B35" s="72" t="s">
+        <v>49</v>
       </c>
       <c r="C35" s="37">
         <v>0</v>
@@ -3533,7 +3771,7 @@
       <c r="F35" s="37">
         <v>3</v>
       </c>
-      <c r="G35" s="77">
+      <c r="G35" s="74">
         <f>VLOOKUP(H35,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -3545,21 +3783,21 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="K35" s="79"/>
-      <c r="L35" s="79"/>
-      <c r="M35" s="79"/>
+      <c r="K35" s="76"/>
+      <c r="L35" s="76"/>
+      <c r="M35" s="76"/>
       <c r="N35" s="52"/>
-      <c r="O35" s="79"/>
-      <c r="P35" s="79"/>
-      <c r="Q35" s="92"/>
+      <c r="O35" s="76"/>
+      <c r="P35" s="76"/>
+      <c r="Q35" s="88"/>
       <c r="R35" s="52"/>
-      <c r="S35" s="79"/>
-      <c r="T35" s="79"/>
-      <c r="U35" s="79"/>
+      <c r="S35" s="76"/>
+      <c r="T35" s="76"/>
+      <c r="U35" s="76"/>
       <c r="V35" s="52"/>
-      <c r="W35" s="79"/>
-      <c r="X35" s="79"/>
-      <c r="Y35" s="79"/>
+      <c r="W35" s="76"/>
+      <c r="X35" s="76"/>
+      <c r="Y35" s="76"/>
       <c r="Z35" s="52"/>
       <c r="AA35" s="44">
         <f t="shared" si="2"/>
@@ -3567,12 +3805,12 @@
       </c>
       <c r="AB35" s="48"/>
     </row>
-    <row r="36" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="35">
         <v>28</v>
       </c>
-      <c r="B36" s="75" t="s">
-        <v>51</v>
+      <c r="B36" s="72" t="s">
+        <v>50</v>
       </c>
       <c r="C36" s="37">
         <v>2</v>
@@ -3586,7 +3824,7 @@
       <c r="F36" s="37">
         <v>8</v>
       </c>
-      <c r="G36" s="77">
+      <c r="G36" s="74">
         <f>VLOOKUP(H36,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -3598,21 +3836,21 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="K36" s="79"/>
-      <c r="L36" s="79"/>
-      <c r="M36" s="79"/>
+      <c r="K36" s="76"/>
+      <c r="L36" s="76"/>
+      <c r="M36" s="76"/>
       <c r="N36" s="52"/>
-      <c r="O36" s="79"/>
-      <c r="P36" s="79"/>
-      <c r="Q36" s="92"/>
+      <c r="O36" s="76"/>
+      <c r="P36" s="76"/>
+      <c r="Q36" s="88"/>
       <c r="R36" s="52"/>
-      <c r="S36" s="79"/>
-      <c r="T36" s="79"/>
-      <c r="U36" s="79"/>
+      <c r="S36" s="76"/>
+      <c r="T36" s="76"/>
+      <c r="U36" s="76"/>
       <c r="V36" s="52"/>
-      <c r="W36" s="79"/>
-      <c r="X36" s="79"/>
-      <c r="Y36" s="79"/>
+      <c r="W36" s="76"/>
+      <c r="X36" s="76"/>
+      <c r="Y36" s="76"/>
       <c r="Z36" s="52"/>
       <c r="AA36" s="44">
         <f t="shared" si="2"/>
@@ -3620,12 +3858,12 @@
       </c>
       <c r="AB36" s="48"/>
     </row>
-    <row r="37" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="35">
         <v>29</v>
       </c>
-      <c r="B37" s="75" t="s">
-        <v>52</v>
+      <c r="B37" s="72" t="s">
+        <v>51</v>
       </c>
       <c r="C37" s="37">
         <v>0</v>
@@ -3639,7 +3877,7 @@
       <c r="F37" s="37">
         <v>4</v>
       </c>
-      <c r="G37" s="77">
+      <c r="G37" s="74">
         <f>VLOOKUP(H37,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -3651,21 +3889,21 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K37" s="79"/>
-      <c r="L37" s="79"/>
-      <c r="M37" s="79"/>
+      <c r="K37" s="76"/>
+      <c r="L37" s="76"/>
+      <c r="M37" s="76"/>
       <c r="N37" s="52"/>
-      <c r="O37" s="79"/>
-      <c r="P37" s="79"/>
-      <c r="Q37" s="92"/>
+      <c r="O37" s="76"/>
+      <c r="P37" s="76"/>
+      <c r="Q37" s="88"/>
       <c r="R37" s="43"/>
-      <c r="S37" s="79"/>
-      <c r="T37" s="79"/>
-      <c r="U37" s="79"/>
+      <c r="S37" s="76"/>
+      <c r="T37" s="76"/>
+      <c r="U37" s="76"/>
       <c r="V37" s="52"/>
-      <c r="W37" s="79"/>
-      <c r="X37" s="79"/>
-      <c r="Y37" s="79"/>
+      <c r="W37" s="76"/>
+      <c r="X37" s="76"/>
+      <c r="Y37" s="76"/>
       <c r="Z37" s="52"/>
       <c r="AA37" s="44">
         <f t="shared" si="2"/>
@@ -3673,12 +3911,12 @@
       </c>
       <c r="AB37" s="48"/>
     </row>
-    <row r="38" spans="1:28" s="46" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="35">
         <v>30</v>
       </c>
-      <c r="B38" s="75" t="s">
-        <v>53</v>
+      <c r="B38" s="72" t="s">
+        <v>52</v>
       </c>
       <c r="C38" s="37">
         <v>5</v>
@@ -3692,7 +3930,7 @@
       <c r="F38" s="37">
         <v>0</v>
       </c>
-      <c r="G38" s="77">
+      <c r="G38" s="74">
         <f>VLOOKUP(H38,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -3704,21 +3942,21 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="K38" s="79"/>
-      <c r="L38" s="79"/>
-      <c r="M38" s="79"/>
+      <c r="K38" s="76"/>
+      <c r="L38" s="76"/>
+      <c r="M38" s="76"/>
       <c r="N38" s="52"/>
-      <c r="O38" s="79"/>
-      <c r="P38" s="79"/>
-      <c r="Q38" s="92"/>
+      <c r="O38" s="76"/>
+      <c r="P38" s="76"/>
+      <c r="Q38" s="88"/>
       <c r="R38" s="52"/>
       <c r="S38" s="42"/>
-      <c r="T38" s="79"/>
-      <c r="U38" s="79"/>
+      <c r="T38" s="76"/>
+      <c r="U38" s="76"/>
       <c r="V38" s="52"/>
-      <c r="W38" s="79"/>
-      <c r="X38" s="79"/>
-      <c r="Y38" s="79"/>
+      <c r="W38" s="76"/>
+      <c r="X38" s="76"/>
+      <c r="Y38" s="76"/>
       <c r="Z38" s="52"/>
       <c r="AA38" s="44">
         <f t="shared" si="2"/>
@@ -3726,12 +3964,12 @@
       </c>
       <c r="AB38" s="48"/>
     </row>
-    <row r="39" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="35">
         <v>31</v>
       </c>
-      <c r="B39" s="75" t="s">
-        <v>54</v>
+      <c r="B39" s="72" t="s">
+        <v>53</v>
       </c>
       <c r="C39" s="37">
         <v>0</v>
@@ -3745,7 +3983,7 @@
       <c r="F39" s="37">
         <v>4</v>
       </c>
-      <c r="G39" s="77">
+      <c r="G39" s="74">
         <f>VLOOKUP(H39,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -3757,21 +3995,21 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K39" s="79"/>
-      <c r="L39" s="79"/>
-      <c r="M39" s="79"/>
+      <c r="K39" s="76"/>
+      <c r="L39" s="76"/>
+      <c r="M39" s="76"/>
       <c r="N39" s="52"/>
-      <c r="O39" s="79"/>
-      <c r="P39" s="79"/>
-      <c r="Q39" s="79"/>
-      <c r="R39" s="92"/>
+      <c r="O39" s="76"/>
+      <c r="P39" s="76"/>
+      <c r="Q39" s="76"/>
+      <c r="R39" s="88"/>
       <c r="S39" s="42"/>
       <c r="T39" s="42"/>
-      <c r="U39" s="79"/>
+      <c r="U39" s="76"/>
       <c r="V39" s="52"/>
-      <c r="W39" s="79"/>
-      <c r="X39" s="79"/>
-      <c r="Y39" s="79"/>
+      <c r="W39" s="76"/>
+      <c r="X39" s="76"/>
+      <c r="Y39" s="76"/>
       <c r="Z39" s="52"/>
       <c r="AA39" s="44">
         <f t="shared" si="2"/>
@@ -3779,12 +4017,12 @@
       </c>
       <c r="AB39" s="48"/>
     </row>
-    <row r="40" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="35">
         <v>32</v>
       </c>
-      <c r="B40" s="75" t="s">
-        <v>55</v>
+      <c r="B40" s="72" t="s">
+        <v>54</v>
       </c>
       <c r="C40" s="37">
         <v>0</v>
@@ -3798,7 +4036,7 @@
       <c r="F40" s="37">
         <v>6</v>
       </c>
-      <c r="G40" s="77">
+      <c r="G40" s="74">
         <f>VLOOKUP(H40,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -3810,21 +4048,21 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="K40" s="79"/>
-      <c r="L40" s="79"/>
-      <c r="M40" s="79"/>
+      <c r="K40" s="76"/>
+      <c r="L40" s="76"/>
+      <c r="M40" s="76"/>
       <c r="N40" s="52"/>
-      <c r="O40" s="79"/>
-      <c r="P40" s="79"/>
-      <c r="Q40" s="79"/>
-      <c r="R40" s="92"/>
-      <c r="S40" s="79"/>
-      <c r="T40" s="79"/>
+      <c r="O40" s="76"/>
+      <c r="P40" s="76"/>
+      <c r="Q40" s="76"/>
+      <c r="R40" s="88"/>
+      <c r="S40" s="76"/>
+      <c r="T40" s="76"/>
       <c r="U40" s="42"/>
       <c r="V40" s="52"/>
-      <c r="W40" s="79"/>
-      <c r="X40" s="79"/>
-      <c r="Y40" s="79"/>
+      <c r="W40" s="76"/>
+      <c r="X40" s="76"/>
+      <c r="Y40" s="76"/>
       <c r="Z40" s="52"/>
       <c r="AA40" s="44">
         <f t="shared" si="2"/>
@@ -3832,12 +4070,12 @@
       </c>
       <c r="AB40" s="48"/>
     </row>
-    <row r="41" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="35">
         <v>33</v>
       </c>
-      <c r="B41" s="75" t="s">
-        <v>56</v>
+      <c r="B41" s="72" t="s">
+        <v>55</v>
       </c>
       <c r="C41" s="37">
         <v>2</v>
@@ -3851,7 +4089,7 @@
       <c r="F41" s="37">
         <v>2</v>
       </c>
-      <c r="G41" s="77">
+      <c r="G41" s="74">
         <f>VLOOKUP(H41,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -3865,21 +4103,21 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="K41" s="79"/>
-      <c r="L41" s="79"/>
-      <c r="M41" s="79"/>
+      <c r="K41" s="76"/>
+      <c r="L41" s="76"/>
+      <c r="M41" s="76"/>
       <c r="N41" s="52"/>
-      <c r="O41" s="79"/>
-      <c r="P41" s="79"/>
+      <c r="O41" s="76"/>
+      <c r="P41" s="76"/>
       <c r="Q41" s="42"/>
-      <c r="R41" s="93"/>
-      <c r="S41" s="79"/>
-      <c r="T41" s="79"/>
-      <c r="U41" s="79"/>
+      <c r="R41" s="70"/>
+      <c r="S41" s="76"/>
+      <c r="T41" s="76"/>
+      <c r="U41" s="76"/>
       <c r="V41" s="52"/>
-      <c r="W41" s="79"/>
-      <c r="X41" s="79"/>
-      <c r="Y41" s="79"/>
+      <c r="W41" s="76"/>
+      <c r="X41" s="76"/>
+      <c r="Y41" s="76"/>
       <c r="Z41" s="52"/>
       <c r="AA41" s="44">
         <f t="shared" si="2"/>
@@ -3887,12 +4125,12 @@
       </c>
       <c r="AB41" s="48"/>
     </row>
-    <row r="42" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="35">
         <v>34</v>
       </c>
-      <c r="B42" s="75" t="s">
-        <v>57</v>
+      <c r="B42" s="72" t="s">
+        <v>56</v>
       </c>
       <c r="C42" s="37">
         <v>0</v>
@@ -3906,33 +4144,33 @@
       <c r="F42" s="37">
         <v>0</v>
       </c>
-      <c r="G42" s="77">
+      <c r="G42" s="74">
         <f>VLOOKUP(H42,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H42" s="39" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I42" s="40"/>
       <c r="J42" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K42" s="79"/>
-      <c r="L42" s="79"/>
-      <c r="M42" s="79"/>
+      <c r="K42" s="76"/>
+      <c r="L42" s="76"/>
+      <c r="M42" s="76"/>
       <c r="N42" s="52"/>
-      <c r="O42" s="79"/>
-      <c r="P42" s="79"/>
-      <c r="Q42" s="79"/>
+      <c r="O42" s="76"/>
+      <c r="P42" s="76"/>
+      <c r="Q42" s="76"/>
       <c r="R42" s="52"/>
-      <c r="S42" s="79"/>
-      <c r="T42" s="79"/>
-      <c r="U42" s="79"/>
+      <c r="S42" s="76"/>
+      <c r="T42" s="76"/>
+      <c r="U42" s="76"/>
       <c r="V42" s="43"/>
-      <c r="W42" s="79"/>
-      <c r="X42" s="79"/>
-      <c r="Y42" s="79"/>
+      <c r="W42" s="76"/>
+      <c r="X42" s="76"/>
+      <c r="Y42" s="76"/>
       <c r="Z42" s="52"/>
       <c r="AA42" s="44">
         <f t="shared" si="2"/>
@@ -3940,12 +4178,12 @@
       </c>
       <c r="AB42" s="48"/>
     </row>
-    <row r="43" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="35">
         <v>35</v>
       </c>
-      <c r="B43" s="75" t="s">
-        <v>58</v>
+      <c r="B43" s="72" t="s">
+        <v>57</v>
       </c>
       <c r="C43" s="37">
         <v>0</v>
@@ -3959,7 +4197,7 @@
       <c r="F43" s="37">
         <v>0</v>
       </c>
-      <c r="G43" s="77">
+      <c r="G43" s="74">
         <f>VLOOKUP(H43,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -3973,21 +4211,21 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K43" s="79"/>
-      <c r="L43" s="79"/>
-      <c r="M43" s="79"/>
+      <c r="K43" s="76"/>
+      <c r="L43" s="76"/>
+      <c r="M43" s="76"/>
       <c r="N43" s="52"/>
-      <c r="O43" s="79"/>
-      <c r="P43" s="79"/>
-      <c r="Q43" s="79"/>
-      <c r="R43" s="92"/>
-      <c r="S43" s="79"/>
-      <c r="T43" s="79"/>
-      <c r="U43" s="79"/>
+      <c r="O43" s="76"/>
+      <c r="P43" s="76"/>
+      <c r="Q43" s="76"/>
+      <c r="R43" s="88"/>
+      <c r="S43" s="76"/>
+      <c r="T43" s="76"/>
+      <c r="U43" s="76"/>
       <c r="V43" s="43"/>
-      <c r="W43" s="79"/>
-      <c r="X43" s="79"/>
-      <c r="Y43" s="79"/>
+      <c r="W43" s="76"/>
+      <c r="X43" s="76"/>
+      <c r="Y43" s="76"/>
       <c r="Z43" s="52"/>
       <c r="AA43" s="44">
         <f t="shared" si="2"/>
@@ -3995,12 +4233,12 @@
       </c>
       <c r="AB43" s="48"/>
     </row>
-    <row r="44" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="35">
         <v>36</v>
       </c>
-      <c r="B44" s="75" t="s">
-        <v>59</v>
+      <c r="B44" s="72" t="s">
+        <v>58</v>
       </c>
       <c r="C44" s="37">
         <v>0</v>
@@ -4014,12 +4252,12 @@
       <c r="F44" s="37">
         <v>0</v>
       </c>
-      <c r="G44" s="77">
+      <c r="G44" s="74">
         <f>VLOOKUP(H44,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H44" s="39" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I44" s="40">
         <v>5</v>
@@ -4028,21 +4266,21 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K44" s="79"/>
-      <c r="L44" s="79"/>
-      <c r="M44" s="79"/>
+      <c r="K44" s="76"/>
+      <c r="L44" s="76"/>
+      <c r="M44" s="76"/>
       <c r="N44" s="52"/>
-      <c r="O44" s="79"/>
-      <c r="P44" s="79"/>
-      <c r="Q44" s="79"/>
+      <c r="O44" s="76"/>
+      <c r="P44" s="76"/>
+      <c r="Q44" s="76"/>
       <c r="R44" s="52"/>
-      <c r="S44" s="79"/>
-      <c r="T44" s="79"/>
-      <c r="U44" s="79"/>
+      <c r="S44" s="76"/>
+      <c r="T44" s="76"/>
+      <c r="U44" s="76"/>
       <c r="V44" s="52"/>
       <c r="W44" s="42"/>
-      <c r="X44" s="79"/>
-      <c r="Y44" s="79"/>
+      <c r="X44" s="76"/>
+      <c r="Y44" s="76"/>
       <c r="Z44" s="52"/>
       <c r="AA44" s="44">
         <f t="shared" si="2"/>
@@ -4050,12 +4288,12 @@
       </c>
       <c r="AB44" s="48"/>
     </row>
-    <row r="45" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="35">
         <v>37</v>
       </c>
-      <c r="B45" s="75" t="s">
-        <v>60</v>
+      <c r="B45" s="72" t="s">
+        <v>59</v>
       </c>
       <c r="C45" s="37">
         <v>7</v>
@@ -4069,7 +4307,7 @@
       <c r="F45" s="37">
         <v>0</v>
       </c>
-      <c r="G45" s="77">
+      <c r="G45" s="74">
         <f>VLOOKUP(H45,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -4081,21 +4319,21 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="K45" s="79"/>
-      <c r="L45" s="79"/>
-      <c r="M45" s="79"/>
+      <c r="K45" s="76"/>
+      <c r="L45" s="76"/>
+      <c r="M45" s="76"/>
       <c r="N45" s="52"/>
-      <c r="O45" s="79"/>
-      <c r="P45" s="79"/>
-      <c r="Q45" s="79"/>
-      <c r="R45" s="92"/>
-      <c r="S45" s="79"/>
-      <c r="T45" s="79"/>
-      <c r="U45" s="79"/>
+      <c r="O45" s="76"/>
+      <c r="P45" s="76"/>
+      <c r="Q45" s="76"/>
+      <c r="R45" s="88"/>
+      <c r="S45" s="76"/>
+      <c r="T45" s="76"/>
+      <c r="U45" s="76"/>
       <c r="V45" s="52"/>
       <c r="W45" s="42"/>
-      <c r="X45" s="79"/>
-      <c r="Y45" s="79"/>
+      <c r="X45" s="76"/>
+      <c r="Y45" s="76"/>
       <c r="Z45" s="52"/>
       <c r="AA45" s="44">
         <f t="shared" si="2"/>
@@ -4103,11 +4341,11 @@
       </c>
       <c r="AB45" s="48"/>
     </row>
-    <row r="46" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" s="141" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="35">
-        <v>38</v>
-      </c>
-      <c r="B46" s="75" t="s">
+        <v>39</v>
+      </c>
+      <c r="B46" s="67" t="s">
         <v>67</v>
       </c>
       <c r="C46" s="37">
@@ -4117,389 +4355,507 @@
         <v>0</v>
       </c>
       <c r="E46" s="37">
-        <v>8.75</v>
+        <v>2.5</v>
       </c>
       <c r="F46" s="37">
         <v>0</v>
       </c>
-      <c r="G46" s="77">
+      <c r="G46" s="74">
         <f>VLOOKUP(H46,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H46" s="39" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I46" s="40">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J46" s="40">
-        <f t="shared" si="1"/>
-        <v>8.75</v>
-      </c>
-      <c r="K46" s="79"/>
-      <c r="L46" s="79"/>
-      <c r="M46" s="79"/>
-      <c r="N46" s="52"/>
-      <c r="O46" s="79"/>
-      <c r="P46" s="79"/>
-      <c r="Q46" s="79"/>
-      <c r="R46" s="120"/>
-      <c r="S46" s="79"/>
-      <c r="T46" s="79"/>
-      <c r="U46" s="79"/>
-      <c r="V46" s="52"/>
-      <c r="W46" s="79"/>
+        <f t="shared" ref="J46" si="3">SUM(C46:F46)</f>
+        <v>2.5</v>
+      </c>
+      <c r="K46" s="42"/>
+      <c r="L46" s="42"/>
+      <c r="M46" s="42"/>
+      <c r="N46" s="43"/>
+      <c r="O46" s="42"/>
+      <c r="P46" s="42"/>
+      <c r="Q46" s="42"/>
+      <c r="R46" s="140"/>
+      <c r="S46" s="42"/>
+      <c r="T46" s="42"/>
+      <c r="U46" s="42"/>
+      <c r="V46" s="43"/>
+      <c r="W46" s="42"/>
       <c r="X46" s="42"/>
-      <c r="Y46" s="79"/>
-      <c r="Z46" s="52"/>
-      <c r="AA46" s="44">
-        <f t="shared" si="2"/>
-        <v>-1.75</v>
-      </c>
+      <c r="Y46" s="42"/>
+      <c r="Z46" s="43"/>
+      <c r="AA46" s="44"/>
       <c r="AB46" s="48"/>
     </row>
-    <row r="47" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" s="141" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="35">
-        <v>39</v>
-      </c>
-      <c r="B47" s="75" t="s">
-        <v>68</v>
+        <v>40</v>
+      </c>
+      <c r="B47" s="67" t="s">
+        <v>75</v>
       </c>
       <c r="C47" s="37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D47" s="37">
         <v>0</v>
       </c>
       <c r="E47" s="37">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="F47" s="37">
         <v>0</v>
       </c>
-      <c r="G47" s="77">
+      <c r="G47" s="74">
         <f>VLOOKUP(H47,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H47" s="39" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I47" s="40">
         <v>8</v>
       </c>
       <c r="J47" s="40">
         <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="K47" s="42"/>
       <c r="L47" s="42"/>
-      <c r="M47" s="79"/>
-      <c r="N47" s="52"/>
-      <c r="O47" s="79"/>
-      <c r="P47" s="79"/>
-      <c r="Q47" s="79"/>
-      <c r="R47" s="122"/>
-      <c r="S47" s="79"/>
-      <c r="T47" s="79"/>
-      <c r="U47" s="79"/>
-      <c r="V47" s="52"/>
-      <c r="W47" s="79"/>
-      <c r="X47" s="79"/>
-      <c r="Y47" s="79"/>
-      <c r="Z47" s="52"/>
-      <c r="AA47" s="121"/>
-      <c r="AB47" s="82"/>
-    </row>
-    <row r="48" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="35">
-        <v>40</v>
-      </c>
-      <c r="B48" s="75"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="37"/>
-      <c r="F48" s="37"/>
-      <c r="G48" s="77"/>
-      <c r="H48" s="39"/>
+      <c r="M47" s="42"/>
+      <c r="N47" s="43"/>
+      <c r="O47" s="42"/>
+      <c r="P47" s="42"/>
+      <c r="Q47" s="42"/>
+      <c r="R47" s="140"/>
+      <c r="S47" s="42"/>
+      <c r="T47" s="42"/>
+      <c r="U47" s="42"/>
+      <c r="V47" s="43"/>
+      <c r="W47" s="42"/>
+      <c r="X47" s="42"/>
+      <c r="Y47" s="42"/>
+      <c r="Z47" s="43"/>
+      <c r="AA47" s="44"/>
+      <c r="AB47" s="48"/>
+    </row>
+    <row r="48" spans="1:28" s="46" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="A48" s="135"/>
+      <c r="B48" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C48" s="84"/>
+      <c r="D48" s="84"/>
+      <c r="E48" s="84"/>
+      <c r="F48" s="84"/>
+      <c r="G48" s="74"/>
+      <c r="H48" s="136"/>
       <c r="I48" s="40"/>
       <c r="J48" s="40">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K48" s="42"/>
-      <c r="L48" s="42"/>
-      <c r="M48" s="79"/>
-      <c r="N48" s="52"/>
-      <c r="O48" s="79"/>
-      <c r="P48" s="79"/>
-      <c r="Q48" s="79"/>
-      <c r="R48" s="122"/>
-      <c r="S48" s="79"/>
-      <c r="T48" s="79"/>
-      <c r="U48" s="79"/>
-      <c r="V48" s="52"/>
-      <c r="W48" s="79"/>
-      <c r="X48" s="79"/>
-      <c r="Y48" s="79"/>
-      <c r="Z48" s="52"/>
-      <c r="AA48" s="121"/>
-      <c r="AB48" s="82"/>
-    </row>
-    <row r="49" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" ref="J48" si="4">SUM(C48:F48)</f>
+        <v>0</v>
+      </c>
+      <c r="K48" s="85"/>
+      <c r="L48" s="85"/>
+      <c r="M48" s="78"/>
+      <c r="N48" s="77"/>
+      <c r="O48" s="78"/>
+      <c r="P48" s="78"/>
+      <c r="Q48" s="78"/>
+      <c r="R48" s="137"/>
+      <c r="S48" s="78"/>
+      <c r="T48" s="42"/>
+      <c r="U48" s="42"/>
+      <c r="V48" s="43"/>
+      <c r="W48" s="78"/>
+      <c r="X48" s="78"/>
+      <c r="Y48" s="78"/>
+      <c r="Z48" s="77"/>
+      <c r="AA48" s="138"/>
+      <c r="AB48" s="139"/>
+    </row>
+    <row r="49" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="35">
-        <v>41</v>
-      </c>
-      <c r="B49" s="75"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="37"/>
-      <c r="E49" s="37"/>
-      <c r="F49" s="37"/>
-      <c r="G49" s="77"/>
-      <c r="H49" s="39"/>
-      <c r="I49" s="40"/>
+        <v>1</v>
+      </c>
+      <c r="B49" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" s="37">
+        <v>0</v>
+      </c>
+      <c r="D49" s="37">
+        <v>0</v>
+      </c>
+      <c r="E49" s="37">
+        <v>8.75</v>
+      </c>
+      <c r="F49" s="37">
+        <v>0</v>
+      </c>
+      <c r="G49" s="74">
+        <f>VLOOKUP(H49,Feuil2!$A$1:$B$3,2,0)</f>
+        <v>100</v>
+      </c>
+      <c r="H49" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="I49" s="40">
+        <v>7</v>
+      </c>
       <c r="J49" s="40">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K49" s="42"/>
-      <c r="L49" s="42"/>
-      <c r="M49" s="79"/>
+        <f>SUM(C49:F49)</f>
+        <v>8.75</v>
+      </c>
+      <c r="K49" s="76"/>
+      <c r="L49" s="76"/>
+      <c r="M49" s="76"/>
       <c r="N49" s="52"/>
-      <c r="O49" s="79"/>
-      <c r="P49" s="79"/>
-      <c r="Q49" s="79"/>
-      <c r="R49" s="122"/>
-      <c r="S49" s="79"/>
-      <c r="T49" s="79"/>
-      <c r="U49" s="79"/>
-      <c r="V49" s="52"/>
-      <c r="W49" s="79"/>
-      <c r="X49" s="79"/>
-      <c r="Y49" s="79"/>
+      <c r="O49" s="76"/>
+      <c r="P49" s="76"/>
+      <c r="Q49" s="76"/>
+      <c r="R49" s="70"/>
+      <c r="S49" s="134"/>
+      <c r="T49" s="42"/>
+      <c r="U49" s="142"/>
+      <c r="V49" s="43"/>
+      <c r="W49" s="76"/>
+      <c r="X49" s="42"/>
+      <c r="Y49" s="76"/>
       <c r="Z49" s="52"/>
-      <c r="AA49" s="121"/>
-      <c r="AB49" s="82"/>
-    </row>
-    <row r="50" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AA49" s="44">
+        <f>I49-J49</f>
+        <v>-1.75</v>
+      </c>
+      <c r="AB49" s="48"/>
+    </row>
+    <row r="50" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="35">
-        <v>42</v>
-      </c>
-      <c r="B50" s="75"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="37"/>
-      <c r="E50" s="37"/>
-      <c r="F50" s="37"/>
-      <c r="G50" s="77"/>
-      <c r="H50" s="39"/>
+        <v>2</v>
+      </c>
+      <c r="B50" s="72" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" s="37">
+        <v>0</v>
+      </c>
+      <c r="D50" s="37">
+        <v>0</v>
+      </c>
+      <c r="E50" s="37">
+        <v>0</v>
+      </c>
+      <c r="F50" s="37">
+        <v>5</v>
+      </c>
+      <c r="G50" s="74">
+        <f>VLOOKUP(H50,Feuil2!$A$1:$B$3,2,0)</f>
+        <v>100</v>
+      </c>
+      <c r="H50" s="39" t="s">
+        <v>5</v>
+      </c>
       <c r="I50" s="40"/>
       <c r="J50" s="40">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K50" s="42"/>
-      <c r="L50" s="42"/>
-      <c r="M50" s="79"/>
+        <f t="shared" ref="J50" si="5">SUM(C50:F50)</f>
+        <v>5</v>
+      </c>
+      <c r="K50" s="76"/>
+      <c r="L50" s="76"/>
+      <c r="M50" s="76"/>
       <c r="N50" s="52"/>
-      <c r="O50" s="79"/>
-      <c r="P50" s="79"/>
-      <c r="Q50" s="79"/>
-      <c r="R50" s="122"/>
-      <c r="S50" s="79"/>
-      <c r="T50" s="79"/>
-      <c r="U50" s="79"/>
-      <c r="V50" s="52"/>
-      <c r="W50" s="79"/>
-      <c r="X50" s="79"/>
-      <c r="Y50" s="79"/>
+      <c r="O50" s="76"/>
+      <c r="P50" s="76"/>
+      <c r="Q50" s="76"/>
+      <c r="R50" s="88"/>
+      <c r="S50" s="134"/>
+      <c r="T50" s="42"/>
+      <c r="U50" s="142"/>
+      <c r="V50" s="43"/>
+      <c r="W50" s="76"/>
+      <c r="X50" s="76"/>
+      <c r="Y50" s="76"/>
       <c r="Z50" s="52"/>
-      <c r="AA50" s="121"/>
-      <c r="AB50" s="82"/>
-    </row>
-    <row r="51" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AA50" s="44">
+        <f t="shared" ref="AA50" si="6">I50-J50</f>
+        <v>-5</v>
+      </c>
+      <c r="AB50" s="48"/>
+    </row>
+    <row r="51" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="35">
-        <v>43</v>
-      </c>
-      <c r="B51" s="75"/>
-      <c r="C51" s="37"/>
-      <c r="D51" s="37"/>
-      <c r="E51" s="37"/>
-      <c r="F51" s="37"/>
-      <c r="G51" s="77"/>
-      <c r="H51" s="39"/>
+        <v>3</v>
+      </c>
+      <c r="B51" s="72" t="s">
+        <v>69</v>
+      </c>
+      <c r="C51" s="37">
+        <v>7</v>
+      </c>
+      <c r="D51" s="37">
+        <v>0</v>
+      </c>
+      <c r="E51" s="37">
+        <v>0</v>
+      </c>
+      <c r="F51" s="37">
+        <v>0</v>
+      </c>
+      <c r="G51" s="74">
+        <f>VLOOKUP(H51,Feuil2!$A$1:$B$3,2,0)</f>
+        <v>100</v>
+      </c>
+      <c r="H51" s="39" t="s">
+        <v>5</v>
+      </c>
       <c r="I51" s="40"/>
       <c r="J51" s="40">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K51" s="42"/>
       <c r="L51" s="42"/>
-      <c r="M51" s="79"/>
+      <c r="M51" s="76"/>
       <c r="N51" s="52"/>
-      <c r="O51" s="79"/>
-      <c r="P51" s="79"/>
-      <c r="Q51" s="79"/>
-      <c r="R51" s="122"/>
-      <c r="S51" s="79"/>
-      <c r="T51" s="79"/>
-      <c r="U51" s="79"/>
-      <c r="V51" s="52"/>
-      <c r="W51" s="79"/>
-      <c r="X51" s="79"/>
-      <c r="Y51" s="79"/>
+      <c r="O51" s="76"/>
+      <c r="P51" s="76"/>
+      <c r="Q51" s="76"/>
+      <c r="R51" s="116"/>
+      <c r="S51" s="134"/>
+      <c r="T51" s="42"/>
+      <c r="U51" s="142"/>
+      <c r="V51" s="43"/>
+      <c r="W51" s="76"/>
+      <c r="X51" s="76"/>
+      <c r="Y51" s="76"/>
       <c r="Z51" s="52"/>
-      <c r="AA51" s="121"/>
-      <c r="AB51" s="82"/>
-    </row>
-    <row r="52" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AA51" s="115"/>
+      <c r="AB51" s="79"/>
+    </row>
+    <row r="52" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="35">
-        <v>44</v>
-      </c>
-      <c r="B52" s="75"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="37"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="37"/>
-      <c r="G52" s="77"/>
-      <c r="H52" s="39"/>
-      <c r="I52" s="40"/>
+        <v>4</v>
+      </c>
+      <c r="B52" s="72" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" s="37">
+        <v>0</v>
+      </c>
+      <c r="D52" s="37">
+        <v>0</v>
+      </c>
+      <c r="E52" s="37">
+        <v>0</v>
+      </c>
+      <c r="F52" s="37">
+        <v>0</v>
+      </c>
+      <c r="G52" s="74">
+        <f>VLOOKUP(H52,Feuil2!$A$1:$B$3,2,0)</f>
+        <v>75</v>
+      </c>
+      <c r="H52" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="I52" s="40">
+        <v>8</v>
+      </c>
       <c r="J52" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K52" s="42"/>
       <c r="L52" s="42"/>
-      <c r="M52" s="79"/>
+      <c r="M52" s="76"/>
       <c r="N52" s="52"/>
-      <c r="O52" s="79"/>
-      <c r="P52" s="79"/>
-      <c r="Q52" s="79"/>
-      <c r="R52" s="122"/>
-      <c r="S52" s="79"/>
-      <c r="T52" s="79"/>
-      <c r="U52" s="79"/>
-      <c r="V52" s="52"/>
-      <c r="W52" s="79"/>
-      <c r="X52" s="79"/>
-      <c r="Y52" s="79"/>
+      <c r="O52" s="76"/>
+      <c r="P52" s="76"/>
+      <c r="Q52" s="76"/>
+      <c r="R52" s="116"/>
+      <c r="S52" s="76"/>
+      <c r="T52" s="42"/>
+      <c r="U52" s="142"/>
+      <c r="V52" s="43"/>
+      <c r="W52" s="76"/>
+      <c r="X52" s="76"/>
+      <c r="Y52" s="76"/>
       <c r="Z52" s="52"/>
-      <c r="AA52" s="121"/>
-      <c r="AB52" s="82"/>
-    </row>
-    <row r="53" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AA52" s="115"/>
+      <c r="AB52" s="79"/>
+    </row>
+    <row r="53" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="35">
-        <v>45</v>
-      </c>
-      <c r="B53" s="75"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="37"/>
-      <c r="E53" s="37"/>
-      <c r="F53" s="37"/>
-      <c r="G53" s="77"/>
-      <c r="H53" s="39"/>
-      <c r="I53" s="40"/>
+        <v>5</v>
+      </c>
+      <c r="B53" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53" s="37">
+        <v>0</v>
+      </c>
+      <c r="D53" s="37">
+        <v>0</v>
+      </c>
+      <c r="E53" s="37">
+        <v>0</v>
+      </c>
+      <c r="F53" s="37">
+        <v>0</v>
+      </c>
+      <c r="G53" s="74">
+        <f>VLOOKUP(H53,Feuil2!$A$1:$B$3,2,0)</f>
+        <v>75</v>
+      </c>
+      <c r="H53" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="I53" s="40">
+        <v>16</v>
+      </c>
       <c r="J53" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K53" s="42"/>
       <c r="L53" s="42"/>
-      <c r="M53" s="79"/>
+      <c r="M53" s="76"/>
       <c r="N53" s="52"/>
-      <c r="O53" s="79"/>
-      <c r="P53" s="79"/>
-      <c r="Q53" s="79"/>
-      <c r="R53" s="122"/>
-      <c r="S53" s="79"/>
-      <c r="T53" s="79"/>
-      <c r="U53" s="79"/>
-      <c r="V53" s="52"/>
-      <c r="W53" s="79"/>
-      <c r="X53" s="79"/>
-      <c r="Y53" s="79"/>
+      <c r="O53" s="76"/>
+      <c r="P53" s="76"/>
+      <c r="Q53" s="76"/>
+      <c r="R53" s="116"/>
+      <c r="S53" s="76"/>
+      <c r="T53" s="42"/>
+      <c r="U53" s="142"/>
+      <c r="V53" s="43"/>
+      <c r="W53" s="76"/>
+      <c r="X53" s="76"/>
+      <c r="Y53" s="76"/>
       <c r="Z53" s="52"/>
-      <c r="AA53" s="121"/>
-      <c r="AB53" s="82"/>
-    </row>
-    <row r="54" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AA53" s="115"/>
+      <c r="AB53" s="79"/>
+    </row>
+    <row r="54" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="35">
-        <v>46</v>
-      </c>
-      <c r="B54" s="75"/>
-      <c r="C54" s="37"/>
-      <c r="D54" s="37"/>
-      <c r="E54" s="37"/>
-      <c r="F54" s="37"/>
-      <c r="G54" s="77"/>
-      <c r="H54" s="39"/>
-      <c r="I54" s="40"/>
+        <v>6</v>
+      </c>
+      <c r="B54" s="72" t="s">
+        <v>72</v>
+      </c>
+      <c r="C54" s="37">
+        <v>0</v>
+      </c>
+      <c r="D54" s="37">
+        <v>0</v>
+      </c>
+      <c r="E54" s="37">
+        <v>0</v>
+      </c>
+      <c r="F54" s="37">
+        <v>0</v>
+      </c>
+      <c r="G54" s="74">
+        <f>VLOOKUP(H54,Feuil2!$A$1:$B$3,2,0)</f>
+        <v>75</v>
+      </c>
+      <c r="H54" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="I54" s="40">
+        <v>8</v>
+      </c>
       <c r="J54" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K54" s="42"/>
       <c r="L54" s="42"/>
-      <c r="M54" s="79"/>
+      <c r="M54" s="76"/>
       <c r="N54" s="52"/>
-      <c r="O54" s="79"/>
-      <c r="P54" s="79"/>
-      <c r="Q54" s="79"/>
-      <c r="R54" s="122"/>
-      <c r="S54" s="79"/>
-      <c r="T54" s="79"/>
-      <c r="U54" s="79"/>
-      <c r="V54" s="52"/>
-      <c r="W54" s="79"/>
-      <c r="X54" s="79"/>
-      <c r="Y54" s="79"/>
+      <c r="O54" s="76"/>
+      <c r="P54" s="76"/>
+      <c r="Q54" s="76"/>
+      <c r="R54" s="116"/>
+      <c r="S54" s="76"/>
+      <c r="T54" s="42"/>
+      <c r="U54" s="142"/>
+      <c r="V54" s="43"/>
+      <c r="W54" s="76"/>
+      <c r="X54" s="76"/>
+      <c r="Y54" s="76"/>
       <c r="Z54" s="52"/>
-      <c r="AA54" s="121"/>
-      <c r="AB54" s="82"/>
-    </row>
-    <row r="55" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AA54" s="115"/>
+      <c r="AB54" s="79"/>
+    </row>
+    <row r="55" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="35">
-        <v>47</v>
-      </c>
-      <c r="B55" s="75"/>
-      <c r="C55" s="37"/>
-      <c r="D55" s="37"/>
-      <c r="E55" s="37"/>
-      <c r="F55" s="37"/>
-      <c r="G55" s="77"/>
-      <c r="H55" s="39"/>
-      <c r="I55" s="40"/>
+        <v>7</v>
+      </c>
+      <c r="B55" s="72" t="s">
+        <v>73</v>
+      </c>
+      <c r="C55" s="37">
+        <v>0</v>
+      </c>
+      <c r="D55" s="37">
+        <v>0</v>
+      </c>
+      <c r="E55" s="37">
+        <v>0</v>
+      </c>
+      <c r="F55" s="37">
+        <v>0</v>
+      </c>
+      <c r="G55" s="74">
+        <f>VLOOKUP(H55,Feuil2!$A$1:$B$3,2,0)</f>
+        <v>75</v>
+      </c>
+      <c r="H55" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="I55" s="40">
+        <v>8</v>
+      </c>
       <c r="J55" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K55" s="42"/>
       <c r="L55" s="42"/>
-      <c r="M55" s="79"/>
+      <c r="M55" s="76"/>
       <c r="N55" s="52"/>
-      <c r="O55" s="79"/>
-      <c r="P55" s="79"/>
-      <c r="Q55" s="79"/>
-      <c r="R55" s="122"/>
-      <c r="S55" s="79"/>
-      <c r="T55" s="79"/>
-      <c r="U55" s="79"/>
-      <c r="V55" s="52"/>
-      <c r="W55" s="79"/>
-      <c r="X55" s="79"/>
-      <c r="Y55" s="79"/>
+      <c r="O55" s="76"/>
+      <c r="P55" s="76"/>
+      <c r="Q55" s="76"/>
+      <c r="R55" s="116"/>
+      <c r="S55" s="76"/>
+      <c r="T55" s="42"/>
+      <c r="U55" s="142"/>
+      <c r="V55" s="43"/>
+      <c r="W55" s="76"/>
+      <c r="X55" s="76"/>
+      <c r="Y55" s="76"/>
       <c r="Z55" s="52"/>
-      <c r="AA55" s="121"/>
-      <c r="AB55" s="82"/>
-    </row>
-    <row r="56" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AA55" s="115"/>
+      <c r="AB55" s="79"/>
+    </row>
+    <row r="56" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="35">
-        <v>48</v>
-      </c>
-      <c r="B56" s="75"/>
+        <v>8</v>
+      </c>
+      <c r="B56" s="72"/>
       <c r="C56" s="37"/>
       <c r="D56" s="37"/>
       <c r="E56" s="37"/>
       <c r="F56" s="37"/>
-      <c r="G56" s="77"/>
+      <c r="G56" s="74"/>
       <c r="H56" s="39"/>
       <c r="I56" s="40"/>
       <c r="J56" s="40">
@@ -4508,33 +4864,33 @@
       </c>
       <c r="K56" s="42"/>
       <c r="L56" s="42"/>
-      <c r="M56" s="79"/>
+      <c r="M56" s="76"/>
       <c r="N56" s="52"/>
-      <c r="O56" s="79"/>
-      <c r="P56" s="79"/>
-      <c r="Q56" s="79"/>
-      <c r="R56" s="122"/>
-      <c r="S56" s="79"/>
-      <c r="T56" s="79"/>
-      <c r="U56" s="79"/>
+      <c r="O56" s="76"/>
+      <c r="P56" s="76"/>
+      <c r="Q56" s="76"/>
+      <c r="R56" s="116"/>
+      <c r="S56" s="76"/>
+      <c r="T56" s="76"/>
+      <c r="U56" s="76"/>
       <c r="V56" s="52"/>
-      <c r="W56" s="79"/>
-      <c r="X56" s="79"/>
-      <c r="Y56" s="79"/>
+      <c r="W56" s="76"/>
+      <c r="X56" s="76"/>
+      <c r="Y56" s="76"/>
       <c r="Z56" s="52"/>
-      <c r="AA56" s="121"/>
-      <c r="AB56" s="82"/>
-    </row>
-    <row r="57" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AA56" s="115"/>
+      <c r="AB56" s="79"/>
+    </row>
+    <row r="57" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="35">
-        <v>49</v>
-      </c>
-      <c r="B57" s="75"/>
+        <v>9</v>
+      </c>
+      <c r="B57" s="72"/>
       <c r="C57" s="37"/>
       <c r="D57" s="37"/>
       <c r="E57" s="37"/>
       <c r="F57" s="37"/>
-      <c r="G57" s="77"/>
+      <c r="G57" s="74"/>
       <c r="H57" s="39"/>
       <c r="I57" s="40"/>
       <c r="J57" s="40">
@@ -4543,33 +4899,33 @@
       </c>
       <c r="K57" s="42"/>
       <c r="L57" s="42"/>
-      <c r="M57" s="79"/>
+      <c r="M57" s="76"/>
       <c r="N57" s="52"/>
-      <c r="O57" s="79"/>
-      <c r="P57" s="79"/>
-      <c r="Q57" s="79"/>
-      <c r="R57" s="122"/>
-      <c r="S57" s="79"/>
-      <c r="T57" s="79"/>
-      <c r="U57" s="79"/>
+      <c r="O57" s="76"/>
+      <c r="P57" s="76"/>
+      <c r="Q57" s="76"/>
+      <c r="R57" s="116"/>
+      <c r="S57" s="76"/>
+      <c r="T57" s="76"/>
+      <c r="U57" s="76"/>
       <c r="V57" s="52"/>
-      <c r="W57" s="79"/>
-      <c r="X57" s="79"/>
-      <c r="Y57" s="79"/>
+      <c r="W57" s="76"/>
+      <c r="X57" s="76"/>
+      <c r="Y57" s="76"/>
       <c r="Z57" s="52"/>
-      <c r="AA57" s="121"/>
-      <c r="AB57" s="82"/>
-    </row>
-    <row r="58" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AA57" s="115"/>
+      <c r="AB57" s="79"/>
+    </row>
+    <row r="58" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="35">
-        <v>50</v>
-      </c>
-      <c r="B58" s="75"/>
+        <v>10</v>
+      </c>
+      <c r="B58" s="72"/>
       <c r="C58" s="37"/>
       <c r="D58" s="37"/>
       <c r="E58" s="37"/>
       <c r="F58" s="37"/>
-      <c r="G58" s="77"/>
+      <c r="G58" s="74"/>
       <c r="H58" s="39"/>
       <c r="I58" s="40"/>
       <c r="J58" s="40">
@@ -4578,33 +4934,33 @@
       </c>
       <c r="K58" s="42"/>
       <c r="L58" s="42"/>
-      <c r="M58" s="79"/>
+      <c r="M58" s="76"/>
       <c r="N58" s="52"/>
-      <c r="O58" s="79"/>
-      <c r="P58" s="79"/>
-      <c r="Q58" s="79"/>
-      <c r="R58" s="122"/>
-      <c r="S58" s="79"/>
-      <c r="T58" s="79"/>
-      <c r="U58" s="79"/>
+      <c r="O58" s="76"/>
+      <c r="P58" s="76"/>
+      <c r="Q58" s="76"/>
+      <c r="R58" s="116"/>
+      <c r="S58" s="76"/>
+      <c r="T58" s="76"/>
+      <c r="U58" s="76"/>
       <c r="V58" s="52"/>
-      <c r="W58" s="79"/>
-      <c r="X58" s="79"/>
-      <c r="Y58" s="79"/>
+      <c r="W58" s="76"/>
+      <c r="X58" s="76"/>
+      <c r="Y58" s="76"/>
       <c r="Z58" s="52"/>
-      <c r="AA58" s="121"/>
-      <c r="AB58" s="82"/>
-    </row>
-    <row r="59" spans="1:28" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AA58" s="115"/>
+      <c r="AB58" s="79"/>
+    </row>
+    <row r="59" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="35">
-        <v>51</v>
-      </c>
-      <c r="B59" s="75"/>
+        <v>11</v>
+      </c>
+      <c r="B59" s="72"/>
       <c r="C59" s="37"/>
       <c r="D59" s="37"/>
       <c r="E59" s="37"/>
       <c r="F59" s="37"/>
-      <c r="G59" s="77"/>
+      <c r="G59" s="74"/>
       <c r="H59" s="39"/>
       <c r="I59" s="40"/>
       <c r="J59" s="40">
@@ -4613,446 +4969,527 @@
       </c>
       <c r="K59" s="42"/>
       <c r="L59" s="42"/>
-      <c r="M59" s="79"/>
+      <c r="M59" s="76"/>
       <c r="N59" s="52"/>
-      <c r="O59" s="79"/>
-      <c r="P59" s="79"/>
-      <c r="Q59" s="79"/>
-      <c r="R59" s="122"/>
-      <c r="S59" s="79"/>
-      <c r="T59" s="79"/>
-      <c r="U59" s="79"/>
+      <c r="O59" s="76"/>
+      <c r="P59" s="76"/>
+      <c r="Q59" s="76"/>
+      <c r="R59" s="116"/>
+      <c r="S59" s="76"/>
+      <c r="T59" s="76"/>
+      <c r="U59" s="76"/>
       <c r="V59" s="52"/>
-      <c r="W59" s="79"/>
-      <c r="X59" s="79"/>
-      <c r="Y59" s="79"/>
+      <c r="W59" s="76"/>
+      <c r="X59" s="76"/>
+      <c r="Y59" s="76"/>
       <c r="Z59" s="52"/>
-      <c r="AA59" s="121"/>
-      <c r="AB59" s="82"/>
-    </row>
-    <row r="60" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AA59" s="115"/>
+      <c r="AB59" s="79"/>
+    </row>
+    <row r="60" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="35">
-        <v>52</v>
-      </c>
-      <c r="B60" s="75"/>
+        <v>12</v>
+      </c>
+      <c r="B60" s="72"/>
       <c r="C60" s="37"/>
       <c r="D60" s="37"/>
       <c r="E60" s="37"/>
       <c r="F60" s="37"/>
-      <c r="G60" s="77"/>
+      <c r="G60" s="74"/>
       <c r="H60" s="39"/>
       <c r="I60" s="40"/>
       <c r="J60" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K60" s="94"/>
-      <c r="L60" s="94"/>
-      <c r="M60" s="94"/>
-      <c r="N60" s="95"/>
-      <c r="O60" s="94"/>
-      <c r="P60" s="94"/>
-      <c r="Q60" s="94"/>
-      <c r="R60" s="95"/>
-      <c r="S60" s="94"/>
-      <c r="T60" s="94"/>
-      <c r="U60" s="94"/>
-      <c r="V60" s="95"/>
-      <c r="W60" s="94"/>
-      <c r="X60" s="94"/>
-      <c r="Y60" s="94"/>
-      <c r="Z60" s="95"/>
-      <c r="AA60" s="96">
+      <c r="K60" s="89"/>
+      <c r="L60" s="89"/>
+      <c r="M60" s="89"/>
+      <c r="N60" s="90"/>
+      <c r="O60" s="89"/>
+      <c r="P60" s="89"/>
+      <c r="Q60" s="89"/>
+      <c r="R60" s="90"/>
+      <c r="S60" s="89"/>
+      <c r="T60" s="89"/>
+      <c r="U60" s="89"/>
+      <c r="V60" s="90"/>
+      <c r="W60" s="89"/>
+      <c r="X60" s="89"/>
+      <c r="Y60" s="89"/>
+      <c r="Z60" s="90"/>
+      <c r="AA60" s="91">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB60" s="97"/>
-    </row>
-    <row r="61" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="137" t="s">
-        <v>61</v>
-      </c>
-      <c r="B61" s="137"/>
-      <c r="C61" s="98">
+      <c r="AB60" s="92"/>
+    </row>
+    <row r="61" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="119" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" s="119"/>
+      <c r="C61" s="93">
         <f>SUM(C10:C60)</f>
-        <v>74.5</v>
-      </c>
-      <c r="D61" s="98">
+        <v>83.5</v>
+      </c>
+      <c r="D61" s="93">
         <f>SUM(D10:D60)</f>
         <v>75</v>
       </c>
-      <c r="E61" s="98">
+      <c r="E61" s="93">
         <f>SUM(E10:E60)</f>
         <v>71.75</v>
       </c>
-      <c r="F61" s="98">
+      <c r="F61" s="93">
         <f>SUM(F10:F60)</f>
-        <v>80</v>
-      </c>
-      <c r="G61" s="99"/>
-      <c r="H61" s="98"/>
-      <c r="I61" s="100"/>
-      <c r="J61" s="98">
+        <v>85</v>
+      </c>
+      <c r="G61" s="94"/>
+      <c r="H61" s="93"/>
+      <c r="I61" s="95"/>
+      <c r="J61" s="93">
         <f t="shared" si="1"/>
-        <v>301.25</v>
-      </c>
-      <c r="K61" s="101"/>
-      <c r="L61" s="101"/>
-      <c r="M61" s="101"/>
-      <c r="N61" s="101"/>
-      <c r="O61" s="101"/>
-      <c r="P61" s="101"/>
-      <c r="Q61" s="101"/>
-      <c r="R61" s="101"/>
-      <c r="S61" s="101"/>
-      <c r="T61" s="101"/>
-      <c r="U61" s="101"/>
-      <c r="V61" s="101"/>
-      <c r="W61" s="101"/>
-      <c r="X61" s="101"/>
-      <c r="Y61" s="101"/>
-      <c r="Z61" s="101"/>
-      <c r="AA61" s="98">
+        <v>315.25</v>
+      </c>
+      <c r="K61" s="96"/>
+      <c r="L61" s="96"/>
+      <c r="M61" s="96"/>
+      <c r="N61" s="96"/>
+      <c r="O61" s="96"/>
+      <c r="P61" s="96"/>
+      <c r="Q61" s="96"/>
+      <c r="R61" s="96"/>
+      <c r="S61" s="96"/>
+      <c r="T61" s="96"/>
+      <c r="U61" s="96"/>
+      <c r="V61" s="96"/>
+      <c r="W61" s="96"/>
+      <c r="X61" s="96"/>
+      <c r="Y61" s="96"/>
+      <c r="Z61" s="96"/>
+      <c r="AA61" s="93">
         <f>SUM(AA10:AA60)</f>
-        <v>13.25</v>
-      </c>
-      <c r="AB61" s="102"/>
-    </row>
-    <row r="62" spans="1:28" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="138" t="s">
-        <v>62</v>
-      </c>
-      <c r="B62" s="138"/>
-      <c r="C62" s="98">
+        <v>8.25</v>
+      </c>
+      <c r="AB61" s="97"/>
+    </row>
+    <row r="62" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="120" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" s="120"/>
+      <c r="C62" s="93">
         <f>135-C61</f>
-        <v>60.5</v>
-      </c>
-      <c r="D62" s="98">
+        <v>51.5</v>
+      </c>
+      <c r="D62" s="93">
         <f>135-D61</f>
         <v>60</v>
       </c>
-      <c r="E62" s="98">
+      <c r="E62" s="93">
         <f>135-E61</f>
         <v>63.25</v>
       </c>
-      <c r="F62" s="98">
+      <c r="F62" s="93">
         <f>135-F61</f>
-        <v>55</v>
-      </c>
-      <c r="G62" s="99"/>
-      <c r="H62" s="98"/>
-      <c r="I62" s="98"/>
-      <c r="J62" s="98">
+        <v>50</v>
+      </c>
+      <c r="G62" s="94"/>
+      <c r="H62" s="93"/>
+      <c r="I62" s="93"/>
+      <c r="J62" s="93">
         <f t="shared" si="1"/>
-        <v>238.75</v>
-      </c>
-      <c r="K62" s="101"/>
-      <c r="L62" s="101"/>
-      <c r="M62" s="101"/>
-      <c r="N62" s="101"/>
-      <c r="O62" s="101"/>
-      <c r="P62" s="101"/>
-      <c r="Q62" s="101"/>
-      <c r="R62" s="101"/>
-      <c r="S62" s="101"/>
-      <c r="T62" s="101"/>
-      <c r="U62" s="101"/>
-      <c r="V62" s="101"/>
-      <c r="W62" s="101"/>
-      <c r="X62" s="101"/>
-      <c r="Y62" s="101"/>
-      <c r="Z62" s="101"/>
-      <c r="AA62" s="101"/>
-      <c r="AB62" s="101"/>
-    </row>
-    <row r="63" spans="1:28" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="139" t="s">
+        <v>224.75</v>
+      </c>
+      <c r="K62" s="96"/>
+      <c r="L62" s="96"/>
+      <c r="M62" s="96"/>
+      <c r="N62" s="96"/>
+      <c r="O62" s="96"/>
+      <c r="P62" s="96"/>
+      <c r="Q62" s="96"/>
+      <c r="R62" s="96"/>
+      <c r="S62" s="96"/>
+      <c r="T62" s="96"/>
+      <c r="U62" s="96"/>
+      <c r="V62" s="96"/>
+      <c r="W62" s="96"/>
+      <c r="X62" s="96"/>
+      <c r="Y62" s="96"/>
+      <c r="Z62" s="96"/>
+      <c r="AA62" s="96"/>
+      <c r="AB62" s="96"/>
+    </row>
+    <row r="63" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="121" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="121"/>
+      <c r="C63" s="93"/>
+      <c r="D63" s="93"/>
+      <c r="E63" s="93"/>
+      <c r="F63" s="93"/>
+      <c r="G63" s="93"/>
+      <c r="H63" s="93"/>
+      <c r="I63" s="93"/>
+      <c r="J63" s="93">
+        <f>C63+D63+F63+E63</f>
+        <v>0</v>
+      </c>
+      <c r="K63" s="96"/>
+      <c r="L63" s="96"/>
+      <c r="M63" s="96"/>
+      <c r="N63" s="96"/>
+      <c r="O63" s="96"/>
+      <c r="P63" s="96"/>
+      <c r="Q63" s="96"/>
+      <c r="R63" s="96"/>
+      <c r="S63" s="96"/>
+      <c r="T63" s="96"/>
+      <c r="U63" s="96"/>
+      <c r="V63" s="96"/>
+      <c r="W63" s="96"/>
+      <c r="X63" s="96"/>
+      <c r="Y63" s="96"/>
+      <c r="Z63" s="96"/>
+      <c r="AA63" s="96"/>
+      <c r="AB63" s="96"/>
+    </row>
+    <row r="64" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="120" t="s">
         <v>63</v>
       </c>
-      <c r="B63" s="139"/>
-      <c r="C63" s="98"/>
-      <c r="D63" s="98"/>
-      <c r="E63" s="98"/>
-      <c r="F63" s="98"/>
-      <c r="G63" s="98"/>
-      <c r="H63" s="98"/>
-      <c r="I63" s="98"/>
-      <c r="J63" s="98">
-        <f>C63+D63+F63+E63</f>
-        <v>0</v>
-      </c>
-      <c r="K63" s="101"/>
-      <c r="L63" s="101"/>
-      <c r="M63" s="101"/>
-      <c r="N63" s="101"/>
-      <c r="O63" s="101"/>
-      <c r="P63" s="101"/>
-      <c r="Q63" s="101"/>
-      <c r="R63" s="101"/>
-      <c r="S63" s="101"/>
-      <c r="T63" s="101"/>
-      <c r="U63" s="101"/>
-      <c r="V63" s="101"/>
-      <c r="W63" s="101"/>
-      <c r="X63" s="101"/>
-      <c r="Y63" s="101"/>
-      <c r="Z63" s="101"/>
-      <c r="AA63" s="101"/>
-      <c r="AB63" s="101"/>
-    </row>
-    <row r="64" spans="1:28" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="138" t="s">
+      <c r="B64" s="120"/>
+      <c r="C64" s="93"/>
+      <c r="D64" s="93"/>
+      <c r="E64" s="98"/>
+      <c r="F64" s="93"/>
+      <c r="G64" s="93"/>
+      <c r="H64" s="93"/>
+      <c r="I64" s="99">
+        <f>SUM(I10:I60)</f>
+        <v>368</v>
+      </c>
+      <c r="J64" s="93">
+        <f>SUM(J10:J60)</f>
+        <v>315.25</v>
+      </c>
+      <c r="K64" s="96"/>
+      <c r="L64" s="96"/>
+      <c r="M64" s="96"/>
+      <c r="N64" s="96"/>
+      <c r="O64" s="96"/>
+      <c r="P64" s="96"/>
+      <c r="Q64" s="96"/>
+      <c r="R64" s="96"/>
+      <c r="S64" s="96"/>
+      <c r="T64" s="96"/>
+      <c r="U64" s="96"/>
+      <c r="V64" s="96"/>
+      <c r="W64" s="96"/>
+      <c r="X64" s="96"/>
+      <c r="Y64" s="96"/>
+      <c r="Z64" s="96"/>
+      <c r="AA64" s="96"/>
+      <c r="AB64" s="96"/>
+    </row>
+    <row r="65" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A65" s="100"/>
+      <c r="B65" s="100"/>
+      <c r="C65" s="101"/>
+      <c r="D65" s="101"/>
+      <c r="E65" s="101"/>
+      <c r="F65" s="101"/>
+      <c r="G65" s="101"/>
+      <c r="H65" s="101"/>
+      <c r="I65" s="101"/>
+      <c r="J65" s="101"/>
+      <c r="K65" s="96"/>
+      <c r="L65" s="96"/>
+      <c r="M65" s="96"/>
+      <c r="N65" s="96"/>
+      <c r="O65" s="96"/>
+      <c r="P65" s="96"/>
+      <c r="Q65" s="96"/>
+      <c r="R65" s="96"/>
+      <c r="S65" s="96"/>
+      <c r="T65" s="96"/>
+      <c r="U65" s="96"/>
+      <c r="V65" s="96"/>
+      <c r="W65" s="96"/>
+      <c r="X65" s="96"/>
+      <c r="Y65" s="96"/>
+      <c r="Z65" s="96"/>
+      <c r="AA65" s="96"/>
+      <c r="AB65" s="96"/>
+    </row>
+    <row r="66" spans="1:28" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="121" t="s">
         <v>64</v>
       </c>
-      <c r="B64" s="138"/>
-      <c r="C64" s="98"/>
-      <c r="D64" s="98"/>
-      <c r="E64" s="103"/>
-      <c r="F64" s="98"/>
-      <c r="G64" s="98"/>
-      <c r="H64" s="98"/>
-      <c r="I64" s="104">
-        <f>SUM(I10:I60)</f>
-        <v>320</v>
-      </c>
-      <c r="J64" s="98">
-        <f>SUM(J10:J60)</f>
-        <v>301.25</v>
-      </c>
-      <c r="K64" s="101"/>
-      <c r="L64" s="101"/>
-      <c r="M64" s="101"/>
-      <c r="N64" s="101"/>
-      <c r="O64" s="101"/>
-      <c r="P64" s="101"/>
-      <c r="Q64" s="101"/>
-      <c r="R64" s="101"/>
-      <c r="S64" s="101"/>
-      <c r="T64" s="101"/>
-      <c r="U64" s="101"/>
-      <c r="V64" s="101"/>
-      <c r="W64" s="101"/>
-      <c r="X64" s="101"/>
-      <c r="Y64" s="101"/>
-      <c r="Z64" s="101"/>
-      <c r="AA64" s="101"/>
-      <c r="AB64" s="101"/>
-    </row>
-    <row r="65" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="105"/>
-      <c r="B65" s="105"/>
-      <c r="C65" s="106"/>
-      <c r="D65" s="106"/>
-      <c r="E65" s="106"/>
-      <c r="F65" s="106"/>
-      <c r="G65" s="106"/>
-      <c r="H65" s="106"/>
-      <c r="I65" s="106"/>
-      <c r="J65" s="106"/>
-      <c r="K65" s="101"/>
-      <c r="L65" s="101"/>
-      <c r="M65" s="101"/>
-      <c r="N65" s="101"/>
-      <c r="O65" s="101"/>
-      <c r="P65" s="101"/>
-      <c r="Q65" s="101"/>
-      <c r="R65" s="101"/>
-      <c r="S65" s="101"/>
-      <c r="T65" s="101"/>
-      <c r="U65" s="101"/>
-      <c r="V65" s="101"/>
-      <c r="W65" s="101"/>
-      <c r="X65" s="101"/>
-      <c r="Y65" s="101"/>
-      <c r="Z65" s="101"/>
-      <c r="AA65" s="101"/>
-      <c r="AB65" s="101"/>
-    </row>
-    <row r="66" spans="1:28" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="139" t="s">
-        <v>65</v>
-      </c>
-      <c r="B66" s="139"/>
-      <c r="C66" s="98">
+      <c r="B66" s="121"/>
+      <c r="C66" s="93">
         <f>135*4</f>
         <v>540</v>
       </c>
-      <c r="D66" s="106"/>
-      <c r="E66" s="106"/>
-      <c r="F66" s="106"/>
-      <c r="G66" s="106"/>
-      <c r="H66" s="106"/>
-      <c r="I66" s="106"/>
-      <c r="J66" s="106"/>
-      <c r="K66" s="101"/>
-      <c r="L66" s="101"/>
-      <c r="M66" s="101"/>
-      <c r="N66" s="101"/>
-      <c r="O66" s="101"/>
-      <c r="P66" s="101"/>
-      <c r="Q66" s="101"/>
-      <c r="R66" s="101"/>
-      <c r="S66" s="101"/>
-      <c r="T66" s="101"/>
-      <c r="U66" s="101"/>
-      <c r="V66" s="101"/>
-      <c r="W66" s="101"/>
-      <c r="X66" s="101"/>
-      <c r="Y66" s="101"/>
-      <c r="Z66" s="101"/>
-      <c r="AA66" s="101"/>
-      <c r="AB66" s="101"/>
-    </row>
-    <row r="67" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="136" t="s">
-        <v>66</v>
-      </c>
-      <c r="B67" s="136"/>
-      <c r="C67" s="98">
+      <c r="D66" s="101"/>
+      <c r="E66" s="101"/>
+      <c r="F66" s="101"/>
+      <c r="G66" s="101"/>
+      <c r="H66" s="101"/>
+      <c r="I66" s="101"/>
+      <c r="J66" s="101"/>
+      <c r="K66" s="96"/>
+      <c r="L66" s="96"/>
+      <c r="M66" s="96"/>
+      <c r="N66" s="96"/>
+      <c r="O66" s="96"/>
+      <c r="P66" s="96"/>
+      <c r="Q66" s="96"/>
+      <c r="R66" s="96"/>
+      <c r="S66" s="96"/>
+      <c r="T66" s="96"/>
+      <c r="U66" s="96"/>
+      <c r="V66" s="96"/>
+      <c r="W66" s="96"/>
+      <c r="X66" s="96"/>
+      <c r="Y66" s="96"/>
+      <c r="Z66" s="96"/>
+      <c r="AA66" s="96"/>
+      <c r="AB66" s="96"/>
+    </row>
+    <row r="67" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="118" t="s">
+        <v>65</v>
+      </c>
+      <c r="B67" s="118"/>
+      <c r="C67" s="93">
         <f>C66-J64</f>
-        <v>238.75</v>
-      </c>
-      <c r="D67" s="106"/>
-      <c r="E67" s="106"/>
-      <c r="F67" s="106"/>
-      <c r="G67" s="106"/>
-      <c r="H67" s="106"/>
-      <c r="I67" s="106"/>
-      <c r="J67" s="106"/>
-      <c r="K67" s="101"/>
-      <c r="L67" s="101"/>
-      <c r="M67" s="101"/>
-      <c r="N67" s="101"/>
-      <c r="O67" s="101"/>
-      <c r="P67" s="101"/>
-      <c r="Q67" s="101"/>
-      <c r="R67" s="101"/>
-      <c r="S67" s="101"/>
-      <c r="T67" s="101"/>
-      <c r="U67" s="101"/>
-      <c r="V67" s="101"/>
-      <c r="W67" s="101"/>
-      <c r="X67" s="101"/>
-      <c r="Y67" s="101"/>
-      <c r="Z67" s="101"/>
-      <c r="AA67" s="101"/>
-      <c r="AB67" s="101"/>
-    </row>
-    <row r="68" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="107"/>
-      <c r="B68" s="105"/>
-      <c r="C68" s="108"/>
-      <c r="D68" s="108"/>
-      <c r="E68" s="108"/>
-      <c r="F68" s="108"/>
-      <c r="G68" s="105"/>
-      <c r="H68" s="109"/>
-      <c r="I68" s="110"/>
-      <c r="J68" s="110"/>
-      <c r="AA68" s="101"/>
-    </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="D69" s="111"/>
-      <c r="E69" s="111"/>
-      <c r="F69" s="111"/>
-    </row>
-    <row r="70" spans="1:28" s="113" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A70" s="112"/>
-      <c r="C70" s="114"/>
-      <c r="D70" s="114"/>
-      <c r="E70" s="114"/>
-      <c r="F70" s="114"/>
-      <c r="H70" s="115"/>
-      <c r="I70" s="116"/>
-      <c r="J70" s="116"/>
-      <c r="N70" s="117"/>
-      <c r="R70" s="117"/>
-      <c r="V70" s="117"/>
-      <c r="Z70" s="117"/>
-      <c r="AA70" s="118"/>
-    </row>
-    <row r="71" spans="1:28" s="113" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C71" s="114"/>
-      <c r="D71" s="114"/>
-      <c r="E71" s="114"/>
-      <c r="F71" s="114"/>
-      <c r="H71" s="115"/>
-      <c r="I71" s="116"/>
-      <c r="J71" s="116"/>
-      <c r="N71" s="117"/>
-      <c r="R71" s="117"/>
-      <c r="V71" s="117"/>
-      <c r="Z71" s="117"/>
-      <c r="AA71" s="118"/>
-    </row>
-    <row r="72" spans="1:28" s="113" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C72" s="114"/>
-      <c r="D72" s="114"/>
-      <c r="E72" s="114"/>
-      <c r="F72" s="114"/>
-      <c r="H72" s="115"/>
-      <c r="I72" s="116"/>
-      <c r="J72" s="116"/>
-      <c r="N72" s="117"/>
-      <c r="R72" s="117"/>
-      <c r="V72" s="117"/>
-      <c r="Z72" s="117"/>
-      <c r="AA72" s="118"/>
+        <v>224.75</v>
+      </c>
+      <c r="D67" s="101"/>
+      <c r="E67" s="101"/>
+      <c r="F67" s="101"/>
+      <c r="G67" s="101"/>
+      <c r="H67" s="101"/>
+      <c r="I67" s="101"/>
+      <c r="J67" s="101"/>
+      <c r="K67" s="96"/>
+      <c r="L67" s="96"/>
+      <c r="M67" s="96"/>
+      <c r="N67" s="96"/>
+      <c r="O67" s="96"/>
+      <c r="P67" s="96"/>
+      <c r="Q67" s="96"/>
+      <c r="R67" s="96"/>
+      <c r="S67" s="96"/>
+      <c r="T67" s="96"/>
+      <c r="U67" s="96"/>
+      <c r="V67" s="96"/>
+      <c r="W67" s="96"/>
+      <c r="X67" s="96"/>
+      <c r="Y67" s="96"/>
+      <c r="Z67" s="96"/>
+      <c r="AA67" s="96"/>
+      <c r="AB67" s="96"/>
+    </row>
+    <row r="68" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A68" s="102"/>
+      <c r="B68" s="100"/>
+      <c r="C68" s="103"/>
+      <c r="D68" s="103"/>
+      <c r="E68" s="103"/>
+      <c r="F68" s="103"/>
+      <c r="G68" s="100"/>
+      <c r="H68" s="104"/>
+      <c r="I68" s="105"/>
+      <c r="J68" s="105"/>
+      <c r="AA68" s="96"/>
+    </row>
+    <row r="69" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="D69" s="106"/>
+      <c r="E69" s="106"/>
+      <c r="F69" s="106"/>
+    </row>
+    <row r="70" spans="1:28" s="108" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="A70" s="107"/>
+      <c r="C70" s="109"/>
+      <c r="D70" s="109"/>
+      <c r="E70" s="109"/>
+      <c r="F70" s="109"/>
+      <c r="H70" s="110"/>
+      <c r="I70" s="111"/>
+      <c r="J70" s="111"/>
+      <c r="N70" s="112"/>
+      <c r="R70" s="112"/>
+      <c r="V70" s="112"/>
+      <c r="Z70" s="112"/>
+      <c r="AA70" s="113"/>
+    </row>
+    <row r="71" spans="1:28" s="108" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="C71" s="109"/>
+      <c r="D71" s="109"/>
+      <c r="E71" s="109"/>
+      <c r="F71" s="109"/>
+      <c r="H71" s="110"/>
+      <c r="I71" s="111"/>
+      <c r="J71" s="111"/>
+      <c r="N71" s="112"/>
+      <c r="R71" s="112"/>
+      <c r="V71" s="112"/>
+      <c r="Z71" s="112"/>
+      <c r="AA71" s="113"/>
+    </row>
+    <row r="72" spans="1:28" s="108" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="C72" s="109"/>
+      <c r="D72" s="109"/>
+      <c r="E72" s="109"/>
+      <c r="F72" s="109"/>
+      <c r="H72" s="110"/>
+      <c r="I72" s="111"/>
+      <c r="J72" s="111"/>
+      <c r="N72" s="112"/>
+      <c r="R72" s="112"/>
+      <c r="V72" s="112"/>
+      <c r="Z72" s="112"/>
+      <c r="AA72" s="113"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:Z7"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
     <mergeCell ref="A67:B67"/>
     <mergeCell ref="A61:B61"/>
     <mergeCell ref="A62:B62"/>
     <mergeCell ref="A63:B63"/>
     <mergeCell ref="A64:B64"/>
     <mergeCell ref="A66:B66"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:Z7"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K6:R6"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="28" priority="23" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H19)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H9:H60">
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="En attente">
+  <conditionalFormatting sqref="H9:H45 H49 H56:H60 H47">
+    <cfRule type="containsText" dxfId="27" priority="24" operator="containsText" text="En attente">
       <formula>NOT(ISERROR(SEARCH("En attente",H9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="26" priority="25" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",H9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9:F60">
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+  <conditionalFormatting sqref="C9:F45 C49:F49 C56:F60 C47:F47">
+    <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="7">
+    <cfRule type="expression" dxfId="23" priority="28">
       <formula>$H9="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9:F60">
-    <cfRule type="expression" dxfId="1" priority="8">
+  <conditionalFormatting sqref="C9:F45 C49:F49 C56:F60 C47:F47">
+    <cfRule type="expression" dxfId="22" priority="29">
       <formula>$H9="En cours"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="9">
+    <cfRule type="expression" dxfId="21" priority="30">
       <formula>$H9="En attente"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H48">
+    <cfRule type="containsText" dxfId="20" priority="15" operator="containsText" text="En attente">
+      <formula>NOT(ISERROR(SEARCH("En attente",H48)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="16" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",H48)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="17" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",H48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48:F48">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="19">
+      <formula>$H48="Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48:F48">
+    <cfRule type="expression" dxfId="15" priority="20">
+      <formula>$H48="En cours"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="21">
+      <formula>$H48="En attente"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H50:H55">
+    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="En attente">
+      <formula>NOT(ISERROR(SEARCH("En attente",H50)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",H50)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",H50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50:F55">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="12">
+      <formula>$H50="Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50:F55">
+    <cfRule type="expression" dxfId="8" priority="13">
+      <formula>$H50="En cours"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="14">
+      <formula>$H50="En attente"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H46">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="En attente">
+      <formula>NOT(ISERROR(SEARCH("En attente",H46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",H46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",H46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C46:F46">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="5">
+      <formula>$H46="Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C46:F46">
+    <cfRule type="expression" dxfId="1" priority="6">
+      <formula>$H46="En cours"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="7">
+      <formula>$H46="En attente"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -5065,7 +5502,7 @@
   <pageMargins left="0.31527777777777799" right="0.31527777777777799" top="0.74791666666666701" bottom="0.55138888888888904" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="J10:J60" unlockedFormula="1"/>
+    <ignoredError sqref="J10:J45 J47 J51:J60" unlockedFormula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -5078,20 +5515,20 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="10.7109375" style="1"/>
+    <col min="1" max="1025" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="119" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="119">
+      <c r="B1" s="114">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -5099,7 +5536,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -5119,9 +5556,9 @@
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="10.7109375" style="1"/>
+    <col min="1" max="1025" width="10.6640625" style="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Updated Semainier for this week
</commit_message>
<xml_diff>
--- a/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
+++ b/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Desktop/marque-sans-nom/Semainiers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abourdeau\source\repos\mrjrdg\marque-sans-nom\Semainiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4D3CC7-15B0-B442-93A0-DE1E3A7477A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B80EA8-BD2F-4DCC-8EC0-0E12E04660BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="77">
   <si>
     <t>UQÀM - Hiver 2020</t>
   </si>
@@ -97,9 +99,6 @@
   </si>
   <si>
     <t>Philippe</t>
-  </si>
-  <si>
-    <t>Alex. H</t>
   </si>
   <si>
     <t>Jordan</t>
@@ -322,10 +321,16 @@
     <t>Babillards de commentaires</t>
   </si>
   <si>
-    <t>Alex . D</t>
-  </si>
-  <si>
     <t>Page Contact</t>
+  </si>
+  <si>
+    <t>Alex D.</t>
+  </si>
+  <si>
+    <t>Alex B.</t>
+  </si>
+  <si>
+    <t>SPRINT 2</t>
   </si>
 </sst>
 </file>
@@ -338,7 +343,7 @@
     <numFmt numFmtId="166" formatCode="[$-C0C]dd/mmm"/>
     <numFmt numFmtId="167" formatCode="\\;;;"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -491,8 +496,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -535,8 +547,14 @@
         <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF9999FF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="33">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -946,6 +964,30 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -960,7 +1002,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1089,10 +1131,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="2" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="167" fontId="14" fillId="0" borderId="16" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
@@ -1125,10 +1163,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1137,19 +1171,14 @@
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="167" fontId="14" fillId="7" borderId="16" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="167" fontId="15" fillId="0" borderId="16" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1168,7 +1197,6 @@
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="4" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="167" fontId="15" fillId="0" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
@@ -1230,7 +1258,6 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="8" applyBorder="1"/>
     <xf numFmtId="167" fontId="14" fillId="0" borderId="8" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
@@ -1300,6 +1327,67 @@
     <xf numFmtId="166" fontId="20" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="5" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="5" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="5" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="7" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1310,76 +1398,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="4" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="4" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="5" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="5" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="5" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="7" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Excel Built-in 60% - Accent4" xfId="7" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Excel Built-in Bad" xfId="6" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Excel Built-in Good" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Excel Built-in Good 1" xfId="8" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Excel Built-in Neutral" xfId="5" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Excel Built-in Normal" xfId="3" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Milliers" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
@@ -1744,7 +1790,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2045,51 +2091,51 @@
   </sheetPr>
   <dimension ref="A1:AMK72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="W49" sqref="W49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="66.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="2" customWidth="1"/>
-    <col min="4" max="5" width="8.1640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="66.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="2" customWidth="1"/>
+    <col min="4" max="5" width="8.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" style="3" customWidth="1"/>
-    <col min="9" max="10" width="9.33203125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" style="3" customWidth="1"/>
+    <col min="9" max="10" width="9.28515625" style="4" customWidth="1"/>
     <col min="11" max="13" width="8" style="1" customWidth="1"/>
     <col min="14" max="14" width="8" style="5" customWidth="1"/>
-    <col min="15" max="16" width="7.6640625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="9.6640625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="7.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.6640625" style="6" customWidth="1"/>
-    <col min="28" max="28" width="22.6640625" style="1" customWidth="1"/>
-    <col min="29" max="1025" width="10.6640625" style="1"/>
+    <col min="15" max="16" width="7.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.7109375" style="6" customWidth="1"/>
+    <col min="28" max="28" width="22.7109375" style="1" customWidth="1"/>
+    <col min="29" max="1025" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="8" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="131" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="131"/>
+    <row r="1" spans="1:28" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="119" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="119"/>
       <c r="C1" s="7"/>
-      <c r="D1" s="132" t="s">
+      <c r="D1" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
-      <c r="J1" s="132"/>
-      <c r="K1" s="132"/>
-      <c r="L1" s="132"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
+      <c r="I1" s="120"/>
+      <c r="J1" s="120"/>
+      <c r="K1" s="120"/>
+      <c r="L1" s="120"/>
       <c r="N1" s="3"/>
       <c r="P1" s="9"/>
       <c r="Q1" s="8" t="s">
@@ -2100,21 +2146,21 @@
       <c r="Z1" s="3"/>
       <c r="AA1" s="10"/>
     </row>
-    <row r="2" spans="1:28" s="8" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="131" t="s">
+    <row r="2" spans="1:28" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="131"/>
+      <c r="B2" s="119"/>
       <c r="C2" s="7"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="131" t="s">
+      <c r="F2" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="131"/>
-      <c r="H2" s="131"/>
-      <c r="I2" s="131"/>
-      <c r="J2" s="131"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="119"/>
+      <c r="I2" s="119"/>
+      <c r="J2" s="119"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
       <c r="N2" s="3"/>
@@ -2127,7 +2173,7 @@
       <c r="Z2" s="3"/>
       <c r="AA2" s="10"/>
     </row>
-    <row r="3" spans="1:28" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:28" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -2145,7 +2191,7 @@
       <c r="Z3" s="3"/>
       <c r="AA3" s="10"/>
     </row>
-    <row r="4" spans="1:28" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:28" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
@@ -2165,7 +2211,7 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="10"/>
     </row>
-    <row r="5" spans="1:28" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:28" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
@@ -2189,7 +2235,7 @@
       </c>
       <c r="AA5" s="10"/>
     </row>
-    <row r="6" spans="1:28" s="8" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:28" s="8" customFormat="1" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
@@ -2197,73 +2243,78 @@
       <c r="H6" s="3"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="133" t="s">
+      <c r="K6" s="121" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="133"/>
-      <c r="M6" s="133"/>
-      <c r="N6" s="133"/>
-      <c r="O6" s="133"/>
-      <c r="P6" s="133"/>
-      <c r="Q6" s="133"/>
-      <c r="R6" s="133"/>
-      <c r="V6" s="17"/>
+      <c r="L6" s="121"/>
+      <c r="M6" s="121"/>
+      <c r="N6" s="121"/>
+      <c r="O6" s="121"/>
+      <c r="P6" s="121"/>
+      <c r="Q6" s="121"/>
+      <c r="R6" s="121"/>
+      <c r="S6" s="141" t="s">
+        <v>76</v>
+      </c>
+      <c r="T6" s="142"/>
+      <c r="U6" s="142"/>
+      <c r="V6" s="143"/>
       <c r="Z6" s="17"/>
       <c r="AA6" s="10"/>
     </row>
-    <row r="7" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="126" t="s">
+    <row r="7" spans="1:28" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="127" t="s">
+      <c r="B7" s="123" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="128" t="s">
+      <c r="C7" s="124" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="128"/>
-      <c r="E7" s="128"/>
-      <c r="F7" s="128"/>
-      <c r="G7" s="129" t="s">
+      <c r="D7" s="124"/>
+      <c r="E7" s="124"/>
+      <c r="F7" s="124"/>
+      <c r="G7" s="125" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="130" t="s">
+      <c r="H7" s="126" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="122" t="s">
+      <c r="I7" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="122" t="s">
+      <c r="J7" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="123" t="s">
+      <c r="K7" s="128" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="123"/>
-      <c r="M7" s="123"/>
-      <c r="N7" s="123"/>
-      <c r="O7" s="123"/>
-      <c r="P7" s="123"/>
-      <c r="Q7" s="123"/>
-      <c r="R7" s="123"/>
-      <c r="S7" s="123"/>
-      <c r="T7" s="123"/>
-      <c r="U7" s="123"/>
-      <c r="V7" s="123"/>
-      <c r="W7" s="123"/>
-      <c r="X7" s="123"/>
-      <c r="Y7" s="123"/>
-      <c r="Z7" s="123"/>
-      <c r="AA7" s="124" t="s">
+      <c r="L7" s="128"/>
+      <c r="M7" s="128"/>
+      <c r="N7" s="128"/>
+      <c r="O7" s="128"/>
+      <c r="P7" s="128"/>
+      <c r="Q7" s="128"/>
+      <c r="R7" s="128"/>
+      <c r="S7" s="128"/>
+      <c r="T7" s="128"/>
+      <c r="U7" s="128"/>
+      <c r="V7" s="128"/>
+      <c r="W7" s="128"/>
+      <c r="X7" s="128"/>
+      <c r="Y7" s="128"/>
+      <c r="Z7" s="128"/>
+      <c r="AA7" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="AB7" s="125" t="s">
+      <c r="AB7" s="130" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="126"/>
-      <c r="B8" s="127"/>
+    <row r="8" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="122"/>
+      <c r="B8" s="123"/>
       <c r="C8" s="20" t="s">
         <v>74</v>
       </c>
@@ -2271,15 +2322,15 @@
         <v>20</v>
       </c>
       <c r="E8" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="129"/>
-      <c r="H8" s="130"/>
-      <c r="I8" s="122"/>
-      <c r="J8" s="122"/>
+      <c r="G8" s="125"/>
+      <c r="H8" s="126"/>
+      <c r="I8" s="127"/>
+      <c r="J8" s="127"/>
       <c r="K8" s="21">
         <v>43838</v>
       </c>
@@ -2307,49 +2358,49 @@
         <f t="shared" si="0"/>
         <v>43880</v>
       </c>
-      <c r="R8" s="117">
+      <c r="R8" s="109">
         <f t="shared" si="0"/>
         <v>43887</v>
       </c>
-      <c r="S8" s="117">
+      <c r="S8" s="109">
         <f t="shared" si="0"/>
         <v>43894</v>
       </c>
-      <c r="T8" s="117">
+      <c r="T8" s="109">
         <f t="shared" si="0"/>
         <v>43901</v>
       </c>
-      <c r="U8" s="117">
+      <c r="U8" s="109">
         <f t="shared" si="0"/>
         <v>43908</v>
       </c>
-      <c r="V8" s="117">
+      <c r="V8" s="109">
         <f t="shared" si="0"/>
         <v>43915</v>
       </c>
-      <c r="W8" s="117">
+      <c r="W8" s="109">
         <f t="shared" si="0"/>
         <v>43922</v>
       </c>
-      <c r="X8" s="117">
+      <c r="X8" s="109">
         <f t="shared" si="0"/>
         <v>43929</v>
       </c>
-      <c r="Y8" s="117">
+      <c r="Y8" s="109">
         <f t="shared" si="0"/>
         <v>43936</v>
       </c>
-      <c r="Z8" s="117">
+      <c r="Z8" s="109">
         <f t="shared" si="0"/>
         <v>43943</v>
       </c>
-      <c r="AA8" s="124"/>
-      <c r="AB8" s="125"/>
-    </row>
-    <row r="9" spans="1:28" ht="19" x14ac:dyDescent="0.2">
+      <c r="AA8" s="129"/>
+      <c r="AB8" s="130"/>
+    </row>
+    <row r="9" spans="1:28" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="25"/>
@@ -2378,12 +2429,12 @@
       <c r="AA9" s="33"/>
       <c r="AB9" s="34"/>
     </row>
-    <row r="10" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="35">
         <v>1</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="37">
         <v>1.5</v>
@@ -2411,34 +2462,34 @@
         <f t="shared" ref="J10:J62" si="1">SUM(C10:F10)</f>
         <v>6</v>
       </c>
-      <c r="K10" s="41"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="43"/>
-      <c r="O10" s="42"/>
-      <c r="P10" s="42"/>
-      <c r="Q10" s="42"/>
-      <c r="R10" s="43"/>
-      <c r="S10" s="42"/>
-      <c r="T10" s="42"/>
-      <c r="U10" s="42"/>
-      <c r="V10" s="43"/>
-      <c r="W10" s="42"/>
-      <c r="X10" s="42"/>
-      <c r="Y10" s="42"/>
-      <c r="Z10" s="43"/>
-      <c r="AA10" s="44">
+      <c r="K10" s="135"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="42"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="41"/>
+      <c r="R10" s="42"/>
+      <c r="S10" s="41"/>
+      <c r="T10" s="41"/>
+      <c r="U10" s="41"/>
+      <c r="V10" s="42"/>
+      <c r="W10" s="41"/>
+      <c r="X10" s="41"/>
+      <c r="Y10" s="41"/>
+      <c r="Z10" s="42"/>
+      <c r="AA10" s="43">
         <f t="shared" ref="AA10:AA60" si="2">I10-J10</f>
         <v>0</v>
       </c>
-      <c r="AB10" s="45"/>
-    </row>
-    <row r="11" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AB10" s="44"/>
+    </row>
+    <row r="11" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="35">
         <v>2</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="37">
         <v>1.5</v>
@@ -2466,34 +2517,34 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="K11" s="41"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="43"/>
-      <c r="O11" s="42"/>
-      <c r="P11" s="42"/>
-      <c r="Q11" s="42"/>
-      <c r="R11" s="43"/>
-      <c r="S11" s="42"/>
-      <c r="T11" s="42"/>
-      <c r="U11" s="42"/>
-      <c r="V11" s="43"/>
-      <c r="W11" s="42"/>
-      <c r="X11" s="42"/>
-      <c r="Y11" s="42"/>
-      <c r="Z11" s="47"/>
-      <c r="AA11" s="44">
+      <c r="K11" s="135"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="42"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="41"/>
+      <c r="R11" s="42"/>
+      <c r="S11" s="41"/>
+      <c r="T11" s="41"/>
+      <c r="U11" s="41"/>
+      <c r="V11" s="42"/>
+      <c r="W11" s="41"/>
+      <c r="X11" s="41"/>
+      <c r="Y11" s="41"/>
+      <c r="Z11" s="46"/>
+      <c r="AA11" s="43">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB11" s="48"/>
-    </row>
-    <row r="12" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AB11" s="47"/>
+    </row>
+    <row r="12" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="35">
         <v>3</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="37">
         <v>3</v>
@@ -2521,33 +2572,33 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="K12" s="42"/>
-      <c r="L12" s="41"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="42"/>
-      <c r="P12" s="42"/>
-      <c r="Q12" s="42"/>
-      <c r="R12" s="43"/>
-      <c r="S12" s="42"/>
-      <c r="T12" s="42"/>
-      <c r="U12" s="42"/>
-      <c r="V12" s="43"/>
-      <c r="W12" s="42"/>
-      <c r="X12" s="42"/>
-      <c r="Y12" s="42"/>
-      <c r="Z12" s="43"/>
-      <c r="AA12" s="44">
+      <c r="K12" s="41"/>
+      <c r="L12" s="135"/>
+      <c r="N12" s="42"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="41"/>
+      <c r="R12" s="42"/>
+      <c r="S12" s="41"/>
+      <c r="T12" s="41"/>
+      <c r="U12" s="41"/>
+      <c r="V12" s="42"/>
+      <c r="W12" s="41"/>
+      <c r="X12" s="41"/>
+      <c r="Y12" s="41"/>
+      <c r="Z12" s="42"/>
+      <c r="AA12" s="43">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB12" s="49"/>
-    </row>
-    <row r="13" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB12" s="48"/>
+    </row>
+    <row r="13" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="35">
         <v>4</v>
       </c>
-      <c r="B13" s="50" t="s">
-        <v>27</v>
+      <c r="B13" s="49" t="s">
+        <v>26</v>
       </c>
       <c r="C13" s="37">
         <v>2</v>
@@ -2575,34 +2626,34 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="K13" s="42"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="43"/>
-      <c r="O13" s="42"/>
-      <c r="P13" s="42"/>
-      <c r="Q13" s="42"/>
-      <c r="R13" s="43"/>
-      <c r="S13" s="42"/>
-      <c r="T13" s="42"/>
-      <c r="U13" s="42"/>
-      <c r="V13" s="43"/>
-      <c r="W13" s="42"/>
-      <c r="X13" s="42"/>
-      <c r="Y13" s="42"/>
-      <c r="Z13" s="43"/>
-      <c r="AA13" s="44">
+      <c r="K13" s="41"/>
+      <c r="L13" s="135"/>
+      <c r="M13" s="135"/>
+      <c r="N13" s="42"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="41"/>
+      <c r="R13" s="42"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
+      <c r="U13" s="41"/>
+      <c r="V13" s="42"/>
+      <c r="W13" s="41"/>
+      <c r="X13" s="41"/>
+      <c r="Y13" s="41"/>
+      <c r="Z13" s="42"/>
+      <c r="AA13" s="43">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB13" s="48"/>
-    </row>
-    <row r="14" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB13" s="47"/>
+    </row>
+    <row r="14" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="35">
         <v>5</v>
       </c>
-      <c r="B14" s="50" t="s">
-        <v>28</v>
+      <c r="B14" s="49" t="s">
+        <v>27</v>
       </c>
       <c r="C14" s="37">
         <v>3</v>
@@ -2630,34 +2681,34 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="K14" s="42"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="43"/>
-      <c r="O14" s="42"/>
-      <c r="P14" s="42"/>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="43"/>
-      <c r="S14" s="42"/>
-      <c r="T14" s="42"/>
-      <c r="U14" s="42"/>
-      <c r="V14" s="43"/>
-      <c r="W14" s="42"/>
-      <c r="X14" s="42"/>
-      <c r="Y14" s="42"/>
-      <c r="Z14" s="43"/>
-      <c r="AA14" s="44">
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="135"/>
+      <c r="N14" s="42"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="41"/>
+      <c r="R14" s="42"/>
+      <c r="S14" s="41"/>
+      <c r="T14" s="41"/>
+      <c r="U14" s="41"/>
+      <c r="V14" s="42"/>
+      <c r="W14" s="41"/>
+      <c r="X14" s="41"/>
+      <c r="Y14" s="41"/>
+      <c r="Z14" s="42"/>
+      <c r="AA14" s="43">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB14" s="48"/>
-    </row>
-    <row r="15" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB14" s="47"/>
+    </row>
+    <row r="15" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="35">
         <v>6</v>
       </c>
-      <c r="B15" s="50" t="s">
-        <v>29</v>
+      <c r="B15" s="49" t="s">
+        <v>28</v>
       </c>
       <c r="C15" s="37">
         <v>2</v>
@@ -2685,34 +2736,34 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K15" s="42"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="51"/>
-      <c r="N15" s="52"/>
-      <c r="O15" s="42"/>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="43"/>
-      <c r="S15" s="42"/>
-      <c r="T15" s="42"/>
-      <c r="U15" s="42"/>
-      <c r="V15" s="43"/>
-      <c r="W15" s="42"/>
-      <c r="X15" s="42"/>
-      <c r="Y15" s="42"/>
-      <c r="Z15" s="43"/>
-      <c r="AA15" s="44">
+      <c r="K15" s="41"/>
+      <c r="L15" s="135"/>
+      <c r="M15" s="50"/>
+      <c r="N15" s="51"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="41"/>
+      <c r="Q15" s="41"/>
+      <c r="R15" s="42"/>
+      <c r="S15" s="41"/>
+      <c r="T15" s="41"/>
+      <c r="U15" s="41"/>
+      <c r="V15" s="42"/>
+      <c r="W15" s="41"/>
+      <c r="X15" s="41"/>
+      <c r="Y15" s="41"/>
+      <c r="Z15" s="42"/>
+      <c r="AA15" s="43">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB15" s="48"/>
-    </row>
-    <row r="16" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB15" s="47"/>
+    </row>
+    <row r="16" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="35">
         <v>7</v>
       </c>
-      <c r="B16" s="50" t="s">
-        <v>30</v>
+      <c r="B16" s="49" t="s">
+        <v>29</v>
       </c>
       <c r="C16" s="37">
         <v>2</v>
@@ -2740,34 +2791,34 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="K16" s="42"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="53"/>
-      <c r="N16" s="54"/>
-      <c r="O16" s="55"/>
-      <c r="P16" s="55"/>
-      <c r="Q16" s="55"/>
-      <c r="R16" s="56"/>
-      <c r="S16" s="55"/>
-      <c r="T16" s="55"/>
-      <c r="U16" s="57"/>
-      <c r="V16" s="43"/>
-      <c r="W16" s="42"/>
-      <c r="X16" s="42"/>
-      <c r="Y16" s="42"/>
-      <c r="Z16" s="43"/>
-      <c r="AA16" s="44">
+      <c r="K16" s="41"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="136"/>
+      <c r="N16" s="136"/>
+      <c r="O16" s="52"/>
+      <c r="P16" s="52"/>
+      <c r="Q16" s="52"/>
+      <c r="R16" s="53"/>
+      <c r="S16" s="52"/>
+      <c r="T16" s="52"/>
+      <c r="U16" s="54"/>
+      <c r="V16" s="42"/>
+      <c r="W16" s="41"/>
+      <c r="X16" s="41"/>
+      <c r="Y16" s="41"/>
+      <c r="Z16" s="42"/>
+      <c r="AA16" s="43">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="AB16" s="48"/>
-    </row>
-    <row r="17" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB16" s="47"/>
+    </row>
+    <row r="17" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="35">
         <v>8</v>
       </c>
-      <c r="B17" s="50" t="s">
-        <v>31</v>
+      <c r="B17" s="49" t="s">
+        <v>30</v>
       </c>
       <c r="C17" s="37">
         <v>2</v>
@@ -2795,34 +2846,34 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K17" s="42"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="58"/>
-      <c r="N17" s="47"/>
-      <c r="O17" s="55"/>
-      <c r="P17" s="55"/>
-      <c r="Q17" s="55"/>
-      <c r="R17" s="56"/>
-      <c r="S17" s="55"/>
-      <c r="T17" s="55"/>
-      <c r="U17" s="57"/>
-      <c r="V17" s="43"/>
-      <c r="W17" s="42"/>
-      <c r="X17" s="42"/>
-      <c r="Y17" s="42"/>
-      <c r="Z17" s="59"/>
-      <c r="AA17" s="44">
+      <c r="K17" s="41"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="136"/>
+      <c r="N17" s="46"/>
+      <c r="O17" s="52"/>
+      <c r="P17" s="52"/>
+      <c r="Q17" s="52"/>
+      <c r="R17" s="53"/>
+      <c r="S17" s="52"/>
+      <c r="T17" s="52"/>
+      <c r="U17" s="54"/>
+      <c r="V17" s="42"/>
+      <c r="W17" s="41"/>
+      <c r="X17" s="41"/>
+      <c r="Y17" s="41"/>
+      <c r="Z17" s="55"/>
+      <c r="AA17" s="43">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB17" s="48"/>
-    </row>
-    <row r="18" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB17" s="47"/>
+    </row>
+    <row r="18" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="35">
         <v>9</v>
       </c>
-      <c r="B18" s="50" t="s">
-        <v>32</v>
+      <c r="B18" s="49" t="s">
+        <v>31</v>
       </c>
       <c r="C18" s="37">
         <v>2</v>
@@ -2850,34 +2901,34 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K18" s="42"/>
-      <c r="L18" s="60"/>
-      <c r="M18" s="61"/>
-      <c r="N18" s="62"/>
-      <c r="O18" s="55"/>
-      <c r="P18" s="55"/>
-      <c r="Q18" s="55"/>
-      <c r="R18" s="61"/>
-      <c r="S18" s="55"/>
-      <c r="T18" s="55"/>
-      <c r="U18" s="57"/>
-      <c r="V18" s="43"/>
-      <c r="W18" s="42"/>
-      <c r="X18" s="42"/>
-      <c r="Y18" s="42"/>
-      <c r="Z18" s="43"/>
-      <c r="AA18" s="44">
+      <c r="K18" s="41"/>
+      <c r="L18" s="56"/>
+      <c r="M18" s="138"/>
+      <c r="N18" s="57"/>
+      <c r="O18" s="52"/>
+      <c r="P18" s="52"/>
+      <c r="Q18" s="52"/>
+      <c r="R18" s="138"/>
+      <c r="S18" s="52"/>
+      <c r="T18" s="52"/>
+      <c r="U18" s="54"/>
+      <c r="V18" s="42"/>
+      <c r="W18" s="41"/>
+      <c r="X18" s="41"/>
+      <c r="Y18" s="41"/>
+      <c r="Z18" s="42"/>
+      <c r="AA18" s="43">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="AB18" s="48"/>
-    </row>
-    <row r="19" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB18" s="47"/>
+    </row>
+    <row r="19" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="35">
         <v>10</v>
       </c>
-      <c r="B19" s="50" t="s">
-        <v>33</v>
+      <c r="B19" s="49" t="s">
+        <v>32</v>
       </c>
       <c r="C19" s="37">
         <v>1.5</v>
@@ -2905,34 +2956,34 @@
         <f t="shared" si="1"/>
         <v>10.5</v>
       </c>
-      <c r="K19" s="42"/>
-      <c r="L19" s="60"/>
-      <c r="M19" s="41"/>
-      <c r="N19" s="63"/>
-      <c r="O19" s="55"/>
-      <c r="P19" s="55"/>
-      <c r="Q19" s="64"/>
-      <c r="R19" s="56"/>
-      <c r="S19" s="55"/>
-      <c r="T19" s="55"/>
-      <c r="U19" s="57"/>
-      <c r="V19" s="43"/>
-      <c r="W19" s="42"/>
-      <c r="X19" s="42"/>
-      <c r="Y19" s="42"/>
-      <c r="Z19" s="43"/>
-      <c r="AA19" s="44">
+      <c r="K19" s="41"/>
+      <c r="L19" s="56"/>
+      <c r="M19" s="135"/>
+      <c r="N19" s="137"/>
+      <c r="O19" s="52"/>
+      <c r="P19" s="52"/>
+      <c r="Q19" s="58"/>
+      <c r="R19" s="53"/>
+      <c r="S19" s="52"/>
+      <c r="T19" s="52"/>
+      <c r="U19" s="54"/>
+      <c r="V19" s="42"/>
+      <c r="W19" s="41"/>
+      <c r="X19" s="41"/>
+      <c r="Y19" s="41"/>
+      <c r="Z19" s="42"/>
+      <c r="AA19" s="43">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
-      <c r="AB19" s="48"/>
-    </row>
-    <row r="20" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB19" s="47"/>
+    </row>
+    <row r="20" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="35">
         <v>11</v>
       </c>
-      <c r="B20" s="50" t="s">
-        <v>34</v>
+      <c r="B20" s="49" t="s">
+        <v>33</v>
       </c>
       <c r="C20" s="37">
         <v>0</v>
@@ -2960,34 +3011,34 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="K20" s="42"/>
-      <c r="L20" s="60"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="47"/>
-      <c r="O20" s="55"/>
-      <c r="P20" s="55"/>
-      <c r="Q20" s="55"/>
-      <c r="R20" s="61"/>
-      <c r="S20" s="55"/>
-      <c r="T20" s="55"/>
-      <c r="U20" s="57"/>
-      <c r="V20" s="43"/>
-      <c r="W20" s="42"/>
-      <c r="X20" s="42"/>
-      <c r="Y20" s="42"/>
-      <c r="Z20" s="43"/>
-      <c r="AA20" s="44">
+      <c r="K20" s="41"/>
+      <c r="L20" s="56"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="46"/>
+      <c r="O20" s="52"/>
+      <c r="P20" s="52"/>
+      <c r="Q20" s="52"/>
+      <c r="R20" s="138"/>
+      <c r="S20" s="52"/>
+      <c r="T20" s="52"/>
+      <c r="U20" s="54"/>
+      <c r="V20" s="42"/>
+      <c r="W20" s="41"/>
+      <c r="X20" s="41"/>
+      <c r="Y20" s="41"/>
+      <c r="Z20" s="42"/>
+      <c r="AA20" s="43">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="AB20" s="48"/>
-    </row>
-    <row r="21" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB20" s="47"/>
+    </row>
+    <row r="21" spans="1:28" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="35">
         <v>12</v>
       </c>
-      <c r="B21" s="50" t="s">
-        <v>35</v>
+      <c r="B21" s="49" t="s">
+        <v>34</v>
       </c>
       <c r="C21" s="37">
         <v>3</v>
@@ -3015,34 +3066,34 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="K21" s="42"/>
-      <c r="L21" s="60"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="47"/>
-      <c r="O21" s="55"/>
-      <c r="P21" s="55"/>
-      <c r="Q21" s="55"/>
-      <c r="R21" s="65"/>
-      <c r="S21" s="66"/>
-      <c r="T21" s="66"/>
-      <c r="U21" s="57"/>
-      <c r="V21" s="43"/>
-      <c r="W21" s="42"/>
-      <c r="X21" s="42"/>
-      <c r="Y21" s="42"/>
-      <c r="Z21" s="43"/>
-      <c r="AA21" s="44">
+      <c r="K21" s="41"/>
+      <c r="L21" s="56"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="46"/>
+      <c r="O21" s="52"/>
+      <c r="P21" s="52"/>
+      <c r="Q21" s="52"/>
+      <c r="R21" s="59"/>
+      <c r="S21" s="60"/>
+      <c r="T21" s="60"/>
+      <c r="U21" s="54"/>
+      <c r="V21" s="42"/>
+      <c r="W21" s="41"/>
+      <c r="X21" s="41"/>
+      <c r="Y21" s="41"/>
+      <c r="Z21" s="42"/>
+      <c r="AA21" s="43">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB21" s="48"/>
-    </row>
-    <row r="22" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB21" s="47"/>
+    </row>
+    <row r="22" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="35">
         <v>13</v>
       </c>
-      <c r="B22" s="67" t="s">
-        <v>36</v>
+      <c r="B22" s="61" t="s">
+        <v>35</v>
       </c>
       <c r="C22" s="37">
         <v>3</v>
@@ -3070,34 +3121,34 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="K22" s="68"/>
-      <c r="L22" s="60"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="63"/>
-      <c r="O22" s="68"/>
-      <c r="P22" s="68"/>
-      <c r="Q22" s="69"/>
-      <c r="R22" s="65"/>
-      <c r="S22" s="66"/>
-      <c r="T22" s="66"/>
-      <c r="U22" s="57"/>
-      <c r="V22" s="43"/>
-      <c r="W22" s="42"/>
-      <c r="X22" s="42"/>
-      <c r="Y22" s="42"/>
-      <c r="Z22" s="43"/>
-      <c r="AA22" s="44">
+      <c r="K22" s="62"/>
+      <c r="L22" s="56"/>
+      <c r="M22" s="135"/>
+      <c r="N22" s="137"/>
+      <c r="O22" s="62"/>
+      <c r="P22" s="62"/>
+      <c r="Q22" s="63"/>
+      <c r="R22" s="59"/>
+      <c r="S22" s="60"/>
+      <c r="T22" s="60"/>
+      <c r="U22" s="54"/>
+      <c r="V22" s="42"/>
+      <c r="W22" s="41"/>
+      <c r="X22" s="41"/>
+      <c r="Y22" s="41"/>
+      <c r="Z22" s="42"/>
+      <c r="AA22" s="43">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="AB22" s="48"/>
-    </row>
-    <row r="23" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB22" s="47"/>
+    </row>
+    <row r="23" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="35">
         <v>14</v>
       </c>
-      <c r="B23" s="67" t="s">
-        <v>37</v>
+      <c r="B23" s="61" t="s">
+        <v>36</v>
       </c>
       <c r="C23" s="37">
         <v>0</v>
@@ -3125,34 +3176,34 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="K23" s="68"/>
-      <c r="L23" s="60"/>
-      <c r="M23" s="41"/>
-      <c r="N23" s="41"/>
-      <c r="O23" s="68"/>
-      <c r="P23" s="68"/>
-      <c r="Q23" s="69"/>
-      <c r="R23" s="56"/>
-      <c r="S23" s="66"/>
-      <c r="T23" s="66"/>
-      <c r="U23" s="57"/>
-      <c r="V23" s="43"/>
-      <c r="W23" s="42"/>
-      <c r="X23" s="42"/>
-      <c r="Y23" s="42"/>
-      <c r="Z23" s="43"/>
-      <c r="AA23" s="44">
+      <c r="K23" s="62"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="135"/>
+      <c r="N23" s="135"/>
+      <c r="O23" s="62"/>
+      <c r="P23" s="62"/>
+      <c r="Q23" s="63"/>
+      <c r="R23" s="53"/>
+      <c r="S23" s="60"/>
+      <c r="T23" s="60"/>
+      <c r="U23" s="54"/>
+      <c r="V23" s="42"/>
+      <c r="W23" s="41"/>
+      <c r="X23" s="41"/>
+      <c r="Y23" s="41"/>
+      <c r="Z23" s="42"/>
+      <c r="AA23" s="43">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="AB23" s="48"/>
-    </row>
-    <row r="24" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB23" s="47"/>
+    </row>
+    <row r="24" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="35">
         <v>15</v>
       </c>
-      <c r="B24" s="67" t="s">
-        <v>38</v>
+      <c r="B24" s="61" t="s">
+        <v>37</v>
       </c>
       <c r="C24" s="37">
         <v>1</v>
@@ -3180,34 +3231,34 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="K24" s="68"/>
-      <c r="L24" s="60"/>
-      <c r="M24" s="41"/>
-      <c r="N24" s="41"/>
-      <c r="O24" s="41"/>
-      <c r="P24" s="41"/>
-      <c r="Q24" s="41"/>
-      <c r="R24" s="70"/>
-      <c r="S24" s="55"/>
-      <c r="T24" s="55"/>
-      <c r="U24" s="57"/>
-      <c r="V24" s="43"/>
-      <c r="W24" s="42"/>
-      <c r="X24" s="42"/>
-      <c r="Y24" s="42"/>
-      <c r="Z24" s="43"/>
-      <c r="AA24" s="44">
+      <c r="K24" s="62"/>
+      <c r="L24" s="56"/>
+      <c r="M24" s="135"/>
+      <c r="N24" s="135"/>
+      <c r="O24" s="135"/>
+      <c r="P24" s="135"/>
+      <c r="Q24" s="135"/>
+      <c r="R24" s="136"/>
+      <c r="S24" s="52"/>
+      <c r="T24" s="52"/>
+      <c r="U24" s="54"/>
+      <c r="V24" s="42"/>
+      <c r="W24" s="41"/>
+      <c r="X24" s="41"/>
+      <c r="Y24" s="41"/>
+      <c r="Z24" s="42"/>
+      <c r="AA24" s="43">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="AB24" s="48"/>
-    </row>
-    <row r="25" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB24" s="47"/>
+    </row>
+    <row r="25" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="35">
         <v>16</v>
       </c>
-      <c r="B25" s="67" t="s">
-        <v>39</v>
+      <c r="B25" s="61" t="s">
+        <v>38</v>
       </c>
       <c r="C25" s="37">
         <v>10</v>
@@ -3235,89 +3286,89 @@
         <f t="shared" si="1"/>
         <v>38.5</v>
       </c>
-      <c r="K25" s="68"/>
-      <c r="L25" s="60"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="41"/>
-      <c r="P25" s="71"/>
-      <c r="Q25" s="41"/>
-      <c r="R25" s="134"/>
-      <c r="S25" s="55"/>
-      <c r="T25" s="55"/>
-      <c r="U25" s="57"/>
-      <c r="V25" s="43"/>
-      <c r="W25" s="42"/>
-      <c r="X25" s="42"/>
-      <c r="Y25" s="42"/>
-      <c r="Z25" s="43"/>
-      <c r="AA25" s="44">
+      <c r="K25" s="62"/>
+      <c r="L25" s="56"/>
+      <c r="M25" s="135"/>
+      <c r="N25" s="135"/>
+      <c r="O25" s="135"/>
+      <c r="P25" s="64"/>
+      <c r="Q25" s="135"/>
+      <c r="R25" s="110"/>
+      <c r="S25" s="52"/>
+      <c r="T25" s="52"/>
+      <c r="U25" s="54"/>
+      <c r="V25" s="42"/>
+      <c r="W25" s="41"/>
+      <c r="X25" s="41"/>
+      <c r="Y25" s="41"/>
+      <c r="Z25" s="42"/>
+      <c r="AA25" s="43">
         <f t="shared" si="2"/>
         <v>-8.5</v>
       </c>
-      <c r="AB25" s="48"/>
-    </row>
-    <row r="26" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB25" s="47"/>
+    </row>
+    <row r="26" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="35">
         <v>17</v>
       </c>
-      <c r="B26" s="72" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="73">
-        <v>2</v>
-      </c>
-      <c r="D26" s="73">
-        <v>2</v>
-      </c>
-      <c r="E26" s="73">
-        <v>2</v>
-      </c>
-      <c r="F26" s="73">
-        <v>2</v>
-      </c>
-      <c r="G26" s="74">
+      <c r="B26" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="66">
+        <v>2</v>
+      </c>
+      <c r="D26" s="66">
+        <v>2</v>
+      </c>
+      <c r="E26" s="66">
+        <v>2</v>
+      </c>
+      <c r="F26" s="66">
+        <v>2</v>
+      </c>
+      <c r="G26" s="67">
         <f>VLOOKUP(H26,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
       <c r="H26" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="I26" s="75">
+      <c r="I26" s="68">
         <v>8</v>
       </c>
       <c r="J26" s="40">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="K26" s="76"/>
-      <c r="L26" s="76"/>
-      <c r="M26" s="76"/>
-      <c r="N26" s="52"/>
-      <c r="O26" s="70"/>
-      <c r="P26" s="42"/>
-      <c r="Q26" s="42"/>
-      <c r="R26" s="77"/>
-      <c r="S26" s="78"/>
-      <c r="T26" s="78"/>
-      <c r="U26" s="76"/>
-      <c r="V26" s="52"/>
-      <c r="W26" s="76"/>
-      <c r="X26" s="76"/>
-      <c r="Y26" s="76"/>
-      <c r="Z26" s="52"/>
-      <c r="AA26" s="44">
+      <c r="K26" s="69"/>
+      <c r="L26" s="69"/>
+      <c r="M26" s="69"/>
+      <c r="N26" s="51"/>
+      <c r="O26" s="136"/>
+      <c r="P26" s="41"/>
+      <c r="Q26" s="41"/>
+      <c r="R26" s="70"/>
+      <c r="S26" s="71"/>
+      <c r="T26" s="71"/>
+      <c r="U26" s="69"/>
+      <c r="V26" s="51"/>
+      <c r="W26" s="69"/>
+      <c r="X26" s="69"/>
+      <c r="Y26" s="69"/>
+      <c r="Z26" s="51"/>
+      <c r="AA26" s="43">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB26" s="79"/>
-    </row>
-    <row r="27" spans="1:28" s="82" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB26" s="72"/>
+    </row>
+    <row r="27" spans="1:28" s="75" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="35">
         <v>18</v>
       </c>
-      <c r="B27" s="80" t="s">
-        <v>41</v>
+      <c r="B27" s="73" t="s">
+        <v>40</v>
       </c>
       <c r="C27" s="37">
         <v>3</v>
@@ -3331,62 +3382,62 @@
       <c r="F27" s="37">
         <v>0</v>
       </c>
-      <c r="G27" s="74">
+      <c r="G27" s="67">
         <f>VLOOKUP(H27,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
       <c r="H27" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="I27" s="81">
+      <c r="I27" s="74">
         <v>21</v>
       </c>
       <c r="J27" s="40">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="K27" s="42"/>
-      <c r="L27" s="42"/>
-      <c r="M27" s="42"/>
-      <c r="N27" s="43"/>
-      <c r="O27" s="70"/>
-      <c r="P27" s="42"/>
-      <c r="Q27" s="42"/>
-      <c r="R27" s="43"/>
-      <c r="S27" s="42"/>
-      <c r="T27" s="42"/>
-      <c r="U27" s="42"/>
-      <c r="V27" s="43"/>
-      <c r="W27" s="42"/>
-      <c r="X27" s="42"/>
-      <c r="Y27" s="42"/>
-      <c r="Z27" s="43"/>
-      <c r="AA27" s="44">
+      <c r="K27" s="41"/>
+      <c r="L27" s="41"/>
+      <c r="M27" s="41"/>
+      <c r="N27" s="42"/>
+      <c r="O27" s="136"/>
+      <c r="P27" s="41"/>
+      <c r="Q27" s="41"/>
+      <c r="R27" s="42"/>
+      <c r="S27" s="41"/>
+      <c r="T27" s="41"/>
+      <c r="U27" s="41"/>
+      <c r="V27" s="42"/>
+      <c r="W27" s="41"/>
+      <c r="X27" s="41"/>
+      <c r="Y27" s="41"/>
+      <c r="Z27" s="42"/>
+      <c r="AA27" s="43">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="AB27" s="48"/>
-    </row>
-    <row r="28" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB27" s="47"/>
+    </row>
+    <row r="28" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="35">
         <v>19</v>
       </c>
-      <c r="B28" s="83" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="84">
-        <v>2</v>
-      </c>
-      <c r="D28" s="84">
-        <v>0</v>
-      </c>
-      <c r="E28" s="84">
-        <v>0</v>
-      </c>
-      <c r="F28" s="84">
+      <c r="B28" s="76" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="77">
+        <v>2</v>
+      </c>
+      <c r="D28" s="77">
+        <v>0</v>
+      </c>
+      <c r="E28" s="77">
+        <v>0</v>
+      </c>
+      <c r="F28" s="77">
         <v>4</v>
       </c>
-      <c r="G28" s="74">
+      <c r="G28" s="67">
         <f>VLOOKUP(H28,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -3400,34 +3451,34 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="K28" s="85"/>
-      <c r="L28" s="85"/>
-      <c r="M28" s="85"/>
-      <c r="N28" s="86"/>
-      <c r="O28" s="42"/>
-      <c r="P28" s="70"/>
-      <c r="Q28" s="42"/>
-      <c r="R28" s="86"/>
-      <c r="S28" s="85"/>
-      <c r="T28" s="85"/>
-      <c r="U28" s="85"/>
-      <c r="V28" s="86"/>
-      <c r="W28" s="85"/>
-      <c r="X28" s="85"/>
-      <c r="Y28" s="85"/>
-      <c r="Z28" s="86"/>
-      <c r="AA28" s="44">
+      <c r="K28" s="78"/>
+      <c r="L28" s="78"/>
+      <c r="M28" s="78"/>
+      <c r="N28" s="79"/>
+      <c r="O28" s="41"/>
+      <c r="P28" s="136"/>
+      <c r="Q28" s="41"/>
+      <c r="R28" s="79"/>
+      <c r="S28" s="78"/>
+      <c r="T28" s="78"/>
+      <c r="U28" s="78"/>
+      <c r="V28" s="79"/>
+      <c r="W28" s="78"/>
+      <c r="X28" s="78"/>
+      <c r="Y28" s="78"/>
+      <c r="Z28" s="79"/>
+      <c r="AA28" s="43">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="AB28" s="48"/>
-    </row>
-    <row r="29" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB28" s="47"/>
+    </row>
+    <row r="29" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="35">
         <v>20</v>
       </c>
-      <c r="B29" s="67" t="s">
-        <v>43</v>
+      <c r="B29" s="61" t="s">
+        <v>42</v>
       </c>
       <c r="C29" s="37">
         <v>6</v>
@@ -3441,7 +3492,7 @@
       <c r="F29" s="37">
         <v>10</v>
       </c>
-      <c r="G29" s="74">
+      <c r="G29" s="67">
         <f>VLOOKUP(H29,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -3455,89 +3506,89 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="K29" s="42"/>
-      <c r="L29" s="42"/>
-      <c r="M29" s="42"/>
-      <c r="N29" s="43"/>
-      <c r="O29" s="42"/>
-      <c r="P29" s="41"/>
-      <c r="Q29" s="42"/>
-      <c r="R29" s="43"/>
-      <c r="S29" s="42"/>
-      <c r="T29" s="42"/>
-      <c r="U29" s="42"/>
-      <c r="V29" s="43"/>
-      <c r="W29" s="42"/>
-      <c r="X29" s="42"/>
-      <c r="Y29" s="42"/>
-      <c r="Z29" s="43"/>
-      <c r="AA29" s="44">
+      <c r="K29" s="41"/>
+      <c r="L29" s="41"/>
+      <c r="M29" s="41"/>
+      <c r="N29" s="42"/>
+      <c r="O29" s="41"/>
+      <c r="P29" s="135"/>
+      <c r="Q29" s="41"/>
+      <c r="R29" s="42"/>
+      <c r="S29" s="41"/>
+      <c r="T29" s="41"/>
+      <c r="U29" s="41"/>
+      <c r="V29" s="42"/>
+      <c r="W29" s="41"/>
+      <c r="X29" s="41"/>
+      <c r="Y29" s="41"/>
+      <c r="Z29" s="42"/>
+      <c r="AA29" s="43">
         <f t="shared" si="2"/>
         <v>-11</v>
       </c>
-      <c r="AB29" s="48"/>
-    </row>
-    <row r="30" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB29" s="47"/>
+    </row>
+    <row r="30" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="35">
         <v>21</v>
       </c>
-      <c r="B30" s="72" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="73">
-        <v>0</v>
-      </c>
-      <c r="D30" s="73">
+      <c r="B30" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="66">
+        <v>0</v>
+      </c>
+      <c r="D30" s="66">
         <v>9</v>
       </c>
-      <c r="E30" s="73">
+      <c r="E30" s="66">
         <v>18.5</v>
       </c>
-      <c r="F30" s="73">
-        <v>0</v>
-      </c>
-      <c r="G30" s="74">
+      <c r="F30" s="66">
+        <v>0</v>
+      </c>
+      <c r="G30" s="67">
         <f>VLOOKUP(H30,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
       <c r="H30" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="I30" s="75">
+      <c r="I30" s="68">
         <v>25</v>
       </c>
       <c r="J30" s="40">
         <f t="shared" si="1"/>
         <v>27.5</v>
       </c>
-      <c r="K30" s="76"/>
-      <c r="L30" s="76"/>
-      <c r="M30" s="76"/>
-      <c r="N30" s="52"/>
-      <c r="O30" s="42"/>
-      <c r="P30" s="70"/>
-      <c r="Q30" s="42"/>
-      <c r="R30" s="61"/>
-      <c r="S30" s="76"/>
-      <c r="T30" s="76"/>
-      <c r="U30" s="76"/>
-      <c r="V30" s="52"/>
-      <c r="W30" s="76"/>
-      <c r="X30" s="76"/>
-      <c r="Y30" s="76"/>
-      <c r="Z30" s="52"/>
-      <c r="AA30" s="44">
+      <c r="K30" s="69"/>
+      <c r="L30" s="69"/>
+      <c r="M30" s="69"/>
+      <c r="N30" s="51"/>
+      <c r="O30" s="41"/>
+      <c r="P30" s="136"/>
+      <c r="Q30" s="41"/>
+      <c r="R30" s="138"/>
+      <c r="S30" s="69"/>
+      <c r="T30" s="69"/>
+      <c r="U30" s="69"/>
+      <c r="V30" s="51"/>
+      <c r="W30" s="69"/>
+      <c r="X30" s="69"/>
+      <c r="Y30" s="69"/>
+      <c r="Z30" s="51"/>
+      <c r="AA30" s="43">
         <f t="shared" si="2"/>
         <v>-2.5</v>
       </c>
-      <c r="AB30" s="48"/>
-    </row>
-    <row r="31" spans="1:28" s="82" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB30" s="47"/>
+    </row>
+    <row r="31" spans="1:28" s="75" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="35">
         <v>22</v>
       </c>
-      <c r="B31" s="80" t="s">
-        <v>45</v>
+      <c r="B31" s="73" t="s">
+        <v>44</v>
       </c>
       <c r="C31" s="37">
         <v>5</v>
@@ -3551,48 +3602,48 @@
       <c r="F31" s="37">
         <v>0</v>
       </c>
-      <c r="G31" s="74">
+      <c r="G31" s="67">
         <f>VLOOKUP(H31,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
       <c r="H31" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="I31" s="81">
+      <c r="I31" s="74">
         <v>12</v>
       </c>
       <c r="J31" s="40">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="K31" s="42"/>
-      <c r="L31" s="42"/>
-      <c r="M31" s="42"/>
-      <c r="N31" s="43"/>
-      <c r="O31" s="42"/>
-      <c r="P31" s="70"/>
-      <c r="Q31" s="42"/>
-      <c r="R31" s="43"/>
-      <c r="S31" s="42"/>
-      <c r="T31" s="42"/>
-      <c r="U31" s="42"/>
-      <c r="V31" s="43"/>
-      <c r="W31" s="42"/>
-      <c r="X31" s="42"/>
-      <c r="Y31" s="42"/>
-      <c r="Z31" s="43"/>
-      <c r="AA31" s="44">
+      <c r="K31" s="41"/>
+      <c r="L31" s="41"/>
+      <c r="M31" s="41"/>
+      <c r="N31" s="42"/>
+      <c r="O31" s="41"/>
+      <c r="P31" s="136"/>
+      <c r="Q31" s="41"/>
+      <c r="R31" s="42"/>
+      <c r="S31" s="41"/>
+      <c r="T31" s="41"/>
+      <c r="U31" s="41"/>
+      <c r="V31" s="42"/>
+      <c r="W31" s="41"/>
+      <c r="X31" s="41"/>
+      <c r="Y31" s="41"/>
+      <c r="Z31" s="42"/>
+      <c r="AA31" s="43">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="AB31" s="48"/>
-    </row>
-    <row r="32" spans="1:28" s="82" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB31" s="47"/>
+    </row>
+    <row r="32" spans="1:28" s="75" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="35">
         <v>23</v>
       </c>
-      <c r="B32" s="80" t="s">
-        <v>46</v>
+      <c r="B32" s="73" t="s">
+        <v>45</v>
       </c>
       <c r="C32" s="37">
         <v>3</v>
@@ -3606,62 +3657,62 @@
       <c r="F32" s="37">
         <v>3</v>
       </c>
-      <c r="G32" s="74">
+      <c r="G32" s="67">
         <f>VLOOKUP(H32,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
       <c r="H32" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="I32" s="81">
+      <c r="I32" s="74">
         <v>12</v>
       </c>
-      <c r="J32" s="81">
+      <c r="J32" s="74">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="K32" s="42"/>
-      <c r="L32" s="42"/>
-      <c r="M32" s="42"/>
-      <c r="N32" s="43"/>
-      <c r="O32" s="42"/>
-      <c r="P32" s="70"/>
-      <c r="Q32" s="42"/>
-      <c r="R32" s="43"/>
-      <c r="S32" s="42"/>
-      <c r="T32" s="42"/>
-      <c r="U32" s="42"/>
-      <c r="V32" s="43"/>
-      <c r="W32" s="42"/>
-      <c r="X32" s="42"/>
-      <c r="Y32" s="42"/>
-      <c r="Z32" s="43"/>
-      <c r="AA32" s="44">
+      <c r="K32" s="41"/>
+      <c r="L32" s="41"/>
+      <c r="M32" s="41"/>
+      <c r="N32" s="42"/>
+      <c r="O32" s="41"/>
+      <c r="P32" s="136"/>
+      <c r="Q32" s="41"/>
+      <c r="R32" s="42"/>
+      <c r="S32" s="41"/>
+      <c r="T32" s="41"/>
+      <c r="U32" s="41"/>
+      <c r="V32" s="42"/>
+      <c r="W32" s="41"/>
+      <c r="X32" s="41"/>
+      <c r="Y32" s="41"/>
+      <c r="Z32" s="42"/>
+      <c r="AA32" s="43">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB32" s="48"/>
-    </row>
-    <row r="33" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB32" s="47"/>
+    </row>
+    <row r="33" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="35">
         <v>24</v>
       </c>
-      <c r="B33" s="87" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" s="84">
-        <v>0</v>
-      </c>
-      <c r="D33" s="84">
-        <v>0</v>
-      </c>
-      <c r="E33" s="84">
+      <c r="B33" s="80" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="77">
+        <v>0</v>
+      </c>
+      <c r="D33" s="77">
+        <v>0</v>
+      </c>
+      <c r="E33" s="77">
         <v>10</v>
       </c>
-      <c r="F33" s="84">
-        <v>0</v>
-      </c>
-      <c r="G33" s="74">
+      <c r="F33" s="77">
+        <v>0</v>
+      </c>
+      <c r="G33" s="67">
         <f>VLOOKUP(H33,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -3675,34 +3726,34 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="K33" s="78"/>
-      <c r="L33" s="78"/>
-      <c r="M33" s="78"/>
-      <c r="N33" s="77"/>
-      <c r="O33" s="42"/>
-      <c r="P33" s="70"/>
-      <c r="Q33" s="70"/>
-      <c r="R33" s="70"/>
-      <c r="S33" s="78"/>
-      <c r="T33" s="78"/>
-      <c r="U33" s="78"/>
-      <c r="V33" s="77"/>
-      <c r="W33" s="78"/>
-      <c r="X33" s="78"/>
-      <c r="Y33" s="78"/>
-      <c r="Z33" s="77"/>
-      <c r="AA33" s="44">
+      <c r="K33" s="71"/>
+      <c r="L33" s="71"/>
+      <c r="M33" s="71"/>
+      <c r="N33" s="70"/>
+      <c r="O33" s="41"/>
+      <c r="P33" s="136"/>
+      <c r="Q33" s="136"/>
+      <c r="R33" s="136"/>
+      <c r="S33" s="71"/>
+      <c r="T33" s="71"/>
+      <c r="U33" s="71"/>
+      <c r="V33" s="70"/>
+      <c r="W33" s="71"/>
+      <c r="X33" s="71"/>
+      <c r="Y33" s="71"/>
+      <c r="Z33" s="70"/>
+      <c r="AA33" s="43">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB33" s="48"/>
-    </row>
-    <row r="34" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB33" s="47"/>
+    </row>
+    <row r="34" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="35">
         <v>25</v>
       </c>
-      <c r="B34" s="72" t="s">
-        <v>48</v>
+      <c r="B34" s="65" t="s">
+        <v>47</v>
       </c>
       <c r="C34" s="37">
         <v>0</v>
@@ -3716,7 +3767,7 @@
       <c r="F34" s="37">
         <v>0</v>
       </c>
-      <c r="G34" s="74">
+      <c r="G34" s="67">
         <f>VLOOKUP(H34,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -3730,34 +3781,34 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="K34" s="76"/>
-      <c r="L34" s="76"/>
-      <c r="M34" s="76"/>
-      <c r="N34" s="52"/>
-      <c r="O34" s="42"/>
-      <c r="P34" s="42"/>
-      <c r="Q34" s="88"/>
-      <c r="R34" s="52"/>
-      <c r="S34" s="76"/>
-      <c r="T34" s="76"/>
-      <c r="U34" s="76"/>
-      <c r="V34" s="52"/>
-      <c r="W34" s="76"/>
-      <c r="X34" s="76"/>
-      <c r="Y34" s="76"/>
-      <c r="Z34" s="52"/>
-      <c r="AA34" s="44">
+      <c r="K34" s="69"/>
+      <c r="L34" s="69"/>
+      <c r="M34" s="69"/>
+      <c r="N34" s="51"/>
+      <c r="O34" s="41"/>
+      <c r="P34" s="41"/>
+      <c r="Q34" s="139"/>
+      <c r="R34" s="51"/>
+      <c r="S34" s="69"/>
+      <c r="T34" s="69"/>
+      <c r="U34" s="69"/>
+      <c r="V34" s="51"/>
+      <c r="W34" s="69"/>
+      <c r="X34" s="69"/>
+      <c r="Y34" s="69"/>
+      <c r="Z34" s="51"/>
+      <c r="AA34" s="43">
         <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
-      <c r="AB34" s="48"/>
-    </row>
-    <row r="35" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB34" s="47"/>
+    </row>
+    <row r="35" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="35">
         <v>27</v>
       </c>
-      <c r="B35" s="72" t="s">
-        <v>49</v>
+      <c r="B35" s="65" t="s">
+        <v>48</v>
       </c>
       <c r="C35" s="37">
         <v>0</v>
@@ -3771,7 +3822,7 @@
       <c r="F35" s="37">
         <v>3</v>
       </c>
-      <c r="G35" s="74">
+      <c r="G35" s="67">
         <f>VLOOKUP(H35,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -3783,34 +3834,34 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="K35" s="76"/>
-      <c r="L35" s="76"/>
-      <c r="M35" s="76"/>
-      <c r="N35" s="52"/>
-      <c r="O35" s="76"/>
-      <c r="P35" s="76"/>
-      <c r="Q35" s="88"/>
-      <c r="R35" s="52"/>
-      <c r="S35" s="76"/>
-      <c r="T35" s="76"/>
-      <c r="U35" s="76"/>
-      <c r="V35" s="52"/>
-      <c r="W35" s="76"/>
-      <c r="X35" s="76"/>
-      <c r="Y35" s="76"/>
-      <c r="Z35" s="52"/>
-      <c r="AA35" s="44">
+      <c r="K35" s="69"/>
+      <c r="L35" s="69"/>
+      <c r="M35" s="69"/>
+      <c r="N35" s="51"/>
+      <c r="O35" s="69"/>
+      <c r="P35" s="69"/>
+      <c r="Q35" s="139"/>
+      <c r="R35" s="51"/>
+      <c r="S35" s="69"/>
+      <c r="T35" s="69"/>
+      <c r="U35" s="69"/>
+      <c r="V35" s="51"/>
+      <c r="W35" s="69"/>
+      <c r="X35" s="69"/>
+      <c r="Y35" s="69"/>
+      <c r="Z35" s="51"/>
+      <c r="AA35" s="43">
         <f t="shared" si="2"/>
         <v>-3</v>
       </c>
-      <c r="AB35" s="48"/>
-    </row>
-    <row r="36" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB35" s="47"/>
+    </row>
+    <row r="36" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="35">
         <v>28</v>
       </c>
-      <c r="B36" s="72" t="s">
-        <v>50</v>
+      <c r="B36" s="65" t="s">
+        <v>49</v>
       </c>
       <c r="C36" s="37">
         <v>2</v>
@@ -3824,7 +3875,7 @@
       <c r="F36" s="37">
         <v>8</v>
       </c>
-      <c r="G36" s="74">
+      <c r="G36" s="67">
         <f>VLOOKUP(H36,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -3836,34 +3887,34 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="K36" s="76"/>
-      <c r="L36" s="76"/>
-      <c r="M36" s="76"/>
-      <c r="N36" s="52"/>
-      <c r="O36" s="76"/>
-      <c r="P36" s="76"/>
-      <c r="Q36" s="88"/>
-      <c r="R36" s="52"/>
-      <c r="S36" s="76"/>
-      <c r="T36" s="76"/>
-      <c r="U36" s="76"/>
-      <c r="V36" s="52"/>
-      <c r="W36" s="76"/>
-      <c r="X36" s="76"/>
-      <c r="Y36" s="76"/>
-      <c r="Z36" s="52"/>
-      <c r="AA36" s="44">
+      <c r="K36" s="69"/>
+      <c r="L36" s="69"/>
+      <c r="M36" s="69"/>
+      <c r="N36" s="51"/>
+      <c r="O36" s="69"/>
+      <c r="P36" s="69"/>
+      <c r="Q36" s="139"/>
+      <c r="R36" s="51"/>
+      <c r="S36" s="69"/>
+      <c r="T36" s="69"/>
+      <c r="U36" s="69"/>
+      <c r="V36" s="51"/>
+      <c r="W36" s="69"/>
+      <c r="X36" s="69"/>
+      <c r="Y36" s="69"/>
+      <c r="Z36" s="51"/>
+      <c r="AA36" s="43">
         <f t="shared" si="2"/>
         <v>-10</v>
       </c>
-      <c r="AB36" s="48"/>
-    </row>
-    <row r="37" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB36" s="47"/>
+    </row>
+    <row r="37" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="35">
         <v>29</v>
       </c>
-      <c r="B37" s="72" t="s">
-        <v>51</v>
+      <c r="B37" s="65" t="s">
+        <v>50</v>
       </c>
       <c r="C37" s="37">
         <v>0</v>
@@ -3877,7 +3928,7 @@
       <c r="F37" s="37">
         <v>4</v>
       </c>
-      <c r="G37" s="74">
+      <c r="G37" s="67">
         <f>VLOOKUP(H37,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -3889,34 +3940,34 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K37" s="76"/>
-      <c r="L37" s="76"/>
-      <c r="M37" s="76"/>
-      <c r="N37" s="52"/>
-      <c r="O37" s="76"/>
-      <c r="P37" s="76"/>
-      <c r="Q37" s="88"/>
-      <c r="R37" s="43"/>
-      <c r="S37" s="76"/>
-      <c r="T37" s="76"/>
-      <c r="U37" s="76"/>
-      <c r="V37" s="52"/>
-      <c r="W37" s="76"/>
-      <c r="X37" s="76"/>
-      <c r="Y37" s="76"/>
-      <c r="Z37" s="52"/>
-      <c r="AA37" s="44">
+      <c r="K37" s="69"/>
+      <c r="L37" s="69"/>
+      <c r="M37" s="69"/>
+      <c r="N37" s="51"/>
+      <c r="O37" s="69"/>
+      <c r="P37" s="69"/>
+      <c r="Q37" s="139"/>
+      <c r="R37" s="42"/>
+      <c r="S37" s="69"/>
+      <c r="T37" s="69"/>
+      <c r="U37" s="69"/>
+      <c r="V37" s="51"/>
+      <c r="W37" s="69"/>
+      <c r="X37" s="69"/>
+      <c r="Y37" s="69"/>
+      <c r="Z37" s="51"/>
+      <c r="AA37" s="43">
         <f t="shared" si="2"/>
         <v>-4</v>
       </c>
-      <c r="AB37" s="48"/>
-    </row>
-    <row r="38" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB37" s="47"/>
+    </row>
+    <row r="38" spans="1:28" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="35">
         <v>30</v>
       </c>
-      <c r="B38" s="72" t="s">
-        <v>52</v>
+      <c r="B38" s="65" t="s">
+        <v>51</v>
       </c>
       <c r="C38" s="37">
         <v>5</v>
@@ -3930,7 +3981,7 @@
       <c r="F38" s="37">
         <v>0</v>
       </c>
-      <c r="G38" s="74">
+      <c r="G38" s="67">
         <f>VLOOKUP(H38,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -3942,34 +3993,34 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="K38" s="76"/>
-      <c r="L38" s="76"/>
-      <c r="M38" s="76"/>
-      <c r="N38" s="52"/>
-      <c r="O38" s="76"/>
-      <c r="P38" s="76"/>
-      <c r="Q38" s="88"/>
-      <c r="R38" s="52"/>
-      <c r="S38" s="42"/>
-      <c r="T38" s="76"/>
-      <c r="U38" s="76"/>
-      <c r="V38" s="52"/>
-      <c r="W38" s="76"/>
-      <c r="X38" s="76"/>
-      <c r="Y38" s="76"/>
-      <c r="Z38" s="52"/>
-      <c r="AA38" s="44">
+      <c r="K38" s="69"/>
+      <c r="L38" s="69"/>
+      <c r="M38" s="69"/>
+      <c r="N38" s="51"/>
+      <c r="O38" s="69"/>
+      <c r="P38" s="69"/>
+      <c r="Q38" s="139"/>
+      <c r="R38" s="51"/>
+      <c r="S38" s="41"/>
+      <c r="T38" s="69"/>
+      <c r="U38" s="69"/>
+      <c r="V38" s="51"/>
+      <c r="W38" s="69"/>
+      <c r="X38" s="69"/>
+      <c r="Y38" s="69"/>
+      <c r="Z38" s="51"/>
+      <c r="AA38" s="43">
         <f t="shared" si="2"/>
         <v>-5</v>
       </c>
-      <c r="AB38" s="48"/>
-    </row>
-    <row r="39" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB38" s="47"/>
+    </row>
+    <row r="39" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="35">
         <v>31</v>
       </c>
-      <c r="B39" s="72" t="s">
-        <v>53</v>
+      <c r="B39" s="65" t="s">
+        <v>52</v>
       </c>
       <c r="C39" s="37">
         <v>0</v>
@@ -3983,7 +4034,7 @@
       <c r="F39" s="37">
         <v>4</v>
       </c>
-      <c r="G39" s="74">
+      <c r="G39" s="67">
         <f>VLOOKUP(H39,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -3995,34 +4046,34 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K39" s="76"/>
-      <c r="L39" s="76"/>
-      <c r="M39" s="76"/>
-      <c r="N39" s="52"/>
-      <c r="O39" s="76"/>
-      <c r="P39" s="76"/>
-      <c r="Q39" s="76"/>
-      <c r="R39" s="88"/>
-      <c r="S39" s="42"/>
-      <c r="T39" s="42"/>
-      <c r="U39" s="76"/>
-      <c r="V39" s="52"/>
-      <c r="W39" s="76"/>
-      <c r="X39" s="76"/>
-      <c r="Y39" s="76"/>
-      <c r="Z39" s="52"/>
-      <c r="AA39" s="44">
+      <c r="K39" s="69"/>
+      <c r="L39" s="69"/>
+      <c r="M39" s="69"/>
+      <c r="N39" s="51"/>
+      <c r="O39" s="69"/>
+      <c r="P39" s="69"/>
+      <c r="Q39" s="69"/>
+      <c r="R39" s="139"/>
+      <c r="S39" s="41"/>
+      <c r="T39" s="41"/>
+      <c r="U39" s="69"/>
+      <c r="V39" s="51"/>
+      <c r="W39" s="69"/>
+      <c r="X39" s="69"/>
+      <c r="Y39" s="69"/>
+      <c r="Z39" s="51"/>
+      <c r="AA39" s="43">
         <f t="shared" si="2"/>
         <v>-4</v>
       </c>
-      <c r="AB39" s="48"/>
-    </row>
-    <row r="40" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB39" s="47"/>
+    </row>
+    <row r="40" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="35">
         <v>32</v>
       </c>
-      <c r="B40" s="72" t="s">
-        <v>54</v>
+      <c r="B40" s="65" t="s">
+        <v>53</v>
       </c>
       <c r="C40" s="37">
         <v>0</v>
@@ -4036,7 +4087,7 @@
       <c r="F40" s="37">
         <v>6</v>
       </c>
-      <c r="G40" s="74">
+      <c r="G40" s="67">
         <f>VLOOKUP(H40,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -4048,34 +4099,34 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="K40" s="76"/>
-      <c r="L40" s="76"/>
-      <c r="M40" s="76"/>
-      <c r="N40" s="52"/>
-      <c r="O40" s="76"/>
-      <c r="P40" s="76"/>
-      <c r="Q40" s="76"/>
-      <c r="R40" s="88"/>
-      <c r="S40" s="76"/>
-      <c r="T40" s="76"/>
-      <c r="U40" s="42"/>
-      <c r="V40" s="52"/>
-      <c r="W40" s="76"/>
-      <c r="X40" s="76"/>
-      <c r="Y40" s="76"/>
-      <c r="Z40" s="52"/>
-      <c r="AA40" s="44">
+      <c r="K40" s="69"/>
+      <c r="L40" s="69"/>
+      <c r="M40" s="69"/>
+      <c r="N40" s="51"/>
+      <c r="O40" s="69"/>
+      <c r="P40" s="69"/>
+      <c r="Q40" s="69"/>
+      <c r="R40" s="139"/>
+      <c r="S40" s="69"/>
+      <c r="T40" s="69"/>
+      <c r="U40" s="41"/>
+      <c r="V40" s="51"/>
+      <c r="W40" s="69"/>
+      <c r="X40" s="69"/>
+      <c r="Y40" s="69"/>
+      <c r="Z40" s="51"/>
+      <c r="AA40" s="43">
         <f t="shared" si="2"/>
         <v>-6</v>
       </c>
-      <c r="AB40" s="48"/>
-    </row>
-    <row r="41" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB40" s="47"/>
+    </row>
+    <row r="41" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="35">
         <v>33</v>
       </c>
-      <c r="B41" s="72" t="s">
-        <v>55</v>
+      <c r="B41" s="65" t="s">
+        <v>54</v>
       </c>
       <c r="C41" s="37">
         <v>2</v>
@@ -4089,7 +4140,7 @@
       <c r="F41" s="37">
         <v>2</v>
       </c>
-      <c r="G41" s="74">
+      <c r="G41" s="67">
         <f>VLOOKUP(H41,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -4103,34 +4154,34 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="K41" s="76"/>
-      <c r="L41" s="76"/>
-      <c r="M41" s="76"/>
-      <c r="N41" s="52"/>
-      <c r="O41" s="76"/>
-      <c r="P41" s="76"/>
-      <c r="Q41" s="42"/>
-      <c r="R41" s="70"/>
-      <c r="S41" s="76"/>
-      <c r="T41" s="76"/>
-      <c r="U41" s="76"/>
-      <c r="V41" s="52"/>
-      <c r="W41" s="76"/>
-      <c r="X41" s="76"/>
-      <c r="Y41" s="76"/>
-      <c r="Z41" s="52"/>
-      <c r="AA41" s="44">
+      <c r="K41" s="69"/>
+      <c r="L41" s="69"/>
+      <c r="M41" s="69"/>
+      <c r="N41" s="51"/>
+      <c r="O41" s="69"/>
+      <c r="P41" s="69"/>
+      <c r="Q41" s="41"/>
+      <c r="R41" s="136"/>
+      <c r="S41" s="69"/>
+      <c r="T41" s="69"/>
+      <c r="U41" s="69"/>
+      <c r="V41" s="51"/>
+      <c r="W41" s="69"/>
+      <c r="X41" s="69"/>
+      <c r="Y41" s="69"/>
+      <c r="Z41" s="51"/>
+      <c r="AA41" s="43">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="AB41" s="48"/>
-    </row>
-    <row r="42" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB41" s="47"/>
+    </row>
+    <row r="42" spans="1:28" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="35">
         <v>34</v>
       </c>
-      <c r="B42" s="72" t="s">
-        <v>56</v>
+      <c r="B42" s="65" t="s">
+        <v>55</v>
       </c>
       <c r="C42" s="37">
         <v>0</v>
@@ -4144,7 +4195,7 @@
       <c r="F42" s="37">
         <v>0</v>
       </c>
-      <c r="G42" s="74">
+      <c r="G42" s="67">
         <f>VLOOKUP(H42,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -4156,34 +4207,34 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K42" s="76"/>
-      <c r="L42" s="76"/>
-      <c r="M42" s="76"/>
-      <c r="N42" s="52"/>
-      <c r="O42" s="76"/>
-      <c r="P42" s="76"/>
-      <c r="Q42" s="76"/>
-      <c r="R42" s="52"/>
-      <c r="S42" s="76"/>
-      <c r="T42" s="76"/>
-      <c r="U42" s="76"/>
-      <c r="V42" s="43"/>
-      <c r="W42" s="76"/>
-      <c r="X42" s="76"/>
-      <c r="Y42" s="76"/>
-      <c r="Z42" s="52"/>
-      <c r="AA42" s="44">
+      <c r="K42" s="69"/>
+      <c r="L42" s="69"/>
+      <c r="M42" s="69"/>
+      <c r="N42" s="51"/>
+      <c r="O42" s="69"/>
+      <c r="P42" s="69"/>
+      <c r="Q42" s="69"/>
+      <c r="R42" s="51"/>
+      <c r="S42" s="69"/>
+      <c r="T42" s="69"/>
+      <c r="U42" s="69"/>
+      <c r="V42" s="42"/>
+      <c r="W42" s="69"/>
+      <c r="X42" s="69"/>
+      <c r="Y42" s="69"/>
+      <c r="Z42" s="51"/>
+      <c r="AA42" s="43">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB42" s="48"/>
-    </row>
-    <row r="43" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB42" s="47"/>
+    </row>
+    <row r="43" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="35">
         <v>35</v>
       </c>
-      <c r="B43" s="72" t="s">
-        <v>57</v>
+      <c r="B43" s="65" t="s">
+        <v>56</v>
       </c>
       <c r="C43" s="37">
         <v>0</v>
@@ -4197,7 +4248,7 @@
       <c r="F43" s="37">
         <v>0</v>
       </c>
-      <c r="G43" s="74">
+      <c r="G43" s="67">
         <f>VLOOKUP(H43,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -4211,34 +4262,34 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K43" s="76"/>
-      <c r="L43" s="76"/>
-      <c r="M43" s="76"/>
-      <c r="N43" s="52"/>
-      <c r="O43" s="76"/>
-      <c r="P43" s="76"/>
-      <c r="Q43" s="76"/>
-      <c r="R43" s="88"/>
-      <c r="S43" s="76"/>
-      <c r="T43" s="76"/>
-      <c r="U43" s="76"/>
-      <c r="V43" s="43"/>
-      <c r="W43" s="76"/>
-      <c r="X43" s="76"/>
-      <c r="Y43" s="76"/>
-      <c r="Z43" s="52"/>
-      <c r="AA43" s="44">
+      <c r="K43" s="69"/>
+      <c r="L43" s="69"/>
+      <c r="M43" s="69"/>
+      <c r="N43" s="51"/>
+      <c r="O43" s="69"/>
+      <c r="P43" s="69"/>
+      <c r="Q43" s="69"/>
+      <c r="R43" s="139"/>
+      <c r="S43" s="69"/>
+      <c r="T43" s="69"/>
+      <c r="U43" s="69"/>
+      <c r="V43" s="42"/>
+      <c r="W43" s="69"/>
+      <c r="X43" s="69"/>
+      <c r="Y43" s="69"/>
+      <c r="Z43" s="51"/>
+      <c r="AA43" s="43">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="AB43" s="48"/>
-    </row>
-    <row r="44" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB43" s="47"/>
+    </row>
+    <row r="44" spans="1:28" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="35">
         <v>36</v>
       </c>
-      <c r="B44" s="72" t="s">
-        <v>58</v>
+      <c r="B44" s="65" t="s">
+        <v>57</v>
       </c>
       <c r="C44" s="37">
         <v>0</v>
@@ -4252,7 +4303,7 @@
       <c r="F44" s="37">
         <v>0</v>
       </c>
-      <c r="G44" s="74">
+      <c r="G44" s="67">
         <f>VLOOKUP(H44,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -4266,34 +4317,34 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K44" s="76"/>
-      <c r="L44" s="76"/>
-      <c r="M44" s="76"/>
-      <c r="N44" s="52"/>
-      <c r="O44" s="76"/>
-      <c r="P44" s="76"/>
-      <c r="Q44" s="76"/>
-      <c r="R44" s="52"/>
-      <c r="S44" s="76"/>
-      <c r="T44" s="76"/>
-      <c r="U44" s="76"/>
-      <c r="V44" s="52"/>
-      <c r="W44" s="42"/>
-      <c r="X44" s="76"/>
-      <c r="Y44" s="76"/>
-      <c r="Z44" s="52"/>
-      <c r="AA44" s="44">
+      <c r="K44" s="69"/>
+      <c r="L44" s="69"/>
+      <c r="M44" s="69"/>
+      <c r="N44" s="51"/>
+      <c r="O44" s="69"/>
+      <c r="P44" s="69"/>
+      <c r="Q44" s="69"/>
+      <c r="R44" s="51"/>
+      <c r="S44" s="69"/>
+      <c r="T44" s="69"/>
+      <c r="U44" s="69"/>
+      <c r="V44" s="51"/>
+      <c r="W44" s="41"/>
+      <c r="X44" s="69"/>
+      <c r="Y44" s="69"/>
+      <c r="Z44" s="51"/>
+      <c r="AA44" s="43">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="AB44" s="48"/>
-    </row>
-    <row r="45" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB44" s="47"/>
+    </row>
+    <row r="45" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="35">
         <v>37</v>
       </c>
-      <c r="B45" s="72" t="s">
-        <v>59</v>
+      <c r="B45" s="65" t="s">
+        <v>58</v>
       </c>
       <c r="C45" s="37">
         <v>7</v>
@@ -4307,7 +4358,7 @@
       <c r="F45" s="37">
         <v>0</v>
       </c>
-      <c r="G45" s="74">
+      <c r="G45" s="67">
         <f>VLOOKUP(H45,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -4319,34 +4370,34 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="K45" s="76"/>
-      <c r="L45" s="76"/>
-      <c r="M45" s="76"/>
-      <c r="N45" s="52"/>
-      <c r="O45" s="76"/>
-      <c r="P45" s="76"/>
-      <c r="Q45" s="76"/>
-      <c r="R45" s="88"/>
-      <c r="S45" s="76"/>
-      <c r="T45" s="76"/>
-      <c r="U45" s="76"/>
-      <c r="V45" s="52"/>
-      <c r="W45" s="42"/>
-      <c r="X45" s="76"/>
-      <c r="Y45" s="76"/>
-      <c r="Z45" s="52"/>
-      <c r="AA45" s="44">
+      <c r="K45" s="69"/>
+      <c r="L45" s="69"/>
+      <c r="M45" s="69"/>
+      <c r="N45" s="51"/>
+      <c r="O45" s="69"/>
+      <c r="P45" s="69"/>
+      <c r="Q45" s="69"/>
+      <c r="R45" s="139"/>
+      <c r="S45" s="69"/>
+      <c r="T45" s="69"/>
+      <c r="U45" s="69"/>
+      <c r="V45" s="51"/>
+      <c r="W45" s="41"/>
+      <c r="X45" s="69"/>
+      <c r="Y45" s="69"/>
+      <c r="Z45" s="51"/>
+      <c r="AA45" s="43">
         <f t="shared" si="2"/>
         <v>-8</v>
       </c>
-      <c r="AB45" s="48"/>
-    </row>
-    <row r="46" spans="1:28" s="141" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB45" s="47"/>
+    </row>
+    <row r="46" spans="1:28" s="117" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="35">
         <v>39</v>
       </c>
-      <c r="B46" s="67" t="s">
-        <v>67</v>
+      <c r="B46" s="61" t="s">
+        <v>66</v>
       </c>
       <c r="C46" s="37">
         <v>0</v>
@@ -4360,7 +4411,7 @@
       <c r="F46" s="37">
         <v>0</v>
       </c>
-      <c r="G46" s="74">
+      <c r="G46" s="67">
         <f>VLOOKUP(H46,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -4374,31 +4425,31 @@
         <f t="shared" ref="J46" si="3">SUM(C46:F46)</f>
         <v>2.5</v>
       </c>
-      <c r="K46" s="42"/>
-      <c r="L46" s="42"/>
-      <c r="M46" s="42"/>
-      <c r="N46" s="43"/>
-      <c r="O46" s="42"/>
-      <c r="P46" s="42"/>
-      <c r="Q46" s="42"/>
-      <c r="R46" s="140"/>
-      <c r="S46" s="42"/>
-      <c r="T46" s="42"/>
-      <c r="U46" s="42"/>
-      <c r="V46" s="43"/>
-      <c r="W46" s="42"/>
-      <c r="X46" s="42"/>
-      <c r="Y46" s="42"/>
-      <c r="Z46" s="43"/>
-      <c r="AA46" s="44"/>
-      <c r="AB46" s="48"/>
-    </row>
-    <row r="47" spans="1:28" s="141" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K46" s="41"/>
+      <c r="L46" s="41"/>
+      <c r="M46" s="41"/>
+      <c r="N46" s="42"/>
+      <c r="O46" s="41"/>
+      <c r="P46" s="41"/>
+      <c r="Q46" s="41"/>
+      <c r="R46" s="116"/>
+      <c r="S46" s="41"/>
+      <c r="T46" s="41"/>
+      <c r="U46" s="41"/>
+      <c r="V46" s="42"/>
+      <c r="W46" s="41"/>
+      <c r="X46" s="41"/>
+      <c r="Y46" s="41"/>
+      <c r="Z46" s="42"/>
+      <c r="AA46" s="43"/>
+      <c r="AB46" s="47"/>
+    </row>
+    <row r="47" spans="1:28" s="117" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="35">
         <v>40</v>
       </c>
-      <c r="B47" s="67" t="s">
-        <v>75</v>
+      <c r="B47" s="61" t="s">
+        <v>73</v>
       </c>
       <c r="C47" s="37">
         <v>2</v>
@@ -4412,7 +4463,7 @@
       <c r="F47" s="37">
         <v>0</v>
       </c>
-      <c r="G47" s="74">
+      <c r="G47" s="67">
         <f>VLOOKUP(H47,Feuil2!$A$1:$B$3,2,0)</f>
         <v>0</v>
       </c>
@@ -4426,66 +4477,63 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="K47" s="42"/>
-      <c r="L47" s="42"/>
-      <c r="M47" s="42"/>
-      <c r="N47" s="43"/>
-      <c r="O47" s="42"/>
-      <c r="P47" s="42"/>
-      <c r="Q47" s="42"/>
-      <c r="R47" s="140"/>
-      <c r="S47" s="42"/>
-      <c r="T47" s="42"/>
-      <c r="U47" s="42"/>
-      <c r="V47" s="43"/>
-      <c r="W47" s="42"/>
-      <c r="X47" s="42"/>
-      <c r="Y47" s="42"/>
-      <c r="Z47" s="43"/>
-      <c r="AA47" s="44"/>
-      <c r="AB47" s="48"/>
-    </row>
-    <row r="48" spans="1:28" s="46" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A48" s="135"/>
+      <c r="K47" s="41"/>
+      <c r="L47" s="41"/>
+      <c r="M47" s="41"/>
+      <c r="N47" s="42"/>
+      <c r="O47" s="41"/>
+      <c r="P47" s="41"/>
+      <c r="Q47" s="41"/>
+      <c r="R47" s="116"/>
+      <c r="S47" s="41"/>
+      <c r="T47" s="41"/>
+      <c r="U47" s="41"/>
+      <c r="V47" s="42"/>
+      <c r="W47" s="41"/>
+      <c r="X47" s="41"/>
+      <c r="Y47" s="41"/>
+      <c r="Z47" s="42"/>
+      <c r="AA47" s="43"/>
+      <c r="AB47" s="47"/>
+    </row>
+    <row r="48" spans="1:28" s="45" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="111"/>
       <c r="B48" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="C48" s="84"/>
-      <c r="D48" s="84"/>
-      <c r="E48" s="84"/>
-      <c r="F48" s="84"/>
-      <c r="G48" s="74"/>
-      <c r="H48" s="136"/>
+        <v>67</v>
+      </c>
+      <c r="C48" s="77"/>
+      <c r="D48" s="77"/>
+      <c r="E48" s="77"/>
+      <c r="F48" s="77"/>
+      <c r="G48" s="67"/>
+      <c r="H48" s="112"/>
       <c r="I48" s="40"/>
-      <c r="J48" s="40">
-        <f t="shared" ref="J48" si="4">SUM(C48:F48)</f>
-        <v>0</v>
-      </c>
-      <c r="K48" s="85"/>
-      <c r="L48" s="85"/>
-      <c r="M48" s="78"/>
-      <c r="N48" s="77"/>
-      <c r="O48" s="78"/>
-      <c r="P48" s="78"/>
-      <c r="Q48" s="78"/>
-      <c r="R48" s="137"/>
-      <c r="S48" s="78"/>
-      <c r="T48" s="42"/>
-      <c r="U48" s="42"/>
-      <c r="V48" s="43"/>
-      <c r="W48" s="78"/>
-      <c r="X48" s="78"/>
-      <c r="Y48" s="78"/>
-      <c r="Z48" s="77"/>
-      <c r="AA48" s="138"/>
-      <c r="AB48" s="139"/>
-    </row>
-    <row r="49" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="J48" s="40"/>
+      <c r="K48" s="78"/>
+      <c r="L48" s="78"/>
+      <c r="M48" s="71"/>
+      <c r="N48" s="70"/>
+      <c r="O48" s="71"/>
+      <c r="P48" s="71"/>
+      <c r="Q48" s="71"/>
+      <c r="R48" s="113"/>
+      <c r="S48" s="71"/>
+      <c r="T48" s="41"/>
+      <c r="U48" s="41"/>
+      <c r="V48" s="42"/>
+      <c r="W48" s="71"/>
+      <c r="X48" s="71"/>
+      <c r="Y48" s="71"/>
+      <c r="Z48" s="70"/>
+      <c r="AA48" s="114"/>
+      <c r="AB48" s="115"/>
+    </row>
+    <row r="49" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="35">
         <v>1</v>
       </c>
-      <c r="B49" s="72" t="s">
-        <v>66</v>
+      <c r="B49" s="65" t="s">
+        <v>65</v>
       </c>
       <c r="C49" s="37">
         <v>0</v>
@@ -4499,7 +4547,7 @@
       <c r="F49" s="37">
         <v>0</v>
       </c>
-      <c r="G49" s="74">
+      <c r="G49" s="67">
         <f>VLOOKUP(H49,Feuil2!$A$1:$B$3,2,0)</f>
         <v>100</v>
       </c>
@@ -4513,34 +4561,34 @@
         <f>SUM(C49:F49)</f>
         <v>8.75</v>
       </c>
-      <c r="K49" s="76"/>
-      <c r="L49" s="76"/>
-      <c r="M49" s="76"/>
-      <c r="N49" s="52"/>
-      <c r="O49" s="76"/>
-      <c r="P49" s="76"/>
-      <c r="Q49" s="76"/>
-      <c r="R49" s="70"/>
-      <c r="S49" s="134"/>
-      <c r="T49" s="42"/>
-      <c r="U49" s="142"/>
-      <c r="V49" s="43"/>
-      <c r="W49" s="76"/>
-      <c r="X49" s="42"/>
-      <c r="Y49" s="76"/>
-      <c r="Z49" s="52"/>
-      <c r="AA49" s="44">
+      <c r="K49" s="69"/>
+      <c r="L49" s="69"/>
+      <c r="M49" s="69"/>
+      <c r="N49" s="51"/>
+      <c r="O49" s="69"/>
+      <c r="P49" s="69"/>
+      <c r="Q49" s="69"/>
+      <c r="R49" s="136"/>
+      <c r="S49" s="110"/>
+      <c r="T49" s="41"/>
+      <c r="U49" s="140"/>
+      <c r="V49" s="118"/>
+      <c r="W49" s="69"/>
+      <c r="X49" s="41"/>
+      <c r="Y49" s="69"/>
+      <c r="Z49" s="51"/>
+      <c r="AA49" s="43">
         <f>I49-J49</f>
         <v>-1.75</v>
       </c>
-      <c r="AB49" s="48"/>
-    </row>
-    <row r="50" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB49" s="47"/>
+    </row>
+    <row r="50" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="35">
         <v>2</v>
       </c>
-      <c r="B50" s="72" t="s">
-        <v>54</v>
+      <c r="B50" s="65" t="s">
+        <v>53</v>
       </c>
       <c r="C50" s="37">
         <v>0</v>
@@ -4554,7 +4602,7 @@
       <c r="F50" s="37">
         <v>5</v>
       </c>
-      <c r="G50" s="74">
+      <c r="G50" s="67">
         <f>VLOOKUP(H50,Feuil2!$A$1:$B$3,2,0)</f>
         <v>100</v>
       </c>
@@ -4563,37 +4611,37 @@
       </c>
       <c r="I50" s="40"/>
       <c r="J50" s="40">
-        <f t="shared" ref="J50" si="5">SUM(C50:F50)</f>
+        <f t="shared" ref="J50" si="4">SUM(C50:F50)</f>
         <v>5</v>
       </c>
-      <c r="K50" s="76"/>
-      <c r="L50" s="76"/>
-      <c r="M50" s="76"/>
-      <c r="N50" s="52"/>
-      <c r="O50" s="76"/>
-      <c r="P50" s="76"/>
-      <c r="Q50" s="76"/>
-      <c r="R50" s="88"/>
-      <c r="S50" s="134"/>
-      <c r="T50" s="42"/>
-      <c r="U50" s="142"/>
-      <c r="V50" s="43"/>
-      <c r="W50" s="76"/>
-      <c r="X50" s="76"/>
-      <c r="Y50" s="76"/>
-      <c r="Z50" s="52"/>
-      <c r="AA50" s="44">
-        <f t="shared" ref="AA50" si="6">I50-J50</f>
+      <c r="K50" s="69"/>
+      <c r="L50" s="69"/>
+      <c r="M50" s="69"/>
+      <c r="N50" s="51"/>
+      <c r="O50" s="69"/>
+      <c r="P50" s="69"/>
+      <c r="Q50" s="69"/>
+      <c r="R50" s="139"/>
+      <c r="S50" s="110"/>
+      <c r="T50" s="41"/>
+      <c r="U50" s="140"/>
+      <c r="V50" s="118"/>
+      <c r="W50" s="69"/>
+      <c r="X50" s="69"/>
+      <c r="Y50" s="69"/>
+      <c r="Z50" s="51"/>
+      <c r="AA50" s="43">
+        <f t="shared" ref="AA50" si="5">I50-J50</f>
         <v>-5</v>
       </c>
-      <c r="AB50" s="48"/>
-    </row>
-    <row r="51" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB50" s="47"/>
+    </row>
+    <row r="51" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="35">
         <v>3</v>
       </c>
-      <c r="B51" s="72" t="s">
-        <v>69</v>
+      <c r="B51" s="65" t="s">
+        <v>68</v>
       </c>
       <c r="C51" s="37">
         <v>7</v>
@@ -4607,7 +4655,7 @@
       <c r="F51" s="37">
         <v>0</v>
       </c>
-      <c r="G51" s="74">
+      <c r="G51" s="67">
         <f>VLOOKUP(H51,Feuil2!$A$1:$B$3,2,0)</f>
         <v>100</v>
       </c>
@@ -4619,31 +4667,31 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="K51" s="42"/>
-      <c r="L51" s="42"/>
-      <c r="M51" s="76"/>
-      <c r="N51" s="52"/>
-      <c r="O51" s="76"/>
-      <c r="P51" s="76"/>
-      <c r="Q51" s="76"/>
-      <c r="R51" s="116"/>
-      <c r="S51" s="134"/>
-      <c r="T51" s="42"/>
-      <c r="U51" s="142"/>
-      <c r="V51" s="43"/>
-      <c r="W51" s="76"/>
-      <c r="X51" s="76"/>
-      <c r="Y51" s="76"/>
-      <c r="Z51" s="52"/>
-      <c r="AA51" s="115"/>
-      <c r="AB51" s="79"/>
-    </row>
-    <row r="52" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K51" s="41"/>
+      <c r="L51" s="41"/>
+      <c r="M51" s="69"/>
+      <c r="N51" s="51"/>
+      <c r="O51" s="69"/>
+      <c r="P51" s="69"/>
+      <c r="Q51" s="69"/>
+      <c r="R51" s="108"/>
+      <c r="S51" s="110"/>
+      <c r="T51" s="41"/>
+      <c r="U51" s="140"/>
+      <c r="V51" s="118"/>
+      <c r="W51" s="69"/>
+      <c r="X51" s="69"/>
+      <c r="Y51" s="69"/>
+      <c r="Z51" s="51"/>
+      <c r="AA51" s="107"/>
+      <c r="AB51" s="72"/>
+    </row>
+    <row r="52" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="35">
         <v>4</v>
       </c>
-      <c r="B52" s="72" t="s">
-        <v>70</v>
+      <c r="B52" s="65" t="s">
+        <v>69</v>
       </c>
       <c r="C52" s="37">
         <v>0</v>
@@ -4657,7 +4705,7 @@
       <c r="F52" s="37">
         <v>0</v>
       </c>
-      <c r="G52" s="74">
+      <c r="G52" s="67">
         <f>VLOOKUP(H52,Feuil2!$A$1:$B$3,2,0)</f>
         <v>75</v>
       </c>
@@ -4671,31 +4719,31 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K52" s="42"/>
-      <c r="L52" s="42"/>
-      <c r="M52" s="76"/>
-      <c r="N52" s="52"/>
-      <c r="O52" s="76"/>
-      <c r="P52" s="76"/>
-      <c r="Q52" s="76"/>
-      <c r="R52" s="116"/>
-      <c r="S52" s="76"/>
-      <c r="T52" s="42"/>
-      <c r="U52" s="142"/>
-      <c r="V52" s="43"/>
-      <c r="W52" s="76"/>
-      <c r="X52" s="76"/>
-      <c r="Y52" s="76"/>
-      <c r="Z52" s="52"/>
-      <c r="AA52" s="115"/>
-      <c r="AB52" s="79"/>
-    </row>
-    <row r="53" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K52" s="41"/>
+      <c r="L52" s="41"/>
+      <c r="M52" s="69"/>
+      <c r="N52" s="51"/>
+      <c r="O52" s="69"/>
+      <c r="P52" s="69"/>
+      <c r="Q52" s="69"/>
+      <c r="R52" s="108"/>
+      <c r="S52" s="69"/>
+      <c r="T52" s="41"/>
+      <c r="U52" s="140"/>
+      <c r="V52" s="118"/>
+      <c r="W52" s="69"/>
+      <c r="X52" s="69"/>
+      <c r="Y52" s="69"/>
+      <c r="Z52" s="51"/>
+      <c r="AA52" s="107"/>
+      <c r="AB52" s="72"/>
+    </row>
+    <row r="53" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="35">
         <v>5</v>
       </c>
-      <c r="B53" s="72" t="s">
-        <v>71</v>
+      <c r="B53" s="65" t="s">
+        <v>70</v>
       </c>
       <c r="C53" s="37">
         <v>0</v>
@@ -4709,7 +4757,7 @@
       <c r="F53" s="37">
         <v>0</v>
       </c>
-      <c r="G53" s="74">
+      <c r="G53" s="67">
         <f>VLOOKUP(H53,Feuil2!$A$1:$B$3,2,0)</f>
         <v>75</v>
       </c>
@@ -4723,31 +4771,31 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K53" s="42"/>
-      <c r="L53" s="42"/>
-      <c r="M53" s="76"/>
-      <c r="N53" s="52"/>
-      <c r="O53" s="76"/>
-      <c r="P53" s="76"/>
-      <c r="Q53" s="76"/>
-      <c r="R53" s="116"/>
-      <c r="S53" s="76"/>
-      <c r="T53" s="42"/>
-      <c r="U53" s="142"/>
-      <c r="V53" s="43"/>
-      <c r="W53" s="76"/>
-      <c r="X53" s="76"/>
-      <c r="Y53" s="76"/>
-      <c r="Z53" s="52"/>
-      <c r="AA53" s="115"/>
-      <c r="AB53" s="79"/>
-    </row>
-    <row r="54" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K53" s="41"/>
+      <c r="L53" s="41"/>
+      <c r="M53" s="69"/>
+      <c r="N53" s="51"/>
+      <c r="O53" s="69"/>
+      <c r="P53" s="69"/>
+      <c r="Q53" s="69"/>
+      <c r="R53" s="108"/>
+      <c r="S53" s="69"/>
+      <c r="T53" s="41"/>
+      <c r="U53" s="140"/>
+      <c r="V53" s="118"/>
+      <c r="W53" s="69"/>
+      <c r="X53" s="69"/>
+      <c r="Y53" s="69"/>
+      <c r="Z53" s="51"/>
+      <c r="AA53" s="107"/>
+      <c r="AB53" s="72"/>
+    </row>
+    <row r="54" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="35">
         <v>6</v>
       </c>
-      <c r="B54" s="72" t="s">
-        <v>72</v>
+      <c r="B54" s="65" t="s">
+        <v>71</v>
       </c>
       <c r="C54" s="37">
         <v>0</v>
@@ -4761,7 +4809,7 @@
       <c r="F54" s="37">
         <v>0</v>
       </c>
-      <c r="G54" s="74">
+      <c r="G54" s="67">
         <f>VLOOKUP(H54,Feuil2!$A$1:$B$3,2,0)</f>
         <v>75</v>
       </c>
@@ -4775,31 +4823,31 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K54" s="42"/>
-      <c r="L54" s="42"/>
-      <c r="M54" s="76"/>
-      <c r="N54" s="52"/>
-      <c r="O54" s="76"/>
-      <c r="P54" s="76"/>
-      <c r="Q54" s="76"/>
-      <c r="R54" s="116"/>
-      <c r="S54" s="76"/>
-      <c r="T54" s="42"/>
-      <c r="U54" s="142"/>
-      <c r="V54" s="43"/>
-      <c r="W54" s="76"/>
-      <c r="X54" s="76"/>
-      <c r="Y54" s="76"/>
-      <c r="Z54" s="52"/>
-      <c r="AA54" s="115"/>
-      <c r="AB54" s="79"/>
-    </row>
-    <row r="55" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K54" s="41"/>
+      <c r="L54" s="41"/>
+      <c r="M54" s="69"/>
+      <c r="N54" s="51"/>
+      <c r="O54" s="69"/>
+      <c r="P54" s="69"/>
+      <c r="Q54" s="69"/>
+      <c r="R54" s="108"/>
+      <c r="S54" s="69"/>
+      <c r="T54" s="41"/>
+      <c r="U54" s="140"/>
+      <c r="V54" s="118"/>
+      <c r="W54" s="69"/>
+      <c r="X54" s="69"/>
+      <c r="Y54" s="69"/>
+      <c r="Z54" s="51"/>
+      <c r="AA54" s="107"/>
+      <c r="AB54" s="72"/>
+    </row>
+    <row r="55" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="35">
         <v>7</v>
       </c>
-      <c r="B55" s="72" t="s">
-        <v>73</v>
+      <c r="B55" s="65" t="s">
+        <v>72</v>
       </c>
       <c r="C55" s="37">
         <v>0</v>
@@ -4813,7 +4861,7 @@
       <c r="F55" s="37">
         <v>0</v>
       </c>
-      <c r="G55" s="74">
+      <c r="G55" s="67">
         <f>VLOOKUP(H55,Feuil2!$A$1:$B$3,2,0)</f>
         <v>75</v>
       </c>
@@ -4827,557 +4875,558 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K55" s="42"/>
-      <c r="L55" s="42"/>
-      <c r="M55" s="76"/>
-      <c r="N55" s="52"/>
-      <c r="O55" s="76"/>
-      <c r="P55" s="76"/>
-      <c r="Q55" s="76"/>
-      <c r="R55" s="116"/>
-      <c r="S55" s="76"/>
-      <c r="T55" s="42"/>
-      <c r="U55" s="142"/>
-      <c r="V55" s="43"/>
-      <c r="W55" s="76"/>
-      <c r="X55" s="76"/>
-      <c r="Y55" s="76"/>
-      <c r="Z55" s="52"/>
-      <c r="AA55" s="115"/>
-      <c r="AB55" s="79"/>
-    </row>
-    <row r="56" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K55" s="41"/>
+      <c r="L55" s="41"/>
+      <c r="M55" s="69"/>
+      <c r="N55" s="51"/>
+      <c r="O55" s="69"/>
+      <c r="P55" s="69"/>
+      <c r="Q55" s="69"/>
+      <c r="R55" s="108"/>
+      <c r="S55" s="69"/>
+      <c r="T55" s="41"/>
+      <c r="U55" s="140"/>
+      <c r="V55" s="118"/>
+      <c r="W55" s="69"/>
+      <c r="X55" s="69"/>
+      <c r="Y55" s="69"/>
+      <c r="Z55" s="51"/>
+      <c r="AA55" s="107"/>
+      <c r="AB55" s="72"/>
+    </row>
+    <row r="56" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="35">
         <v>8</v>
       </c>
-      <c r="B56" s="72"/>
+      <c r="B56" s="65"/>
       <c r="C56" s="37"/>
       <c r="D56" s="37"/>
       <c r="E56" s="37"/>
       <c r="F56" s="37"/>
-      <c r="G56" s="74"/>
+      <c r="G56" s="67"/>
       <c r="H56" s="39"/>
       <c r="I56" s="40"/>
       <c r="J56" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K56" s="42"/>
-      <c r="L56" s="42"/>
-      <c r="M56" s="76"/>
-      <c r="N56" s="52"/>
-      <c r="O56" s="76"/>
-      <c r="P56" s="76"/>
-      <c r="Q56" s="76"/>
-      <c r="R56" s="116"/>
-      <c r="S56" s="76"/>
-      <c r="T56" s="76"/>
-      <c r="U56" s="76"/>
-      <c r="V56" s="52"/>
-      <c r="W56" s="76"/>
-      <c r="X56" s="76"/>
-      <c r="Y56" s="76"/>
-      <c r="Z56" s="52"/>
-      <c r="AA56" s="115"/>
-      <c r="AB56" s="79"/>
-    </row>
-    <row r="57" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K56" s="41"/>
+      <c r="L56" s="41"/>
+      <c r="M56" s="69"/>
+      <c r="N56" s="51"/>
+      <c r="O56" s="69"/>
+      <c r="P56" s="69"/>
+      <c r="Q56" s="69"/>
+      <c r="R56" s="108"/>
+      <c r="S56" s="69"/>
+      <c r="T56" s="69"/>
+      <c r="U56" s="69"/>
+      <c r="V56" s="51"/>
+      <c r="W56" s="69"/>
+      <c r="X56" s="69"/>
+      <c r="Y56" s="69"/>
+      <c r="Z56" s="51"/>
+      <c r="AA56" s="107"/>
+      <c r="AB56" s="72"/>
+    </row>
+    <row r="57" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="35">
         <v>9</v>
       </c>
-      <c r="B57" s="72"/>
+      <c r="B57" s="65"/>
       <c r="C57" s="37"/>
       <c r="D57" s="37"/>
       <c r="E57" s="37"/>
       <c r="F57" s="37"/>
-      <c r="G57" s="74"/>
+      <c r="G57" s="67"/>
       <c r="H57" s="39"/>
       <c r="I57" s="40"/>
       <c r="J57" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K57" s="42"/>
-      <c r="L57" s="42"/>
-      <c r="M57" s="76"/>
-      <c r="N57" s="52"/>
-      <c r="O57" s="76"/>
-      <c r="P57" s="76"/>
-      <c r="Q57" s="76"/>
-      <c r="R57" s="116"/>
-      <c r="S57" s="76"/>
-      <c r="T57" s="76"/>
-      <c r="U57" s="76"/>
-      <c r="V57" s="52"/>
-      <c r="W57" s="76"/>
-      <c r="X57" s="76"/>
-      <c r="Y57" s="76"/>
-      <c r="Z57" s="52"/>
-      <c r="AA57" s="115"/>
-      <c r="AB57" s="79"/>
-    </row>
-    <row r="58" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K57" s="41"/>
+      <c r="L57" s="41"/>
+      <c r="M57" s="69"/>
+      <c r="N57" s="51"/>
+      <c r="O57" s="69"/>
+      <c r="P57" s="69"/>
+      <c r="Q57" s="69"/>
+      <c r="R57" s="108"/>
+      <c r="S57" s="69"/>
+      <c r="T57" s="69"/>
+      <c r="U57" s="69"/>
+      <c r="V57" s="51"/>
+      <c r="W57" s="69"/>
+      <c r="X57" s="69"/>
+      <c r="Y57" s="69"/>
+      <c r="Z57" s="51"/>
+      <c r="AA57" s="107"/>
+      <c r="AB57" s="72"/>
+    </row>
+    <row r="58" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="35">
         <v>10</v>
       </c>
-      <c r="B58" s="72"/>
+      <c r="B58" s="65"/>
       <c r="C58" s="37"/>
       <c r="D58" s="37"/>
       <c r="E58" s="37"/>
       <c r="F58" s="37"/>
-      <c r="G58" s="74"/>
+      <c r="G58" s="67"/>
       <c r="H58" s="39"/>
       <c r="I58" s="40"/>
       <c r="J58" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K58" s="42"/>
-      <c r="L58" s="42"/>
-      <c r="M58" s="76"/>
-      <c r="N58" s="52"/>
-      <c r="O58" s="76"/>
-      <c r="P58" s="76"/>
-      <c r="Q58" s="76"/>
-      <c r="R58" s="116"/>
-      <c r="S58" s="76"/>
-      <c r="T58" s="76"/>
-      <c r="U58" s="76"/>
-      <c r="V58" s="52"/>
-      <c r="W58" s="76"/>
-      <c r="X58" s="76"/>
-      <c r="Y58" s="76"/>
-      <c r="Z58" s="52"/>
-      <c r="AA58" s="115"/>
-      <c r="AB58" s="79"/>
-    </row>
-    <row r="59" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K58" s="41"/>
+      <c r="L58" s="41"/>
+      <c r="M58" s="69"/>
+      <c r="N58" s="51"/>
+      <c r="O58" s="69"/>
+      <c r="P58" s="69"/>
+      <c r="Q58" s="69"/>
+      <c r="R58" s="108"/>
+      <c r="S58" s="69"/>
+      <c r="T58" s="69"/>
+      <c r="U58" s="69"/>
+      <c r="V58" s="51"/>
+      <c r="W58" s="69"/>
+      <c r="X58" s="69"/>
+      <c r="Y58" s="69"/>
+      <c r="Z58" s="51"/>
+      <c r="AA58" s="107"/>
+      <c r="AB58" s="72"/>
+    </row>
+    <row r="59" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="35">
         <v>11</v>
       </c>
-      <c r="B59" s="72"/>
+      <c r="B59" s="65"/>
       <c r="C59" s="37"/>
       <c r="D59" s="37"/>
       <c r="E59" s="37"/>
       <c r="F59" s="37"/>
-      <c r="G59" s="74"/>
+      <c r="G59" s="67"/>
       <c r="H59" s="39"/>
       <c r="I59" s="40"/>
       <c r="J59" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K59" s="42"/>
-      <c r="L59" s="42"/>
-      <c r="M59" s="76"/>
-      <c r="N59" s="52"/>
-      <c r="O59" s="76"/>
-      <c r="P59" s="76"/>
-      <c r="Q59" s="76"/>
-      <c r="R59" s="116"/>
-      <c r="S59" s="76"/>
-      <c r="T59" s="76"/>
-      <c r="U59" s="76"/>
-      <c r="V59" s="52"/>
-      <c r="W59" s="76"/>
-      <c r="X59" s="76"/>
-      <c r="Y59" s="76"/>
-      <c r="Z59" s="52"/>
-      <c r="AA59" s="115"/>
-      <c r="AB59" s="79"/>
-    </row>
-    <row r="60" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K59" s="41"/>
+      <c r="L59" s="41"/>
+      <c r="M59" s="69"/>
+      <c r="N59" s="51"/>
+      <c r="O59" s="69"/>
+      <c r="P59" s="69"/>
+      <c r="Q59" s="69"/>
+      <c r="R59" s="108"/>
+      <c r="S59" s="69"/>
+      <c r="T59" s="69"/>
+      <c r="U59" s="69"/>
+      <c r="V59" s="51"/>
+      <c r="W59" s="69"/>
+      <c r="X59" s="69"/>
+      <c r="Y59" s="69"/>
+      <c r="Z59" s="51"/>
+      <c r="AA59" s="107"/>
+      <c r="AB59" s="72"/>
+    </row>
+    <row r="60" spans="1:28" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="35">
         <v>12</v>
       </c>
-      <c r="B60" s="72"/>
+      <c r="B60" s="65"/>
       <c r="C60" s="37"/>
       <c r="D60" s="37"/>
       <c r="E60" s="37"/>
       <c r="F60" s="37"/>
-      <c r="G60" s="74"/>
+      <c r="G60" s="67"/>
       <c r="H60" s="39"/>
       <c r="I60" s="40"/>
       <c r="J60" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K60" s="89"/>
-      <c r="L60" s="89"/>
-      <c r="M60" s="89"/>
-      <c r="N60" s="90"/>
-      <c r="O60" s="89"/>
-      <c r="P60" s="89"/>
-      <c r="Q60" s="89"/>
-      <c r="R60" s="90"/>
-      <c r="S60" s="89"/>
-      <c r="T60" s="89"/>
-      <c r="U60" s="89"/>
-      <c r="V60" s="90"/>
-      <c r="W60" s="89"/>
-      <c r="X60" s="89"/>
-      <c r="Y60" s="89"/>
-      <c r="Z60" s="90"/>
-      <c r="AA60" s="91">
+      <c r="K60" s="81"/>
+      <c r="L60" s="81"/>
+      <c r="M60" s="81"/>
+      <c r="N60" s="82"/>
+      <c r="O60" s="81"/>
+      <c r="P60" s="81"/>
+      <c r="Q60" s="81"/>
+      <c r="R60" s="82"/>
+      <c r="S60" s="81"/>
+      <c r="T60" s="81"/>
+      <c r="U60" s="81"/>
+      <c r="V60" s="82"/>
+      <c r="W60" s="81"/>
+      <c r="X60" s="81"/>
+      <c r="Y60" s="81"/>
+      <c r="Z60" s="82"/>
+      <c r="AA60" s="83">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB60" s="92"/>
-    </row>
-    <row r="61" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="119" t="s">
-        <v>60</v>
-      </c>
-      <c r="B61" s="119"/>
-      <c r="C61" s="93">
+      <c r="AB60" s="84"/>
+    </row>
+    <row r="61" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="132" t="s">
+        <v>59</v>
+      </c>
+      <c r="B61" s="132"/>
+      <c r="C61" s="85">
         <f>SUM(C10:C60)</f>
         <v>83.5</v>
       </c>
-      <c r="D61" s="93">
+      <c r="D61" s="85">
         <f>SUM(D10:D60)</f>
         <v>75</v>
       </c>
-      <c r="E61" s="93">
+      <c r="E61" s="85">
         <f>SUM(E10:E60)</f>
         <v>71.75</v>
       </c>
-      <c r="F61" s="93">
+      <c r="F61" s="85">
         <f>SUM(F10:F60)</f>
         <v>85</v>
       </c>
-      <c r="G61" s="94"/>
-      <c r="H61" s="93"/>
-      <c r="I61" s="95"/>
-      <c r="J61" s="93">
+      <c r="G61" s="86"/>
+      <c r="H61" s="85"/>
+      <c r="I61" s="87"/>
+      <c r="J61" s="85">
         <f t="shared" si="1"/>
         <v>315.25</v>
       </c>
-      <c r="K61" s="96"/>
-      <c r="L61" s="96"/>
-      <c r="M61" s="96"/>
-      <c r="N61" s="96"/>
-      <c r="O61" s="96"/>
-      <c r="P61" s="96"/>
-      <c r="Q61" s="96"/>
-      <c r="R61" s="96"/>
-      <c r="S61" s="96"/>
-      <c r="T61" s="96"/>
-      <c r="U61" s="96"/>
-      <c r="V61" s="96"/>
-      <c r="W61" s="96"/>
-      <c r="X61" s="96"/>
-      <c r="Y61" s="96"/>
-      <c r="Z61" s="96"/>
-      <c r="AA61" s="93">
+      <c r="K61" s="88"/>
+      <c r="L61" s="88"/>
+      <c r="M61" s="88"/>
+      <c r="N61" s="88"/>
+      <c r="O61" s="88"/>
+      <c r="P61" s="88"/>
+      <c r="Q61" s="88"/>
+      <c r="R61" s="88"/>
+      <c r="S61" s="88"/>
+      <c r="T61" s="88"/>
+      <c r="U61" s="88"/>
+      <c r="V61" s="88"/>
+      <c r="W61" s="88"/>
+      <c r="X61" s="88"/>
+      <c r="Y61" s="88"/>
+      <c r="Z61" s="88"/>
+      <c r="AA61" s="85">
         <f>SUM(AA10:AA60)</f>
         <v>8.25</v>
       </c>
-      <c r="AB61" s="97"/>
-    </row>
-    <row r="62" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="120" t="s">
-        <v>61</v>
-      </c>
-      <c r="B62" s="120"/>
-      <c r="C62" s="93">
+      <c r="AB61" s="89"/>
+    </row>
+    <row r="62" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="133" t="s">
+        <v>60</v>
+      </c>
+      <c r="B62" s="133"/>
+      <c r="C62" s="85">
         <f>135-C61</f>
         <v>51.5</v>
       </c>
-      <c r="D62" s="93">
+      <c r="D62" s="85">
         <f>135-D61</f>
         <v>60</v>
       </c>
-      <c r="E62" s="93">
+      <c r="E62" s="85">
         <f>135-E61</f>
         <v>63.25</v>
       </c>
-      <c r="F62" s="93">
+      <c r="F62" s="85">
         <f>135-F61</f>
         <v>50</v>
       </c>
-      <c r="G62" s="94"/>
-      <c r="H62" s="93"/>
-      <c r="I62" s="93"/>
-      <c r="J62" s="93">
+      <c r="G62" s="86"/>
+      <c r="H62" s="85"/>
+      <c r="I62" s="85"/>
+      <c r="J62" s="85">
         <f t="shared" si="1"/>
         <v>224.75</v>
       </c>
-      <c r="K62" s="96"/>
-      <c r="L62" s="96"/>
-      <c r="M62" s="96"/>
-      <c r="N62" s="96"/>
-      <c r="O62" s="96"/>
-      <c r="P62" s="96"/>
-      <c r="Q62" s="96"/>
-      <c r="R62" s="96"/>
-      <c r="S62" s="96"/>
-      <c r="T62" s="96"/>
-      <c r="U62" s="96"/>
-      <c r="V62" s="96"/>
-      <c r="W62" s="96"/>
-      <c r="X62" s="96"/>
-      <c r="Y62" s="96"/>
-      <c r="Z62" s="96"/>
-      <c r="AA62" s="96"/>
-      <c r="AB62" s="96"/>
-    </row>
-    <row r="63" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="121" t="s">
+      <c r="K62" s="88"/>
+      <c r="L62" s="88"/>
+      <c r="M62" s="88"/>
+      <c r="N62" s="88"/>
+      <c r="O62" s="88"/>
+      <c r="P62" s="88"/>
+      <c r="Q62" s="88"/>
+      <c r="R62" s="88"/>
+      <c r="S62" s="88"/>
+      <c r="T62" s="88"/>
+      <c r="U62" s="88"/>
+      <c r="V62" s="88"/>
+      <c r="W62" s="88"/>
+      <c r="X62" s="88"/>
+      <c r="Y62" s="88"/>
+      <c r="Z62" s="88"/>
+      <c r="AA62" s="88"/>
+      <c r="AB62" s="88"/>
+    </row>
+    <row r="63" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="134" t="s">
+        <v>61</v>
+      </c>
+      <c r="B63" s="134"/>
+      <c r="C63" s="85"/>
+      <c r="D63" s="85"/>
+      <c r="E63" s="85"/>
+      <c r="F63" s="85"/>
+      <c r="G63" s="85"/>
+      <c r="H63" s="85"/>
+      <c r="I63" s="85"/>
+      <c r="J63" s="85">
+        <f>C63+D63+F63+E63</f>
+        <v>0</v>
+      </c>
+      <c r="K63" s="88"/>
+      <c r="L63" s="88"/>
+      <c r="M63" s="88"/>
+      <c r="N63" s="88"/>
+      <c r="O63" s="88"/>
+      <c r="P63" s="88"/>
+      <c r="Q63" s="88"/>
+      <c r="R63" s="88"/>
+      <c r="S63" s="88"/>
+      <c r="T63" s="88"/>
+      <c r="U63" s="88"/>
+      <c r="V63" s="88"/>
+      <c r="W63" s="88"/>
+      <c r="X63" s="88"/>
+      <c r="Y63" s="88"/>
+      <c r="Z63" s="88"/>
+      <c r="AA63" s="88"/>
+      <c r="AB63" s="88"/>
+    </row>
+    <row r="64" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="133" t="s">
         <v>62</v>
       </c>
-      <c r="B63" s="121"/>
-      <c r="C63" s="93"/>
-      <c r="D63" s="93"/>
-      <c r="E63" s="93"/>
-      <c r="F63" s="93"/>
-      <c r="G63" s="93"/>
-      <c r="H63" s="93"/>
-      <c r="I63" s="93"/>
-      <c r="J63" s="93">
-        <f>C63+D63+F63+E63</f>
-        <v>0</v>
-      </c>
-      <c r="K63" s="96"/>
-      <c r="L63" s="96"/>
-      <c r="M63" s="96"/>
-      <c r="N63" s="96"/>
-      <c r="O63" s="96"/>
-      <c r="P63" s="96"/>
-      <c r="Q63" s="96"/>
-      <c r="R63" s="96"/>
-      <c r="S63" s="96"/>
-      <c r="T63" s="96"/>
-      <c r="U63" s="96"/>
-      <c r="V63" s="96"/>
-      <c r="W63" s="96"/>
-      <c r="X63" s="96"/>
-      <c r="Y63" s="96"/>
-      <c r="Z63" s="96"/>
-      <c r="AA63" s="96"/>
-      <c r="AB63" s="96"/>
-    </row>
-    <row r="64" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="120" t="s">
-        <v>63</v>
-      </c>
-      <c r="B64" s="120"/>
-      <c r="C64" s="93"/>
-      <c r="D64" s="93"/>
-      <c r="E64" s="98"/>
-      <c r="F64" s="93"/>
-      <c r="G64" s="93"/>
-      <c r="H64" s="93"/>
-      <c r="I64" s="99">
+      <c r="B64" s="133"/>
+      <c r="C64" s="85"/>
+      <c r="D64" s="85"/>
+      <c r="E64" s="90"/>
+      <c r="F64" s="85"/>
+      <c r="G64" s="85"/>
+      <c r="H64" s="85"/>
+      <c r="I64" s="91">
         <f>SUM(I10:I60)</f>
         <v>368</v>
       </c>
-      <c r="J64" s="93">
+      <c r="J64" s="85">
         <f>SUM(J10:J60)</f>
         <v>315.25</v>
       </c>
-      <c r="K64" s="96"/>
-      <c r="L64" s="96"/>
-      <c r="M64" s="96"/>
-      <c r="N64" s="96"/>
-      <c r="O64" s="96"/>
-      <c r="P64" s="96"/>
-      <c r="Q64" s="96"/>
-      <c r="R64" s="96"/>
-      <c r="S64" s="96"/>
-      <c r="T64" s="96"/>
-      <c r="U64" s="96"/>
-      <c r="V64" s="96"/>
-      <c r="W64" s="96"/>
-      <c r="X64" s="96"/>
-      <c r="Y64" s="96"/>
-      <c r="Z64" s="96"/>
-      <c r="AA64" s="96"/>
-      <c r="AB64" s="96"/>
-    </row>
-    <row r="65" spans="1:28" ht="16" x14ac:dyDescent="0.2">
-      <c r="A65" s="100"/>
-      <c r="B65" s="100"/>
-      <c r="C65" s="101"/>
-      <c r="D65" s="101"/>
-      <c r="E65" s="101"/>
-      <c r="F65" s="101"/>
-      <c r="G65" s="101"/>
-      <c r="H65" s="101"/>
-      <c r="I65" s="101"/>
-      <c r="J65" s="101"/>
-      <c r="K65" s="96"/>
-      <c r="L65" s="96"/>
-      <c r="M65" s="96"/>
-      <c r="N65" s="96"/>
-      <c r="O65" s="96"/>
-      <c r="P65" s="96"/>
-      <c r="Q65" s="96"/>
-      <c r="R65" s="96"/>
-      <c r="S65" s="96"/>
-      <c r="T65" s="96"/>
-      <c r="U65" s="96"/>
-      <c r="V65" s="96"/>
-      <c r="W65" s="96"/>
-      <c r="X65" s="96"/>
-      <c r="Y65" s="96"/>
-      <c r="Z65" s="96"/>
-      <c r="AA65" s="96"/>
-      <c r="AB65" s="96"/>
-    </row>
-    <row r="66" spans="1:28" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="121" t="s">
-        <v>64</v>
-      </c>
-      <c r="B66" s="121"/>
-      <c r="C66" s="93">
+      <c r="K64" s="88"/>
+      <c r="L64" s="88"/>
+      <c r="M64" s="88"/>
+      <c r="N64" s="88"/>
+      <c r="O64" s="88"/>
+      <c r="P64" s="88"/>
+      <c r="Q64" s="88"/>
+      <c r="R64" s="88"/>
+      <c r="S64" s="88"/>
+      <c r="T64" s="88"/>
+      <c r="U64" s="88"/>
+      <c r="V64" s="88"/>
+      <c r="W64" s="88"/>
+      <c r="X64" s="88"/>
+      <c r="Y64" s="88"/>
+      <c r="Z64" s="88"/>
+      <c r="AA64" s="88"/>
+      <c r="AB64" s="88"/>
+    </row>
+    <row r="65" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="92"/>
+      <c r="B65" s="92"/>
+      <c r="C65" s="93"/>
+      <c r="D65" s="93"/>
+      <c r="E65" s="93"/>
+      <c r="F65" s="93"/>
+      <c r="G65" s="93"/>
+      <c r="H65" s="93"/>
+      <c r="I65" s="93"/>
+      <c r="J65" s="93"/>
+      <c r="K65" s="88"/>
+      <c r="L65" s="88"/>
+      <c r="M65" s="88"/>
+      <c r="N65" s="88"/>
+      <c r="O65" s="88"/>
+      <c r="P65" s="88"/>
+      <c r="Q65" s="88"/>
+      <c r="R65" s="88"/>
+      <c r="S65" s="88"/>
+      <c r="T65" s="88"/>
+      <c r="U65" s="88"/>
+      <c r="V65" s="88"/>
+      <c r="W65" s="88"/>
+      <c r="X65" s="88"/>
+      <c r="Y65" s="88"/>
+      <c r="Z65" s="88"/>
+      <c r="AA65" s="88"/>
+      <c r="AB65" s="88"/>
+    </row>
+    <row r="66" spans="1:28" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="134" t="s">
+        <v>63</v>
+      </c>
+      <c r="B66" s="134"/>
+      <c r="C66" s="85">
         <f>135*4</f>
         <v>540</v>
       </c>
-      <c r="D66" s="101"/>
-      <c r="E66" s="101"/>
-      <c r="F66" s="101"/>
-      <c r="G66" s="101"/>
-      <c r="H66" s="101"/>
-      <c r="I66" s="101"/>
-      <c r="J66" s="101"/>
-      <c r="K66" s="96"/>
-      <c r="L66" s="96"/>
-      <c r="M66" s="96"/>
-      <c r="N66" s="96"/>
-      <c r="O66" s="96"/>
-      <c r="P66" s="96"/>
-      <c r="Q66" s="96"/>
-      <c r="R66" s="96"/>
-      <c r="S66" s="96"/>
-      <c r="T66" s="96"/>
-      <c r="U66" s="96"/>
-      <c r="V66" s="96"/>
-      <c r="W66" s="96"/>
-      <c r="X66" s="96"/>
-      <c r="Y66" s="96"/>
-      <c r="Z66" s="96"/>
-      <c r="AA66" s="96"/>
-      <c r="AB66" s="96"/>
-    </row>
-    <row r="67" spans="1:28" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="118" t="s">
-        <v>65</v>
-      </c>
-      <c r="B67" s="118"/>
-      <c r="C67" s="93">
+      <c r="D66" s="93"/>
+      <c r="E66" s="93"/>
+      <c r="F66" s="93"/>
+      <c r="G66" s="93"/>
+      <c r="H66" s="93"/>
+      <c r="I66" s="93"/>
+      <c r="J66" s="93"/>
+      <c r="K66" s="88"/>
+      <c r="L66" s="88"/>
+      <c r="M66" s="88"/>
+      <c r="N66" s="88"/>
+      <c r="O66" s="88"/>
+      <c r="P66" s="88"/>
+      <c r="Q66" s="88"/>
+      <c r="R66" s="88"/>
+      <c r="S66" s="88"/>
+      <c r="T66" s="88"/>
+      <c r="U66" s="88"/>
+      <c r="V66" s="88"/>
+      <c r="W66" s="88"/>
+      <c r="X66" s="88"/>
+      <c r="Y66" s="88"/>
+      <c r="Z66" s="88"/>
+      <c r="AA66" s="88"/>
+      <c r="AB66" s="88"/>
+    </row>
+    <row r="67" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="131" t="s">
+        <v>64</v>
+      </c>
+      <c r="B67" s="131"/>
+      <c r="C67" s="85">
         <f>C66-J64</f>
         <v>224.75</v>
       </c>
-      <c r="D67" s="101"/>
-      <c r="E67" s="101"/>
-      <c r="F67" s="101"/>
-      <c r="G67" s="101"/>
-      <c r="H67" s="101"/>
-      <c r="I67" s="101"/>
-      <c r="J67" s="101"/>
-      <c r="K67" s="96"/>
-      <c r="L67" s="96"/>
-      <c r="M67" s="96"/>
-      <c r="N67" s="96"/>
-      <c r="O67" s="96"/>
-      <c r="P67" s="96"/>
-      <c r="Q67" s="96"/>
-      <c r="R67" s="96"/>
-      <c r="S67" s="96"/>
-      <c r="T67" s="96"/>
-      <c r="U67" s="96"/>
-      <c r="V67" s="96"/>
-      <c r="W67" s="96"/>
-      <c r="X67" s="96"/>
-      <c r="Y67" s="96"/>
-      <c r="Z67" s="96"/>
-      <c r="AA67" s="96"/>
-      <c r="AB67" s="96"/>
-    </row>
-    <row r="68" spans="1:28" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="102"/>
-      <c r="B68" s="100"/>
-      <c r="C68" s="103"/>
-      <c r="D68" s="103"/>
-      <c r="E68" s="103"/>
-      <c r="F68" s="103"/>
-      <c r="G68" s="100"/>
-      <c r="H68" s="104"/>
-      <c r="I68" s="105"/>
-      <c r="J68" s="105"/>
-      <c r="AA68" s="96"/>
-    </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="D69" s="106"/>
-      <c r="E69" s="106"/>
-      <c r="F69" s="106"/>
-    </row>
-    <row r="70" spans="1:28" s="108" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="A70" s="107"/>
-      <c r="C70" s="109"/>
-      <c r="D70" s="109"/>
-      <c r="E70" s="109"/>
-      <c r="F70" s="109"/>
-      <c r="H70" s="110"/>
-      <c r="I70" s="111"/>
-      <c r="J70" s="111"/>
-      <c r="N70" s="112"/>
-      <c r="R70" s="112"/>
-      <c r="V70" s="112"/>
-      <c r="Z70" s="112"/>
-      <c r="AA70" s="113"/>
-    </row>
-    <row r="71" spans="1:28" s="108" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="C71" s="109"/>
-      <c r="D71" s="109"/>
-      <c r="E71" s="109"/>
-      <c r="F71" s="109"/>
-      <c r="H71" s="110"/>
-      <c r="I71" s="111"/>
-      <c r="J71" s="111"/>
-      <c r="N71" s="112"/>
-      <c r="R71" s="112"/>
-      <c r="V71" s="112"/>
-      <c r="Z71" s="112"/>
-      <c r="AA71" s="113"/>
-    </row>
-    <row r="72" spans="1:28" s="108" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="C72" s="109"/>
-      <c r="D72" s="109"/>
-      <c r="E72" s="109"/>
-      <c r="F72" s="109"/>
-      <c r="H72" s="110"/>
-      <c r="I72" s="111"/>
-      <c r="J72" s="111"/>
-      <c r="N72" s="112"/>
-      <c r="R72" s="112"/>
-      <c r="V72" s="112"/>
-      <c r="Z72" s="112"/>
-      <c r="AA72" s="113"/>
+      <c r="D67" s="93"/>
+      <c r="E67" s="93"/>
+      <c r="F67" s="93"/>
+      <c r="G67" s="93"/>
+      <c r="H67" s="93"/>
+      <c r="I67" s="93"/>
+      <c r="J67" s="93"/>
+      <c r="K67" s="88"/>
+      <c r="L67" s="88"/>
+      <c r="M67" s="88"/>
+      <c r="N67" s="88"/>
+      <c r="O67" s="88"/>
+      <c r="P67" s="88"/>
+      <c r="Q67" s="88"/>
+      <c r="R67" s="88"/>
+      <c r="S67" s="88"/>
+      <c r="T67" s="88"/>
+      <c r="U67" s="88"/>
+      <c r="V67" s="88"/>
+      <c r="W67" s="88"/>
+      <c r="X67" s="88"/>
+      <c r="Y67" s="88"/>
+      <c r="Z67" s="88"/>
+      <c r="AA67" s="88"/>
+      <c r="AB67" s="88"/>
+    </row>
+    <row r="68" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="94"/>
+      <c r="B68" s="92"/>
+      <c r="C68" s="95"/>
+      <c r="D68" s="95"/>
+      <c r="E68" s="95"/>
+      <c r="F68" s="95"/>
+      <c r="G68" s="92"/>
+      <c r="H68" s="96"/>
+      <c r="I68" s="97"/>
+      <c r="J68" s="97"/>
+      <c r="AA68" s="88"/>
+    </row>
+    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="D69" s="98"/>
+      <c r="E69" s="98"/>
+      <c r="F69" s="98"/>
+    </row>
+    <row r="70" spans="1:28" s="100" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A70" s="99"/>
+      <c r="C70" s="101"/>
+      <c r="D70" s="101"/>
+      <c r="E70" s="101"/>
+      <c r="F70" s="101"/>
+      <c r="H70" s="102"/>
+      <c r="I70" s="103"/>
+      <c r="J70" s="103"/>
+      <c r="N70" s="104"/>
+      <c r="R70" s="104"/>
+      <c r="V70" s="104"/>
+      <c r="Z70" s="104"/>
+      <c r="AA70" s="105"/>
+    </row>
+    <row r="71" spans="1:28" s="100" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C71" s="101"/>
+      <c r="D71" s="101"/>
+      <c r="E71" s="101"/>
+      <c r="F71" s="101"/>
+      <c r="H71" s="102"/>
+      <c r="I71" s="103"/>
+      <c r="J71" s="103"/>
+      <c r="N71" s="104"/>
+      <c r="R71" s="104"/>
+      <c r="V71" s="104"/>
+      <c r="Z71" s="104"/>
+      <c r="AA71" s="105"/>
+    </row>
+    <row r="72" spans="1:28" s="100" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C72" s="101"/>
+      <c r="D72" s="101"/>
+      <c r="E72" s="101"/>
+      <c r="F72" s="101"/>
+      <c r="H72" s="102"/>
+      <c r="I72" s="103"/>
+      <c r="J72" s="103"/>
+      <c r="N72" s="104"/>
+      <c r="R72" s="104"/>
+      <c r="V72" s="104"/>
+      <c r="Z72" s="104"/>
+      <c r="AA72" s="105"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:Z7"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
+  <mergeCells count="22">
+    <mergeCell ref="S6:V6"/>
     <mergeCell ref="A67:B67"/>
     <mergeCell ref="A61:B61"/>
     <mergeCell ref="A62:B62"/>
     <mergeCell ref="A63:B63"/>
     <mergeCell ref="A64:B64"/>
     <mergeCell ref="A66:B66"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:Z7"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K6:R6"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
     <cfRule type="containsText" dxfId="28" priority="23" operator="containsText" text="En cours">
@@ -5515,20 +5564,20 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="10.6640625" style="1"/>
+    <col min="1" max="1025" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="106" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="114">
+      <c r="B1" s="106">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -5536,7 +5585,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -5556,9 +5605,9 @@
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="10.6640625" style="1"/>
+    <col min="1" max="1025" width="10.7109375" style="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Semainiers de du 11mars
</commit_message>
<xml_diff>
--- a/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
+++ b/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abourdeau\source\repos\mrjrdg\marque-sans-nom\Semainiers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Desktop/marque-sans-nom/Semainiers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B80EA8-BD2F-4DCC-8EC0-0E12E04660BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1EB6F3-9CFC-CB4E-B0EC-8D2732FE16C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4660" yWindow="460" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -1352,52 +1350,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="7" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="4" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1417,15 +1369,61 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Excel Built-in 60% - Accent4" xfId="7" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Excel Built-in Bad" xfId="6" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Excel Built-in Good" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Excel Built-in Good 1" xfId="8" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Excel Built-in Neutral" xfId="5" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Excel Built-in Normal" xfId="3" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Milliers" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
@@ -1790,7 +1788,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2091,51 +2089,51 @@
   </sheetPr>
   <dimension ref="A1:AMK72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="W49" sqref="W49"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="66.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="2" customWidth="1"/>
-    <col min="4" max="5" width="8.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="66.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="8.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" style="3" customWidth="1"/>
-    <col min="9" max="10" width="9.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="3" customWidth="1"/>
+    <col min="9" max="10" width="9.33203125" style="4" customWidth="1"/>
     <col min="11" max="13" width="8" style="1" customWidth="1"/>
     <col min="14" max="14" width="8" style="5" customWidth="1"/>
-    <col min="15" max="16" width="7.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.7109375" style="6" customWidth="1"/>
-    <col min="28" max="28" width="22.7109375" style="1" customWidth="1"/>
-    <col min="29" max="1025" width="10.7109375" style="1"/>
+    <col min="15" max="16" width="7.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="7.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.6640625" style="6" customWidth="1"/>
+    <col min="28" max="28" width="22.6640625" style="1" customWidth="1"/>
+    <col min="29" max="1025" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="119" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="119"/>
+    <row r="1" spans="1:28" s="8" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="141"/>
       <c r="C1" s="7"/>
-      <c r="D1" s="120" t="s">
+      <c r="D1" s="142" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
-      <c r="J1" s="120"/>
-      <c r="K1" s="120"/>
-      <c r="L1" s="120"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
+      <c r="J1" s="142"/>
+      <c r="K1" s="142"/>
+      <c r="L1" s="142"/>
       <c r="N1" s="3"/>
       <c r="P1" s="9"/>
       <c r="Q1" s="8" t="s">
@@ -2146,21 +2144,21 @@
       <c r="Z1" s="3"/>
       <c r="AA1" s="10"/>
     </row>
-    <row r="2" spans="1:28" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="119" t="s">
+    <row r="2" spans="1:28" s="8" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="141" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="119"/>
+      <c r="B2" s="141"/>
       <c r="C2" s="7"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="119" t="s">
+      <c r="F2" s="141" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="119"/>
-      <c r="H2" s="119"/>
-      <c r="I2" s="119"/>
-      <c r="J2" s="119"/>
+      <c r="G2" s="141"/>
+      <c r="H2" s="141"/>
+      <c r="I2" s="141"/>
+      <c r="J2" s="141"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
       <c r="N2" s="3"/>
@@ -2173,7 +2171,7 @@
       <c r="Z2" s="3"/>
       <c r="AA2" s="10"/>
     </row>
-    <row r="3" spans="1:28" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -2191,7 +2189,7 @@
       <c r="Z3" s="3"/>
       <c r="AA3" s="10"/>
     </row>
-    <row r="4" spans="1:28" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
@@ -2211,7 +2209,7 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="10"/>
     </row>
-    <row r="5" spans="1:28" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.2">
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
@@ -2235,7 +2233,7 @@
       </c>
       <c r="AA5" s="10"/>
     </row>
-    <row r="6" spans="1:28" s="8" customFormat="1" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" s="8" customFormat="1" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
@@ -2243,78 +2241,78 @@
       <c r="H6" s="3"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="121" t="s">
+      <c r="K6" s="143" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="121"/>
-      <c r="M6" s="121"/>
-      <c r="N6" s="121"/>
-      <c r="O6" s="121"/>
-      <c r="P6" s="121"/>
-      <c r="Q6" s="121"/>
-      <c r="R6" s="121"/>
-      <c r="S6" s="141" t="s">
+      <c r="L6" s="143"/>
+      <c r="M6" s="143"/>
+      <c r="N6" s="143"/>
+      <c r="O6" s="143"/>
+      <c r="P6" s="143"/>
+      <c r="Q6" s="143"/>
+      <c r="R6" s="143"/>
+      <c r="S6" s="125" t="s">
         <v>76</v>
       </c>
-      <c r="T6" s="142"/>
-      <c r="U6" s="142"/>
-      <c r="V6" s="143"/>
+      <c r="T6" s="126"/>
+      <c r="U6" s="126"/>
+      <c r="V6" s="127"/>
       <c r="Z6" s="17"/>
       <c r="AA6" s="10"/>
     </row>
-    <row r="7" spans="1:28" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="122" t="s">
+    <row r="7" spans="1:28" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="136" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="123" t="s">
+      <c r="B7" s="137" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="124" t="s">
+      <c r="C7" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="124"/>
-      <c r="E7" s="124"/>
-      <c r="F7" s="124"/>
-      <c r="G7" s="125" t="s">
+      <c r="D7" s="138"/>
+      <c r="E7" s="138"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="139" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="126" t="s">
+      <c r="H7" s="140" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="127" t="s">
+      <c r="I7" s="132" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="127" t="s">
+      <c r="J7" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="128" t="s">
+      <c r="K7" s="133" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="128"/>
-      <c r="M7" s="128"/>
-      <c r="N7" s="128"/>
-      <c r="O7" s="128"/>
-      <c r="P7" s="128"/>
-      <c r="Q7" s="128"/>
-      <c r="R7" s="128"/>
-      <c r="S7" s="128"/>
-      <c r="T7" s="128"/>
-      <c r="U7" s="128"/>
-      <c r="V7" s="128"/>
-      <c r="W7" s="128"/>
-      <c r="X7" s="128"/>
-      <c r="Y7" s="128"/>
-      <c r="Z7" s="128"/>
-      <c r="AA7" s="129" t="s">
+      <c r="L7" s="133"/>
+      <c r="M7" s="133"/>
+      <c r="N7" s="133"/>
+      <c r="O7" s="133"/>
+      <c r="P7" s="133"/>
+      <c r="Q7" s="133"/>
+      <c r="R7" s="133"/>
+      <c r="S7" s="133"/>
+      <c r="T7" s="133"/>
+      <c r="U7" s="133"/>
+      <c r="V7" s="133"/>
+      <c r="W7" s="133"/>
+      <c r="X7" s="133"/>
+      <c r="Y7" s="133"/>
+      <c r="Z7" s="133"/>
+      <c r="AA7" s="134" t="s">
         <v>18</v>
       </c>
-      <c r="AB7" s="130" t="s">
+      <c r="AB7" s="135" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="122"/>
-      <c r="B8" s="123"/>
+    <row r="8" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="136"/>
+      <c r="B8" s="137"/>
       <c r="C8" s="20" t="s">
         <v>74</v>
       </c>
@@ -2327,10 +2325,10 @@
       <c r="F8" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="125"/>
-      <c r="H8" s="126"/>
-      <c r="I8" s="127"/>
-      <c r="J8" s="127"/>
+      <c r="G8" s="139"/>
+      <c r="H8" s="140"/>
+      <c r="I8" s="132"/>
+      <c r="J8" s="132"/>
       <c r="K8" s="21">
         <v>43838</v>
       </c>
@@ -2394,10 +2392,10 @@
         <f t="shared" si="0"/>
         <v>43943</v>
       </c>
-      <c r="AA8" s="129"/>
-      <c r="AB8" s="130"/>
-    </row>
-    <row r="9" spans="1:28" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="AA8" s="134"/>
+      <c r="AB8" s="135"/>
+    </row>
+    <row r="9" spans="1:28" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>22</v>
@@ -2429,7 +2427,7 @@
       <c r="AA9" s="33"/>
       <c r="AB9" s="34"/>
     </row>
-    <row r="10" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="35">
         <v>1</v>
       </c>
@@ -2462,7 +2460,7 @@
         <f t="shared" ref="J10:J62" si="1">SUM(C10:F10)</f>
         <v>6</v>
       </c>
-      <c r="K10" s="135"/>
+      <c r="K10" s="119"/>
       <c r="L10" s="41"/>
       <c r="M10" s="41"/>
       <c r="N10" s="42"/>
@@ -2484,7 +2482,7 @@
       </c>
       <c r="AB10" s="44"/>
     </row>
-    <row r="11" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="35">
         <v>2</v>
       </c>
@@ -2517,7 +2515,7 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="K11" s="135"/>
+      <c r="K11" s="119"/>
       <c r="L11" s="41"/>
       <c r="M11" s="41"/>
       <c r="N11" s="42"/>
@@ -2539,7 +2537,7 @@
       </c>
       <c r="AB11" s="47"/>
     </row>
-    <row r="12" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="35">
         <v>3</v>
       </c>
@@ -2573,7 +2571,7 @@
         <v>12</v>
       </c>
       <c r="K12" s="41"/>
-      <c r="L12" s="135"/>
+      <c r="L12" s="119"/>
       <c r="N12" s="42"/>
       <c r="O12" s="41"/>
       <c r="P12" s="41"/>
@@ -2593,7 +2591,7 @@
       </c>
       <c r="AB12" s="48"/>
     </row>
-    <row r="13" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="35">
         <v>4</v>
       </c>
@@ -2627,8 +2625,8 @@
         <v>8</v>
       </c>
       <c r="K13" s="41"/>
-      <c r="L13" s="135"/>
-      <c r="M13" s="135"/>
+      <c r="L13" s="119"/>
+      <c r="M13" s="119"/>
       <c r="N13" s="42"/>
       <c r="O13" s="41"/>
       <c r="P13" s="41"/>
@@ -2648,7 +2646,7 @@
       </c>
       <c r="AB13" s="47"/>
     </row>
-    <row r="14" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="35">
         <v>5</v>
       </c>
@@ -2683,7 +2681,7 @@
       </c>
       <c r="K14" s="41"/>
       <c r="L14" s="41"/>
-      <c r="M14" s="135"/>
+      <c r="M14" s="119"/>
       <c r="N14" s="42"/>
       <c r="O14" s="41"/>
       <c r="P14" s="41"/>
@@ -2703,7 +2701,7 @@
       </c>
       <c r="AB14" s="47"/>
     </row>
-    <row r="15" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="35">
         <v>6</v>
       </c>
@@ -2737,7 +2735,7 @@
         <v>4</v>
       </c>
       <c r="K15" s="41"/>
-      <c r="L15" s="135"/>
+      <c r="L15" s="119"/>
       <c r="M15" s="50"/>
       <c r="N15" s="51"/>
       <c r="O15" s="41"/>
@@ -2758,7 +2756,7 @@
       </c>
       <c r="AB15" s="47"/>
     </row>
-    <row r="16" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="35">
         <v>7</v>
       </c>
@@ -2793,8 +2791,8 @@
       </c>
       <c r="K16" s="41"/>
       <c r="L16" s="41"/>
-      <c r="M16" s="136"/>
-      <c r="N16" s="136"/>
+      <c r="M16" s="120"/>
+      <c r="N16" s="120"/>
       <c r="O16" s="52"/>
       <c r="P16" s="52"/>
       <c r="Q16" s="52"/>
@@ -2813,7 +2811,7 @@
       </c>
       <c r="AB16" s="47"/>
     </row>
-    <row r="17" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="35">
         <v>8</v>
       </c>
@@ -2848,7 +2846,7 @@
       </c>
       <c r="K17" s="41"/>
       <c r="L17" s="41"/>
-      <c r="M17" s="136"/>
+      <c r="M17" s="120"/>
       <c r="N17" s="46"/>
       <c r="O17" s="52"/>
       <c r="P17" s="52"/>
@@ -2868,7 +2866,7 @@
       </c>
       <c r="AB17" s="47"/>
     </row>
-    <row r="18" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="35">
         <v>9</v>
       </c>
@@ -2903,12 +2901,12 @@
       </c>
       <c r="K18" s="41"/>
       <c r="L18" s="56"/>
-      <c r="M18" s="138"/>
+      <c r="M18" s="122"/>
       <c r="N18" s="57"/>
       <c r="O18" s="52"/>
       <c r="P18" s="52"/>
       <c r="Q18" s="52"/>
-      <c r="R18" s="138"/>
+      <c r="R18" s="122"/>
       <c r="S18" s="52"/>
       <c r="T18" s="52"/>
       <c r="U18" s="54"/>
@@ -2923,7 +2921,7 @@
       </c>
       <c r="AB18" s="47"/>
     </row>
-    <row r="19" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="35">
         <v>10</v>
       </c>
@@ -2958,8 +2956,8 @@
       </c>
       <c r="K19" s="41"/>
       <c r="L19" s="56"/>
-      <c r="M19" s="135"/>
-      <c r="N19" s="137"/>
+      <c r="M19" s="119"/>
+      <c r="N19" s="121"/>
       <c r="O19" s="52"/>
       <c r="P19" s="52"/>
       <c r="Q19" s="58"/>
@@ -2978,7 +2976,7 @@
       </c>
       <c r="AB19" s="47"/>
     </row>
-    <row r="20" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="35">
         <v>11</v>
       </c>
@@ -3018,7 +3016,7 @@
       <c r="O20" s="52"/>
       <c r="P20" s="52"/>
       <c r="Q20" s="52"/>
-      <c r="R20" s="138"/>
+      <c r="R20" s="122"/>
       <c r="S20" s="52"/>
       <c r="T20" s="52"/>
       <c r="U20" s="54"/>
@@ -3033,7 +3031,7 @@
       </c>
       <c r="AB20" s="47"/>
     </row>
-    <row r="21" spans="1:28" s="45" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="35">
         <v>12</v>
       </c>
@@ -3088,7 +3086,7 @@
       </c>
       <c r="AB21" s="47"/>
     </row>
-    <row r="22" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="35">
         <v>13</v>
       </c>
@@ -3123,8 +3121,8 @@
       </c>
       <c r="K22" s="62"/>
       <c r="L22" s="56"/>
-      <c r="M22" s="135"/>
-      <c r="N22" s="137"/>
+      <c r="M22" s="119"/>
+      <c r="N22" s="121"/>
       <c r="O22" s="62"/>
       <c r="P22" s="62"/>
       <c r="Q22" s="63"/>
@@ -3143,7 +3141,7 @@
       </c>
       <c r="AB22" s="47"/>
     </row>
-    <row r="23" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="35">
         <v>14</v>
       </c>
@@ -3178,8 +3176,8 @@
       </c>
       <c r="K23" s="62"/>
       <c r="L23" s="56"/>
-      <c r="M23" s="135"/>
-      <c r="N23" s="135"/>
+      <c r="M23" s="119"/>
+      <c r="N23" s="119"/>
       <c r="O23" s="62"/>
       <c r="P23" s="62"/>
       <c r="Q23" s="63"/>
@@ -3198,7 +3196,7 @@
       </c>
       <c r="AB23" s="47"/>
     </row>
-    <row r="24" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="35">
         <v>15</v>
       </c>
@@ -3233,12 +3231,12 @@
       </c>
       <c r="K24" s="62"/>
       <c r="L24" s="56"/>
-      <c r="M24" s="135"/>
-      <c r="N24" s="135"/>
-      <c r="O24" s="135"/>
-      <c r="P24" s="135"/>
-      <c r="Q24" s="135"/>
-      <c r="R24" s="136"/>
+      <c r="M24" s="119"/>
+      <c r="N24" s="119"/>
+      <c r="O24" s="119"/>
+      <c r="P24" s="119"/>
+      <c r="Q24" s="119"/>
+      <c r="R24" s="120"/>
       <c r="S24" s="52"/>
       <c r="T24" s="52"/>
       <c r="U24" s="54"/>
@@ -3253,7 +3251,7 @@
       </c>
       <c r="AB24" s="47"/>
     </row>
-    <row r="25" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="35">
         <v>16</v>
       </c>
@@ -3288,11 +3286,11 @@
       </c>
       <c r="K25" s="62"/>
       <c r="L25" s="56"/>
-      <c r="M25" s="135"/>
-      <c r="N25" s="135"/>
-      <c r="O25" s="135"/>
+      <c r="M25" s="119"/>
+      <c r="N25" s="119"/>
+      <c r="O25" s="119"/>
       <c r="P25" s="64"/>
-      <c r="Q25" s="135"/>
+      <c r="Q25" s="119"/>
       <c r="R25" s="110"/>
       <c r="S25" s="52"/>
       <c r="T25" s="52"/>
@@ -3308,7 +3306,7 @@
       </c>
       <c r="AB25" s="47"/>
     </row>
-    <row r="26" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="35">
         <v>17</v>
       </c>
@@ -3345,7 +3343,7 @@
       <c r="L26" s="69"/>
       <c r="M26" s="69"/>
       <c r="N26" s="51"/>
-      <c r="O26" s="136"/>
+      <c r="O26" s="120"/>
       <c r="P26" s="41"/>
       <c r="Q26" s="41"/>
       <c r="R26" s="70"/>
@@ -3363,7 +3361,7 @@
       </c>
       <c r="AB26" s="72"/>
     </row>
-    <row r="27" spans="1:28" s="75" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" s="75" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="35">
         <v>18</v>
       </c>
@@ -3400,7 +3398,7 @@
       <c r="L27" s="41"/>
       <c r="M27" s="41"/>
       <c r="N27" s="42"/>
-      <c r="O27" s="136"/>
+      <c r="O27" s="120"/>
       <c r="P27" s="41"/>
       <c r="Q27" s="41"/>
       <c r="R27" s="42"/>
@@ -3418,7 +3416,7 @@
       </c>
       <c r="AB27" s="47"/>
     </row>
-    <row r="28" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="35">
         <v>19</v>
       </c>
@@ -3456,7 +3454,7 @@
       <c r="M28" s="78"/>
       <c r="N28" s="79"/>
       <c r="O28" s="41"/>
-      <c r="P28" s="136"/>
+      <c r="P28" s="120"/>
       <c r="Q28" s="41"/>
       <c r="R28" s="79"/>
       <c r="S28" s="78"/>
@@ -3473,7 +3471,7 @@
       </c>
       <c r="AB28" s="47"/>
     </row>
-    <row r="29" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="35">
         <v>20</v>
       </c>
@@ -3511,7 +3509,7 @@
       <c r="M29" s="41"/>
       <c r="N29" s="42"/>
       <c r="O29" s="41"/>
-      <c r="P29" s="135"/>
+      <c r="P29" s="119"/>
       <c r="Q29" s="41"/>
       <c r="R29" s="42"/>
       <c r="S29" s="41"/>
@@ -3528,7 +3526,7 @@
       </c>
       <c r="AB29" s="47"/>
     </row>
-    <row r="30" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="35">
         <v>21</v>
       </c>
@@ -3566,9 +3564,9 @@
       <c r="M30" s="69"/>
       <c r="N30" s="51"/>
       <c r="O30" s="41"/>
-      <c r="P30" s="136"/>
+      <c r="P30" s="120"/>
       <c r="Q30" s="41"/>
-      <c r="R30" s="138"/>
+      <c r="R30" s="122"/>
       <c r="S30" s="69"/>
       <c r="T30" s="69"/>
       <c r="U30" s="69"/>
@@ -3583,7 +3581,7 @@
       </c>
       <c r="AB30" s="47"/>
     </row>
-    <row r="31" spans="1:28" s="75" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" s="75" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="35">
         <v>22</v>
       </c>
@@ -3621,7 +3619,7 @@
       <c r="M31" s="41"/>
       <c r="N31" s="42"/>
       <c r="O31" s="41"/>
-      <c r="P31" s="136"/>
+      <c r="P31" s="120"/>
       <c r="Q31" s="41"/>
       <c r="R31" s="42"/>
       <c r="S31" s="41"/>
@@ -3638,7 +3636,7 @@
       </c>
       <c r="AB31" s="47"/>
     </row>
-    <row r="32" spans="1:28" s="75" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" s="75" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="35">
         <v>23</v>
       </c>
@@ -3676,7 +3674,7 @@
       <c r="M32" s="41"/>
       <c r="N32" s="42"/>
       <c r="O32" s="41"/>
-      <c r="P32" s="136"/>
+      <c r="P32" s="120"/>
       <c r="Q32" s="41"/>
       <c r="R32" s="42"/>
       <c r="S32" s="41"/>
@@ -3693,7 +3691,7 @@
       </c>
       <c r="AB32" s="47"/>
     </row>
-    <row r="33" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="35">
         <v>24</v>
       </c>
@@ -3731,9 +3729,9 @@
       <c r="M33" s="71"/>
       <c r="N33" s="70"/>
       <c r="O33" s="41"/>
-      <c r="P33" s="136"/>
-      <c r="Q33" s="136"/>
-      <c r="R33" s="136"/>
+      <c r="P33" s="120"/>
+      <c r="Q33" s="120"/>
+      <c r="R33" s="120"/>
       <c r="S33" s="71"/>
       <c r="T33" s="71"/>
       <c r="U33" s="71"/>
@@ -3748,7 +3746,7 @@
       </c>
       <c r="AB33" s="47"/>
     </row>
-    <row r="34" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="35">
         <v>25</v>
       </c>
@@ -3787,7 +3785,7 @@
       <c r="N34" s="51"/>
       <c r="O34" s="41"/>
       <c r="P34" s="41"/>
-      <c r="Q34" s="139"/>
+      <c r="Q34" s="123"/>
       <c r="R34" s="51"/>
       <c r="S34" s="69"/>
       <c r="T34" s="69"/>
@@ -3803,7 +3801,7 @@
       </c>
       <c r="AB34" s="47"/>
     </row>
-    <row r="35" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="35">
         <v>27</v>
       </c>
@@ -3840,7 +3838,7 @@
       <c r="N35" s="51"/>
       <c r="O35" s="69"/>
       <c r="P35" s="69"/>
-      <c r="Q35" s="139"/>
+      <c r="Q35" s="123"/>
       <c r="R35" s="51"/>
       <c r="S35" s="69"/>
       <c r="T35" s="69"/>
@@ -3856,7 +3854,7 @@
       </c>
       <c r="AB35" s="47"/>
     </row>
-    <row r="36" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="35">
         <v>28</v>
       </c>
@@ -3893,7 +3891,7 @@
       <c r="N36" s="51"/>
       <c r="O36" s="69"/>
       <c r="P36" s="69"/>
-      <c r="Q36" s="139"/>
+      <c r="Q36" s="123"/>
       <c r="R36" s="51"/>
       <c r="S36" s="69"/>
       <c r="T36" s="69"/>
@@ -3909,7 +3907,7 @@
       </c>
       <c r="AB36" s="47"/>
     </row>
-    <row r="37" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="35">
         <v>29</v>
       </c>
@@ -3946,7 +3944,7 @@
       <c r="N37" s="51"/>
       <c r="O37" s="69"/>
       <c r="P37" s="69"/>
-      <c r="Q37" s="139"/>
+      <c r="Q37" s="123"/>
       <c r="R37" s="42"/>
       <c r="S37" s="69"/>
       <c r="T37" s="69"/>
@@ -3962,7 +3960,7 @@
       </c>
       <c r="AB37" s="47"/>
     </row>
-    <row r="38" spans="1:28" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="35">
         <v>30</v>
       </c>
@@ -3999,7 +3997,7 @@
       <c r="N38" s="51"/>
       <c r="O38" s="69"/>
       <c r="P38" s="69"/>
-      <c r="Q38" s="139"/>
+      <c r="Q38" s="123"/>
       <c r="R38" s="51"/>
       <c r="S38" s="41"/>
       <c r="T38" s="69"/>
@@ -4015,7 +4013,7 @@
       </c>
       <c r="AB38" s="47"/>
     </row>
-    <row r="39" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="35">
         <v>31</v>
       </c>
@@ -4053,7 +4051,7 @@
       <c r="O39" s="69"/>
       <c r="P39" s="69"/>
       <c r="Q39" s="69"/>
-      <c r="R39" s="139"/>
+      <c r="R39" s="123"/>
       <c r="S39" s="41"/>
       <c r="T39" s="41"/>
       <c r="U39" s="69"/>
@@ -4068,7 +4066,7 @@
       </c>
       <c r="AB39" s="47"/>
     </row>
-    <row r="40" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="35">
         <v>32</v>
       </c>
@@ -4106,7 +4104,7 @@
       <c r="O40" s="69"/>
       <c r="P40" s="69"/>
       <c r="Q40" s="69"/>
-      <c r="R40" s="139"/>
+      <c r="R40" s="123"/>
       <c r="S40" s="69"/>
       <c r="T40" s="69"/>
       <c r="U40" s="41"/>
@@ -4121,7 +4119,7 @@
       </c>
       <c r="AB40" s="47"/>
     </row>
-    <row r="41" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="35">
         <v>33</v>
       </c>
@@ -4161,7 +4159,7 @@
       <c r="O41" s="69"/>
       <c r="P41" s="69"/>
       <c r="Q41" s="41"/>
-      <c r="R41" s="136"/>
+      <c r="R41" s="120"/>
       <c r="S41" s="69"/>
       <c r="T41" s="69"/>
       <c r="U41" s="69"/>
@@ -4176,7 +4174,7 @@
       </c>
       <c r="AB41" s="47"/>
     </row>
-    <row r="42" spans="1:28" s="45" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="35">
         <v>34</v>
       </c>
@@ -4229,7 +4227,7 @@
       </c>
       <c r="AB42" s="47"/>
     </row>
-    <row r="43" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="35">
         <v>35</v>
       </c>
@@ -4269,7 +4267,7 @@
       <c r="O43" s="69"/>
       <c r="P43" s="69"/>
       <c r="Q43" s="69"/>
-      <c r="R43" s="139"/>
+      <c r="R43" s="123"/>
       <c r="S43" s="69"/>
       <c r="T43" s="69"/>
       <c r="U43" s="69"/>
@@ -4284,7 +4282,7 @@
       </c>
       <c r="AB43" s="47"/>
     </row>
-    <row r="44" spans="1:28" s="45" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="35">
         <v>36</v>
       </c>
@@ -4339,7 +4337,7 @@
       </c>
       <c r="AB44" s="47"/>
     </row>
-    <row r="45" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="35">
         <v>37</v>
       </c>
@@ -4377,7 +4375,7 @@
       <c r="O45" s="69"/>
       <c r="P45" s="69"/>
       <c r="Q45" s="69"/>
-      <c r="R45" s="139"/>
+      <c r="R45" s="123"/>
       <c r="S45" s="69"/>
       <c r="T45" s="69"/>
       <c r="U45" s="69"/>
@@ -4392,7 +4390,7 @@
       </c>
       <c r="AB45" s="47"/>
     </row>
-    <row r="46" spans="1:28" s="117" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" s="117" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="35">
         <v>39</v>
       </c>
@@ -4444,7 +4442,7 @@
       <c r="AA46" s="43"/>
       <c r="AB46" s="47"/>
     </row>
-    <row r="47" spans="1:28" s="117" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" s="117" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="35">
         <v>40</v>
       </c>
@@ -4496,7 +4494,7 @@
       <c r="AA47" s="43"/>
       <c r="AB47" s="47"/>
     </row>
-    <row r="48" spans="1:28" s="45" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" s="45" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A48" s="111"/>
       <c r="B48" s="24" t="s">
         <v>67</v>
@@ -4528,7 +4526,7 @@
       <c r="AA48" s="114"/>
       <c r="AB48" s="115"/>
     </row>
-    <row r="49" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="35">
         <v>1</v>
       </c>
@@ -4568,10 +4566,10 @@
       <c r="O49" s="69"/>
       <c r="P49" s="69"/>
       <c r="Q49" s="69"/>
-      <c r="R49" s="136"/>
+      <c r="R49" s="120"/>
       <c r="S49" s="110"/>
       <c r="T49" s="41"/>
-      <c r="U49" s="140"/>
+      <c r="U49" s="124"/>
       <c r="V49" s="118"/>
       <c r="W49" s="69"/>
       <c r="X49" s="41"/>
@@ -4583,7 +4581,7 @@
       </c>
       <c r="AB49" s="47"/>
     </row>
-    <row r="50" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="35">
         <v>2</v>
       </c>
@@ -4604,10 +4602,10 @@
       </c>
       <c r="G50" s="67">
         <f>VLOOKUP(H50,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H50" s="39" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I50" s="40"/>
       <c r="J50" s="40">
@@ -4621,10 +4619,10 @@
       <c r="O50" s="69"/>
       <c r="P50" s="69"/>
       <c r="Q50" s="69"/>
-      <c r="R50" s="139"/>
+      <c r="R50" s="123"/>
       <c r="S50" s="110"/>
       <c r="T50" s="41"/>
-      <c r="U50" s="140"/>
+      <c r="U50" s="124"/>
       <c r="V50" s="118"/>
       <c r="W50" s="69"/>
       <c r="X50" s="69"/>
@@ -4636,7 +4634,7 @@
       </c>
       <c r="AB50" s="47"/>
     </row>
-    <row r="51" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="35">
         <v>3</v>
       </c>
@@ -4657,10 +4655,10 @@
       </c>
       <c r="G51" s="67">
         <f>VLOOKUP(H51,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H51" s="39" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I51" s="40"/>
       <c r="J51" s="40">
@@ -4677,7 +4675,7 @@
       <c r="R51" s="108"/>
       <c r="S51" s="110"/>
       <c r="T51" s="41"/>
-      <c r="U51" s="140"/>
+      <c r="U51" s="124"/>
       <c r="V51" s="118"/>
       <c r="W51" s="69"/>
       <c r="X51" s="69"/>
@@ -4686,7 +4684,7 @@
       <c r="AA51" s="107"/>
       <c r="AB51" s="72"/>
     </row>
-    <row r="52" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="35">
         <v>4</v>
       </c>
@@ -4694,7 +4692,7 @@
         <v>69</v>
       </c>
       <c r="C52" s="37">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D52" s="37">
         <v>0</v>
@@ -4707,17 +4705,17 @@
       </c>
       <c r="G52" s="67">
         <f>VLOOKUP(H52,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="H52" s="39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I52" s="40">
         <v>8</v>
       </c>
       <c r="J52" s="40">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K52" s="41"/>
       <c r="L52" s="41"/>
@@ -4729,7 +4727,7 @@
       <c r="R52" s="108"/>
       <c r="S52" s="69"/>
       <c r="T52" s="41"/>
-      <c r="U52" s="140"/>
+      <c r="U52" s="124"/>
       <c r="V52" s="118"/>
       <c r="W52" s="69"/>
       <c r="X52" s="69"/>
@@ -4738,7 +4736,7 @@
       <c r="AA52" s="107"/>
       <c r="AB52" s="72"/>
     </row>
-    <row r="53" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="35">
         <v>5</v>
       </c>
@@ -4746,7 +4744,7 @@
         <v>70</v>
       </c>
       <c r="C53" s="37">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D53" s="37">
         <v>0</v>
@@ -4759,17 +4757,17 @@
       </c>
       <c r="G53" s="67">
         <f>VLOOKUP(H53,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="H53" s="39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I53" s="40">
         <v>16</v>
       </c>
       <c r="J53" s="40">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K53" s="41"/>
       <c r="L53" s="41"/>
@@ -4781,7 +4779,7 @@
       <c r="R53" s="108"/>
       <c r="S53" s="69"/>
       <c r="T53" s="41"/>
-      <c r="U53" s="140"/>
+      <c r="U53" s="124"/>
       <c r="V53" s="118"/>
       <c r="W53" s="69"/>
       <c r="X53" s="69"/>
@@ -4790,7 +4788,7 @@
       <c r="AA53" s="107"/>
       <c r="AB53" s="72"/>
     </row>
-    <row r="54" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="35">
         <v>6</v>
       </c>
@@ -4807,21 +4805,21 @@
         <v>0</v>
       </c>
       <c r="F54" s="37">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G54" s="67">
         <f>VLOOKUP(H54,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="H54" s="39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I54" s="40">
         <v>8</v>
       </c>
       <c r="J54" s="40">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K54" s="41"/>
       <c r="L54" s="41"/>
@@ -4833,7 +4831,7 @@
       <c r="R54" s="108"/>
       <c r="S54" s="69"/>
       <c r="T54" s="41"/>
-      <c r="U54" s="140"/>
+      <c r="U54" s="124"/>
       <c r="V54" s="118"/>
       <c r="W54" s="69"/>
       <c r="X54" s="69"/>
@@ -4842,7 +4840,7 @@
       <c r="AA54" s="107"/>
       <c r="AB54" s="72"/>
     </row>
-    <row r="55" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="35">
         <v>7</v>
       </c>
@@ -4885,7 +4883,7 @@
       <c r="R55" s="108"/>
       <c r="S55" s="69"/>
       <c r="T55" s="41"/>
-      <c r="U55" s="140"/>
+      <c r="U55" s="124"/>
       <c r="V55" s="118"/>
       <c r="W55" s="69"/>
       <c r="X55" s="69"/>
@@ -4894,7 +4892,7 @@
       <c r="AA55" s="107"/>
       <c r="AB55" s="72"/>
     </row>
-    <row r="56" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="35">
         <v>8</v>
       </c>
@@ -4929,7 +4927,7 @@
       <c r="AA56" s="107"/>
       <c r="AB56" s="72"/>
     </row>
-    <row r="57" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="35">
         <v>9</v>
       </c>
@@ -4964,7 +4962,7 @@
       <c r="AA57" s="107"/>
       <c r="AB57" s="72"/>
     </row>
-    <row r="58" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="35">
         <v>10</v>
       </c>
@@ -4999,7 +4997,7 @@
       <c r="AA58" s="107"/>
       <c r="AB58" s="72"/>
     </row>
-    <row r="59" spans="1:28" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="35">
         <v>11</v>
       </c>
@@ -5034,7 +5032,7 @@
       <c r="AA59" s="107"/>
       <c r="AB59" s="72"/>
     </row>
-    <row r="60" spans="1:28" s="45" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="35">
         <v>12</v>
       </c>
@@ -5072,14 +5070,14 @@
       </c>
       <c r="AB60" s="84"/>
     </row>
-    <row r="61" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="132" t="s">
+    <row r="61" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="129" t="s">
         <v>59</v>
       </c>
-      <c r="B61" s="132"/>
+      <c r="B61" s="129"/>
       <c r="C61" s="85">
         <f>SUM(C10:C60)</f>
-        <v>83.5</v>
+        <v>94.5</v>
       </c>
       <c r="D61" s="85">
         <f>SUM(D10:D60)</f>
@@ -5091,14 +5089,14 @@
       </c>
       <c r="F61" s="85">
         <f>SUM(F10:F60)</f>
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="G61" s="86"/>
       <c r="H61" s="85"/>
       <c r="I61" s="87"/>
       <c r="J61" s="85">
         <f t="shared" si="1"/>
-        <v>315.25</v>
+        <v>336.25</v>
       </c>
       <c r="K61" s="88"/>
       <c r="L61" s="88"/>
@@ -5122,14 +5120,14 @@
       </c>
       <c r="AB61" s="89"/>
     </row>
-    <row r="62" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="133" t="s">
+    <row r="62" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="130" t="s">
         <v>60</v>
       </c>
-      <c r="B62" s="133"/>
+      <c r="B62" s="130"/>
       <c r="C62" s="85">
         <f>135-C61</f>
-        <v>51.5</v>
+        <v>40.5</v>
       </c>
       <c r="D62" s="85">
         <f>135-D61</f>
@@ -5141,14 +5139,14 @@
       </c>
       <c r="F62" s="85">
         <f>135-F61</f>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G62" s="86"/>
       <c r="H62" s="85"/>
       <c r="I62" s="85"/>
       <c r="J62" s="85">
         <f t="shared" si="1"/>
-        <v>224.75</v>
+        <v>203.75</v>
       </c>
       <c r="K62" s="88"/>
       <c r="L62" s="88"/>
@@ -5169,11 +5167,11 @@
       <c r="AA62" s="88"/>
       <c r="AB62" s="88"/>
     </row>
-    <row r="63" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="134" t="s">
+    <row r="63" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="131" t="s">
         <v>61</v>
       </c>
-      <c r="B63" s="134"/>
+      <c r="B63" s="131"/>
       <c r="C63" s="85"/>
       <c r="D63" s="85"/>
       <c r="E63" s="85"/>
@@ -5204,11 +5202,11 @@
       <c r="AA63" s="88"/>
       <c r="AB63" s="88"/>
     </row>
-    <row r="64" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="133" t="s">
+    <row r="64" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="130" t="s">
         <v>62</v>
       </c>
-      <c r="B64" s="133"/>
+      <c r="B64" s="130"/>
       <c r="C64" s="85"/>
       <c r="D64" s="85"/>
       <c r="E64" s="90"/>
@@ -5221,7 +5219,7 @@
       </c>
       <c r="J64" s="85">
         <f>SUM(J10:J60)</f>
-        <v>315.25</v>
+        <v>336.25</v>
       </c>
       <c r="K64" s="88"/>
       <c r="L64" s="88"/>
@@ -5242,7 +5240,7 @@
       <c r="AA64" s="88"/>
       <c r="AB64" s="88"/>
     </row>
-    <row r="65" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="92"/>
       <c r="B65" s="92"/>
       <c r="C65" s="93"/>
@@ -5272,11 +5270,11 @@
       <c r="AA65" s="88"/>
       <c r="AB65" s="88"/>
     </row>
-    <row r="66" spans="1:28" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="134" t="s">
+    <row r="66" spans="1:28" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="131" t="s">
         <v>63</v>
       </c>
-      <c r="B66" s="134"/>
+      <c r="B66" s="131"/>
       <c r="C66" s="85">
         <f>135*4</f>
         <v>540</v>
@@ -5307,14 +5305,14 @@
       <c r="AA66" s="88"/>
       <c r="AB66" s="88"/>
     </row>
-    <row r="67" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="131" t="s">
+    <row r="67" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="128" t="s">
         <v>64</v>
       </c>
-      <c r="B67" s="131"/>
+      <c r="B67" s="128"/>
       <c r="C67" s="85">
         <f>C66-J64</f>
-        <v>224.75</v>
+        <v>203.75</v>
       </c>
       <c r="D67" s="93"/>
       <c r="E67" s="93"/>
@@ -5342,7 +5340,7 @@
       <c r="AA67" s="88"/>
       <c r="AB67" s="88"/>
     </row>
-    <row r="68" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="94"/>
       <c r="B68" s="92"/>
       <c r="C68" s="95"/>
@@ -5355,12 +5353,12 @@
       <c r="J68" s="97"/>
       <c r="AA68" s="88"/>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D69" s="98"/>
       <c r="E69" s="98"/>
       <c r="F69" s="98"/>
     </row>
-    <row r="70" spans="1:28" s="100" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:28" s="100" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A70" s="99"/>
       <c r="C70" s="101"/>
       <c r="D70" s="101"/>
@@ -5375,7 +5373,7 @@
       <c r="Z70" s="104"/>
       <c r="AA70" s="105"/>
     </row>
-    <row r="71" spans="1:28" s="100" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:28" s="100" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="C71" s="101"/>
       <c r="D71" s="101"/>
       <c r="E71" s="101"/>
@@ -5389,7 +5387,7 @@
       <c r="Z71" s="104"/>
       <c r="AA71" s="105"/>
     </row>
-    <row r="72" spans="1:28" s="100" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:28" s="100" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="C72" s="101"/>
       <c r="D72" s="101"/>
       <c r="E72" s="101"/>
@@ -5405,6 +5403,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
     <mergeCell ref="S6:V6"/>
     <mergeCell ref="A67:B67"/>
     <mergeCell ref="A61:B61"/>
@@ -5415,18 +5425,6 @@
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:Z7"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K6:R6"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
     <cfRule type="containsText" dxfId="28" priority="23" operator="containsText" text="En cours">
@@ -5564,12 +5562,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="10.7109375" style="1"/>
+    <col min="1" max="1025" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="106" t="s">
         <v>6</v>
       </c>
@@ -5577,7 +5575,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -5585,7 +5583,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -5605,9 +5603,9 @@
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="10.7109375" style="1"/>
+    <col min="1" max="1025" width="10.6640625" style="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Partially fixed issue #34
</commit_message>
<xml_diff>
--- a/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
+++ b/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alxbo\Source\Repos\mrjrdg\marque-sans-nom\Semainiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654CDC8F-ECC5-44F5-B67C-C6F7AC854DC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA9EC5C-8CDB-4EB9-AAAC-584E85702F4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1370,6 +1370,36 @@
     <xf numFmtId="0" fontId="19" fillId="9" borderId="16" xfId="8" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1385,36 +1415,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -2225,7 +2225,7 @@
   <dimension ref="A1:AMK78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+      <selection activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2253,22 +2253,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="9" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="143" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="143"/>
+      <c r="A1" s="129" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="129"/>
       <c r="C1" s="8"/>
-      <c r="D1" s="144" t="s">
+      <c r="D1" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="144"/>
-      <c r="F1" s="144"/>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
-      <c r="I1" s="144"/>
-      <c r="J1" s="144"/>
-      <c r="K1" s="144"/>
-      <c r="L1" s="144"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="130"/>
+      <c r="L1" s="130"/>
       <c r="N1" s="4"/>
       <c r="P1" s="10"/>
       <c r="Q1" s="9" t="s">
@@ -2280,20 +2280,20 @@
       <c r="AA1" s="11"/>
     </row>
     <row r="2" spans="1:28" s="9" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="143" t="s">
+      <c r="A2" s="129" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="143"/>
+      <c r="B2" s="129"/>
       <c r="C2" s="8"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
-      <c r="F2" s="143" t="s">
+      <c r="F2" s="129" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="143"/>
-      <c r="H2" s="143"/>
-      <c r="I2" s="143"/>
-      <c r="J2" s="143"/>
+      <c r="G2" s="129"/>
+      <c r="H2" s="129"/>
+      <c r="I2" s="129"/>
+      <c r="J2" s="129"/>
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
       <c r="N2" s="4"/>
@@ -2376,78 +2376,78 @@
       <c r="H6" s="4"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="135" t="s">
+      <c r="K6" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="135"/>
-      <c r="M6" s="135"/>
-      <c r="N6" s="135"/>
-      <c r="O6" s="135"/>
-      <c r="P6" s="135"/>
-      <c r="Q6" s="135"/>
-      <c r="R6" s="135"/>
-      <c r="S6" s="135" t="s">
+      <c r="L6" s="131"/>
+      <c r="M6" s="131"/>
+      <c r="N6" s="131"/>
+      <c r="O6" s="131"/>
+      <c r="P6" s="131"/>
+      <c r="Q6" s="131"/>
+      <c r="R6" s="131"/>
+      <c r="S6" s="131" t="s">
         <v>10</v>
       </c>
-      <c r="T6" s="135"/>
-      <c r="U6" s="135"/>
-      <c r="V6" s="135"/>
+      <c r="T6" s="131"/>
+      <c r="U6" s="131"/>
+      <c r="V6" s="131"/>
       <c r="Z6" s="18"/>
       <c r="AA6" s="11"/>
     </row>
     <row r="7" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="136" t="s">
+      <c r="A7" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="137" t="s">
+      <c r="B7" s="133" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="138" t="s">
+      <c r="C7" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="138"/>
-      <c r="E7" s="138"/>
-      <c r="F7" s="138"/>
-      <c r="G7" s="139" t="s">
+      <c r="D7" s="134"/>
+      <c r="E7" s="134"/>
+      <c r="F7" s="134"/>
+      <c r="G7" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="140" t="s">
+      <c r="H7" s="136" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="141" t="s">
+      <c r="I7" s="137" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="141" t="s">
+      <c r="J7" s="137" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="142" t="s">
+      <c r="K7" s="138" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="142"/>
-      <c r="M7" s="142"/>
-      <c r="N7" s="142"/>
-      <c r="O7" s="142"/>
-      <c r="P7" s="142"/>
-      <c r="Q7" s="142"/>
-      <c r="R7" s="142"/>
-      <c r="S7" s="142"/>
-      <c r="T7" s="142"/>
-      <c r="U7" s="142"/>
-      <c r="V7" s="142"/>
-      <c r="W7" s="142"/>
-      <c r="X7" s="142"/>
-      <c r="Y7" s="142"/>
-      <c r="Z7" s="142"/>
-      <c r="AA7" s="132" t="s">
+      <c r="L7" s="138"/>
+      <c r="M7" s="138"/>
+      <c r="N7" s="138"/>
+      <c r="O7" s="138"/>
+      <c r="P7" s="138"/>
+      <c r="Q7" s="138"/>
+      <c r="R7" s="138"/>
+      <c r="S7" s="138"/>
+      <c r="T7" s="138"/>
+      <c r="U7" s="138"/>
+      <c r="V7" s="138"/>
+      <c r="W7" s="138"/>
+      <c r="X7" s="138"/>
+      <c r="Y7" s="138"/>
+      <c r="Z7" s="138"/>
+      <c r="AA7" s="142" t="s">
         <v>19</v>
       </c>
-      <c r="AB7" s="133" t="s">
+      <c r="AB7" s="143" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="136"/>
-      <c r="B8" s="137"/>
+      <c r="A8" s="132"/>
+      <c r="B8" s="133"/>
       <c r="C8" s="21" t="s">
         <v>21</v>
       </c>
@@ -2460,10 +2460,10 @@
       <c r="F8" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="139"/>
-      <c r="H8" s="140"/>
-      <c r="I8" s="141"/>
-      <c r="J8" s="141"/>
+      <c r="G8" s="135"/>
+      <c r="H8" s="136"/>
+      <c r="I8" s="137"/>
+      <c r="J8" s="137"/>
       <c r="K8" s="22">
         <v>43838</v>
       </c>
@@ -2527,8 +2527,8 @@
         <f t="shared" si="0"/>
         <v>43943</v>
       </c>
-      <c r="AA8" s="132"/>
-      <c r="AB8" s="133"/>
+      <c r="AA8" s="142"/>
+      <c r="AB8" s="143"/>
     </row>
     <row r="9" spans="1:28" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="24"/>
@@ -5353,7 +5353,7 @@
         <v>0</v>
       </c>
       <c r="E62" s="38">
-        <v>3.25</v>
+        <v>4.25</v>
       </c>
       <c r="F62" s="38">
         <v>0</v>
@@ -5366,11 +5366,11 @@
         <v>2</v>
       </c>
       <c r="I62" s="41">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J62" s="41">
         <f t="shared" si="3"/>
-        <v>3.25</v>
+        <v>4.25</v>
       </c>
       <c r="K62" s="43"/>
       <c r="L62" s="43"/>
@@ -5575,10 +5575,10 @@
       <c r="AB66" s="99"/>
     </row>
     <row r="67" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="134" t="s">
+      <c r="A67" s="144" t="s">
         <v>70</v>
       </c>
-      <c r="B67" s="134"/>
+      <c r="B67" s="144"/>
       <c r="C67" s="100">
         <f>SUM(C10:C66)</f>
         <v>99.5</v>
@@ -5589,7 +5589,7 @@
       </c>
       <c r="E67" s="100">
         <f>SUM(E10:E66)</f>
-        <v>83.75</v>
+        <v>84.75</v>
       </c>
       <c r="F67" s="100">
         <f>SUM(F10:F66)</f>
@@ -5600,7 +5600,7 @@
       <c r="I67" s="102"/>
       <c r="J67" s="100">
         <f t="shared" si="3"/>
-        <v>370.25</v>
+        <v>371.25</v>
       </c>
       <c r="K67" s="103"/>
       <c r="L67" s="103"/>
@@ -5625,10 +5625,10 @@
       <c r="AB67" s="104"/>
     </row>
     <row r="68" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="129" t="s">
+      <c r="A68" s="139" t="s">
         <v>71</v>
       </c>
-      <c r="B68" s="129"/>
+      <c r="B68" s="139"/>
       <c r="C68" s="100">
         <f>135-C67</f>
         <v>35.5</v>
@@ -5639,7 +5639,7 @@
       </c>
       <c r="E68" s="100">
         <f>135-E67</f>
-        <v>51.25</v>
+        <v>50.25</v>
       </c>
       <c r="F68" s="100">
         <f>135-F67</f>
@@ -5650,7 +5650,7 @@
       <c r="I68" s="100"/>
       <c r="J68" s="100">
         <f t="shared" si="3"/>
-        <v>169.75</v>
+        <v>168.75</v>
       </c>
       <c r="K68" s="103"/>
       <c r="L68" s="103"/>
@@ -5672,10 +5672,10 @@
       <c r="AB68" s="103"/>
     </row>
     <row r="69" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="130" t="s">
+      <c r="A69" s="140" t="s">
         <v>72</v>
       </c>
-      <c r="B69" s="130"/>
+      <c r="B69" s="140"/>
       <c r="C69" s="100"/>
       <c r="D69" s="100"/>
       <c r="E69" s="100"/>
@@ -5707,10 +5707,10 @@
       <c r="AB69" s="103"/>
     </row>
     <row r="70" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="129" t="s">
+      <c r="A70" s="139" t="s">
         <v>73</v>
       </c>
-      <c r="B70" s="129"/>
+      <c r="B70" s="139"/>
       <c r="C70" s="100"/>
       <c r="D70" s="100"/>
       <c r="E70" s="105"/>
@@ -5719,11 +5719,11 @@
       <c r="H70" s="100"/>
       <c r="I70" s="106">
         <f>SUM(I10:I66)</f>
-        <v>394.75</v>
+        <v>396.75</v>
       </c>
       <c r="J70" s="100">
         <f>SUM(J10:J66)</f>
-        <v>370.25</v>
+        <v>371.25</v>
       </c>
       <c r="K70" s="103"/>
       <c r="L70" s="103"/>
@@ -5775,10 +5775,10 @@
       <c r="AB71" s="103"/>
     </row>
     <row r="72" spans="1:28" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="130" t="s">
+      <c r="A72" s="140" t="s">
         <v>74</v>
       </c>
-      <c r="B72" s="130"/>
+      <c r="B72" s="140"/>
       <c r="C72" s="100">
         <f>135*4</f>
         <v>540</v>
@@ -5810,13 +5810,13 @@
       <c r="AB72" s="103"/>
     </row>
     <row r="73" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="131" t="s">
+      <c r="A73" s="141" t="s">
         <v>75</v>
       </c>
-      <c r="B73" s="131"/>
+      <c r="B73" s="141"/>
       <c r="C73" s="100">
         <f>C72-J70</f>
-        <v>169.75</v>
+        <v>168.75</v>
       </c>
       <c r="D73" s="108"/>
       <c r="E73" s="108"/>
@@ -5907,11 +5907,14 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
     <mergeCell ref="S6:V6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
@@ -5921,14 +5924,11 @@
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:Z7"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K6:R6"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
     <cfRule type="containsText" dxfId="42" priority="16" operator="containsText" text="En cours">

</xml_diff>

<commit_message>
ajout des heures 8 Avril et rapport sprint 2
</commit_message>
<xml_diff>
--- a/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
+++ b/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alxbo\Source\Repos\mrjrdg\marque-sans-nom\Semainiers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Desktop/marque-sans-nom/Semainiers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC91031-07DC-4DE4-8941-6428FBBB0011}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC516814-8EFC-8949-8AED-572F1E3C3D41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="87">
   <si>
     <t>UQÀM - Hiver 2020</t>
   </si>
@@ -240,12 +238,6 @@
   </si>
   <si>
     <t>Pages gestion d'entreprises (Create,Edit)</t>
-  </si>
-  <si>
-    <t>Pages gestion d'evenement (Create,Edit,Delete)</t>
-  </si>
-  <si>
-    <t>Babillards de commentaires</t>
   </si>
   <si>
     <t>Nombre d'heures totales accordées au projet par personne</t>
@@ -356,6 +348,18 @@
   <si>
     <t>Améliorer le visuel (administration)</t>
   </si>
+  <si>
+    <t>Correctifs et modifications sur la supression d'entreprise et rejoindre evenement</t>
+  </si>
+  <si>
+    <t>Babillards de commentaires - Repousser au 3 ieme Sprint</t>
+  </si>
+  <si>
+    <t>Pages gestion d'evenement (Create,Edit,Delete) - Edit et Delete repousser 3ieme Sprint</t>
+  </si>
+  <si>
+    <t>Correction et visuel de la messagerie</t>
+  </si>
 </sst>
 </file>
 
@@ -367,7 +371,7 @@
     <numFmt numFmtId="166" formatCode="[$-C0C]dd/mmm"/>
     <numFmt numFmtId="167" formatCode="\\;;;"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -514,8 +518,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -569,6 +595,12 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAAAC4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="33">
     <border>
@@ -994,7 +1026,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
@@ -1367,36 +1399,6 @@
     <xf numFmtId="0" fontId="19" fillId="9" borderId="16" xfId="8" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1413,19 +1415,95 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Excel Built-in 60% - Accent4" xfId="7" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Excel Built-in Bad" xfId="6" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Excel Built-in Good" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Excel Built-in Neutral" xfId="5" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Excel Built-in Normal" xfId="3" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Milliers" xfId="1" builtinId="3"/>
+    <cellStyle name="Good" xfId="8" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Satisfaisant" xfId="8" builtinId="26"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="46">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1907,6 +1985,10 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFFAAAC4"/>
+      <color rgb="FFFF788F"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1920,7 +2002,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2221,19 +2303,19 @@
   </sheetPr>
   <dimension ref="A1:AMK78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V48" sqref="V48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="66.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="66.1640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" style="3" customWidth="1"/>
-    <col min="4" max="5" width="8.109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.1640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="4" customWidth="1"/>
     <col min="9" max="10" width="9.33203125" style="5" customWidth="1"/>
     <col min="11" max="13" width="8" style="2" customWidth="1"/>
     <col min="14" max="14" width="8" style="6" customWidth="1"/>
@@ -2249,23 +2331,23 @@
     <col min="29" max="1025" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="9" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="129" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="129"/>
+    <row r="1" spans="1:28" s="9" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="143" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="143"/>
       <c r="C1" s="8"/>
-      <c r="D1" s="130" t="s">
+      <c r="D1" s="144" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="130"/>
-      <c r="J1" s="130"/>
-      <c r="K1" s="130"/>
-      <c r="L1" s="130"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="144"/>
+      <c r="G1" s="144"/>
+      <c r="H1" s="144"/>
+      <c r="I1" s="144"/>
+      <c r="J1" s="144"/>
+      <c r="K1" s="144"/>
+      <c r="L1" s="144"/>
       <c r="N1" s="4"/>
       <c r="P1" s="10"/>
       <c r="Q1" s="9" t="s">
@@ -2276,21 +2358,21 @@
       <c r="Z1" s="4"/>
       <c r="AA1" s="11"/>
     </row>
-    <row r="2" spans="1:28" s="9" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="129" t="s">
+    <row r="2" spans="1:28" s="9" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="143" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="129"/>
+      <c r="B2" s="143"/>
       <c r="C2" s="8"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
-      <c r="F2" s="129" t="s">
+      <c r="F2" s="143" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="129"/>
-      <c r="H2" s="129"/>
-      <c r="I2" s="129"/>
-      <c r="J2" s="129"/>
+      <c r="G2" s="143"/>
+      <c r="H2" s="143"/>
+      <c r="I2" s="143"/>
+      <c r="J2" s="143"/>
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
       <c r="N2" s="4"/>
@@ -2303,7 +2385,7 @@
       <c r="Z2" s="4"/>
       <c r="AA2" s="11"/>
     </row>
-    <row r="3" spans="1:28" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -2321,7 +2403,7 @@
       <c r="Z3" s="4"/>
       <c r="AA3" s="11"/>
     </row>
-    <row r="4" spans="1:28" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="C4" s="15"/>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -2341,7 +2423,7 @@
       <c r="Z4" s="4"/>
       <c r="AA4" s="11"/>
     </row>
-    <row r="5" spans="1:28" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -2365,7 +2447,7 @@
       </c>
       <c r="AA5" s="11"/>
     </row>
-    <row r="6" spans="1:28" s="9" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" s="9" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -2373,78 +2455,78 @@
       <c r="H6" s="4"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="131" t="s">
+      <c r="K6" s="135" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="131"/>
-      <c r="M6" s="131"/>
-      <c r="N6" s="131"/>
-      <c r="O6" s="131"/>
-      <c r="P6" s="131"/>
-      <c r="Q6" s="131"/>
-      <c r="R6" s="131"/>
-      <c r="S6" s="131" t="s">
+      <c r="L6" s="135"/>
+      <c r="M6" s="135"/>
+      <c r="N6" s="135"/>
+      <c r="O6" s="135"/>
+      <c r="P6" s="135"/>
+      <c r="Q6" s="135"/>
+      <c r="R6" s="135"/>
+      <c r="S6" s="135" t="s">
         <v>10</v>
       </c>
-      <c r="T6" s="131"/>
-      <c r="U6" s="131"/>
-      <c r="V6" s="131"/>
+      <c r="T6" s="135"/>
+      <c r="U6" s="135"/>
+      <c r="V6" s="135"/>
       <c r="Z6" s="18"/>
       <c r="AA6" s="11"/>
     </row>
-    <row r="7" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="132" t="s">
+    <row r="7" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="133" t="s">
+      <c r="B7" s="137" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="134" t="s">
+      <c r="C7" s="138" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="134"/>
-      <c r="E7" s="134"/>
-      <c r="F7" s="134"/>
-      <c r="G7" s="135" t="s">
+      <c r="D7" s="138"/>
+      <c r="E7" s="138"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="139" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="136" t="s">
+      <c r="H7" s="140" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="137" t="s">
+      <c r="I7" s="141" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="137" t="s">
+      <c r="J7" s="141" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="138" t="s">
+      <c r="K7" s="142" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="138"/>
-      <c r="M7" s="138"/>
-      <c r="N7" s="138"/>
-      <c r="O7" s="138"/>
-      <c r="P7" s="138"/>
-      <c r="Q7" s="138"/>
-      <c r="R7" s="138"/>
-      <c r="S7" s="138"/>
-      <c r="T7" s="138"/>
-      <c r="U7" s="138"/>
-      <c r="V7" s="138"/>
-      <c r="W7" s="138"/>
-      <c r="X7" s="138"/>
-      <c r="Y7" s="138"/>
-      <c r="Z7" s="138"/>
-      <c r="AA7" s="142" t="s">
+      <c r="L7" s="142"/>
+      <c r="M7" s="142"/>
+      <c r="N7" s="142"/>
+      <c r="O7" s="142"/>
+      <c r="P7" s="142"/>
+      <c r="Q7" s="142"/>
+      <c r="R7" s="142"/>
+      <c r="S7" s="142"/>
+      <c r="T7" s="142"/>
+      <c r="U7" s="142"/>
+      <c r="V7" s="142"/>
+      <c r="W7" s="142"/>
+      <c r="X7" s="142"/>
+      <c r="Y7" s="142"/>
+      <c r="Z7" s="142"/>
+      <c r="AA7" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="AB7" s="143" t="s">
+      <c r="AB7" s="133" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="132"/>
-      <c r="B8" s="133"/>
+    <row r="8" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="136"/>
+      <c r="B8" s="137"/>
       <c r="C8" s="21" t="s">
         <v>21</v>
       </c>
@@ -2457,10 +2539,10 @@
       <c r="F8" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="135"/>
-      <c r="H8" s="136"/>
-      <c r="I8" s="137"/>
-      <c r="J8" s="137"/>
+      <c r="G8" s="139"/>
+      <c r="H8" s="140"/>
+      <c r="I8" s="141"/>
+      <c r="J8" s="141"/>
       <c r="K8" s="22">
         <v>43838</v>
       </c>
@@ -2524,10 +2606,10 @@
         <f t="shared" si="0"/>
         <v>43943</v>
       </c>
-      <c r="AA8" s="142"/>
-      <c r="AB8" s="143"/>
-    </row>
-    <row r="9" spans="1:28" ht="18" x14ac:dyDescent="0.3">
+      <c r="AA8" s="132"/>
+      <c r="AB8" s="133"/>
+    </row>
+    <row r="9" spans="1:28" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="24"/>
       <c r="B9" s="25" t="s">
         <v>25</v>
@@ -2559,7 +2641,7 @@
       <c r="AA9" s="34"/>
       <c r="AB9" s="35"/>
     </row>
-    <row r="10" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="36">
         <v>1</v>
       </c>
@@ -2614,7 +2696,7 @@
       </c>
       <c r="AB10" s="46"/>
     </row>
-    <row r="11" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="36">
         <v>2</v>
       </c>
@@ -2669,7 +2751,7 @@
       </c>
       <c r="AB11" s="49"/>
     </row>
-    <row r="12" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="36">
         <v>3</v>
       </c>
@@ -2723,7 +2805,7 @@
       </c>
       <c r="AB12" s="50"/>
     </row>
-    <row r="13" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="36">
         <v>4</v>
       </c>
@@ -2778,7 +2860,7 @@
       </c>
       <c r="AB13" s="49"/>
     </row>
-    <row r="14" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="36">
         <v>5</v>
       </c>
@@ -2833,7 +2915,7 @@
       </c>
       <c r="AB14" s="49"/>
     </row>
-    <row r="15" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="36">
         <v>6</v>
       </c>
@@ -2888,7 +2970,7 @@
       </c>
       <c r="AB15" s="49"/>
     </row>
-    <row r="16" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="36">
         <v>7</v>
       </c>
@@ -2943,7 +3025,7 @@
       </c>
       <c r="AB16" s="49"/>
     </row>
-    <row r="17" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="36">
         <v>8</v>
       </c>
@@ -2998,7 +3080,7 @@
       </c>
       <c r="AB17" s="49"/>
     </row>
-    <row r="18" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="36">
         <v>9</v>
       </c>
@@ -3053,7 +3135,7 @@
       </c>
       <c r="AB18" s="49"/>
     </row>
-    <row r="19" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="36">
         <v>10</v>
       </c>
@@ -3108,7 +3190,7 @@
       </c>
       <c r="AB19" s="49"/>
     </row>
-    <row r="20" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="36">
         <v>11</v>
       </c>
@@ -3163,7 +3245,7 @@
       </c>
       <c r="AB20" s="49"/>
     </row>
-    <row r="21" spans="1:28" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="36">
         <v>12</v>
       </c>
@@ -3218,7 +3300,7 @@
       </c>
       <c r="AB21" s="49"/>
     </row>
-    <row r="22" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="36">
         <v>13</v>
       </c>
@@ -3273,7 +3355,7 @@
       </c>
       <c r="AB22" s="49"/>
     </row>
-    <row r="23" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="36">
         <v>14</v>
       </c>
@@ -3328,7 +3410,7 @@
       </c>
       <c r="AB23" s="49"/>
     </row>
-    <row r="24" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="36">
         <v>15</v>
       </c>
@@ -3383,7 +3465,7 @@
       </c>
       <c r="AB24" s="49"/>
     </row>
-    <row r="25" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="36">
         <v>16</v>
       </c>
@@ -3438,7 +3520,7 @@
       </c>
       <c r="AB25" s="49"/>
     </row>
-    <row r="26" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="36">
         <v>17</v>
       </c>
@@ -3493,7 +3575,7 @@
       </c>
       <c r="AB26" s="77"/>
     </row>
-    <row r="27" spans="1:28" s="80" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" s="80" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="36">
         <v>18</v>
       </c>
@@ -3548,7 +3630,7 @@
       </c>
       <c r="AB27" s="49"/>
     </row>
-    <row r="28" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="36">
         <v>19</v>
       </c>
@@ -3603,7 +3685,7 @@
       </c>
       <c r="AB28" s="49"/>
     </row>
-    <row r="29" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="36">
         <v>20</v>
       </c>
@@ -3658,7 +3740,7 @@
       </c>
       <c r="AB29" s="49"/>
     </row>
-    <row r="30" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="36">
         <v>21</v>
       </c>
@@ -3713,7 +3795,7 @@
       </c>
       <c r="AB30" s="49"/>
     </row>
-    <row r="31" spans="1:28" s="80" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" s="80" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="36">
         <v>22</v>
       </c>
@@ -3768,7 +3850,7 @@
       </c>
       <c r="AB31" s="49"/>
     </row>
-    <row r="32" spans="1:28" s="80" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" s="80" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="36">
         <v>23</v>
       </c>
@@ -3823,7 +3905,7 @@
       </c>
       <c r="AB32" s="49"/>
     </row>
-    <row r="33" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="36">
         <v>24</v>
       </c>
@@ -3878,7 +3960,7 @@
       </c>
       <c r="AB33" s="49"/>
     </row>
-    <row r="34" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="36">
         <v>25</v>
       </c>
@@ -3933,7 +4015,7 @@
       </c>
       <c r="AB34" s="49"/>
     </row>
-    <row r="35" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="36">
         <v>27</v>
       </c>
@@ -3986,7 +4068,7 @@
       </c>
       <c r="AB35" s="49"/>
     </row>
-    <row r="36" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="36">
         <v>28</v>
       </c>
@@ -4039,7 +4121,7 @@
       </c>
       <c r="AB36" s="49"/>
     </row>
-    <row r="37" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="36">
         <v>29</v>
       </c>
@@ -4092,7 +4174,7 @@
       </c>
       <c r="AB37" s="49"/>
     </row>
-    <row r="38" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="36">
         <v>30</v>
       </c>
@@ -4145,7 +4227,7 @@
       </c>
       <c r="AB38" s="49"/>
     </row>
-    <row r="39" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="36">
         <v>31</v>
       </c>
@@ -4198,7 +4280,7 @@
       </c>
       <c r="AB39" s="49"/>
     </row>
-    <row r="40" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="36">
         <v>32</v>
       </c>
@@ -4251,7 +4333,7 @@
       </c>
       <c r="AB40" s="49"/>
     </row>
-    <row r="41" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="36">
         <v>33</v>
       </c>
@@ -4306,7 +4388,7 @@
       </c>
       <c r="AB41" s="49"/>
     </row>
-    <row r="42" spans="1:28" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="36">
         <v>34</v>
       </c>
@@ -4359,7 +4441,7 @@
       </c>
       <c r="AB42" s="49"/>
     </row>
-    <row r="43" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="36">
         <v>35</v>
       </c>
@@ -4414,7 +4496,7 @@
       </c>
       <c r="AB43" s="49"/>
     </row>
-    <row r="44" spans="1:28" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="36">
         <v>36</v>
       </c>
@@ -4469,7 +4551,7 @@
       </c>
       <c r="AB44" s="49"/>
     </row>
-    <row r="45" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="36">
         <v>37</v>
       </c>
@@ -4522,7 +4604,7 @@
       </c>
       <c r="AB45" s="49"/>
     </row>
-    <row r="46" spans="1:28" s="87" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:28" s="87" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="36">
         <v>39</v>
       </c>
@@ -4574,7 +4656,7 @@
       <c r="AA46" s="45"/>
       <c r="AB46" s="49"/>
     </row>
-    <row r="47" spans="1:28" s="87" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:28" s="87" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="36">
         <v>40</v>
       </c>
@@ -4626,7 +4708,7 @@
       <c r="AA47" s="45"/>
       <c r="AB47" s="49"/>
     </row>
-    <row r="48" spans="1:28" s="47" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:28" s="47" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A48" s="88"/>
       <c r="B48" s="25" t="s">
         <v>64</v>
@@ -4658,7 +4740,7 @@
       <c r="AA48" s="91"/>
       <c r="AB48" s="92"/>
     </row>
-    <row r="49" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="36">
         <v>1</v>
       </c>
@@ -4679,10 +4761,10 @@
       </c>
       <c r="G49" s="72">
         <f>VLOOKUP(H49,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H49" s="40" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I49" s="41">
         <v>7</v>
@@ -4699,7 +4781,7 @@
       <c r="P49" s="74"/>
       <c r="Q49" s="74"/>
       <c r="R49" s="54"/>
-      <c r="S49" s="69"/>
+      <c r="S49" s="54"/>
       <c r="T49" s="43"/>
       <c r="U49" s="93"/>
       <c r="V49" s="124"/>
@@ -4713,7 +4795,7 @@
       </c>
       <c r="AB49" s="49"/>
     </row>
-    <row r="50" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="36">
         <v>2</v>
       </c>
@@ -4752,7 +4834,7 @@
       <c r="P50" s="74"/>
       <c r="Q50" s="74"/>
       <c r="R50" s="54"/>
-      <c r="S50" s="69"/>
+      <c r="S50" s="54"/>
       <c r="T50" s="43"/>
       <c r="U50" s="93"/>
       <c r="V50" s="124"/>
@@ -4766,7 +4848,7 @@
       </c>
       <c r="AB50" s="49"/>
     </row>
-    <row r="51" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="36">
         <v>3</v>
       </c>
@@ -4805,7 +4887,7 @@
       <c r="P51" s="74"/>
       <c r="Q51" s="74"/>
       <c r="R51" s="94"/>
-      <c r="S51" s="69"/>
+      <c r="S51" s="54"/>
       <c r="T51" s="43"/>
       <c r="U51" s="93"/>
       <c r="V51" s="124"/>
@@ -4816,7 +4898,7 @@
       <c r="AA51" s="95"/>
       <c r="AB51" s="77"/>
     </row>
-    <row r="52" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="36">
         <v>4</v>
       </c>
@@ -4837,10 +4919,10 @@
       </c>
       <c r="G52" s="72">
         <f>VLOOKUP(H52,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H52" s="40" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I52" s="41">
         <v>8</v>
@@ -4862,18 +4944,18 @@
       <c r="U52" s="93"/>
       <c r="V52" s="124"/>
       <c r="W52" s="74"/>
-      <c r="X52" s="123"/>
+      <c r="X52" s="69"/>
       <c r="Y52" s="74"/>
       <c r="Z52" s="53"/>
       <c r="AA52" s="95"/>
       <c r="AB52" s="77"/>
     </row>
-    <row r="53" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="36">
+    <row r="53" spans="1:28" s="47" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="145">
         <v>5</v>
       </c>
-      <c r="B53" s="70" t="s">
-        <v>68</v>
+      <c r="B53" s="146" t="s">
+        <v>85</v>
       </c>
       <c r="C53" s="38">
         <v>8</v>
@@ -4920,12 +5002,12 @@
       <c r="AA53" s="95"/>
       <c r="AB53" s="77"/>
     </row>
-    <row r="54" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="36">
         <v>6</v>
       </c>
       <c r="B54" s="70" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C54" s="38">
         <v>0</v>
@@ -4941,10 +5023,10 @@
       </c>
       <c r="G54" s="72">
         <f>VLOOKUP(H54,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H54" s="40" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I54" s="41">
         <v>8</v>
@@ -4972,12 +5054,12 @@
       <c r="AA54" s="95"/>
       <c r="AB54" s="77"/>
     </row>
-    <row r="55" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="36">
+    <row r="55" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="147">
         <v>7</v>
       </c>
-      <c r="B55" s="70" t="s">
-        <v>69</v>
+      <c r="B55" s="148" t="s">
+        <v>84</v>
       </c>
       <c r="C55" s="38">
         <v>0</v>
@@ -5018,18 +5100,18 @@
       <c r="U55" s="93"/>
       <c r="V55" s="124"/>
       <c r="W55" s="74"/>
-      <c r="X55" s="123"/>
+      <c r="X55" s="69"/>
       <c r="Y55" s="74"/>
       <c r="Z55" s="53"/>
       <c r="AA55" s="95"/>
       <c r="AB55" s="77"/>
     </row>
-    <row r="56" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="36">
         <v>8</v>
       </c>
       <c r="B56" s="70" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C56" s="38">
         <v>5</v>
@@ -5045,10 +5127,10 @@
       </c>
       <c r="G56" s="72">
         <f>VLOOKUP(H56,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H56" s="40" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I56" s="41">
         <v>8</v>
@@ -5076,12 +5158,12 @@
       <c r="AA56" s="95"/>
       <c r="AB56" s="77"/>
     </row>
-    <row r="57" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="36">
         <v>9</v>
       </c>
       <c r="B57" s="70" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C57" s="38">
         <v>0</v>
@@ -5128,12 +5210,12 @@
       <c r="AA57" s="95"/>
       <c r="AB57" s="77"/>
     </row>
-    <row r="58" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="36">
         <v>10</v>
       </c>
       <c r="B58" s="70" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C58" s="38">
         <v>0</v>
@@ -5180,12 +5262,12 @@
       <c r="AA58" s="95"/>
       <c r="AB58" s="77"/>
     </row>
-    <row r="59" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="36">
         <v>11</v>
       </c>
       <c r="B59" s="70" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C59" s="38">
         <v>0</v>
@@ -5232,12 +5314,12 @@
       <c r="AA59" s="95"/>
       <c r="AB59" s="77"/>
     </row>
-    <row r="60" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="36">
         <v>12</v>
       </c>
       <c r="B60" s="70" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C60" s="38">
         <v>0</v>
@@ -5284,12 +5366,12 @@
       <c r="AA60" s="95"/>
       <c r="AB60" s="77"/>
     </row>
-    <row r="61" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="36">
         <v>13</v>
       </c>
       <c r="B61" s="70" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C61" s="38">
         <v>0</v>
@@ -5336,12 +5418,12 @@
       <c r="AA61" s="95"/>
       <c r="AB61" s="77"/>
     </row>
-    <row r="62" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="36">
         <v>14</v>
       </c>
       <c r="B62" s="70" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C62" s="38">
         <v>0</v>
@@ -5388,12 +5470,12 @@
       <c r="AA62" s="95"/>
       <c r="AB62" s="77"/>
     </row>
-    <row r="63" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="36">
         <v>15</v>
       </c>
       <c r="B63" s="70" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C63" s="38">
         <v>0</v>
@@ -5440,24 +5522,38 @@
       <c r="AA63" s="95"/>
       <c r="AB63" s="77"/>
     </row>
-    <row r="64" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="36">
         <v>16</v>
       </c>
-      <c r="B64" s="70"/>
-      <c r="C64" s="38"/>
-      <c r="D64" s="38"/>
-      <c r="E64" s="38"/>
-      <c r="F64" s="38"/>
-      <c r="G64" s="72" t="e">
+      <c r="B64" s="70" t="s">
+        <v>83</v>
+      </c>
+      <c r="C64" s="38">
+        <v>8</v>
+      </c>
+      <c r="D64" s="38">
+        <v>0</v>
+      </c>
+      <c r="E64" s="38">
+        <v>0</v>
+      </c>
+      <c r="F64" s="38">
+        <v>0</v>
+      </c>
+      <c r="G64" s="72">
         <f>VLOOKUP(H64,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H64" s="40"/>
-      <c r="I64" s="41"/>
+        <v>0</v>
+      </c>
+      <c r="H64" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="I64" s="41">
+        <v>0</v>
+      </c>
       <c r="J64" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K64" s="43"/>
       <c r="L64" s="43"/>
@@ -5472,30 +5568,44 @@
       <c r="U64" s="74"/>
       <c r="V64" s="53"/>
       <c r="W64" s="74"/>
-      <c r="X64" s="74"/>
+      <c r="X64" s="127"/>
       <c r="Y64" s="74"/>
       <c r="Z64" s="53"/>
       <c r="AA64" s="95"/>
       <c r="AB64" s="77"/>
     </row>
-    <row r="65" spans="1:28" s="47" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:28" s="47" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="36">
         <v>17</v>
       </c>
-      <c r="B65" s="70"/>
-      <c r="C65" s="38"/>
-      <c r="D65" s="38"/>
-      <c r="E65" s="38"/>
-      <c r="F65" s="38"/>
-      <c r="G65" s="72" t="e">
+      <c r="B65" s="70" t="s">
+        <v>86</v>
+      </c>
+      <c r="C65" s="38">
+        <v>2</v>
+      </c>
+      <c r="D65" s="38">
+        <v>0</v>
+      </c>
+      <c r="E65" s="38">
+        <v>0</v>
+      </c>
+      <c r="F65" s="38">
+        <v>5</v>
+      </c>
+      <c r="G65" s="72">
         <f>VLOOKUP(H65,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H65" s="40"/>
-      <c r="I65" s="41"/>
+        <v>0</v>
+      </c>
+      <c r="H65" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="I65" s="41">
+        <v>1</v>
+      </c>
       <c r="J65" s="41">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" ref="J65" si="4">SUM(C65:F65)</f>
+        <v>7</v>
       </c>
       <c r="K65" s="43"/>
       <c r="L65" s="43"/>
@@ -5510,13 +5620,13 @@
       <c r="U65" s="74"/>
       <c r="V65" s="53"/>
       <c r="W65" s="74"/>
-      <c r="X65" s="74"/>
+      <c r="X65" s="127"/>
       <c r="Y65" s="74"/>
       <c r="Z65" s="53"/>
       <c r="AA65" s="95"/>
       <c r="AB65" s="77"/>
     </row>
-    <row r="66" spans="1:28" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:28" s="47" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="36">
         <v>19</v>
       </c>
@@ -5557,14 +5667,14 @@
       </c>
       <c r="AB66" s="99"/>
     </row>
-    <row r="67" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="144" t="s">
-        <v>70</v>
-      </c>
-      <c r="B67" s="144"/>
+    <row r="67" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="134" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67" s="134"/>
       <c r="C67" s="100">
         <f>SUM(C10:C66)</f>
-        <v>99.5</v>
+        <v>109.5</v>
       </c>
       <c r="D67" s="100">
         <f>SUM(D10:D66)</f>
@@ -5576,14 +5686,14 @@
       </c>
       <c r="F67" s="100">
         <f>SUM(F10:F66)</f>
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="G67" s="101"/>
       <c r="H67" s="100"/>
       <c r="I67" s="102"/>
       <c r="J67" s="100">
         <f t="shared" si="3"/>
-        <v>369.5</v>
+        <v>384.5</v>
       </c>
       <c r="K67" s="103"/>
       <c r="L67" s="103"/>
@@ -5607,14 +5717,14 @@
       </c>
       <c r="AB67" s="104"/>
     </row>
-    <row r="68" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="139" t="s">
-        <v>71</v>
-      </c>
-      <c r="B68" s="139"/>
+    <row r="68" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="129" t="s">
+        <v>69</v>
+      </c>
+      <c r="B68" s="129"/>
       <c r="C68" s="100">
         <f>135-C67</f>
-        <v>35.5</v>
+        <v>25.5</v>
       </c>
       <c r="D68" s="100">
         <f>135-D67</f>
@@ -5626,14 +5736,14 @@
       </c>
       <c r="F68" s="100">
         <f>135-F67</f>
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G68" s="101"/>
       <c r="H68" s="100"/>
       <c r="I68" s="100"/>
       <c r="J68" s="100">
         <f t="shared" si="3"/>
-        <v>170.5</v>
+        <v>155.5</v>
       </c>
       <c r="K68" s="103"/>
       <c r="L68" s="103"/>
@@ -5654,11 +5764,11 @@
       <c r="AA68" s="103"/>
       <c r="AB68" s="103"/>
     </row>
-    <row r="69" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="140" t="s">
-        <v>72</v>
-      </c>
-      <c r="B69" s="140"/>
+    <row r="69" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="130" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69" s="130"/>
       <c r="C69" s="100"/>
       <c r="D69" s="100"/>
       <c r="E69" s="100"/>
@@ -5689,11 +5799,11 @@
       <c r="AA69" s="103"/>
       <c r="AB69" s="103"/>
     </row>
-    <row r="70" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="139" t="s">
-        <v>73</v>
-      </c>
-      <c r="B70" s="139"/>
+    <row r="70" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="129" t="s">
+        <v>71</v>
+      </c>
+      <c r="B70" s="129"/>
       <c r="C70" s="100"/>
       <c r="D70" s="100"/>
       <c r="E70" s="105"/>
@@ -5702,11 +5812,11 @@
       <c r="H70" s="100"/>
       <c r="I70" s="106">
         <f>SUM(I10:I66)</f>
-        <v>393.75</v>
+        <v>394.75</v>
       </c>
       <c r="J70" s="100">
         <f>SUM(J10:J66)</f>
-        <v>369.5</v>
+        <v>384.5</v>
       </c>
       <c r="K70" s="103"/>
       <c r="L70" s="103"/>
@@ -5727,7 +5837,7 @@
       <c r="AA70" s="103"/>
       <c r="AB70" s="103"/>
     </row>
-    <row r="71" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="107"/>
       <c r="B71" s="107"/>
       <c r="C71" s="108"/>
@@ -5757,11 +5867,11 @@
       <c r="AA71" s="103"/>
       <c r="AB71" s="103"/>
     </row>
-    <row r="72" spans="1:28" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="140" t="s">
-        <v>74</v>
-      </c>
-      <c r="B72" s="140"/>
+    <row r="72" spans="1:28" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="130" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" s="130"/>
       <c r="C72" s="100">
         <f>135*4</f>
         <v>540</v>
@@ -5792,14 +5902,14 @@
       <c r="AA72" s="103"/>
       <c r="AB72" s="103"/>
     </row>
-    <row r="73" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="141" t="s">
-        <v>75</v>
-      </c>
-      <c r="B73" s="141"/>
+    <row r="73" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A73" s="131" t="s">
+        <v>73</v>
+      </c>
+      <c r="B73" s="131"/>
       <c r="C73" s="100">
         <f>C72-J70</f>
-        <v>170.5</v>
+        <v>155.5</v>
       </c>
       <c r="D73" s="108"/>
       <c r="E73" s="108"/>
@@ -5827,7 +5937,7 @@
       <c r="AA73" s="103"/>
       <c r="AB73" s="103"/>
     </row>
-    <row r="74" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="109"/>
       <c r="B74" s="107"/>
       <c r="C74" s="110"/>
@@ -5840,12 +5950,12 @@
       <c r="J74" s="112"/>
       <c r="AA74" s="103"/>
     </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D75" s="113"/>
       <c r="E75" s="113"/>
       <c r="F75" s="113"/>
     </row>
-    <row r="76" spans="1:28" s="115" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:28" s="115" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A76" s="114"/>
       <c r="C76" s="116"/>
       <c r="D76" s="116"/>
@@ -5860,7 +5970,7 @@
       <c r="Z76" s="119"/>
       <c r="AA76" s="120"/>
     </row>
-    <row r="77" spans="1:28" s="115" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:28" s="115" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="C77" s="116"/>
       <c r="D77" s="116"/>
       <c r="E77" s="116"/>
@@ -5874,7 +5984,7 @@
       <c r="Z77" s="119"/>
       <c r="AA77" s="120"/>
     </row>
-    <row r="78" spans="1:28" s="115" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:28" s="115" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="C78" s="116"/>
       <c r="D78" s="116"/>
       <c r="E78" s="116"/>
@@ -5890,14 +6000,11 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K6:R6"/>
     <mergeCell ref="S6:V6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
@@ -5907,177 +6014,191 @@
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:Z7"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
-    <cfRule type="containsText" dxfId="42" priority="16" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="45" priority="19" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H19)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H9:H45 H49 H64:H66 H47">
-    <cfRule type="containsText" dxfId="41" priority="17" operator="containsText" text="En attente">
+  <conditionalFormatting sqref="H9:H45 H49 H66 H47">
+    <cfRule type="containsText" dxfId="44" priority="20" operator="containsText" text="En attente">
       <formula>NOT(ISERROR(SEARCH("En attente",H9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="18" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="43" priority="21" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="19" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="42" priority="22" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",H9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9:F45 C49:F49 C64:F66 C47:F47">
-    <cfRule type="cellIs" dxfId="38" priority="20" operator="equal">
+  <conditionalFormatting sqref="C9:F45 C49:F49 C47:F47 C64:F66">
+    <cfRule type="cellIs" dxfId="41" priority="23" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="21">
+    <cfRule type="expression" dxfId="40" priority="24">
       <formula>$H9="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9:F45 C49:F49 C64:F66 C47:F47">
-    <cfRule type="expression" dxfId="36" priority="22">
+  <conditionalFormatting sqref="C9:F45 C49:F49 C47:F47 C64:F66">
+    <cfRule type="expression" dxfId="39" priority="25">
       <formula>$H9="En cours"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="23">
+    <cfRule type="expression" dxfId="38" priority="26">
       <formula>$H9="En attente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="containsText" dxfId="34" priority="24" operator="containsText" text="En attente">
+    <cfRule type="containsText" dxfId="37" priority="27" operator="containsText" text="En attente">
       <formula>NOT(ISERROR(SEARCH("En attente",H48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="25" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="36" priority="28" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="26" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="35" priority="29" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",H48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:F48">
-    <cfRule type="cellIs" dxfId="31" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="30" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="28">
+    <cfRule type="expression" dxfId="33" priority="31">
       <formula>$H48="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:F48">
-    <cfRule type="expression" dxfId="29" priority="29">
+    <cfRule type="expression" dxfId="32" priority="32">
       <formula>$H48="En cours"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="30">
+    <cfRule type="expression" dxfId="31" priority="33">
       <formula>$H48="En attente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50:H55">
-    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="En attente">
+    <cfRule type="containsText" dxfId="30" priority="34" operator="containsText" text="En attente">
       <formula>NOT(ISERROR(SEARCH("En attente",H50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="32" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="29" priority="35" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="33" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="28" priority="36" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",H50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50:F55">
-    <cfRule type="cellIs" dxfId="24" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="37" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="35">
+    <cfRule type="expression" dxfId="26" priority="38">
       <formula>$H50="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50:F55">
-    <cfRule type="expression" dxfId="22" priority="36">
+    <cfRule type="expression" dxfId="25" priority="39">
       <formula>$H50="En cours"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="37">
+    <cfRule type="expression" dxfId="24" priority="40">
       <formula>$H50="En attente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46">
-    <cfRule type="containsText" dxfId="20" priority="38" operator="containsText" text="En attente">
+    <cfRule type="containsText" dxfId="23" priority="41" operator="containsText" text="En attente">
       <formula>NOT(ISERROR(SEARCH("En attente",H46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="39" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="22" priority="42" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="40" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="21" priority="43" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",H46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:F46">
-    <cfRule type="cellIs" dxfId="17" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="44" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="42">
+    <cfRule type="expression" dxfId="19" priority="45">
       <formula>$H46="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:F46">
-    <cfRule type="expression" dxfId="15" priority="43">
+    <cfRule type="expression" dxfId="18" priority="46">
       <formula>$H46="En cours"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="44">
+    <cfRule type="expression" dxfId="17" priority="47">
       <formula>$H46="En attente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H56">
-    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="En attente">
+    <cfRule type="containsText" dxfId="16" priority="11" operator="containsText" text="En attente">
       <formula>NOT(ISERROR(SEARCH("En attente",H56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",H56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:F56">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="12">
+    <cfRule type="expression" dxfId="12" priority="15">
       <formula>$H56="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:F56">
-    <cfRule type="expression" dxfId="8" priority="13">
+    <cfRule type="expression" dxfId="11" priority="16">
       <formula>$H56="En cours"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="14">
+    <cfRule type="expression" dxfId="10" priority="17">
       <formula>$H56="En attente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57:H63">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="En attente">
+    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="En attente">
       <formula>NOT(ISERROR(SEARCH("En attente",H57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",H57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57:F63">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="5">
+    <cfRule type="expression" dxfId="5" priority="8">
       <formula>$H57="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57:F63">
-    <cfRule type="expression" dxfId="1" priority="6">
+    <cfRule type="expression" dxfId="4" priority="9">
       <formula>$H57="En cours"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="7">
+    <cfRule type="expression" dxfId="3" priority="10">
       <formula>$H57="En attente"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H64:H65">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="En attente">
+      <formula>NOT(ISERROR(SEARCH("En attente",H64)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",H64)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",H64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -6100,12 +6221,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1025" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="121" t="s">
         <v>6</v>
       </c>
@@ -6113,7 +6234,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -6121,7 +6242,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -6141,7 +6262,7 @@
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1025" width="10.6640625" style="2"/>
   </cols>

</xml_diff>

<commit_message>
Ajout du semainier 08 Avril
</commit_message>
<xml_diff>
--- a/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
+++ b/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alxbo\Source\Repos\mrjrdg\marque-sans-nom\Semainiers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Desktop/marque-sans-nom/Semainiers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACDF28A4-31EE-425E-A700-86D9A9A293D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C830DF5A-379C-4D47-B5E8-8D3D9BE70EE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="30720" windowHeight="18740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="89">
   <si>
     <t>UQÀM - Hiver 2020</t>
   </si>
@@ -364,6 +362,9 @@
   </si>
   <si>
     <t>Améliorer le visuel (business-create, business-list, business-edit, business-delete)</t>
+  </si>
+  <si>
+    <t>Ajuster ( - 2 semaines Covid-19)</t>
   </si>
 </sst>
 </file>
@@ -538,7 +539,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -614,8 +615,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="38">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -1083,6 +1090,49 @@
       <left/>
       <right style="thin">
         <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
       <top style="thin">
         <color auto="1"/>
@@ -1106,7 +1156,7 @@
     <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1543,6 +1593,36 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1559,49 +1639,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="11" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="11" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="14" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
+    <cellStyle name="Bad" xfId="10" builtinId="27"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Excel Built-in 60% - Accent4" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Excel Built-in Bad" xfId="6" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Excel Built-in Good" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Excel Built-in Neutral" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Excel Built-in Normal" xfId="3" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Insatisfaisant" xfId="10" builtinId="27"/>
-    <cellStyle name="Milliers" xfId="1" builtinId="3"/>
-    <cellStyle name="Neutre" xfId="9" builtinId="28"/>
+    <cellStyle name="Good" xfId="8" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="9" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Satisfaisant" xfId="8" builtinId="26"/>
   </cellStyles>
   <dxfs count="52">
     <dxf>
@@ -2493,19 +2555,19 @@
   </sheetPr>
   <dimension ref="A1:AMK80"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AD7" sqref="AD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="74.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="74.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" style="2" customWidth="1"/>
-    <col min="4" max="5" width="8.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="3" customWidth="1"/>
     <col min="9" max="10" width="9.33203125" style="4" customWidth="1"/>
     <col min="11" max="13" width="8" style="1" customWidth="1"/>
     <col min="14" max="14" width="8" style="5" customWidth="1"/>
@@ -2521,23 +2583,23 @@
     <col min="29" max="1025" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="8" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="160" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="160"/>
+    <row r="1" spans="1:28" s="8" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="146" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="146"/>
       <c r="C1" s="7"/>
-      <c r="D1" s="161" t="s">
+      <c r="D1" s="147" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="161"/>
-      <c r="F1" s="161"/>
-      <c r="G1" s="161"/>
-      <c r="H1" s="161"/>
-      <c r="I1" s="161"/>
-      <c r="J1" s="161"/>
-      <c r="K1" s="161"/>
-      <c r="L1" s="161"/>
+      <c r="E1" s="147"/>
+      <c r="F1" s="147"/>
+      <c r="G1" s="147"/>
+      <c r="H1" s="147"/>
+      <c r="I1" s="147"/>
+      <c r="J1" s="147"/>
+      <c r="K1" s="147"/>
+      <c r="L1" s="147"/>
       <c r="N1" s="3"/>
       <c r="P1" s="9"/>
       <c r="Q1" s="8" t="s">
@@ -2548,21 +2610,21 @@
       <c r="Z1" s="3"/>
       <c r="AA1" s="10"/>
     </row>
-    <row r="2" spans="1:28" s="8" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="160" t="s">
+    <row r="2" spans="1:28" s="8" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="146" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="160"/>
+      <c r="B2" s="146"/>
       <c r="C2" s="7"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="160" t="s">
+      <c r="F2" s="146" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="160"/>
-      <c r="H2" s="160"/>
-      <c r="I2" s="160"/>
-      <c r="J2" s="160"/>
+      <c r="G2" s="146"/>
+      <c r="H2" s="146"/>
+      <c r="I2" s="146"/>
+      <c r="J2" s="146"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
       <c r="N2" s="3"/>
@@ -2575,7 +2637,7 @@
       <c r="Z2" s="3"/>
       <c r="AA2" s="10"/>
     </row>
-    <row r="3" spans="1:28" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -2593,7 +2655,7 @@
       <c r="Z3" s="3"/>
       <c r="AA3" s="10"/>
     </row>
-    <row r="4" spans="1:28" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
@@ -2613,7 +2675,7 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="10"/>
     </row>
-    <row r="5" spans="1:28" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
@@ -2637,7 +2699,7 @@
       </c>
       <c r="AA5" s="10"/>
     </row>
-    <row r="6" spans="1:28" s="8" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" s="8" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
@@ -2645,78 +2707,78 @@
       <c r="H6" s="3"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="152" t="s">
+      <c r="K6" s="148" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="152"/>
-      <c r="M6" s="152"/>
-      <c r="N6" s="152"/>
-      <c r="O6" s="152"/>
-      <c r="P6" s="152"/>
-      <c r="Q6" s="152"/>
-      <c r="R6" s="152"/>
-      <c r="S6" s="152" t="s">
+      <c r="L6" s="148"/>
+      <c r="M6" s="148"/>
+      <c r="N6" s="148"/>
+      <c r="O6" s="148"/>
+      <c r="P6" s="148"/>
+      <c r="Q6" s="148"/>
+      <c r="R6" s="148"/>
+      <c r="S6" s="148" t="s">
         <v>10</v>
       </c>
-      <c r="T6" s="152"/>
-      <c r="U6" s="152"/>
-      <c r="V6" s="152"/>
+      <c r="T6" s="148"/>
+      <c r="U6" s="148"/>
+      <c r="V6" s="148"/>
       <c r="Z6" s="17"/>
       <c r="AA6" s="10"/>
     </row>
-    <row r="7" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="153" t="s">
+    <row r="7" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="149" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="154" t="s">
+      <c r="B7" s="150" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="155" t="s">
+      <c r="C7" s="151" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="155"/>
-      <c r="E7" s="155"/>
-      <c r="F7" s="155"/>
-      <c r="G7" s="156" t="s">
+      <c r="D7" s="151"/>
+      <c r="E7" s="151"/>
+      <c r="F7" s="151"/>
+      <c r="G7" s="152" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="157" t="s">
+      <c r="H7" s="153" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="158" t="s">
+      <c r="I7" s="154" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="158" t="s">
+      <c r="J7" s="154" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="159" t="s">
+      <c r="K7" s="155" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="159"/>
-      <c r="M7" s="159"/>
-      <c r="N7" s="159"/>
-      <c r="O7" s="159"/>
-      <c r="P7" s="159"/>
-      <c r="Q7" s="159"/>
-      <c r="R7" s="159"/>
-      <c r="S7" s="159"/>
-      <c r="T7" s="159"/>
-      <c r="U7" s="159"/>
-      <c r="V7" s="159"/>
-      <c r="W7" s="159"/>
-      <c r="X7" s="159"/>
-      <c r="Y7" s="159"/>
-      <c r="Z7" s="159"/>
-      <c r="AA7" s="149" t="s">
+      <c r="L7" s="155"/>
+      <c r="M7" s="155"/>
+      <c r="N7" s="155"/>
+      <c r="O7" s="155"/>
+      <c r="P7" s="155"/>
+      <c r="Q7" s="155"/>
+      <c r="R7" s="155"/>
+      <c r="S7" s="155"/>
+      <c r="T7" s="155"/>
+      <c r="U7" s="155"/>
+      <c r="V7" s="155"/>
+      <c r="W7" s="155"/>
+      <c r="X7" s="155"/>
+      <c r="Y7" s="155"/>
+      <c r="Z7" s="155"/>
+      <c r="AA7" s="159" t="s">
         <v>19</v>
       </c>
-      <c r="AB7" s="150" t="s">
+      <c r="AB7" s="160" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="153"/>
-      <c r="B8" s="154"/>
+    <row r="8" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="149"/>
+      <c r="B8" s="150"/>
       <c r="C8" s="20" t="s">
         <v>21</v>
       </c>
@@ -2729,10 +2791,10 @@
       <c r="F8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="156"/>
-      <c r="H8" s="157"/>
-      <c r="I8" s="158"/>
-      <c r="J8" s="158"/>
+      <c r="G8" s="152"/>
+      <c r="H8" s="153"/>
+      <c r="I8" s="154"/>
+      <c r="J8" s="154"/>
       <c r="K8" s="21">
         <v>43838</v>
       </c>
@@ -2796,10 +2858,10 @@
         <f t="shared" si="0"/>
         <v>43943</v>
       </c>
-      <c r="AA8" s="149"/>
-      <c r="AB8" s="150"/>
-    </row>
-    <row r="9" spans="1:28" ht="18" x14ac:dyDescent="0.3">
+      <c r="AA8" s="159"/>
+      <c r="AB8" s="160"/>
+    </row>
+    <row r="9" spans="1:28" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>25</v>
@@ -2831,7 +2893,7 @@
       <c r="AA9" s="33"/>
       <c r="AB9" s="34"/>
     </row>
-    <row r="10" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="35">
         <v>1</v>
       </c>
@@ -2886,7 +2948,7 @@
       </c>
       <c r="AB10" s="45"/>
     </row>
-    <row r="11" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="35">
         <v>2</v>
       </c>
@@ -2941,7 +3003,7 @@
       </c>
       <c r="AB11" s="48"/>
     </row>
-    <row r="12" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="35">
         <v>3</v>
       </c>
@@ -2995,7 +3057,7 @@
       </c>
       <c r="AB12" s="49"/>
     </row>
-    <row r="13" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="35">
         <v>4</v>
       </c>
@@ -3050,7 +3112,7 @@
       </c>
       <c r="AB13" s="48"/>
     </row>
-    <row r="14" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="35">
         <v>5</v>
       </c>
@@ -3105,7 +3167,7 @@
       </c>
       <c r="AB14" s="48"/>
     </row>
-    <row r="15" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="35">
         <v>6</v>
       </c>
@@ -3160,7 +3222,7 @@
       </c>
       <c r="AB15" s="48"/>
     </row>
-    <row r="16" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="35">
         <v>7</v>
       </c>
@@ -3215,7 +3277,7 @@
       </c>
       <c r="AB16" s="48"/>
     </row>
-    <row r="17" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="35">
         <v>8</v>
       </c>
@@ -3270,7 +3332,7 @@
       </c>
       <c r="AB17" s="48"/>
     </row>
-    <row r="18" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="35">
         <v>9</v>
       </c>
@@ -3325,7 +3387,7 @@
       </c>
       <c r="AB18" s="48"/>
     </row>
-    <row r="19" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="35">
         <v>10</v>
       </c>
@@ -3380,7 +3442,7 @@
       </c>
       <c r="AB19" s="48"/>
     </row>
-    <row r="20" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="35">
         <v>11</v>
       </c>
@@ -3435,7 +3497,7 @@
       </c>
       <c r="AB20" s="48"/>
     </row>
-    <row r="21" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="35">
         <v>12</v>
       </c>
@@ -3490,7 +3552,7 @@
       </c>
       <c r="AB21" s="48"/>
     </row>
-    <row r="22" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="35">
         <v>13</v>
       </c>
@@ -3545,7 +3607,7 @@
       </c>
       <c r="AB22" s="48"/>
     </row>
-    <row r="23" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="35">
         <v>14</v>
       </c>
@@ -3600,7 +3662,7 @@
       </c>
       <c r="AB23" s="48"/>
     </row>
-    <row r="24" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="35">
         <v>15</v>
       </c>
@@ -3655,7 +3717,7 @@
       </c>
       <c r="AB24" s="48"/>
     </row>
-    <row r="25" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="35">
         <v>16</v>
       </c>
@@ -3710,7 +3772,7 @@
       </c>
       <c r="AB25" s="48"/>
     </row>
-    <row r="26" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="35">
         <v>17</v>
       </c>
@@ -3765,7 +3827,7 @@
       </c>
       <c r="AB26" s="76"/>
     </row>
-    <row r="27" spans="1:28" s="79" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" s="79" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="35">
         <v>18</v>
       </c>
@@ -3820,7 +3882,7 @@
       </c>
       <c r="AB27" s="48"/>
     </row>
-    <row r="28" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="35">
         <v>19</v>
       </c>
@@ -3875,7 +3937,7 @@
       </c>
       <c r="AB28" s="48"/>
     </row>
-    <row r="29" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="35">
         <v>20</v>
       </c>
@@ -3930,7 +3992,7 @@
       </c>
       <c r="AB29" s="48"/>
     </row>
-    <row r="30" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="35">
         <v>21</v>
       </c>
@@ -3985,7 +4047,7 @@
       </c>
       <c r="AB30" s="48"/>
     </row>
-    <row r="31" spans="1:28" s="79" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" s="79" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="35">
         <v>22</v>
       </c>
@@ -4040,7 +4102,7 @@
       </c>
       <c r="AB31" s="48"/>
     </row>
-    <row r="32" spans="1:28" s="79" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" s="79" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="35">
         <v>23</v>
       </c>
@@ -4095,7 +4157,7 @@
       </c>
       <c r="AB32" s="48"/>
     </row>
-    <row r="33" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="35">
         <v>24</v>
       </c>
@@ -4150,7 +4212,7 @@
       </c>
       <c r="AB33" s="48"/>
     </row>
-    <row r="34" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="35">
         <v>25</v>
       </c>
@@ -4205,7 +4267,7 @@
       </c>
       <c r="AB34" s="48"/>
     </row>
-    <row r="35" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="35">
         <v>27</v>
       </c>
@@ -4258,7 +4320,7 @@
       </c>
       <c r="AB35" s="48"/>
     </row>
-    <row r="36" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="35">
         <v>28</v>
       </c>
@@ -4311,7 +4373,7 @@
       </c>
       <c r="AB36" s="48"/>
     </row>
-    <row r="37" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="35">
         <v>29</v>
       </c>
@@ -4364,7 +4426,7 @@
       </c>
       <c r="AB37" s="48"/>
     </row>
-    <row r="38" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="35">
         <v>30</v>
       </c>
@@ -4417,7 +4479,7 @@
       </c>
       <c r="AB38" s="48"/>
     </row>
-    <row r="39" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="35">
         <v>31</v>
       </c>
@@ -4470,7 +4532,7 @@
       </c>
       <c r="AB39" s="48"/>
     </row>
-    <row r="40" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="35">
         <v>32</v>
       </c>
@@ -4523,7 +4585,7 @@
       </c>
       <c r="AB40" s="48"/>
     </row>
-    <row r="41" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="35">
         <v>33</v>
       </c>
@@ -4578,7 +4640,7 @@
       </c>
       <c r="AB41" s="48"/>
     </row>
-    <row r="42" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="35">
         <v>34</v>
       </c>
@@ -4631,7 +4693,7 @@
       </c>
       <c r="AB42" s="48"/>
     </row>
-    <row r="43" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="35">
         <v>35</v>
       </c>
@@ -4686,7 +4748,7 @@
       </c>
       <c r="AB43" s="48"/>
     </row>
-    <row r="44" spans="1:28" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="35">
         <v>36</v>
       </c>
@@ -4741,7 +4803,7 @@
       </c>
       <c r="AB44" s="48"/>
     </row>
-    <row r="45" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="35">
         <v>37</v>
       </c>
@@ -4794,7 +4856,7 @@
       </c>
       <c r="AB45" s="48"/>
     </row>
-    <row r="46" spans="1:28" s="86" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:28" s="86" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="35">
         <v>39</v>
       </c>
@@ -4846,7 +4908,7 @@
       <c r="AA46" s="44"/>
       <c r="AB46" s="48"/>
     </row>
-    <row r="47" spans="1:28" s="86" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:28" s="86" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="35">
         <v>40</v>
       </c>
@@ -4898,7 +4960,7 @@
       <c r="AA47" s="44"/>
       <c r="AB47" s="48"/>
     </row>
-    <row r="48" spans="1:28" s="46" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:28" s="46" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A48" s="87"/>
       <c r="B48" s="24" t="s">
         <v>64</v>
@@ -4930,7 +4992,7 @@
       <c r="AA48" s="90"/>
       <c r="AB48" s="91"/>
     </row>
-    <row r="49" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="35">
         <v>1</v>
       </c>
@@ -4985,7 +5047,7 @@
       </c>
       <c r="AB49" s="48"/>
     </row>
-    <row r="50" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="35">
         <v>2</v>
       </c>
@@ -5038,7 +5100,7 @@
       </c>
       <c r="AB50" s="48"/>
     </row>
-    <row r="51" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="35">
         <v>3</v>
       </c>
@@ -5088,7 +5150,7 @@
       <c r="AA51" s="94"/>
       <c r="AB51" s="76"/>
     </row>
-    <row r="52" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="35">
         <v>4</v>
       </c>
@@ -5140,7 +5202,7 @@
       <c r="AA52" s="94"/>
       <c r="AB52" s="76"/>
     </row>
-    <row r="53" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="143">
         <v>5</v>
       </c>
@@ -5192,7 +5254,7 @@
       <c r="AA53" s="94"/>
       <c r="AB53" s="76"/>
     </row>
-    <row r="54" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="35">
         <v>6</v>
       </c>
@@ -5244,7 +5306,7 @@
       <c r="AA54" s="94"/>
       <c r="AB54" s="76"/>
     </row>
-    <row r="55" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="35">
         <v>7</v>
       </c>
@@ -5296,7 +5358,7 @@
       <c r="AA55" s="94"/>
       <c r="AB55" s="76"/>
     </row>
-    <row r="56" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="35">
         <v>8</v>
       </c>
@@ -5348,7 +5410,7 @@
       <c r="AA56" s="94"/>
       <c r="AB56" s="76"/>
     </row>
-    <row r="57" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="35">
         <v>9</v>
       </c>
@@ -5400,7 +5462,7 @@
       <c r="AA57" s="94"/>
       <c r="AB57" s="76"/>
     </row>
-    <row r="58" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="35">
         <v>10</v>
       </c>
@@ -5452,7 +5514,7 @@
       <c r="AA58" s="94"/>
       <c r="AB58" s="76"/>
     </row>
-    <row r="59" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="35">
         <v>11</v>
       </c>
@@ -5504,7 +5566,7 @@
       <c r="AA59" s="94"/>
       <c r="AB59" s="76"/>
     </row>
-    <row r="60" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="35">
         <v>12</v>
       </c>
@@ -5556,7 +5618,7 @@
       <c r="AA60" s="94"/>
       <c r="AB60" s="76"/>
     </row>
-    <row r="61" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="35">
         <v>13</v>
       </c>
@@ -5608,7 +5670,7 @@
       <c r="AA61" s="94"/>
       <c r="AB61" s="76"/>
     </row>
-    <row r="62" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="35">
         <v>14</v>
       </c>
@@ -5660,7 +5722,7 @@
       <c r="AA62" s="94"/>
       <c r="AB62" s="76"/>
     </row>
-    <row r="63" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="35">
         <v>15</v>
       </c>
@@ -5712,7 +5774,7 @@
       <c r="AA63" s="94"/>
       <c r="AB63" s="76"/>
     </row>
-    <row r="64" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="143">
         <v>16</v>
       </c>
@@ -5753,13 +5815,13 @@
       <c r="U64" s="73"/>
       <c r="V64" s="52"/>
       <c r="W64" s="73"/>
-      <c r="X64" s="128"/>
+      <c r="X64" s="124"/>
       <c r="Y64" s="73"/>
       <c r="Z64" s="52"/>
       <c r="AA64" s="94"/>
       <c r="AB64" s="76"/>
     </row>
-    <row r="65" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="35">
         <v>17</v>
       </c>
@@ -5780,7 +5842,7 @@
       </c>
       <c r="G65" s="71"/>
       <c r="H65" s="39" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I65" s="40">
         <v>3</v>
@@ -5808,7 +5870,7 @@
       <c r="AA65" s="94"/>
       <c r="AB65" s="76"/>
     </row>
-    <row r="66" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="35">
         <v>18</v>
       </c>
@@ -5857,7 +5919,7 @@
       <c r="AA66" s="94"/>
       <c r="AB66" s="76"/>
     </row>
-    <row r="67" spans="1:28" s="46" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:28" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="35"/>
       <c r="B67" s="69"/>
       <c r="C67" s="37"/>
@@ -5887,7 +5949,7 @@
       <c r="AA67" s="94"/>
       <c r="AB67" s="76"/>
     </row>
-    <row r="68" spans="1:28" s="46" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:28" s="46" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="135"/>
       <c r="B68" s="136"/>
       <c r="C68" s="137"/>
@@ -5917,11 +5979,11 @@
       <c r="AA68" s="97"/>
       <c r="AB68" s="98"/>
     </row>
-    <row r="69" spans="1:28" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="151" t="s">
+    <row r="69" spans="1:28" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="161" t="s">
         <v>68</v>
       </c>
-      <c r="B69" s="151"/>
+      <c r="B69" s="161"/>
       <c r="C69" s="99">
         <f>SUM(C10:C68)</f>
         <v>111</v>
@@ -5967,33 +6029,33 @@
       </c>
       <c r="AB69" s="133"/>
     </row>
-    <row r="70" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="146" t="s">
+    <row r="70" spans="1:28" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="156" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="146"/>
+      <c r="B70" s="156"/>
       <c r="C70" s="99">
-        <f>135-C69</f>
-        <v>24</v>
+        <f>117-C69</f>
+        <v>6</v>
       </c>
       <c r="D70" s="99">
-        <f>135-D69</f>
-        <v>44.5</v>
+        <f>117-D69</f>
+        <v>26.5</v>
       </c>
       <c r="E70" s="99">
-        <f>135-E69</f>
-        <v>42.5</v>
+        <f>117-E69</f>
+        <v>24.5</v>
       </c>
       <c r="F70" s="99">
-        <f>135-F69</f>
-        <v>27</v>
+        <f>117-F69</f>
+        <v>9</v>
       </c>
       <c r="G70" s="100"/>
       <c r="H70" s="99"/>
       <c r="I70" s="99"/>
       <c r="J70" s="99">
         <f>SUM(C70:F70)</f>
-        <v>138</v>
+        <v>66</v>
       </c>
       <c r="K70" s="102"/>
       <c r="L70" s="102"/>
@@ -6014,11 +6076,11 @@
       <c r="AA70" s="102"/>
       <c r="AB70" s="102"/>
     </row>
-    <row r="71" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="147" t="s">
+    <row r="71" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="157" t="s">
         <v>70</v>
       </c>
-      <c r="B71" s="147"/>
+      <c r="B71" s="157"/>
       <c r="C71" s="99"/>
       <c r="D71" s="99"/>
       <c r="E71" s="99"/>
@@ -6049,11 +6111,11 @@
       <c r="AA71" s="102"/>
       <c r="AB71" s="102"/>
     </row>
-    <row r="72" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="146" t="s">
+    <row r="72" spans="1:28" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="156" t="s">
         <v>71</v>
       </c>
-      <c r="B72" s="146"/>
+      <c r="B72" s="156"/>
       <c r="C72" s="99"/>
       <c r="D72" s="99"/>
       <c r="E72" s="103"/>
@@ -6087,14 +6149,16 @@
       <c r="AA72" s="102"/>
       <c r="AB72" s="102"/>
     </row>
-    <row r="73" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:28" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="105"/>
       <c r="B73" s="105"/>
       <c r="C73" s="106"/>
-      <c r="D73" s="106"/>
-      <c r="E73" s="106"/>
-      <c r="F73" s="106"/>
-      <c r="G73" s="106"/>
+      <c r="D73" s="165" t="s">
+        <v>88</v>
+      </c>
+      <c r="E73" s="165"/>
+      <c r="F73" s="165"/>
+      <c r="G73" s="165"/>
       <c r="H73" s="106"/>
       <c r="I73" s="106"/>
       <c r="J73" s="106"/>
@@ -6117,16 +6181,18 @@
       <c r="AA73" s="102"/>
       <c r="AB73" s="102"/>
     </row>
-    <row r="74" spans="1:28" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="147" t="s">
+    <row r="74" spans="1:28" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="157" t="s">
         <v>72</v>
       </c>
-      <c r="B74" s="147"/>
-      <c r="C74" s="99">
+      <c r="B74" s="157"/>
+      <c r="C74" s="162">
         <f>135*4</f>
         <v>540</v>
       </c>
-      <c r="D74" s="106"/>
+      <c r="D74" s="163">
+        <v>468</v>
+      </c>
       <c r="E74" s="106"/>
       <c r="F74" s="106"/>
       <c r="G74" s="106"/>
@@ -6152,16 +6218,18 @@
       <c r="AA74" s="102"/>
       <c r="AB74" s="102"/>
     </row>
-    <row r="75" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="148" t="s">
+    <row r="75" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="158" t="s">
         <v>73</v>
       </c>
-      <c r="B75" s="148"/>
-      <c r="C75" s="99">
+      <c r="B75" s="158"/>
+      <c r="C75" s="162">
         <f>C74-J72</f>
         <v>138</v>
       </c>
-      <c r="D75" s="106"/>
+      <c r="D75" s="164">
+        <v>66</v>
+      </c>
       <c r="E75" s="106"/>
       <c r="F75" s="106"/>
       <c r="G75" s="106"/>
@@ -6187,7 +6255,7 @@
       <c r="AA75" s="102"/>
       <c r="AB75" s="102"/>
     </row>
-    <row r="76" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="107"/>
       <c r="B76" s="105"/>
       <c r="C76" s="108"/>
@@ -6200,12 +6268,12 @@
       <c r="J76" s="110"/>
       <c r="AA76" s="102"/>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:28" x14ac:dyDescent="0.2">
       <c r="D77" s="111"/>
       <c r="E77" s="111"/>
       <c r="F77" s="111"/>
     </row>
-    <row r="78" spans="1:28" s="113" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:28" s="113" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A78" s="112"/>
       <c r="C78" s="114"/>
       <c r="D78" s="114"/>
@@ -6220,7 +6288,7 @@
       <c r="Z78" s="117"/>
       <c r="AA78" s="118"/>
     </row>
-    <row r="79" spans="1:28" s="113" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:28" s="113" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="C79" s="114"/>
       <c r="D79" s="114"/>
       <c r="E79" s="114"/>
@@ -6234,7 +6302,7 @@
       <c r="Z79" s="117"/>
       <c r="AA79" s="118"/>
     </row>
-    <row r="80" spans="1:28" s="113" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:28" s="113" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="C80" s="114"/>
       <c r="D80" s="114"/>
       <c r="E80" s="114"/>
@@ -6249,12 +6317,16 @@
       <c r="AA80" s="118"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K6:R6"/>
+  <mergeCells count="23">
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D73:G73"/>
     <mergeCell ref="S6:V6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
@@ -6264,14 +6336,11 @@
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:Z7"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K6:R6"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
     <cfRule type="containsText" dxfId="51" priority="33" operator="containsText" text="En cours">
@@ -6473,7 +6542,7 @@
       <formula>NOT(ISERROR(SEARCH("Terminé",H66)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H9:H68" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"En attente,En cours,Terminé"</formula1>
       <formula2>0</formula2>
@@ -6481,7 +6550,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31527777777777799" right="0.31527777777777799" top="0.74791666666666701" bottom="0.55138888888888904" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup scale="37" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -6493,12 +6562,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1025" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="119" t="s">
         <v>6</v>
       </c>
@@ -6506,7 +6575,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -6514,7 +6583,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -6534,7 +6603,7 @@
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1025" width="10.6640625" style="1"/>
   </cols>

</xml_diff>

<commit_message>
Partially fixed issue #64
</commit_message>
<xml_diff>
--- a/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
+++ b/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alxbo\Source\Repos\mrjrdg\marque-sans-nom\Semainiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617FD861-5697-4C34-BEC8-F89CE0F9ADAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135EE3CE-9E38-4987-822E-96195C620AB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="112">
   <si>
     <t>UQÀM - Hiver 2020</t>
   </si>
@@ -433,6 +433,9 @@
   </si>
   <si>
     <t>Régler un bug (event-create, event-edit)</t>
+  </si>
+  <si>
+    <t>Afficher les avatars (event-view, profile-edit, navbar)</t>
   </si>
 </sst>
 </file>
@@ -1525,63 +1528,7 @@
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="12" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="11" xfId="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -1596,6 +1543,62 @@
     <xf numFmtId="164" fontId="18" fillId="0" borderId="33" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="34" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="35" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="12" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Excel Built-in 60% - Accent4" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -2596,16 +2599,16 @@
   <dimension ref="A1:AMK101"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="76.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="142" customWidth="1"/>
-    <col min="4" max="4" width="8.109375" style="142" customWidth="1"/>
-    <col min="5" max="6" width="8.77734375" style="142" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="123" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" style="123" customWidth="1"/>
+    <col min="5" max="6" width="8.77734375" style="123" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.44140625" style="2" customWidth="1"/>
     <col min="9" max="10" width="9.33203125" style="3" customWidth="1"/>
@@ -2624,22 +2627,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="6" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="140" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="140"/>
-      <c r="C1" s="142"/>
-      <c r="D1" s="141" t="s">
+      <c r="A1" s="132" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="132"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="141"/>
-      <c r="F1" s="141"/>
-      <c r="G1" s="141"/>
-      <c r="H1" s="141"/>
-      <c r="I1" s="141"/>
-      <c r="J1" s="141"/>
-      <c r="K1" s="141"/>
-      <c r="L1" s="141"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
+      <c r="J1" s="133"/>
+      <c r="K1" s="133"/>
+      <c r="L1" s="133"/>
       <c r="N1" s="2"/>
       <c r="P1" s="7"/>
       <c r="Q1" s="6" t="s">
@@ -2651,20 +2654,20 @@
       <c r="AA1" s="8"/>
     </row>
     <row r="2" spans="1:28" s="6" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="140" t="s">
+      <c r="A2" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="140"/>
-      <c r="C2" s="142"/>
-      <c r="D2" s="142"/>
-      <c r="E2" s="142"/>
-      <c r="F2" s="140" t="s">
+      <c r="B2" s="132"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="132" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="140"/>
-      <c r="H2" s="140"/>
-      <c r="I2" s="140"/>
-      <c r="J2" s="140"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="132"/>
+      <c r="J2" s="132"/>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
       <c r="N2" s="2"/>
@@ -2678,10 +2681,10 @@
       <c r="AA2" s="8"/>
     </row>
     <row r="3" spans="1:28" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="C3" s="142"/>
-      <c r="D3" s="142"/>
-      <c r="E3" s="142"/>
-      <c r="F3" s="142"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="123"/>
       <c r="H3" s="2"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -2696,10 +2699,10 @@
       <c r="AA3" s="8"/>
     </row>
     <row r="4" spans="1:28" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="C4" s="142"/>
-      <c r="D4" s="142"/>
-      <c r="E4" s="142"/>
-      <c r="F4" s="142"/>
+      <c r="C4" s="123"/>
+      <c r="D4" s="123"/>
+      <c r="E4" s="123"/>
+      <c r="F4" s="123"/>
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -2716,10 +2719,10 @@
       <c r="AA4" s="8"/>
     </row>
     <row r="5" spans="1:28" s="6" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="142"/>
-      <c r="D5" s="142"/>
-      <c r="E5" s="142"/>
-      <c r="F5" s="142"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="123"/>
+      <c r="F5" s="123"/>
       <c r="H5" s="2"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -2740,106 +2743,106 @@
       <c r="AA5" s="8"/>
     </row>
     <row r="6" spans="1:28" s="6" customFormat="1" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="142"/>
-      <c r="D6" s="142"/>
-      <c r="E6" s="142"/>
-      <c r="F6" s="142"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
       <c r="H6" s="2"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="130" t="s">
+      <c r="K6" s="134" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="130"/>
-      <c r="M6" s="130"/>
-      <c r="N6" s="130"/>
-      <c r="O6" s="130"/>
-      <c r="P6" s="130"/>
-      <c r="Q6" s="130"/>
-      <c r="R6" s="130"/>
-      <c r="S6" s="130" t="s">
+      <c r="L6" s="134"/>
+      <c r="M6" s="134"/>
+      <c r="N6" s="134"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="134"/>
+      <c r="Q6" s="134"/>
+      <c r="R6" s="134"/>
+      <c r="S6" s="134" t="s">
         <v>10</v>
       </c>
-      <c r="T6" s="130"/>
-      <c r="U6" s="130"/>
-      <c r="V6" s="130"/>
-      <c r="W6" s="137" t="s">
+      <c r="T6" s="134"/>
+      <c r="U6" s="134"/>
+      <c r="V6" s="134"/>
+      <c r="W6" s="142" t="s">
         <v>93</v>
       </c>
-      <c r="X6" s="138"/>
-      <c r="Y6" s="138"/>
-      <c r="Z6" s="139"/>
+      <c r="X6" s="143"/>
+      <c r="Y6" s="143"/>
+      <c r="Z6" s="144"/>
       <c r="AA6" s="8"/>
     </row>
     <row r="7" spans="1:28" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="131" t="s">
+      <c r="A7" s="135" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="132" t="s">
+      <c r="B7" s="136" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="143" t="s">
+      <c r="C7" s="137" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="143"/>
-      <c r="E7" s="143"/>
-      <c r="F7" s="143"/>
-      <c r="G7" s="133" t="s">
+      <c r="D7" s="137"/>
+      <c r="E7" s="137"/>
+      <c r="F7" s="137"/>
+      <c r="G7" s="138" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="134" t="s">
+      <c r="H7" s="139" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="135" t="s">
+      <c r="I7" s="140" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="135" t="s">
+      <c r="J7" s="140" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="136" t="s">
+      <c r="K7" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="136"/>
-      <c r="M7" s="136"/>
-      <c r="N7" s="136"/>
-      <c r="O7" s="136"/>
-      <c r="P7" s="136"/>
-      <c r="Q7" s="136"/>
-      <c r="R7" s="136"/>
-      <c r="S7" s="136"/>
-      <c r="T7" s="136"/>
-      <c r="U7" s="136"/>
-      <c r="V7" s="136"/>
-      <c r="W7" s="136"/>
-      <c r="X7" s="136"/>
-      <c r="Y7" s="136"/>
-      <c r="Z7" s="136"/>
-      <c r="AA7" s="126" t="s">
+      <c r="L7" s="141"/>
+      <c r="M7" s="141"/>
+      <c r="N7" s="141"/>
+      <c r="O7" s="141"/>
+      <c r="P7" s="141"/>
+      <c r="Q7" s="141"/>
+      <c r="R7" s="141"/>
+      <c r="S7" s="141"/>
+      <c r="T7" s="141"/>
+      <c r="U7" s="141"/>
+      <c r="V7" s="141"/>
+      <c r="W7" s="141"/>
+      <c r="X7" s="141"/>
+      <c r="Y7" s="141"/>
+      <c r="Z7" s="141"/>
+      <c r="AA7" s="148" t="s">
         <v>19</v>
       </c>
-      <c r="AB7" s="127" t="s">
+      <c r="AB7" s="149" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="131"/>
-      <c r="B8" s="132"/>
-      <c r="C8" s="144" t="s">
+      <c r="A8" s="135"/>
+      <c r="B8" s="136"/>
+      <c r="C8" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="144" t="s">
+      <c r="D8" s="124" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="144" t="s">
+      <c r="E8" s="124" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="144" t="s">
+      <c r="F8" s="124" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="133"/>
-      <c r="H8" s="134"/>
-      <c r="I8" s="135"/>
-      <c r="J8" s="135"/>
+      <c r="G8" s="138"/>
+      <c r="H8" s="139"/>
+      <c r="I8" s="140"/>
+      <c r="J8" s="140"/>
       <c r="K8" s="16">
         <v>43838</v>
       </c>
@@ -2903,18 +2906,18 @@
         <f>Y8+7</f>
         <v>43943</v>
       </c>
-      <c r="AA8" s="126"/>
-      <c r="AB8" s="127"/>
+      <c r="AA8" s="148"/>
+      <c r="AB8" s="149"/>
     </row>
     <row r="9" spans="1:28" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="18"/>
       <c r="B9" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="145"/>
-      <c r="D9" s="145"/>
-      <c r="E9" s="145"/>
-      <c r="F9" s="145"/>
+      <c r="C9" s="125"/>
+      <c r="D9" s="125"/>
+      <c r="E9" s="125"/>
+      <c r="F9" s="125"/>
       <c r="G9" s="20"/>
       <c r="H9" s="21"/>
       <c r="I9" s="22"/>
@@ -2945,16 +2948,16 @@
       <c r="B10" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="146">
+      <c r="C10" s="126">
         <v>1.5</v>
       </c>
-      <c r="D10" s="146">
+      <c r="D10" s="126">
         <v>1.5</v>
       </c>
-      <c r="E10" s="146">
+      <c r="E10" s="126">
         <v>1.5</v>
       </c>
-      <c r="F10" s="146">
+      <c r="F10" s="126">
         <v>1.5</v>
       </c>
       <c r="G10" s="31">
@@ -3000,16 +3003,16 @@
       <c r="B11" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="146">
+      <c r="C11" s="126">
         <v>1.5</v>
       </c>
-      <c r="D11" s="146">
+      <c r="D11" s="126">
         <v>1.5</v>
       </c>
-      <c r="E11" s="146">
+      <c r="E11" s="126">
         <v>1.5</v>
       </c>
-      <c r="F11" s="146">
+      <c r="F11" s="126">
         <v>1.5</v>
       </c>
       <c r="G11" s="31">
@@ -3055,16 +3058,16 @@
       <c r="B12" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="146">
+      <c r="C12" s="126">
         <v>3</v>
       </c>
-      <c r="D12" s="146">
+      <c r="D12" s="126">
         <v>3</v>
       </c>
-      <c r="E12" s="146">
+      <c r="E12" s="126">
         <v>3</v>
       </c>
-      <c r="F12" s="146">
+      <c r="F12" s="126">
         <v>3</v>
       </c>
       <c r="G12" s="31">
@@ -3109,16 +3112,16 @@
       <c r="B13" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="146">
-        <v>2</v>
-      </c>
-      <c r="D13" s="146">
-        <v>2</v>
-      </c>
-      <c r="E13" s="146">
-        <v>2</v>
-      </c>
-      <c r="F13" s="146">
+      <c r="C13" s="126">
+        <v>2</v>
+      </c>
+      <c r="D13" s="126">
+        <v>2</v>
+      </c>
+      <c r="E13" s="126">
+        <v>2</v>
+      </c>
+      <c r="F13" s="126">
         <v>2</v>
       </c>
       <c r="G13" s="31">
@@ -3164,16 +3167,16 @@
       <c r="B14" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="146">
+      <c r="C14" s="126">
         <v>3</v>
       </c>
-      <c r="D14" s="146">
+      <c r="D14" s="126">
         <v>3</v>
       </c>
-      <c r="E14" s="146">
-        <v>0</v>
-      </c>
-      <c r="F14" s="146">
+      <c r="E14" s="126">
+        <v>0</v>
+      </c>
+      <c r="F14" s="126">
         <v>3</v>
       </c>
       <c r="G14" s="31">
@@ -3219,16 +3222,16 @@
       <c r="B15" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="146">
-        <v>2</v>
-      </c>
-      <c r="D15" s="146">
-        <v>2</v>
-      </c>
-      <c r="E15" s="146">
-        <v>0</v>
-      </c>
-      <c r="F15" s="146">
+      <c r="C15" s="126">
+        <v>2</v>
+      </c>
+      <c r="D15" s="126">
+        <v>2</v>
+      </c>
+      <c r="E15" s="126">
+        <v>0</v>
+      </c>
+      <c r="F15" s="126">
         <v>0</v>
       </c>
       <c r="G15" s="31">
@@ -3274,16 +3277,16 @@
       <c r="B16" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="146">
-        <v>2</v>
-      </c>
-      <c r="D16" s="146">
-        <v>0</v>
-      </c>
-      <c r="E16" s="146">
-        <v>0</v>
-      </c>
-      <c r="F16" s="146">
+      <c r="C16" s="126">
+        <v>2</v>
+      </c>
+      <c r="D16" s="126">
+        <v>0</v>
+      </c>
+      <c r="E16" s="126">
+        <v>0</v>
+      </c>
+      <c r="F16" s="126">
         <v>0</v>
       </c>
       <c r="G16" s="31">
@@ -3329,16 +3332,16 @@
       <c r="B17" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="146">
-        <v>2</v>
-      </c>
-      <c r="D17" s="146">
-        <v>2</v>
-      </c>
-      <c r="E17" s="146">
-        <v>0</v>
-      </c>
-      <c r="F17" s="146">
+      <c r="C17" s="126">
+        <v>2</v>
+      </c>
+      <c r="D17" s="126">
+        <v>2</v>
+      </c>
+      <c r="E17" s="126">
+        <v>0</v>
+      </c>
+      <c r="F17" s="126">
         <v>0</v>
       </c>
       <c r="G17" s="31">
@@ -3384,16 +3387,16 @@
       <c r="B18" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="146">
-        <v>2</v>
-      </c>
-      <c r="D18" s="146">
-        <v>0</v>
-      </c>
-      <c r="E18" s="146">
-        <v>0</v>
-      </c>
-      <c r="F18" s="146">
+      <c r="C18" s="126">
+        <v>2</v>
+      </c>
+      <c r="D18" s="126">
+        <v>0</v>
+      </c>
+      <c r="E18" s="126">
+        <v>0</v>
+      </c>
+      <c r="F18" s="126">
         <v>2</v>
       </c>
       <c r="G18" s="31">
@@ -3439,16 +3442,16 @@
       <c r="B19" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="146">
+      <c r="C19" s="126">
         <v>1.5</v>
       </c>
-      <c r="D19" s="146">
+      <c r="D19" s="126">
         <v>6</v>
       </c>
-      <c r="E19" s="146">
+      <c r="E19" s="126">
         <v>3</v>
       </c>
-      <c r="F19" s="146">
+      <c r="F19" s="126">
         <v>0</v>
       </c>
       <c r="G19" s="31">
@@ -3494,16 +3497,16 @@
       <c r="B20" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="146">
-        <v>0</v>
-      </c>
-      <c r="D20" s="146">
+      <c r="C20" s="126">
+        <v>0</v>
+      </c>
+      <c r="D20" s="126">
         <v>3</v>
       </c>
-      <c r="E20" s="146">
-        <v>0</v>
-      </c>
-      <c r="F20" s="146">
+      <c r="E20" s="126">
+        <v>0</v>
+      </c>
+      <c r="F20" s="126">
         <v>0</v>
       </c>
       <c r="G20" s="31">
@@ -3549,16 +3552,16 @@
       <c r="B21" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="146">
+      <c r="C21" s="126">
         <v>3</v>
       </c>
-      <c r="D21" s="146">
-        <v>0</v>
-      </c>
-      <c r="E21" s="146">
-        <v>0</v>
-      </c>
-      <c r="F21" s="146">
+      <c r="D21" s="126">
+        <v>0</v>
+      </c>
+      <c r="E21" s="126">
+        <v>0</v>
+      </c>
+      <c r="F21" s="126">
         <v>3</v>
       </c>
       <c r="G21" s="31">
@@ -3604,16 +3607,16 @@
       <c r="B22" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="146">
+      <c r="C22" s="126">
         <v>3</v>
       </c>
-      <c r="D22" s="146">
+      <c r="D22" s="126">
         <v>3</v>
       </c>
-      <c r="E22" s="146">
+      <c r="E22" s="126">
         <v>3</v>
       </c>
-      <c r="F22" s="146">
+      <c r="F22" s="126">
         <v>3</v>
       </c>
       <c r="G22" s="31">
@@ -3659,16 +3662,16 @@
       <c r="B23" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="146">
-        <v>0</v>
-      </c>
-      <c r="D23" s="146">
+      <c r="C23" s="126">
+        <v>0</v>
+      </c>
+      <c r="D23" s="126">
         <v>10</v>
       </c>
-      <c r="E23" s="146">
-        <v>0</v>
-      </c>
-      <c r="F23" s="146">
+      <c r="E23" s="126">
+        <v>0</v>
+      </c>
+      <c r="F23" s="126">
         <v>0</v>
       </c>
       <c r="G23" s="31">
@@ -3714,16 +3717,16 @@
       <c r="B24" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="146">
+      <c r="C24" s="126">
         <v>1</v>
       </c>
-      <c r="D24" s="146">
+      <c r="D24" s="126">
         <v>10</v>
       </c>
-      <c r="E24" s="146">
-        <v>2</v>
-      </c>
-      <c r="F24" s="146">
+      <c r="E24" s="126">
+        <v>2</v>
+      </c>
+      <c r="F24" s="126">
         <v>0</v>
       </c>
       <c r="G24" s="31">
@@ -3769,16 +3772,16 @@
       <c r="B25" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="146">
+      <c r="C25" s="126">
         <v>10</v>
       </c>
-      <c r="D25" s="146">
+      <c r="D25" s="126">
         <v>18</v>
       </c>
-      <c r="E25" s="146">
+      <c r="E25" s="126">
         <v>3.5</v>
       </c>
-      <c r="F25" s="146">
+      <c r="F25" s="126">
         <v>15</v>
       </c>
       <c r="G25" s="31">
@@ -3824,16 +3827,16 @@
       <c r="B26" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="147">
-        <v>2</v>
-      </c>
-      <c r="D26" s="147">
-        <v>2</v>
-      </c>
-      <c r="E26" s="147">
-        <v>2</v>
-      </c>
-      <c r="F26" s="147">
+      <c r="C26" s="127">
+        <v>2</v>
+      </c>
+      <c r="D26" s="127">
+        <v>2</v>
+      </c>
+      <c r="E26" s="127">
+        <v>2</v>
+      </c>
+      <c r="F26" s="127">
         <v>2</v>
       </c>
       <c r="G26" s="63">
@@ -3879,16 +3882,16 @@
       <c r="B27" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="146">
+      <c r="C27" s="126">
         <v>3</v>
       </c>
-      <c r="D27" s="146">
+      <c r="D27" s="126">
         <v>1</v>
       </c>
-      <c r="E27" s="146">
+      <c r="E27" s="126">
         <v>1</v>
       </c>
-      <c r="F27" s="146">
+      <c r="F27" s="126">
         <v>0</v>
       </c>
       <c r="G27" s="63">
@@ -3934,16 +3937,16 @@
       <c r="B28" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="145">
-        <v>2</v>
-      </c>
-      <c r="D28" s="145">
-        <v>0</v>
-      </c>
-      <c r="E28" s="145">
-        <v>0</v>
-      </c>
-      <c r="F28" s="145">
+      <c r="C28" s="125">
+        <v>2</v>
+      </c>
+      <c r="D28" s="125">
+        <v>0</v>
+      </c>
+      <c r="E28" s="125">
+        <v>0</v>
+      </c>
+      <c r="F28" s="125">
         <v>4</v>
       </c>
       <c r="G28" s="63">
@@ -3989,16 +3992,16 @@
       <c r="B29" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="146">
+      <c r="C29" s="126">
         <v>6</v>
       </c>
-      <c r="D29" s="146">
-        <v>0</v>
-      </c>
-      <c r="E29" s="146">
-        <v>0</v>
-      </c>
-      <c r="F29" s="146">
+      <c r="D29" s="126">
+        <v>0</v>
+      </c>
+      <c r="E29" s="126">
+        <v>0</v>
+      </c>
+      <c r="F29" s="126">
         <v>10</v>
       </c>
       <c r="G29" s="63">
@@ -4044,16 +4047,16 @@
       <c r="B30" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="147">
-        <v>0</v>
-      </c>
-      <c r="D30" s="147">
+      <c r="C30" s="127">
+        <v>0</v>
+      </c>
+      <c r="D30" s="127">
         <v>9</v>
       </c>
-      <c r="E30" s="147">
+      <c r="E30" s="127">
         <v>18.5</v>
       </c>
-      <c r="F30" s="147">
+      <c r="F30" s="127">
         <v>0</v>
       </c>
       <c r="G30" s="63">
@@ -4099,16 +4102,16 @@
       <c r="B31" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="146">
+      <c r="C31" s="126">
         <v>5</v>
       </c>
-      <c r="D31" s="146">
-        <v>0</v>
-      </c>
-      <c r="E31" s="146">
-        <v>0</v>
-      </c>
-      <c r="F31" s="146">
+      <c r="D31" s="126">
+        <v>0</v>
+      </c>
+      <c r="E31" s="126">
+        <v>0</v>
+      </c>
+      <c r="F31" s="126">
         <v>0</v>
       </c>
       <c r="G31" s="63">
@@ -4154,16 +4157,16 @@
       <c r="B32" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="146">
+      <c r="C32" s="126">
         <v>3</v>
       </c>
-      <c r="D32" s="146">
+      <c r="D32" s="126">
         <v>3</v>
       </c>
-      <c r="E32" s="146">
+      <c r="E32" s="126">
         <v>3</v>
       </c>
-      <c r="F32" s="146">
+      <c r="F32" s="126">
         <v>3</v>
       </c>
       <c r="G32" s="63">
@@ -4209,16 +4212,16 @@
       <c r="B33" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="145">
-        <v>0</v>
-      </c>
-      <c r="D33" s="145">
-        <v>0</v>
-      </c>
-      <c r="E33" s="145">
+      <c r="C33" s="125">
+        <v>0</v>
+      </c>
+      <c r="D33" s="125">
+        <v>0</v>
+      </c>
+      <c r="E33" s="125">
         <v>10</v>
       </c>
-      <c r="F33" s="145">
+      <c r="F33" s="125">
         <v>0</v>
       </c>
       <c r="G33" s="63">
@@ -4264,16 +4267,16 @@
       <c r="B34" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="146">
-        <v>0</v>
-      </c>
-      <c r="D34" s="146">
-        <v>0</v>
-      </c>
-      <c r="E34" s="146">
+      <c r="C34" s="126">
+        <v>0</v>
+      </c>
+      <c r="D34" s="126">
+        <v>0</v>
+      </c>
+      <c r="E34" s="126">
         <v>0.5</v>
       </c>
-      <c r="F34" s="146">
+      <c r="F34" s="126">
         <v>0</v>
       </c>
       <c r="G34" s="63">
@@ -4319,16 +4322,16 @@
       <c r="B35" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="146">
-        <v>0</v>
-      </c>
-      <c r="D35" s="146">
-        <v>0</v>
-      </c>
-      <c r="E35" s="146">
-        <v>0</v>
-      </c>
-      <c r="F35" s="146">
+      <c r="C35" s="126">
+        <v>0</v>
+      </c>
+      <c r="D35" s="126">
+        <v>0</v>
+      </c>
+      <c r="E35" s="126">
+        <v>0</v>
+      </c>
+      <c r="F35" s="126">
         <v>3</v>
       </c>
       <c r="G35" s="63">
@@ -4372,16 +4375,16 @@
       <c r="B36" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="146">
-        <v>2</v>
-      </c>
-      <c r="D36" s="146">
-        <v>0</v>
-      </c>
-      <c r="E36" s="146">
-        <v>0</v>
-      </c>
-      <c r="F36" s="146">
+      <c r="C36" s="126">
+        <v>2</v>
+      </c>
+      <c r="D36" s="126">
+        <v>0</v>
+      </c>
+      <c r="E36" s="126">
+        <v>0</v>
+      </c>
+      <c r="F36" s="126">
         <v>8</v>
       </c>
       <c r="G36" s="63">
@@ -4425,16 +4428,16 @@
       <c r="B37" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="146">
-        <v>0</v>
-      </c>
-      <c r="D37" s="146">
-        <v>0</v>
-      </c>
-      <c r="E37" s="146">
-        <v>0</v>
-      </c>
-      <c r="F37" s="146">
+      <c r="C37" s="126">
+        <v>0</v>
+      </c>
+      <c r="D37" s="126">
+        <v>0</v>
+      </c>
+      <c r="E37" s="126">
+        <v>0</v>
+      </c>
+      <c r="F37" s="126">
         <v>4</v>
       </c>
       <c r="G37" s="63">
@@ -4478,16 +4481,16 @@
       <c r="B38" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="146">
+      <c r="C38" s="126">
         <v>5</v>
       </c>
-      <c r="D38" s="146">
-        <v>0</v>
-      </c>
-      <c r="E38" s="146">
-        <v>0</v>
-      </c>
-      <c r="F38" s="146">
+      <c r="D38" s="126">
+        <v>0</v>
+      </c>
+      <c r="E38" s="126">
+        <v>0</v>
+      </c>
+      <c r="F38" s="126">
         <v>0</v>
       </c>
       <c r="G38" s="63">
@@ -4531,16 +4534,16 @@
       <c r="B39" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="146">
-        <v>0</v>
-      </c>
-      <c r="D39" s="146">
-        <v>0</v>
-      </c>
-      <c r="E39" s="146">
-        <v>0</v>
-      </c>
-      <c r="F39" s="146">
+      <c r="C39" s="126">
+        <v>0</v>
+      </c>
+      <c r="D39" s="126">
+        <v>0</v>
+      </c>
+      <c r="E39" s="126">
+        <v>0</v>
+      </c>
+      <c r="F39" s="126">
         <v>4</v>
       </c>
       <c r="G39" s="63">
@@ -4584,16 +4587,16 @@
       <c r="B40" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="146">
-        <v>0</v>
-      </c>
-      <c r="D40" s="146">
-        <v>0</v>
-      </c>
-      <c r="E40" s="146">
-        <v>0</v>
-      </c>
-      <c r="F40" s="146">
+      <c r="C40" s="126">
+        <v>0</v>
+      </c>
+      <c r="D40" s="126">
+        <v>0</v>
+      </c>
+      <c r="E40" s="126">
+        <v>0</v>
+      </c>
+      <c r="F40" s="126">
         <v>6</v>
       </c>
       <c r="G40" s="63">
@@ -4637,16 +4640,16 @@
       <c r="B41" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="146">
-        <v>2</v>
-      </c>
-      <c r="D41" s="146">
-        <v>2</v>
-      </c>
-      <c r="E41" s="146">
-        <v>2</v>
-      </c>
-      <c r="F41" s="146">
+      <c r="C41" s="126">
+        <v>2</v>
+      </c>
+      <c r="D41" s="126">
+        <v>2</v>
+      </c>
+      <c r="E41" s="126">
+        <v>2</v>
+      </c>
+      <c r="F41" s="126">
         <v>2</v>
       </c>
       <c r="G41" s="63">
@@ -4692,16 +4695,16 @@
       <c r="B42" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="146">
-        <v>0</v>
-      </c>
-      <c r="D42" s="146">
-        <v>0</v>
-      </c>
-      <c r="E42" s="146">
-        <v>0</v>
-      </c>
-      <c r="F42" s="146">
+      <c r="C42" s="126">
+        <v>0</v>
+      </c>
+      <c r="D42" s="126">
+        <v>0</v>
+      </c>
+      <c r="E42" s="126">
+        <v>0</v>
+      </c>
+      <c r="F42" s="126">
         <v>0</v>
       </c>
       <c r="G42" s="63">
@@ -4745,16 +4748,16 @@
       <c r="B43" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="146">
-        <v>0</v>
-      </c>
-      <c r="D43" s="146">
+      <c r="C43" s="126">
+        <v>0</v>
+      </c>
+      <c r="D43" s="126">
         <v>1</v>
       </c>
-      <c r="E43" s="146">
-        <v>0</v>
-      </c>
-      <c r="F43" s="146">
+      <c r="E43" s="126">
+        <v>0</v>
+      </c>
+      <c r="F43" s="126">
         <v>0</v>
       </c>
       <c r="G43" s="63">
@@ -4800,16 +4803,16 @@
       <c r="B44" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="146">
-        <v>0</v>
-      </c>
-      <c r="D44" s="146">
-        <v>0</v>
-      </c>
-      <c r="E44" s="146">
+      <c r="C44" s="126">
+        <v>0</v>
+      </c>
+      <c r="D44" s="126">
+        <v>0</v>
+      </c>
+      <c r="E44" s="126">
         <v>4</v>
       </c>
-      <c r="F44" s="146">
+      <c r="F44" s="126">
         <v>0</v>
       </c>
       <c r="G44" s="63">
@@ -4855,16 +4858,16 @@
       <c r="B45" s="62" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="146">
+      <c r="C45" s="126">
         <v>7</v>
       </c>
-      <c r="D45" s="146">
+      <c r="D45" s="126">
         <v>1</v>
       </c>
-      <c r="E45" s="146">
-        <v>0</v>
-      </c>
-      <c r="F45" s="146">
+      <c r="E45" s="126">
+        <v>0</v>
+      </c>
+      <c r="F45" s="126">
         <v>0</v>
       </c>
       <c r="G45" s="63">
@@ -4908,16 +4911,16 @@
       <c r="B46" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="146">
-        <v>0</v>
-      </c>
-      <c r="D46" s="146">
-        <v>0</v>
-      </c>
-      <c r="E46" s="146">
+      <c r="C46" s="126">
+        <v>0</v>
+      </c>
+      <c r="D46" s="126">
+        <v>0</v>
+      </c>
+      <c r="E46" s="126">
         <v>2.5</v>
       </c>
-      <c r="F46" s="146">
+      <c r="F46" s="126">
         <v>0</v>
       </c>
       <c r="G46" s="63">
@@ -4960,16 +4963,16 @@
       <c r="B47" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="146">
-        <v>2</v>
-      </c>
-      <c r="D47" s="146">
-        <v>0</v>
-      </c>
-      <c r="E47" s="146">
-        <v>0</v>
-      </c>
-      <c r="F47" s="146">
+      <c r="C47" s="126">
+        <v>2</v>
+      </c>
+      <c r="D47" s="126">
+        <v>0</v>
+      </c>
+      <c r="E47" s="126">
+        <v>0</v>
+      </c>
+      <c r="F47" s="126">
         <v>0</v>
       </c>
       <c r="G47" s="63">
@@ -5010,10 +5013,10 @@
       <c r="B48" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="145"/>
-      <c r="D48" s="145"/>
-      <c r="E48" s="145"/>
-      <c r="F48" s="145"/>
+      <c r="C48" s="125"/>
+      <c r="D48" s="125"/>
+      <c r="E48" s="125"/>
+      <c r="F48" s="125"/>
       <c r="G48" s="63"/>
       <c r="H48" s="79"/>
       <c r="I48" s="33"/>
@@ -5044,16 +5047,16 @@
       <c r="B49" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="146">
-        <v>0</v>
-      </c>
-      <c r="D49" s="146">
-        <v>0</v>
-      </c>
-      <c r="E49" s="146">
+      <c r="C49" s="126">
+        <v>0</v>
+      </c>
+      <c r="D49" s="126">
+        <v>0</v>
+      </c>
+      <c r="E49" s="126">
         <v>8.75</v>
       </c>
-      <c r="F49" s="146">
+      <c r="F49" s="126">
         <v>0</v>
       </c>
       <c r="G49" s="63">
@@ -5099,16 +5102,16 @@
       <c r="B50" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="146">
-        <v>0</v>
-      </c>
-      <c r="D50" s="146">
-        <v>0</v>
-      </c>
-      <c r="E50" s="146">
-        <v>0</v>
-      </c>
-      <c r="F50" s="146">
+      <c r="C50" s="126">
+        <v>0</v>
+      </c>
+      <c r="D50" s="126">
+        <v>0</v>
+      </c>
+      <c r="E50" s="126">
+        <v>0</v>
+      </c>
+      <c r="F50" s="126">
         <v>5</v>
       </c>
       <c r="G50" s="63">
@@ -5152,16 +5155,16 @@
       <c r="B51" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="C51" s="146">
+      <c r="C51" s="126">
         <v>7</v>
       </c>
-      <c r="D51" s="146">
-        <v>0</v>
-      </c>
-      <c r="E51" s="146">
-        <v>0</v>
-      </c>
-      <c r="F51" s="146">
+      <c r="D51" s="126">
+        <v>0</v>
+      </c>
+      <c r="E51" s="126">
+        <v>0</v>
+      </c>
+      <c r="F51" s="126">
         <v>0</v>
       </c>
       <c r="G51" s="63">
@@ -5202,16 +5205,16 @@
       <c r="B52" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="146">
+      <c r="C52" s="126">
         <v>3</v>
       </c>
-      <c r="D52" s="146">
+      <c r="D52" s="126">
         <v>5</v>
       </c>
-      <c r="E52" s="146">
-        <v>0</v>
-      </c>
-      <c r="F52" s="146">
+      <c r="E52" s="126">
+        <v>0</v>
+      </c>
+      <c r="F52" s="126">
         <v>0</v>
       </c>
       <c r="G52" s="63">
@@ -5254,16 +5257,16 @@
       <c r="B53" s="121" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="146">
+      <c r="C53" s="126">
         <v>8</v>
       </c>
-      <c r="D53" s="146">
-        <v>0</v>
-      </c>
-      <c r="E53" s="146">
-        <v>0</v>
-      </c>
-      <c r="F53" s="146">
+      <c r="D53" s="126">
+        <v>0</v>
+      </c>
+      <c r="E53" s="126">
+        <v>0</v>
+      </c>
+      <c r="F53" s="126">
         <v>0</v>
       </c>
       <c r="G53" s="63">
@@ -5306,16 +5309,16 @@
       <c r="B54" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="C54" s="146">
-        <v>0</v>
-      </c>
-      <c r="D54" s="146">
-        <v>0</v>
-      </c>
-      <c r="E54" s="146">
-        <v>0</v>
-      </c>
-      <c r="F54" s="146">
+      <c r="C54" s="126">
+        <v>0</v>
+      </c>
+      <c r="D54" s="126">
+        <v>0</v>
+      </c>
+      <c r="E54" s="126">
+        <v>0</v>
+      </c>
+      <c r="F54" s="126">
         <v>10</v>
       </c>
       <c r="G54" s="63">
@@ -5358,16 +5361,16 @@
       <c r="B55" s="62" t="s">
         <v>76</v>
       </c>
-      <c r="C55" s="146">
+      <c r="C55" s="126">
         <v>5</v>
       </c>
-      <c r="D55" s="146">
-        <v>0</v>
-      </c>
-      <c r="E55" s="146">
-        <v>0</v>
-      </c>
-      <c r="F55" s="146">
+      <c r="D55" s="126">
+        <v>0</v>
+      </c>
+      <c r="E55" s="126">
+        <v>0</v>
+      </c>
+      <c r="F55" s="126">
         <v>0</v>
       </c>
       <c r="G55" s="63">
@@ -5410,16 +5413,16 @@
       <c r="B56" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="C56" s="146">
-        <v>0</v>
-      </c>
-      <c r="D56" s="146">
-        <v>0</v>
-      </c>
-      <c r="E56" s="146">
-        <v>0</v>
-      </c>
-      <c r="F56" s="146">
+      <c r="C56" s="126">
+        <v>0</v>
+      </c>
+      <c r="D56" s="126">
+        <v>0</v>
+      </c>
+      <c r="E56" s="126">
+        <v>0</v>
+      </c>
+      <c r="F56" s="126">
         <v>8</v>
       </c>
       <c r="G56" s="63">
@@ -5462,16 +5465,16 @@
       <c r="B57" s="113" t="s">
         <v>81</v>
       </c>
-      <c r="C57" s="146">
-        <v>0</v>
-      </c>
-      <c r="D57" s="146">
-        <v>0</v>
-      </c>
-      <c r="E57" s="146">
+      <c r="C57" s="126">
+        <v>0</v>
+      </c>
+      <c r="D57" s="126">
+        <v>0</v>
+      </c>
+      <c r="E57" s="126">
         <v>11.5</v>
       </c>
-      <c r="F57" s="146">
+      <c r="F57" s="126">
         <v>0</v>
       </c>
       <c r="G57" s="63">
@@ -5514,16 +5517,16 @@
       <c r="B58" s="113" t="s">
         <v>82</v>
       </c>
-      <c r="C58" s="146">
-        <v>0</v>
-      </c>
-      <c r="D58" s="146">
-        <v>0</v>
-      </c>
-      <c r="E58" s="146">
+      <c r="C58" s="126">
+        <v>0</v>
+      </c>
+      <c r="D58" s="126">
+        <v>0</v>
+      </c>
+      <c r="E58" s="126">
         <v>0.75</v>
       </c>
-      <c r="F58" s="146">
+      <c r="F58" s="126">
         <v>0</v>
       </c>
       <c r="G58" s="63">
@@ -5566,16 +5569,16 @@
       <c r="B59" s="113" t="s">
         <v>77</v>
       </c>
-      <c r="C59" s="146">
-        <v>0</v>
-      </c>
-      <c r="D59" s="146">
-        <v>0</v>
-      </c>
-      <c r="E59" s="146">
+      <c r="C59" s="126">
+        <v>0</v>
+      </c>
+      <c r="D59" s="126">
+        <v>0</v>
+      </c>
+      <c r="E59" s="126">
         <v>4</v>
       </c>
-      <c r="F59" s="146">
+      <c r="F59" s="126">
         <v>0</v>
       </c>
       <c r="G59" s="63">
@@ -5618,16 +5621,16 @@
       <c r="B60" s="113" t="s">
         <v>83</v>
       </c>
-      <c r="C60" s="146">
-        <v>0</v>
-      </c>
-      <c r="D60" s="146">
-        <v>0</v>
-      </c>
-      <c r="E60" s="146">
+      <c r="C60" s="126">
+        <v>0</v>
+      </c>
+      <c r="D60" s="126">
+        <v>0</v>
+      </c>
+      <c r="E60" s="126">
         <v>0.25</v>
       </c>
-      <c r="F60" s="146">
+      <c r="F60" s="126">
         <v>0</v>
       </c>
       <c r="G60" s="63">
@@ -5670,16 +5673,16 @@
       <c r="B61" s="113" t="s">
         <v>87</v>
       </c>
-      <c r="C61" s="146">
-        <v>0</v>
-      </c>
-      <c r="D61" s="146">
-        <v>0</v>
-      </c>
-      <c r="E61" s="146">
+      <c r="C61" s="126">
+        <v>0</v>
+      </c>
+      <c r="D61" s="126">
+        <v>0</v>
+      </c>
+      <c r="E61" s="126">
         <v>2.75</v>
       </c>
-      <c r="F61" s="146">
+      <c r="F61" s="126">
         <v>0</v>
       </c>
       <c r="G61" s="63">
@@ -5722,16 +5725,16 @@
       <c r="B62" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="C62" s="146">
+      <c r="C62" s="126">
         <v>8</v>
       </c>
-      <c r="D62" s="146">
-        <v>0</v>
-      </c>
-      <c r="E62" s="146">
-        <v>0</v>
-      </c>
-      <c r="F62" s="146">
+      <c r="D62" s="126">
+        <v>0</v>
+      </c>
+      <c r="E62" s="126">
+        <v>0</v>
+      </c>
+      <c r="F62" s="126">
         <v>0</v>
       </c>
       <c r="G62" s="63">
@@ -5774,16 +5777,16 @@
       <c r="B63" s="62" t="s">
         <v>80</v>
       </c>
-      <c r="C63" s="146">
-        <v>2</v>
-      </c>
-      <c r="D63" s="146">
-        <v>0</v>
-      </c>
-      <c r="E63" s="146">
-        <v>0</v>
-      </c>
-      <c r="F63" s="146">
+      <c r="C63" s="126">
+        <v>2</v>
+      </c>
+      <c r="D63" s="126">
+        <v>0</v>
+      </c>
+      <c r="E63" s="126">
+        <v>0</v>
+      </c>
+      <c r="F63" s="126">
         <v>5</v>
       </c>
       <c r="G63" s="63">
@@ -5826,16 +5829,16 @@
       <c r="B64" s="118" t="s">
         <v>85</v>
       </c>
-      <c r="C64" s="146">
-        <v>0</v>
-      </c>
-      <c r="D64" s="146">
-        <v>0</v>
-      </c>
-      <c r="E64" s="146">
-        <v>0</v>
-      </c>
-      <c r="F64" s="146">
+      <c r="C64" s="126">
+        <v>0</v>
+      </c>
+      <c r="D64" s="126">
+        <v>0</v>
+      </c>
+      <c r="E64" s="126">
+        <v>0</v>
+      </c>
+      <c r="F64" s="126">
         <v>0</v>
       </c>
       <c r="G64" s="63"/>
@@ -5873,16 +5876,16 @@
       <c r="B65" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="C65" s="146">
+      <c r="C65" s="126">
         <v>1.5</v>
       </c>
-      <c r="D65" s="146">
+      <c r="D65" s="126">
         <v>0.5</v>
       </c>
-      <c r="E65" s="146">
+      <c r="E65" s="126">
         <v>1.5</v>
       </c>
-      <c r="F65" s="146">
+      <c r="F65" s="126">
         <v>0</v>
       </c>
       <c r="G65" s="63"/>
@@ -5922,16 +5925,16 @@
       <c r="B66" s="69" t="s">
         <v>86</v>
       </c>
-      <c r="C66" s="146">
-        <v>0</v>
-      </c>
-      <c r="D66" s="146">
+      <c r="C66" s="126">
+        <v>0</v>
+      </c>
+      <c r="D66" s="126">
         <v>1</v>
       </c>
-      <c r="E66" s="146">
-        <v>0</v>
-      </c>
-      <c r="F66" s="146">
+      <c r="E66" s="126">
+        <v>0</v>
+      </c>
+      <c r="F66" s="126">
         <v>0</v>
       </c>
       <c r="G66" s="63"/>
@@ -5969,10 +5972,10 @@
       <c r="B67" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="C67" s="146"/>
-      <c r="D67" s="146"/>
-      <c r="E67" s="146"/>
-      <c r="F67" s="146"/>
+      <c r="C67" s="126"/>
+      <c r="D67" s="126"/>
+      <c r="E67" s="126"/>
+      <c r="F67" s="126"/>
       <c r="G67" s="63"/>
       <c r="H67" s="32"/>
       <c r="I67" s="33"/>
@@ -6003,16 +6006,16 @@
       <c r="B68" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="C68" s="146">
+      <c r="C68" s="126">
         <v>3</v>
       </c>
-      <c r="D68" s="146">
+      <c r="D68" s="126">
         <v>3</v>
       </c>
-      <c r="E68" s="146">
+      <c r="E68" s="126">
         <v>3</v>
       </c>
-      <c r="F68" s="146">
+      <c r="F68" s="126">
         <v>3</v>
       </c>
       <c r="G68" s="63">
@@ -6055,16 +6058,16 @@
       <c r="B69" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="C69" s="146">
-        <v>0</v>
-      </c>
-      <c r="D69" s="146">
+      <c r="C69" s="126">
+        <v>0</v>
+      </c>
+      <c r="D69" s="126">
         <v>7</v>
       </c>
-      <c r="E69" s="146">
-        <v>0</v>
-      </c>
-      <c r="F69" s="146">
+      <c r="E69" s="126">
+        <v>0</v>
+      </c>
+      <c r="F69" s="126">
         <v>0</v>
       </c>
       <c r="G69" s="63">
@@ -6107,16 +6110,16 @@
       <c r="B70" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="C70" s="146">
-        <v>0</v>
-      </c>
-      <c r="D70" s="146">
-        <v>0</v>
-      </c>
-      <c r="E70" s="146">
+      <c r="C70" s="126">
+        <v>0</v>
+      </c>
+      <c r="D70" s="126">
+        <v>0</v>
+      </c>
+      <c r="E70" s="126">
         <v>0.75</v>
       </c>
-      <c r="F70" s="146">
+      <c r="F70" s="126">
         <v>0</v>
       </c>
       <c r="G70" s="63">
@@ -6159,16 +6162,16 @@
       <c r="B71" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="C71" s="146">
-        <v>0</v>
-      </c>
-      <c r="D71" s="146">
-        <v>0</v>
-      </c>
-      <c r="E71" s="146">
+      <c r="C71" s="126">
+        <v>0</v>
+      </c>
+      <c r="D71" s="126">
+        <v>0</v>
+      </c>
+      <c r="E71" s="126">
         <v>1.25</v>
       </c>
-      <c r="F71" s="146">
+      <c r="F71" s="126">
         <v>0</v>
       </c>
       <c r="G71" s="63">
@@ -6211,16 +6214,16 @@
       <c r="B72" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="C72" s="146">
-        <v>0</v>
-      </c>
-      <c r="D72" s="146">
-        <v>0</v>
-      </c>
-      <c r="E72" s="146">
+      <c r="C72" s="126">
+        <v>0</v>
+      </c>
+      <c r="D72" s="126">
+        <v>0</v>
+      </c>
+      <c r="E72" s="126">
         <v>1</v>
       </c>
-      <c r="F72" s="146">
+      <c r="F72" s="126">
         <v>0</v>
       </c>
       <c r="G72" s="63">
@@ -6263,16 +6266,16 @@
       <c r="B73" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="C73" s="146">
-        <v>0</v>
-      </c>
-      <c r="D73" s="146">
-        <v>0</v>
-      </c>
-      <c r="E73" s="146">
-        <v>2</v>
-      </c>
-      <c r="F73" s="146">
+      <c r="C73" s="126">
+        <v>0</v>
+      </c>
+      <c r="D73" s="126">
+        <v>0</v>
+      </c>
+      <c r="E73" s="126">
+        <v>2</v>
+      </c>
+      <c r="F73" s="126">
         <v>0</v>
       </c>
       <c r="G73" s="63">
@@ -6315,16 +6318,16 @@
       <c r="B74" s="57" t="s">
         <v>97</v>
       </c>
-      <c r="C74" s="146">
-        <v>2</v>
-      </c>
-      <c r="D74" s="146">
-        <v>0</v>
-      </c>
-      <c r="E74" s="146">
-        <v>0</v>
-      </c>
-      <c r="F74" s="146">
+      <c r="C74" s="126">
+        <v>2</v>
+      </c>
+      <c r="D74" s="126">
+        <v>0</v>
+      </c>
+      <c r="E74" s="126">
+        <v>0</v>
+      </c>
+      <c r="F74" s="126">
         <v>1</v>
       </c>
       <c r="G74" s="63">
@@ -6367,16 +6370,16 @@
       <c r="B75" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="C75" s="146">
+      <c r="C75" s="126">
         <v>4</v>
       </c>
-      <c r="D75" s="146">
-        <v>0</v>
-      </c>
-      <c r="E75" s="146">
-        <v>0</v>
-      </c>
-      <c r="F75" s="146">
+      <c r="D75" s="126">
+        <v>0</v>
+      </c>
+      <c r="E75" s="126">
+        <v>0</v>
+      </c>
+      <c r="F75" s="126">
         <v>0</v>
       </c>
       <c r="G75" s="63">
@@ -6419,16 +6422,16 @@
       <c r="B76" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="C76" s="146">
-        <v>2</v>
-      </c>
-      <c r="D76" s="146">
-        <v>0</v>
-      </c>
-      <c r="E76" s="146">
-        <v>0</v>
-      </c>
-      <c r="F76" s="146">
+      <c r="C76" s="126">
+        <v>2</v>
+      </c>
+      <c r="D76" s="126">
+        <v>0</v>
+      </c>
+      <c r="E76" s="126">
+        <v>0</v>
+      </c>
+      <c r="F76" s="126">
         <v>0</v>
       </c>
       <c r="G76" s="63">
@@ -6471,16 +6474,16 @@
       <c r="B77" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="C77" s="146">
-        <v>2</v>
-      </c>
-      <c r="D77" s="146">
-        <v>0</v>
-      </c>
-      <c r="E77" s="146">
-        <v>0</v>
-      </c>
-      <c r="F77" s="146">
+      <c r="C77" s="126">
+        <v>2</v>
+      </c>
+      <c r="D77" s="126">
+        <v>0</v>
+      </c>
+      <c r="E77" s="126">
+        <v>0</v>
+      </c>
+      <c r="F77" s="126">
         <v>0</v>
       </c>
       <c r="G77" s="63">
@@ -6523,16 +6526,16 @@
       <c r="B78" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="C78" s="146">
-        <v>2</v>
-      </c>
-      <c r="D78" s="146">
-        <v>0</v>
-      </c>
-      <c r="E78" s="146">
-        <v>0</v>
-      </c>
-      <c r="F78" s="146">
+      <c r="C78" s="126">
+        <v>2</v>
+      </c>
+      <c r="D78" s="126">
+        <v>0</v>
+      </c>
+      <c r="E78" s="126">
+        <v>0</v>
+      </c>
+      <c r="F78" s="126">
         <v>0</v>
       </c>
       <c r="G78" s="63">
@@ -6575,16 +6578,16 @@
       <c r="B79" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="C79" s="146">
-        <v>2</v>
-      </c>
-      <c r="D79" s="146">
-        <v>0</v>
-      </c>
-      <c r="E79" s="146">
-        <v>0</v>
-      </c>
-      <c r="F79" s="146">
+      <c r="C79" s="126">
+        <v>2</v>
+      </c>
+      <c r="D79" s="126">
+        <v>0</v>
+      </c>
+      <c r="E79" s="126">
+        <v>0</v>
+      </c>
+      <c r="F79" s="126">
         <v>2</v>
       </c>
       <c r="G79" s="63">
@@ -6627,16 +6630,16 @@
       <c r="B80" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="C80" s="146">
+      <c r="C80" s="126">
         <v>0.5</v>
       </c>
-      <c r="D80" s="146">
-        <v>0</v>
-      </c>
-      <c r="E80" s="146">
-        <v>0</v>
-      </c>
-      <c r="F80" s="146">
+      <c r="D80" s="126">
+        <v>0</v>
+      </c>
+      <c r="E80" s="126">
+        <v>0</v>
+      </c>
+      <c r="F80" s="126">
         <v>0</v>
       </c>
       <c r="G80" s="63">
@@ -6679,16 +6682,16 @@
       <c r="B81" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="C81" s="146">
-        <v>2</v>
-      </c>
-      <c r="D81" s="146">
-        <v>0</v>
-      </c>
-      <c r="E81" s="146">
-        <v>0</v>
-      </c>
-      <c r="F81" s="146">
+      <c r="C81" s="126">
+        <v>2</v>
+      </c>
+      <c r="D81" s="126">
+        <v>0</v>
+      </c>
+      <c r="E81" s="126">
+        <v>0</v>
+      </c>
+      <c r="F81" s="126">
         <v>0</v>
       </c>
       <c r="G81" s="63">
@@ -6731,16 +6734,16 @@
       <c r="B82" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="C82" s="146">
-        <v>0</v>
-      </c>
-      <c r="D82" s="146">
-        <v>0</v>
-      </c>
-      <c r="E82" s="146">
+      <c r="C82" s="126">
+        <v>0</v>
+      </c>
+      <c r="D82" s="126">
+        <v>0</v>
+      </c>
+      <c r="E82" s="126">
         <v>3.25</v>
       </c>
-      <c r="F82" s="146">
+      <c r="F82" s="126">
         <v>0</v>
       </c>
       <c r="G82" s="63">
@@ -6783,16 +6786,16 @@
       <c r="B83" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="C83" s="146">
-        <v>0</v>
-      </c>
-      <c r="D83" s="146">
-        <v>2</v>
-      </c>
-      <c r="E83" s="146">
-        <v>0</v>
-      </c>
-      <c r="F83" s="146">
+      <c r="C83" s="126">
+        <v>0</v>
+      </c>
+      <c r="D83" s="126">
+        <v>2</v>
+      </c>
+      <c r="E83" s="126">
+        <v>0</v>
+      </c>
+      <c r="F83" s="126">
         <v>0</v>
       </c>
       <c r="G83" s="63">
@@ -6835,16 +6838,16 @@
       <c r="B84" s="57" t="s">
         <v>110</v>
       </c>
-      <c r="C84" s="146">
-        <v>0</v>
-      </c>
-      <c r="D84" s="146">
-        <v>0</v>
-      </c>
-      <c r="E84" s="146">
+      <c r="C84" s="126">
+        <v>0</v>
+      </c>
+      <c r="D84" s="126">
+        <v>0</v>
+      </c>
+      <c r="E84" s="126">
         <v>1</v>
       </c>
-      <c r="F84" s="146">
+      <c r="F84" s="126">
         <v>0</v>
       </c>
       <c r="G84" s="63">
@@ -6881,21 +6884,35 @@
       <c r="AB84" s="41"/>
     </row>
     <row r="85" spans="1:28" s="77" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="29"/>
-      <c r="B85" s="57"/>
-      <c r="C85" s="146"/>
-      <c r="D85" s="146"/>
-      <c r="E85" s="146"/>
-      <c r="F85" s="146"/>
-      <c r="G85" s="63" t="e">
+      <c r="A85" s="29">
+        <v>19</v>
+      </c>
+      <c r="B85" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="C85" s="126">
+        <v>0</v>
+      </c>
+      <c r="D85" s="126">
+        <v>0</v>
+      </c>
+      <c r="E85" s="126">
+        <v>1.5</v>
+      </c>
+      <c r="F85" s="126">
+        <v>0</v>
+      </c>
+      <c r="G85" s="63">
         <f>VLOOKUP(H85,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H85" s="32"/>
+        <v>100</v>
+      </c>
+      <c r="H85" s="32" t="s">
+        <v>5</v>
+      </c>
       <c r="I85" s="33"/>
       <c r="J85" s="33">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="K85" s="35"/>
       <c r="L85" s="35"/>
@@ -6911,7 +6928,7 @@
       <c r="V85" s="36"/>
       <c r="W85" s="35"/>
       <c r="X85" s="120"/>
-      <c r="Y85" s="35"/>
+      <c r="Y85" s="122"/>
       <c r="Z85" s="36"/>
       <c r="AA85" s="37"/>
       <c r="AB85" s="41"/>
@@ -6919,10 +6936,10 @@
     <row r="86" spans="1:28" s="77" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="29"/>
       <c r="B86" s="57"/>
-      <c r="C86" s="146"/>
-      <c r="D86" s="146"/>
-      <c r="E86" s="146"/>
-      <c r="F86" s="146"/>
+      <c r="C86" s="126"/>
+      <c r="D86" s="126"/>
+      <c r="E86" s="126"/>
+      <c r="F86" s="126"/>
       <c r="G86" s="63" t="e">
         <f>VLOOKUP(H86,Feuil2!$A$1:$B$3,2,0)</f>
         <v>#N/A</v>
@@ -6955,10 +6972,10 @@
     <row r="87" spans="1:28" s="77" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="29"/>
       <c r="B87" s="57"/>
-      <c r="C87" s="146"/>
-      <c r="D87" s="146"/>
-      <c r="E87" s="146"/>
-      <c r="F87" s="146"/>
+      <c r="C87" s="126"/>
+      <c r="D87" s="126"/>
+      <c r="E87" s="126"/>
+      <c r="F87" s="126"/>
       <c r="G87" s="63" t="e">
         <f>VLOOKUP(H87,Feuil2!$A$1:$B$3,2,0)</f>
         <v>#N/A</v>
@@ -6995,16 +7012,16 @@
       <c r="B88" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="C88" s="146">
-        <v>0</v>
-      </c>
-      <c r="D88" s="146">
-        <v>0</v>
-      </c>
-      <c r="E88" s="146">
+      <c r="C88" s="126">
+        <v>0</v>
+      </c>
+      <c r="D88" s="126">
+        <v>0</v>
+      </c>
+      <c r="E88" s="126">
         <v>0.75</v>
       </c>
-      <c r="F88" s="146">
+      <c r="F88" s="126">
         <v>0</v>
       </c>
       <c r="G88" s="63">
@@ -7043,10 +7060,10 @@
     <row r="89" spans="1:28" s="77" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="29"/>
       <c r="B89" s="57"/>
-      <c r="C89" s="146"/>
-      <c r="D89" s="146"/>
-      <c r="E89" s="146"/>
-      <c r="F89" s="146"/>
+      <c r="C89" s="126"/>
+      <c r="D89" s="126"/>
+      <c r="E89" s="126"/>
+      <c r="F89" s="126"/>
       <c r="G89" s="63"/>
       <c r="H89" s="32"/>
       <c r="I89" s="33"/>
@@ -7071,23 +7088,23 @@
       <c r="AB89" s="41"/>
     </row>
     <row r="90" spans="1:28" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="128" t="s">
+      <c r="A90" s="150" t="s">
         <v>68</v>
       </c>
-      <c r="B90" s="128"/>
-      <c r="C90" s="144">
+      <c r="B90" s="150"/>
+      <c r="C90" s="124">
         <f>SUM(C10:C89)</f>
         <v>130.5</v>
       </c>
-      <c r="D90" s="144">
+      <c r="D90" s="124">
         <f>SUM(D10:D89)</f>
         <v>102.5</v>
       </c>
-      <c r="E90" s="144">
+      <c r="E90" s="124">
         <f>SUM(E10:E89)</f>
-        <v>105.5</v>
-      </c>
-      <c r="F90" s="144">
+        <v>107</v>
+      </c>
+      <c r="F90" s="124">
         <f>SUM(F10:F89)</f>
         <v>114</v>
       </c>
@@ -7096,7 +7113,7 @@
       <c r="I90" s="88"/>
       <c r="J90" s="86">
         <f>SUM(C90:F90)</f>
-        <v>452.5</v>
+        <v>454</v>
       </c>
       <c r="K90" s="89"/>
       <c r="L90" s="89"/>
@@ -7121,23 +7138,23 @@
       <c r="AB90" s="115"/>
     </row>
     <row r="91" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="123" t="s">
+      <c r="A91" s="145" t="s">
         <v>69</v>
       </c>
-      <c r="B91" s="123"/>
-      <c r="C91" s="144">
+      <c r="B91" s="145"/>
+      <c r="C91" s="124">
         <f>117-C90</f>
         <v>-13.5</v>
       </c>
-      <c r="D91" s="144">
+      <c r="D91" s="124">
         <f>117-D90</f>
         <v>14.5</v>
       </c>
-      <c r="E91" s="144">
+      <c r="E91" s="124">
         <f>117-E90</f>
-        <v>11.5</v>
-      </c>
-      <c r="F91" s="144">
+        <v>10</v>
+      </c>
+      <c r="F91" s="124">
         <f>117-F90</f>
         <v>3</v>
       </c>
@@ -7146,7 +7163,7 @@
       <c r="I91" s="86"/>
       <c r="J91" s="86">
         <f>SUM(C91:F91)</f>
-        <v>15.5</v>
+        <v>14</v>
       </c>
       <c r="K91" s="89"/>
       <c r="L91" s="89"/>
@@ -7168,14 +7185,14 @@
       <c r="AB91" s="89"/>
     </row>
     <row r="92" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="124" t="s">
+      <c r="A92" s="146" t="s">
         <v>70</v>
       </c>
-      <c r="B92" s="124"/>
-      <c r="C92" s="144"/>
-      <c r="D92" s="144"/>
-      <c r="E92" s="144"/>
-      <c r="F92" s="144"/>
+      <c r="B92" s="146"/>
+      <c r="C92" s="124"/>
+      <c r="D92" s="124"/>
+      <c r="E92" s="124"/>
+      <c r="F92" s="124"/>
       <c r="G92" s="86"/>
       <c r="H92" s="86"/>
       <c r="I92" s="86"/>
@@ -7203,14 +7220,14 @@
       <c r="AB92" s="89"/>
     </row>
     <row r="93" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="123" t="s">
+      <c r="A93" s="145" t="s">
         <v>71</v>
       </c>
-      <c r="B93" s="123"/>
-      <c r="C93" s="144"/>
-      <c r="D93" s="144"/>
-      <c r="E93" s="148"/>
-      <c r="F93" s="144"/>
+      <c r="B93" s="145"/>
+      <c r="C93" s="124"/>
+      <c r="D93" s="124"/>
+      <c r="E93" s="128"/>
+      <c r="F93" s="124"/>
       <c r="G93" s="86"/>
       <c r="H93" s="86"/>
       <c r="I93" s="90">
@@ -7219,7 +7236,7 @@
       </c>
       <c r="J93" s="86">
         <f>SUM(J10:J89)</f>
-        <v>452.5</v>
+        <v>454</v>
       </c>
       <c r="K93" s="89"/>
       <c r="L93" s="89"/>
@@ -7243,12 +7260,12 @@
     <row r="94" spans="1:28" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="91"/>
       <c r="B94" s="91"/>
-      <c r="D94" s="129" t="s">
+      <c r="D94" s="151" t="s">
         <v>88</v>
       </c>
-      <c r="E94" s="129"/>
-      <c r="F94" s="129"/>
-      <c r="G94" s="129"/>
+      <c r="E94" s="151"/>
+      <c r="F94" s="151"/>
+      <c r="G94" s="151"/>
       <c r="H94" s="92"/>
       <c r="I94" s="92"/>
       <c r="J94" s="92"/>
@@ -7272,15 +7289,15 @@
       <c r="AB94" s="89"/>
     </row>
     <row r="95" spans="1:28" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="124" t="s">
+      <c r="A95" s="146" t="s">
         <v>72</v>
       </c>
-      <c r="B95" s="124"/>
-      <c r="C95" s="149">
+      <c r="B95" s="146"/>
+      <c r="C95" s="129">
         <f>135*4</f>
         <v>540</v>
       </c>
-      <c r="D95" s="150">
+      <c r="D95" s="130">
         <v>468</v>
       </c>
       <c r="G95" s="92"/>
@@ -7307,15 +7324,15 @@
       <c r="AB95" s="89"/>
     </row>
     <row r="96" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="125" t="s">
+      <c r="A96" s="147" t="s">
         <v>73</v>
       </c>
-      <c r="B96" s="125"/>
-      <c r="C96" s="149">
+      <c r="B96" s="147"/>
+      <c r="C96" s="129">
         <f>C95-J93</f>
-        <v>87.5</v>
-      </c>
-      <c r="D96" s="151">
+        <v>86</v>
+      </c>
+      <c r="D96" s="131">
         <v>66</v>
       </c>
       <c r="G96" s="92"/>
@@ -7352,10 +7369,10 @@
     </row>
     <row r="99" spans="1:27" s="97" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A99" s="96"/>
-      <c r="C99" s="142"/>
-      <c r="D99" s="142"/>
-      <c r="E99" s="142"/>
-      <c r="F99" s="142"/>
+      <c r="C99" s="123"/>
+      <c r="D99" s="123"/>
+      <c r="E99" s="123"/>
+      <c r="F99" s="123"/>
       <c r="H99" s="98"/>
       <c r="I99" s="99"/>
       <c r="J99" s="99"/>
@@ -7366,10 +7383,10 @@
       <c r="AA99" s="101"/>
     </row>
     <row r="100" spans="1:27" s="97" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="C100" s="142"/>
-      <c r="D100" s="142"/>
-      <c r="E100" s="142"/>
-      <c r="F100" s="142"/>
+      <c r="C100" s="123"/>
+      <c r="D100" s="123"/>
+      <c r="E100" s="123"/>
+      <c r="F100" s="123"/>
       <c r="H100" s="98"/>
       <c r="I100" s="99"/>
       <c r="J100" s="99"/>
@@ -7380,10 +7397,10 @@
       <c r="AA100" s="101"/>
     </row>
     <row r="101" spans="1:27" s="97" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="C101" s="142"/>
-      <c r="D101" s="142"/>
-      <c r="E101" s="142"/>
-      <c r="F101" s="142"/>
+      <c r="C101" s="123"/>
+      <c r="D101" s="123"/>
+      <c r="E101" s="123"/>
+      <c r="F101" s="123"/>
       <c r="H101" s="98"/>
       <c r="I101" s="99"/>
       <c r="J101" s="99"/>
@@ -7395,11 +7412,15 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="D94:G94"/>
     <mergeCell ref="S6:V6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
@@ -7410,15 +7431,11 @@
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:Z7"/>
     <mergeCell ref="W6:Z6"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="D94:G94"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K6:R6"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
     <cfRule type="containsText" dxfId="62" priority="75" operator="containsText" text="En cours">

</xml_diff>

<commit_message>
Partially fixed issue #53
</commit_message>
<xml_diff>
--- a/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
+++ b/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alxbo\Source\Repos\mrjrdg\marque-sans-nom\Semainiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60D8539-197D-46C7-B069-7834C34A2D37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D90BED-93DF-46D7-A3AF-A23DEA5527D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="113">
   <si>
     <t>UQÀM - Hiver 2020</t>
   </si>
@@ -436,6 +436,9 @@
   </si>
   <si>
     <t>Afficher les avatars (event-view, profile-edit, navbar)</t>
+  </si>
+  <si>
+    <t>Améliorer le visuel (profile-view)</t>
   </si>
 </sst>
 </file>
@@ -1543,6 +1546,43 @@
     <xf numFmtId="164" fontId="18" fillId="0" borderId="33" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="34" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="35" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1561,43 +1601,6 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="12" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -2596,10 +2599,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AMK101"/>
+  <dimension ref="A1:AMK106"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2627,22 +2630,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="6" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="150" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="150"/>
+      <c r="A1" s="132" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="132"/>
       <c r="C1" s="123"/>
-      <c r="D1" s="151" t="s">
+      <c r="D1" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
-      <c r="G1" s="151"/>
-      <c r="H1" s="151"/>
-      <c r="I1" s="151"/>
-      <c r="J1" s="151"/>
-      <c r="K1" s="151"/>
-      <c r="L1" s="151"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
+      <c r="J1" s="133"/>
+      <c r="K1" s="133"/>
+      <c r="L1" s="133"/>
       <c r="N1" s="2"/>
       <c r="P1" s="7"/>
       <c r="Q1" s="6" t="s">
@@ -2654,20 +2657,20 @@
       <c r="AA1" s="8"/>
     </row>
     <row r="2" spans="1:28" s="6" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="150"/>
+      <c r="B2" s="132"/>
       <c r="C2" s="123"/>
       <c r="D2" s="123"/>
       <c r="E2" s="123"/>
-      <c r="F2" s="150" t="s">
+      <c r="F2" s="132" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="150"/>
-      <c r="H2" s="150"/>
-      <c r="I2" s="150"/>
-      <c r="J2" s="150"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="132"/>
+      <c r="J2" s="132"/>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
       <c r="N2" s="2"/>
@@ -2750,83 +2753,83 @@
       <c r="H6" s="2"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="139" t="s">
+      <c r="K6" s="134" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="139"/>
-      <c r="M6" s="139"/>
-      <c r="N6" s="139"/>
-      <c r="O6" s="139"/>
-      <c r="P6" s="139"/>
-      <c r="Q6" s="139"/>
-      <c r="R6" s="139"/>
-      <c r="S6" s="139" t="s">
+      <c r="L6" s="134"/>
+      <c r="M6" s="134"/>
+      <c r="N6" s="134"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="134"/>
+      <c r="Q6" s="134"/>
+      <c r="R6" s="134"/>
+      <c r="S6" s="134" t="s">
         <v>10</v>
       </c>
-      <c r="T6" s="139"/>
-      <c r="U6" s="139"/>
-      <c r="V6" s="139"/>
-      <c r="W6" s="147" t="s">
+      <c r="T6" s="134"/>
+      <c r="U6" s="134"/>
+      <c r="V6" s="134"/>
+      <c r="W6" s="142" t="s">
         <v>93</v>
       </c>
-      <c r="X6" s="148"/>
-      <c r="Y6" s="148"/>
-      <c r="Z6" s="149"/>
+      <c r="X6" s="143"/>
+      <c r="Y6" s="143"/>
+      <c r="Z6" s="144"/>
       <c r="AA6" s="8"/>
     </row>
     <row r="7" spans="1:28" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="140" t="s">
+      <c r="A7" s="135" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="141" t="s">
+      <c r="B7" s="136" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="142" t="s">
+      <c r="C7" s="137" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="142"/>
-      <c r="E7" s="142"/>
-      <c r="F7" s="142"/>
-      <c r="G7" s="143" t="s">
+      <c r="D7" s="137"/>
+      <c r="E7" s="137"/>
+      <c r="F7" s="137"/>
+      <c r="G7" s="138" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="144" t="s">
+      <c r="H7" s="139" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="145" t="s">
+      <c r="I7" s="140" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="145" t="s">
+      <c r="J7" s="140" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="146" t="s">
+      <c r="K7" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="146"/>
-      <c r="M7" s="146"/>
-      <c r="N7" s="146"/>
-      <c r="O7" s="146"/>
-      <c r="P7" s="146"/>
-      <c r="Q7" s="146"/>
-      <c r="R7" s="146"/>
-      <c r="S7" s="146"/>
-      <c r="T7" s="146"/>
-      <c r="U7" s="146"/>
-      <c r="V7" s="146"/>
-      <c r="W7" s="146"/>
-      <c r="X7" s="146"/>
-      <c r="Y7" s="146"/>
-      <c r="Z7" s="146"/>
-      <c r="AA7" s="135" t="s">
+      <c r="L7" s="141"/>
+      <c r="M7" s="141"/>
+      <c r="N7" s="141"/>
+      <c r="O7" s="141"/>
+      <c r="P7" s="141"/>
+      <c r="Q7" s="141"/>
+      <c r="R7" s="141"/>
+      <c r="S7" s="141"/>
+      <c r="T7" s="141"/>
+      <c r="U7" s="141"/>
+      <c r="V7" s="141"/>
+      <c r="W7" s="141"/>
+      <c r="X7" s="141"/>
+      <c r="Y7" s="141"/>
+      <c r="Z7" s="141"/>
+      <c r="AA7" s="148" t="s">
         <v>19</v>
       </c>
-      <c r="AB7" s="136" t="s">
+      <c r="AB7" s="149" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="140"/>
-      <c r="B8" s="141"/>
+      <c r="A8" s="135"/>
+      <c r="B8" s="136"/>
       <c r="C8" s="124" t="s">
         <v>21</v>
       </c>
@@ -2839,10 +2842,10 @@
       <c r="F8" s="124" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="143"/>
-      <c r="H8" s="144"/>
-      <c r="I8" s="145"/>
-      <c r="J8" s="145"/>
+      <c r="G8" s="138"/>
+      <c r="H8" s="139"/>
+      <c r="I8" s="140"/>
+      <c r="J8" s="140"/>
       <c r="K8" s="16">
         <v>43838</v>
       </c>
@@ -2906,8 +2909,8 @@
         <f>Y8+7</f>
         <v>43943</v>
       </c>
-      <c r="AA8" s="135"/>
-      <c r="AB8" s="136"/>
+      <c r="AA8" s="148"/>
+      <c r="AB8" s="149"/>
     </row>
     <row r="9" spans="1:28" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="18"/>
@@ -6029,7 +6032,7 @@
         <v>12</v>
       </c>
       <c r="J68" s="33">
-        <f t="shared" ref="J68:J88" si="7">SUM(C68:F68)</f>
+        <f t="shared" ref="J68:J93" si="7">SUM(C68:F68)</f>
         <v>12</v>
       </c>
       <c r="K68" s="35"/>
@@ -6934,21 +6937,33 @@
       <c r="AB85" s="41"/>
     </row>
     <row r="86" spans="1:28" s="77" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="29"/>
-      <c r="B86" s="57"/>
-      <c r="C86" s="126"/>
-      <c r="D86" s="126"/>
-      <c r="E86" s="126"/>
+      <c r="A86" s="29">
+        <v>20</v>
+      </c>
+      <c r="B86" s="57" t="s">
+        <v>112</v>
+      </c>
+      <c r="C86" s="126">
+        <v>0</v>
+      </c>
+      <c r="D86" s="126">
+        <v>0</v>
+      </c>
+      <c r="E86" s="126">
+        <v>0.5</v>
+      </c>
       <c r="F86" s="126"/>
-      <c r="G86" s="63" t="e">
+      <c r="G86" s="63">
         <f>VLOOKUP(H86,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H86" s="32"/>
+        <v>100</v>
+      </c>
+      <c r="H86" s="32" t="s">
+        <v>5</v>
+      </c>
       <c r="I86" s="33"/>
       <c r="J86" s="33">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K86" s="35"/>
       <c r="L86" s="35"/>
@@ -6964,7 +6979,7 @@
       <c r="V86" s="36"/>
       <c r="W86" s="35"/>
       <c r="X86" s="120"/>
-      <c r="Y86" s="35"/>
+      <c r="Y86" s="122"/>
       <c r="Z86" s="36"/>
       <c r="AA86" s="37"/>
       <c r="AB86" s="41"/>
@@ -6976,16 +6991,10 @@
       <c r="D87" s="126"/>
       <c r="E87" s="126"/>
       <c r="F87" s="126"/>
-      <c r="G87" s="63" t="e">
-        <f>VLOOKUP(H87,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>#N/A</v>
-      </c>
+      <c r="G87" s="63"/>
       <c r="H87" s="32"/>
       <c r="I87" s="33"/>
-      <c r="J87" s="33">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="J87" s="33"/>
       <c r="K87" s="35"/>
       <c r="L87" s="35"/>
       <c r="M87" s="35"/>
@@ -7000,44 +7009,22 @@
       <c r="V87" s="36"/>
       <c r="W87" s="35"/>
       <c r="X87" s="120"/>
-      <c r="Y87" s="35"/>
+      <c r="Y87" s="122"/>
       <c r="Z87" s="36"/>
       <c r="AA87" s="37"/>
       <c r="AB87" s="41"/>
     </row>
     <row r="88" spans="1:28" s="77" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="B88" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="C88" s="126">
-        <v>0</v>
-      </c>
-      <c r="D88" s="126">
-        <v>0</v>
-      </c>
-      <c r="E88" s="126">
-        <v>0.75</v>
-      </c>
-      <c r="F88" s="126">
-        <v>0</v>
-      </c>
-      <c r="G88" s="63">
-        <f>VLOOKUP(H88,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>100</v>
-      </c>
-      <c r="H88" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="I88" s="33">
-        <v>12</v>
-      </c>
-      <c r="J88" s="33">
-        <f t="shared" si="7"/>
-        <v>0.75</v>
-      </c>
+      <c r="A88" s="29"/>
+      <c r="B88" s="57"/>
+      <c r="C88" s="126"/>
+      <c r="D88" s="126"/>
+      <c r="E88" s="126"/>
+      <c r="F88" s="126"/>
+      <c r="G88" s="63"/>
+      <c r="H88" s="32"/>
+      <c r="I88" s="33"/>
+      <c r="J88" s="33"/>
       <c r="K88" s="35"/>
       <c r="L88" s="35"/>
       <c r="M88" s="35"/>
@@ -7057,7 +7044,7 @@
       <c r="AA88" s="37"/>
       <c r="AB88" s="41"/>
     </row>
-    <row r="89" spans="1:28" s="77" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:28" s="77" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="29"/>
       <c r="B89" s="57"/>
       <c r="C89" s="126"/>
@@ -7082,228 +7069,217 @@
       <c r="V89" s="36"/>
       <c r="W89" s="35"/>
       <c r="X89" s="120"/>
-      <c r="Y89" s="35"/>
+      <c r="Y89" s="122"/>
       <c r="Z89" s="36"/>
       <c r="AA89" s="37"/>
       <c r="AB89" s="41"/>
     </row>
-    <row r="90" spans="1:28" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="137" t="s">
+    <row r="90" spans="1:28" s="77" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="29"/>
+      <c r="B90" s="57"/>
+      <c r="C90" s="126"/>
+      <c r="D90" s="126"/>
+      <c r="E90" s="126"/>
+      <c r="F90" s="126"/>
+      <c r="G90" s="63"/>
+      <c r="H90" s="32"/>
+      <c r="I90" s="33"/>
+      <c r="J90" s="33"/>
+      <c r="K90" s="35"/>
+      <c r="L90" s="35"/>
+      <c r="M90" s="35"/>
+      <c r="N90" s="36"/>
+      <c r="O90" s="35"/>
+      <c r="P90" s="35"/>
+      <c r="Q90" s="35"/>
+      <c r="R90" s="35"/>
+      <c r="S90" s="35"/>
+      <c r="T90" s="35"/>
+      <c r="U90" s="35"/>
+      <c r="V90" s="36"/>
+      <c r="W90" s="35"/>
+      <c r="X90" s="120"/>
+      <c r="Y90" s="122"/>
+      <c r="Z90" s="36"/>
+      <c r="AA90" s="37"/>
+      <c r="AB90" s="41"/>
+    </row>
+    <row r="91" spans="1:28" s="77" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="29"/>
+      <c r="B91" s="57"/>
+      <c r="C91" s="126"/>
+      <c r="D91" s="126"/>
+      <c r="E91" s="126"/>
+      <c r="F91" s="126"/>
+      <c r="G91" s="63"/>
+      <c r="H91" s="32"/>
+      <c r="I91" s="33"/>
+      <c r="J91" s="33"/>
+      <c r="K91" s="35"/>
+      <c r="L91" s="35"/>
+      <c r="M91" s="35"/>
+      <c r="N91" s="36"/>
+      <c r="O91" s="35"/>
+      <c r="P91" s="35"/>
+      <c r="Q91" s="35"/>
+      <c r="R91" s="35"/>
+      <c r="S91" s="35"/>
+      <c r="T91" s="35"/>
+      <c r="U91" s="35"/>
+      <c r="V91" s="36"/>
+      <c r="W91" s="35"/>
+      <c r="X91" s="120"/>
+      <c r="Y91" s="122"/>
+      <c r="Z91" s="36"/>
+      <c r="AA91" s="37"/>
+      <c r="AB91" s="41"/>
+    </row>
+    <row r="92" spans="1:28" s="77" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="29"/>
+      <c r="B92" s="57"/>
+      <c r="C92" s="126"/>
+      <c r="D92" s="126"/>
+      <c r="E92" s="126"/>
+      <c r="F92" s="126"/>
+      <c r="G92" s="63" t="e">
+        <f>VLOOKUP(H92,Feuil2!$A$1:$B$3,2,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H92" s="32"/>
+      <c r="I92" s="33"/>
+      <c r="J92" s="33">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K92" s="35"/>
+      <c r="L92" s="35"/>
+      <c r="M92" s="35"/>
+      <c r="N92" s="36"/>
+      <c r="O92" s="35"/>
+      <c r="P92" s="35"/>
+      <c r="Q92" s="35"/>
+      <c r="R92" s="35"/>
+      <c r="S92" s="35"/>
+      <c r="T92" s="35"/>
+      <c r="U92" s="35"/>
+      <c r="V92" s="36"/>
+      <c r="W92" s="35"/>
+      <c r="X92" s="120"/>
+      <c r="Y92" s="35"/>
+      <c r="Z92" s="36"/>
+      <c r="AA92" s="37"/>
+      <c r="AB92" s="41"/>
+    </row>
+    <row r="93" spans="1:28" s="77" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B93" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C93" s="126">
+        <v>0</v>
+      </c>
+      <c r="D93" s="126">
+        <v>0</v>
+      </c>
+      <c r="E93" s="126">
+        <v>0.75</v>
+      </c>
+      <c r="F93" s="126">
+        <v>0</v>
+      </c>
+      <c r="G93" s="63">
+        <f>VLOOKUP(H93,Feuil2!$A$1:$B$3,2,0)</f>
+        <v>100</v>
+      </c>
+      <c r="H93" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="I93" s="33">
+        <v>12</v>
+      </c>
+      <c r="J93" s="33">
+        <f t="shared" si="7"/>
+        <v>0.75</v>
+      </c>
+      <c r="K93" s="35"/>
+      <c r="L93" s="35"/>
+      <c r="M93" s="35"/>
+      <c r="N93" s="36"/>
+      <c r="O93" s="35"/>
+      <c r="P93" s="35"/>
+      <c r="Q93" s="35"/>
+      <c r="R93" s="35"/>
+      <c r="S93" s="35"/>
+      <c r="T93" s="35"/>
+      <c r="U93" s="35"/>
+      <c r="V93" s="36"/>
+      <c r="W93" s="35"/>
+      <c r="X93" s="120"/>
+      <c r="Y93" s="122"/>
+      <c r="Z93" s="36"/>
+      <c r="AA93" s="37"/>
+      <c r="AB93" s="41"/>
+    </row>
+    <row r="94" spans="1:28" s="77" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="29"/>
+      <c r="B94" s="57"/>
+      <c r="C94" s="126"/>
+      <c r="D94" s="126"/>
+      <c r="E94" s="126"/>
+      <c r="F94" s="126"/>
+      <c r="G94" s="63"/>
+      <c r="H94" s="32"/>
+      <c r="I94" s="33"/>
+      <c r="J94" s="33"/>
+      <c r="K94" s="35"/>
+      <c r="L94" s="35"/>
+      <c r="M94" s="35"/>
+      <c r="N94" s="36"/>
+      <c r="O94" s="35"/>
+      <c r="P94" s="35"/>
+      <c r="Q94" s="35"/>
+      <c r="R94" s="35"/>
+      <c r="S94" s="35"/>
+      <c r="T94" s="35"/>
+      <c r="U94" s="35"/>
+      <c r="V94" s="36"/>
+      <c r="W94" s="35"/>
+      <c r="X94" s="120"/>
+      <c r="Y94" s="35"/>
+      <c r="Z94" s="36"/>
+      <c r="AA94" s="37"/>
+      <c r="AB94" s="41"/>
+    </row>
+    <row r="95" spans="1:28" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="150" t="s">
         <v>68</v>
       </c>
-      <c r="B90" s="137"/>
-      <c r="C90" s="124">
-        <f>SUM(C10:C89)</f>
+      <c r="B95" s="150"/>
+      <c r="C95" s="124">
+        <f>SUM(C10:C94)</f>
         <v>130.5</v>
       </c>
-      <c r="D90" s="124">
-        <f>SUM(D10:D89)</f>
+      <c r="D95" s="124">
+        <f>SUM(D10:D94)</f>
         <v>102.5</v>
       </c>
-      <c r="E90" s="124">
-        <f>SUM(E10:E89)</f>
-        <v>107.25</v>
-      </c>
-      <c r="F90" s="124">
-        <f>SUM(F10:F89)</f>
+      <c r="E95" s="124">
+        <f>SUM(E10:E94)</f>
+        <v>107.75</v>
+      </c>
+      <c r="F95" s="124">
+        <f>SUM(F10:F94)</f>
         <v>114</v>
       </c>
-      <c r="G90" s="87"/>
-      <c r="H90" s="86"/>
-      <c r="I90" s="88"/>
-      <c r="J90" s="86">
-        <f>SUM(C90:F90)</f>
-        <v>454.25</v>
-      </c>
-      <c r="K90" s="89"/>
-      <c r="L90" s="89"/>
-      <c r="M90" s="89"/>
-      <c r="N90" s="89"/>
-      <c r="O90" s="89"/>
-      <c r="P90" s="89"/>
-      <c r="Q90" s="89"/>
-      <c r="R90" s="89"/>
-      <c r="S90" s="89"/>
-      <c r="T90" s="89"/>
-      <c r="U90" s="89"/>
-      <c r="V90" s="89"/>
-      <c r="W90" s="89"/>
-      <c r="X90" s="89"/>
-      <c r="Y90" s="89"/>
-      <c r="Z90" s="89"/>
-      <c r="AA90" s="114">
-        <f>SUM(AA10:AA89)</f>
-        <v>-0.75</v>
-      </c>
-      <c r="AB90" s="115"/>
-    </row>
-    <row r="91" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="132" t="s">
-        <v>69</v>
-      </c>
-      <c r="B91" s="132"/>
-      <c r="C91" s="124">
-        <f>117-C90</f>
-        <v>-13.5</v>
-      </c>
-      <c r="D91" s="124">
-        <f>117-D90</f>
-        <v>14.5</v>
-      </c>
-      <c r="E91" s="124">
-        <f>117-E90</f>
-        <v>9.75</v>
-      </c>
-      <c r="F91" s="124">
-        <f>117-F90</f>
-        <v>3</v>
-      </c>
-      <c r="G91" s="87"/>
-      <c r="H91" s="86"/>
-      <c r="I91" s="86"/>
-      <c r="J91" s="86">
-        <f>SUM(C91:F91)</f>
-        <v>13.75</v>
-      </c>
-      <c r="K91" s="89"/>
-      <c r="L91" s="89"/>
-      <c r="M91" s="89"/>
-      <c r="N91" s="89"/>
-      <c r="O91" s="89"/>
-      <c r="P91" s="89"/>
-      <c r="Q91" s="89"/>
-      <c r="R91" s="89"/>
-      <c r="S91" s="89"/>
-      <c r="T91" s="89"/>
-      <c r="U91" s="89"/>
-      <c r="V91" s="89"/>
-      <c r="W91" s="89"/>
-      <c r="X91" s="89"/>
-      <c r="Y91" s="89"/>
-      <c r="Z91" s="89"/>
-      <c r="AA91" s="89"/>
-      <c r="AB91" s="89"/>
-    </row>
-    <row r="92" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="133" t="s">
-        <v>70</v>
-      </c>
-      <c r="B92" s="133"/>
-      <c r="C92" s="124"/>
-      <c r="D92" s="124"/>
-      <c r="E92" s="124"/>
-      <c r="F92" s="124"/>
-      <c r="G92" s="86"/>
-      <c r="H92" s="86"/>
-      <c r="I92" s="86"/>
-      <c r="J92" s="86">
-        <f>C92+D92+F92+E92</f>
-        <v>0</v>
-      </c>
-      <c r="K92" s="89"/>
-      <c r="L92" s="89"/>
-      <c r="M92" s="89"/>
-      <c r="N92" s="89"/>
-      <c r="O92" s="89"/>
-      <c r="P92" s="89"/>
-      <c r="Q92" s="89"/>
-      <c r="R92" s="89"/>
-      <c r="S92" s="89"/>
-      <c r="T92" s="89"/>
-      <c r="U92" s="89"/>
-      <c r="V92" s="89"/>
-      <c r="W92" s="89"/>
-      <c r="X92" s="89"/>
-      <c r="Y92" s="89"/>
-      <c r="Z92" s="89"/>
-      <c r="AA92" s="89"/>
-      <c r="AB92" s="89"/>
-    </row>
-    <row r="93" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="132" t="s">
-        <v>71</v>
-      </c>
-      <c r="B93" s="132"/>
-      <c r="C93" s="124"/>
-      <c r="D93" s="124"/>
-      <c r="E93" s="128"/>
-      <c r="F93" s="124"/>
-      <c r="G93" s="86"/>
-      <c r="H93" s="86"/>
-      <c r="I93" s="90">
-        <f>SUM(I10:I89)</f>
-        <v>483.25</v>
-      </c>
-      <c r="J93" s="86">
-        <f>SUM(J10:J89)</f>
-        <v>454.25</v>
-      </c>
-      <c r="K93" s="89"/>
-      <c r="L93" s="89"/>
-      <c r="M93" s="89"/>
-      <c r="N93" s="89"/>
-      <c r="O93" s="89"/>
-      <c r="P93" s="89"/>
-      <c r="Q93" s="89"/>
-      <c r="R93" s="89"/>
-      <c r="S93" s="89"/>
-      <c r="T93" s="89"/>
-      <c r="U93" s="89"/>
-      <c r="V93" s="89"/>
-      <c r="W93" s="89"/>
-      <c r="X93" s="89"/>
-      <c r="Y93" s="89"/>
-      <c r="Z93" s="89"/>
-      <c r="AA93" s="89"/>
-      <c r="AB93" s="89"/>
-    </row>
-    <row r="94" spans="1:28" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="91"/>
-      <c r="B94" s="91"/>
-      <c r="D94" s="138" t="s">
-        <v>88</v>
-      </c>
-      <c r="E94" s="138"/>
-      <c r="F94" s="138"/>
-      <c r="G94" s="138"/>
-      <c r="H94" s="92"/>
-      <c r="I94" s="92"/>
-      <c r="J94" s="92"/>
-      <c r="K94" s="89"/>
-      <c r="L94" s="89"/>
-      <c r="M94" s="89"/>
-      <c r="N94" s="89"/>
-      <c r="O94" s="89"/>
-      <c r="P94" s="89"/>
-      <c r="Q94" s="89"/>
-      <c r="R94" s="89"/>
-      <c r="S94" s="89"/>
-      <c r="T94" s="89"/>
-      <c r="U94" s="89"/>
-      <c r="V94" s="89"/>
-      <c r="W94" s="89"/>
-      <c r="X94" s="89"/>
-      <c r="Y94" s="89"/>
-      <c r="Z94" s="89"/>
-      <c r="AA94" s="89"/>
-      <c r="AB94" s="89"/>
-    </row>
-    <row r="95" spans="1:28" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="133" t="s">
-        <v>72</v>
-      </c>
-      <c r="B95" s="133"/>
-      <c r="C95" s="129">
-        <f>135*4</f>
-        <v>540</v>
-      </c>
-      <c r="D95" s="130">
-        <v>468</v>
-      </c>
-      <c r="G95" s="92"/>
-      <c r="H95" s="92"/>
-      <c r="I95" s="92"/>
-      <c r="J95" s="92"/>
+      <c r="G95" s="87"/>
+      <c r="H95" s="86"/>
+      <c r="I95" s="88"/>
+      <c r="J95" s="86">
+        <f>SUM(C95:F95)</f>
+        <v>454.75</v>
+      </c>
       <c r="K95" s="89"/>
       <c r="L95" s="89"/>
       <c r="M95" s="89"/>
@@ -7320,25 +7296,40 @@
       <c r="X95" s="89"/>
       <c r="Y95" s="89"/>
       <c r="Z95" s="89"/>
-      <c r="AA95" s="89"/>
-      <c r="AB95" s="89"/>
-    </row>
-    <row r="96" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="134" t="s">
-        <v>73</v>
-      </c>
-      <c r="B96" s="134"/>
-      <c r="C96" s="129">
-        <f>C95-J93</f>
-        <v>85.75</v>
-      </c>
-      <c r="D96" s="131">
-        <v>66</v>
-      </c>
-      <c r="G96" s="92"/>
-      <c r="H96" s="92"/>
-      <c r="I96" s="92"/>
-      <c r="J96" s="92"/>
+      <c r="AA95" s="114">
+        <f>SUM(AA10:AA94)</f>
+        <v>-0.75</v>
+      </c>
+      <c r="AB95" s="115"/>
+    </row>
+    <row r="96" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="145" t="s">
+        <v>69</v>
+      </c>
+      <c r="B96" s="145"/>
+      <c r="C96" s="124">
+        <f>117-C95</f>
+        <v>-13.5</v>
+      </c>
+      <c r="D96" s="124">
+        <f>117-D95</f>
+        <v>14.5</v>
+      </c>
+      <c r="E96" s="124">
+        <f>117-E95</f>
+        <v>9.25</v>
+      </c>
+      <c r="F96" s="124">
+        <f>117-F95</f>
+        <v>3</v>
+      </c>
+      <c r="G96" s="87"/>
+      <c r="H96" s="86"/>
+      <c r="I96" s="86"/>
+      <c r="J96" s="86">
+        <f>SUM(C96:F96)</f>
+        <v>13.25</v>
+      </c>
       <c r="K96" s="89"/>
       <c r="L96" s="89"/>
       <c r="M96" s="89"/>
@@ -7358,65 +7349,243 @@
       <c r="AA96" s="89"/>
       <c r="AB96" s="89"/>
     </row>
-    <row r="97" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A97" s="93"/>
-      <c r="B97" s="91"/>
-      <c r="G97" s="91"/>
-      <c r="H97" s="94"/>
-      <c r="I97" s="95"/>
-      <c r="J97" s="95"/>
+    <row r="97" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="146" t="s">
+        <v>70</v>
+      </c>
+      <c r="B97" s="146"/>
+      <c r="C97" s="124"/>
+      <c r="D97" s="124"/>
+      <c r="E97" s="124"/>
+      <c r="F97" s="124"/>
+      <c r="G97" s="86"/>
+      <c r="H97" s="86"/>
+      <c r="I97" s="86"/>
+      <c r="J97" s="86">
+        <f>C97+D97+F97+E97</f>
+        <v>0</v>
+      </c>
+      <c r="K97" s="89"/>
+      <c r="L97" s="89"/>
+      <c r="M97" s="89"/>
+      <c r="N97" s="89"/>
+      <c r="O97" s="89"/>
+      <c r="P97" s="89"/>
+      <c r="Q97" s="89"/>
+      <c r="R97" s="89"/>
+      <c r="S97" s="89"/>
+      <c r="T97" s="89"/>
+      <c r="U97" s="89"/>
+      <c r="V97" s="89"/>
+      <c r="W97" s="89"/>
+      <c r="X97" s="89"/>
+      <c r="Y97" s="89"/>
+      <c r="Z97" s="89"/>
       <c r="AA97" s="89"/>
-    </row>
-    <row r="99" spans="1:27" s="97" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A99" s="96"/>
-      <c r="C99" s="123"/>
-      <c r="D99" s="123"/>
-      <c r="E99" s="123"/>
-      <c r="F99" s="123"/>
-      <c r="H99" s="98"/>
-      <c r="I99" s="99"/>
-      <c r="J99" s="99"/>
-      <c r="N99" s="100"/>
-      <c r="R99" s="100"/>
-      <c r="V99" s="100"/>
-      <c r="Z99" s="100"/>
-      <c r="AA99" s="101"/>
-    </row>
-    <row r="100" spans="1:27" s="97" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="C100" s="123"/>
-      <c r="D100" s="123"/>
-      <c r="E100" s="123"/>
-      <c r="F100" s="123"/>
-      <c r="H100" s="98"/>
-      <c r="I100" s="99"/>
-      <c r="J100" s="99"/>
-      <c r="N100" s="100"/>
-      <c r="R100" s="100"/>
-      <c r="V100" s="100"/>
-      <c r="Z100" s="100"/>
-      <c r="AA100" s="101"/>
-    </row>
-    <row r="101" spans="1:27" s="97" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="C101" s="123"/>
-      <c r="D101" s="123"/>
-      <c r="E101" s="123"/>
-      <c r="F101" s="123"/>
-      <c r="H101" s="98"/>
-      <c r="I101" s="99"/>
-      <c r="J101" s="99"/>
-      <c r="N101" s="100"/>
-      <c r="R101" s="100"/>
-      <c r="V101" s="100"/>
-      <c r="Z101" s="100"/>
-      <c r="AA101" s="101"/>
+      <c r="AB97" s="89"/>
+    </row>
+    <row r="98" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="145" t="s">
+        <v>71</v>
+      </c>
+      <c r="B98" s="145"/>
+      <c r="C98" s="124"/>
+      <c r="D98" s="124"/>
+      <c r="E98" s="128"/>
+      <c r="F98" s="124"/>
+      <c r="G98" s="86"/>
+      <c r="H98" s="86"/>
+      <c r="I98" s="90">
+        <f>SUM(I10:I94)</f>
+        <v>483.25</v>
+      </c>
+      <c r="J98" s="86">
+        <f>SUM(J10:J94)</f>
+        <v>454.75</v>
+      </c>
+      <c r="K98" s="89"/>
+      <c r="L98" s="89"/>
+      <c r="M98" s="89"/>
+      <c r="N98" s="89"/>
+      <c r="O98" s="89"/>
+      <c r="P98" s="89"/>
+      <c r="Q98" s="89"/>
+      <c r="R98" s="89"/>
+      <c r="S98" s="89"/>
+      <c r="T98" s="89"/>
+      <c r="U98" s="89"/>
+      <c r="V98" s="89"/>
+      <c r="W98" s="89"/>
+      <c r="X98" s="89"/>
+      <c r="Y98" s="89"/>
+      <c r="Z98" s="89"/>
+      <c r="AA98" s="89"/>
+      <c r="AB98" s="89"/>
+    </row>
+    <row r="99" spans="1:28" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="91"/>
+      <c r="B99" s="91"/>
+      <c r="D99" s="151" t="s">
+        <v>88</v>
+      </c>
+      <c r="E99" s="151"/>
+      <c r="F99" s="151"/>
+      <c r="G99" s="151"/>
+      <c r="H99" s="92"/>
+      <c r="I99" s="92"/>
+      <c r="J99" s="92"/>
+      <c r="K99" s="89"/>
+      <c r="L99" s="89"/>
+      <c r="M99" s="89"/>
+      <c r="N99" s="89"/>
+      <c r="O99" s="89"/>
+      <c r="P99" s="89"/>
+      <c r="Q99" s="89"/>
+      <c r="R99" s="89"/>
+      <c r="S99" s="89"/>
+      <c r="T99" s="89"/>
+      <c r="U99" s="89"/>
+      <c r="V99" s="89"/>
+      <c r="W99" s="89"/>
+      <c r="X99" s="89"/>
+      <c r="Y99" s="89"/>
+      <c r="Z99" s="89"/>
+      <c r="AA99" s="89"/>
+      <c r="AB99" s="89"/>
+    </row>
+    <row r="100" spans="1:28" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="146" t="s">
+        <v>72</v>
+      </c>
+      <c r="B100" s="146"/>
+      <c r="C100" s="129">
+        <f>135*4</f>
+        <v>540</v>
+      </c>
+      <c r="D100" s="130">
+        <v>468</v>
+      </c>
+      <c r="G100" s="92"/>
+      <c r="H100" s="92"/>
+      <c r="I100" s="92"/>
+      <c r="J100" s="92"/>
+      <c r="K100" s="89"/>
+      <c r="L100" s="89"/>
+      <c r="M100" s="89"/>
+      <c r="N100" s="89"/>
+      <c r="O100" s="89"/>
+      <c r="P100" s="89"/>
+      <c r="Q100" s="89"/>
+      <c r="R100" s="89"/>
+      <c r="S100" s="89"/>
+      <c r="T100" s="89"/>
+      <c r="U100" s="89"/>
+      <c r="V100" s="89"/>
+      <c r="W100" s="89"/>
+      <c r="X100" s="89"/>
+      <c r="Y100" s="89"/>
+      <c r="Z100" s="89"/>
+      <c r="AA100" s="89"/>
+      <c r="AB100" s="89"/>
+    </row>
+    <row r="101" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="147" t="s">
+        <v>73</v>
+      </c>
+      <c r="B101" s="147"/>
+      <c r="C101" s="129">
+        <f>C100-J98</f>
+        <v>85.25</v>
+      </c>
+      <c r="D101" s="131">
+        <v>66</v>
+      </c>
+      <c r="G101" s="92"/>
+      <c r="H101" s="92"/>
+      <c r="I101" s="92"/>
+      <c r="J101" s="92"/>
+      <c r="K101" s="89"/>
+      <c r="L101" s="89"/>
+      <c r="M101" s="89"/>
+      <c r="N101" s="89"/>
+      <c r="O101" s="89"/>
+      <c r="P101" s="89"/>
+      <c r="Q101" s="89"/>
+      <c r="R101" s="89"/>
+      <c r="S101" s="89"/>
+      <c r="T101" s="89"/>
+      <c r="U101" s="89"/>
+      <c r="V101" s="89"/>
+      <c r="W101" s="89"/>
+      <c r="X101" s="89"/>
+      <c r="Y101" s="89"/>
+      <c r="Z101" s="89"/>
+      <c r="AA101" s="89"/>
+      <c r="AB101" s="89"/>
+    </row>
+    <row r="102" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A102" s="93"/>
+      <c r="B102" s="91"/>
+      <c r="G102" s="91"/>
+      <c r="H102" s="94"/>
+      <c r="I102" s="95"/>
+      <c r="J102" s="95"/>
+      <c r="AA102" s="89"/>
+    </row>
+    <row r="104" spans="1:28" s="97" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A104" s="96"/>
+      <c r="C104" s="123"/>
+      <c r="D104" s="123"/>
+      <c r="E104" s="123"/>
+      <c r="F104" s="123"/>
+      <c r="H104" s="98"/>
+      <c r="I104" s="99"/>
+      <c r="J104" s="99"/>
+      <c r="N104" s="100"/>
+      <c r="R104" s="100"/>
+      <c r="V104" s="100"/>
+      <c r="Z104" s="100"/>
+      <c r="AA104" s="101"/>
+    </row>
+    <row r="105" spans="1:28" s="97" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="C105" s="123"/>
+      <c r="D105" s="123"/>
+      <c r="E105" s="123"/>
+      <c r="F105" s="123"/>
+      <c r="H105" s="98"/>
+      <c r="I105" s="99"/>
+      <c r="J105" s="99"/>
+      <c r="N105" s="100"/>
+      <c r="R105" s="100"/>
+      <c r="V105" s="100"/>
+      <c r="Z105" s="100"/>
+      <c r="AA105" s="101"/>
+    </row>
+    <row r="106" spans="1:28" s="97" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="C106" s="123"/>
+      <c r="D106" s="123"/>
+      <c r="E106" s="123"/>
+      <c r="F106" s="123"/>
+      <c r="H106" s="98"/>
+      <c r="I106" s="99"/>
+      <c r="J106" s="99"/>
+      <c r="N106" s="100"/>
+      <c r="R106" s="100"/>
+      <c r="V106" s="100"/>
+      <c r="Z106" s="100"/>
+      <c r="AA106" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D99:G99"/>
     <mergeCell ref="S6:V6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
@@ -7427,22 +7596,18 @@
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:Z7"/>
     <mergeCell ref="W6:Z6"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="D94:G94"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K6:R6"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
     <cfRule type="containsText" dxfId="62" priority="75" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H19)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H9:H68 H70:H80 H82:H89">
+  <conditionalFormatting sqref="H9:H68 H70:H80 H82:H94">
     <cfRule type="containsText" dxfId="61" priority="76" operator="containsText" text="En attente">
       <formula>NOT(ISERROR(SEARCH("En attente",H9)))</formula>
     </cfRule>
@@ -7453,7 +7618,7 @@
       <formula>NOT(ISERROR(SEARCH("Terminé",H9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9:F45 C47:F47 C56:F64 C49:F54 C66:F68 C70:F80 C82:F89">
+  <conditionalFormatting sqref="C9:F45 C47:F47 C56:F64 C49:F54 C66:F68 C70:F80 C82:F94">
     <cfRule type="cellIs" dxfId="58" priority="79" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -7461,7 +7626,7 @@
       <formula>$H9="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9:F45 C47:F47 C56:F64 C49:F54 C66:F68 C70:F80 C82:F89">
+  <conditionalFormatting sqref="C9:F45 C47:F47 C56:F64 C49:F54 C66:F68 C70:F80 C82:F94">
     <cfRule type="expression" dxfId="56" priority="81">
       <formula>$H9="En cours"</formula>
     </cfRule>
@@ -7549,31 +7714,31 @@
       <formula>$H66="En attente"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C89:F89">
+  <conditionalFormatting sqref="C94:F94">
     <cfRule type="expression" dxfId="34" priority="36">
-      <formula>$H89="En cours"</formula>
+      <formula>$H94="En cours"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="33" priority="37">
-      <formula>$H89="En attente"</formula>
+      <formula>$H94="En attente"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H89">
+  <conditionalFormatting sqref="H94">
     <cfRule type="containsText" dxfId="32" priority="40" operator="containsText" text="En attente">
-      <formula>NOT(ISERROR(SEARCH("En attente",H89)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En attente",H94)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="31" priority="41" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",H89)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",H94)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="30" priority="42" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",H89)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",H94)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C89:F89">
+  <conditionalFormatting sqref="C94:F94">
     <cfRule type="cellIs" dxfId="29" priority="38" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="28" priority="39">
-      <formula>$H89="Terminé"</formula>
+      <formula>$H94="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69">
@@ -7685,7 +7850,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H9:H89" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H9:H94" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"En attente,En cours,Terminé"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Partially fixed issue #49
</commit_message>
<xml_diff>
--- a/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
+++ b/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alxbo\Source\Repos\mrjrdg\marque-sans-nom\Semainiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D90BED-93DF-46D7-A3AF-A23DEA5527D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F100B9E8-FB8D-4746-8A79-644E1537507A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="114">
   <si>
     <t>UQÀM - Hiver 2020</t>
   </si>
@@ -439,6 +439,9 @@
   </si>
   <si>
     <t>Améliorer le visuel (profile-view)</t>
+  </si>
+  <si>
+    <t>Améliorer le visuel (user-create)</t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1172,7 @@
     <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyAlignment="1">
@@ -1546,11 +1549,24 @@
     <xf numFmtId="164" fontId="18" fillId="0" borderId="33" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="34" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="35" xfId="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="12" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1583,24 +1599,15 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="12" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="20" fillId="0" borderId="16" xfId="9" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -2601,8 +2608,8 @@
   </sheetPr>
   <dimension ref="A1:AMK106"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2630,22 +2637,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="6" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="132" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="132"/>
+      <c r="A1" s="150" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="150"/>
       <c r="C1" s="123"/>
-      <c r="D1" s="133" t="s">
+      <c r="D1" s="151" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="133"/>
-      <c r="F1" s="133"/>
-      <c r="G1" s="133"/>
-      <c r="H1" s="133"/>
-      <c r="I1" s="133"/>
-      <c r="J1" s="133"/>
-      <c r="K1" s="133"/>
-      <c r="L1" s="133"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
+      <c r="G1" s="151"/>
+      <c r="H1" s="151"/>
+      <c r="I1" s="151"/>
+      <c r="J1" s="151"/>
+      <c r="K1" s="151"/>
+      <c r="L1" s="151"/>
       <c r="N1" s="2"/>
       <c r="P1" s="7"/>
       <c r="Q1" s="6" t="s">
@@ -2657,20 +2664,20 @@
       <c r="AA1" s="8"/>
     </row>
     <row r="2" spans="1:28" s="6" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="132" t="s">
+      <c r="A2" s="150" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="132"/>
+      <c r="B2" s="150"/>
       <c r="C2" s="123"/>
       <c r="D2" s="123"/>
       <c r="E2" s="123"/>
-      <c r="F2" s="132" t="s">
+      <c r="F2" s="150" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="132"/>
-      <c r="H2" s="132"/>
-      <c r="I2" s="132"/>
-      <c r="J2" s="132"/>
+      <c r="G2" s="150"/>
+      <c r="H2" s="150"/>
+      <c r="I2" s="150"/>
+      <c r="J2" s="150"/>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
       <c r="N2" s="2"/>
@@ -2753,83 +2760,83 @@
       <c r="H6" s="2"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="134" t="s">
+      <c r="K6" s="139" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="134"/>
-      <c r="M6" s="134"/>
-      <c r="N6" s="134"/>
-      <c r="O6" s="134"/>
-      <c r="P6" s="134"/>
-      <c r="Q6" s="134"/>
-      <c r="R6" s="134"/>
-      <c r="S6" s="134" t="s">
+      <c r="L6" s="139"/>
+      <c r="M6" s="139"/>
+      <c r="N6" s="139"/>
+      <c r="O6" s="139"/>
+      <c r="P6" s="139"/>
+      <c r="Q6" s="139"/>
+      <c r="R6" s="139"/>
+      <c r="S6" s="139" t="s">
         <v>10</v>
       </c>
-      <c r="T6" s="134"/>
-      <c r="U6" s="134"/>
-      <c r="V6" s="134"/>
-      <c r="W6" s="142" t="s">
+      <c r="T6" s="139"/>
+      <c r="U6" s="139"/>
+      <c r="V6" s="139"/>
+      <c r="W6" s="147" t="s">
         <v>93</v>
       </c>
-      <c r="X6" s="143"/>
-      <c r="Y6" s="143"/>
-      <c r="Z6" s="144"/>
+      <c r="X6" s="148"/>
+      <c r="Y6" s="148"/>
+      <c r="Z6" s="149"/>
       <c r="AA6" s="8"/>
     </row>
     <row r="7" spans="1:28" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="135" t="s">
+      <c r="A7" s="140" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="136" t="s">
+      <c r="B7" s="141" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="137" t="s">
+      <c r="C7" s="142" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="137"/>
-      <c r="E7" s="137"/>
-      <c r="F7" s="137"/>
-      <c r="G7" s="138" t="s">
+      <c r="D7" s="142"/>
+      <c r="E7" s="142"/>
+      <c r="F7" s="142"/>
+      <c r="G7" s="143" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="139" t="s">
+      <c r="H7" s="144" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="140" t="s">
+      <c r="I7" s="145" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="140" t="s">
+      <c r="J7" s="145" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="141" t="s">
+      <c r="K7" s="146" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="141"/>
-      <c r="M7" s="141"/>
-      <c r="N7" s="141"/>
-      <c r="O7" s="141"/>
-      <c r="P7" s="141"/>
-      <c r="Q7" s="141"/>
-      <c r="R7" s="141"/>
-      <c r="S7" s="141"/>
-      <c r="T7" s="141"/>
-      <c r="U7" s="141"/>
-      <c r="V7" s="141"/>
-      <c r="W7" s="141"/>
-      <c r="X7" s="141"/>
-      <c r="Y7" s="141"/>
-      <c r="Z7" s="141"/>
-      <c r="AA7" s="148" t="s">
+      <c r="L7" s="146"/>
+      <c r="M7" s="146"/>
+      <c r="N7" s="146"/>
+      <c r="O7" s="146"/>
+      <c r="P7" s="146"/>
+      <c r="Q7" s="146"/>
+      <c r="R7" s="146"/>
+      <c r="S7" s="146"/>
+      <c r="T7" s="146"/>
+      <c r="U7" s="146"/>
+      <c r="V7" s="146"/>
+      <c r="W7" s="146"/>
+      <c r="X7" s="146"/>
+      <c r="Y7" s="146"/>
+      <c r="Z7" s="146"/>
+      <c r="AA7" s="135" t="s">
         <v>19</v>
       </c>
-      <c r="AB7" s="149" t="s">
+      <c r="AB7" s="136" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="135"/>
-      <c r="B8" s="136"/>
+      <c r="A8" s="140"/>
+      <c r="B8" s="141"/>
       <c r="C8" s="124" t="s">
         <v>21</v>
       </c>
@@ -2842,10 +2849,10 @@
       <c r="F8" s="124" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="138"/>
-      <c r="H8" s="139"/>
-      <c r="I8" s="140"/>
-      <c r="J8" s="140"/>
+      <c r="G8" s="143"/>
+      <c r="H8" s="144"/>
+      <c r="I8" s="145"/>
+      <c r="J8" s="145"/>
       <c r="K8" s="16">
         <v>43838</v>
       </c>
@@ -2909,8 +2916,8 @@
         <f>Y8+7</f>
         <v>43943</v>
       </c>
-      <c r="AA8" s="148"/>
-      <c r="AB8" s="149"/>
+      <c r="AA8" s="135"/>
+      <c r="AB8" s="136"/>
     </row>
     <row r="9" spans="1:28" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="18"/>
@@ -6985,16 +6992,33 @@
       <c r="AB86" s="41"/>
     </row>
     <row r="87" spans="1:28" s="77" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="29"/>
-      <c r="B87" s="57"/>
-      <c r="C87" s="126"/>
-      <c r="D87" s="126"/>
-      <c r="E87" s="126"/>
-      <c r="F87" s="126"/>
+      <c r="A87" s="29">
+        <v>21</v>
+      </c>
+      <c r="B87" s="57" t="s">
+        <v>113</v>
+      </c>
+      <c r="C87" s="126">
+        <v>0</v>
+      </c>
+      <c r="D87" s="126">
+        <v>0</v>
+      </c>
+      <c r="E87" s="126">
+        <v>0.25</v>
+      </c>
+      <c r="F87" s="126">
+        <v>0</v>
+      </c>
       <c r="G87" s="63"/>
-      <c r="H87" s="32"/>
+      <c r="H87" s="32" t="s">
+        <v>5</v>
+      </c>
       <c r="I87" s="33"/>
-      <c r="J87" s="33"/>
+      <c r="J87" s="33">
+        <f t="shared" si="7"/>
+        <v>0.25</v>
+      </c>
       <c r="K87" s="35"/>
       <c r="L87" s="35"/>
       <c r="M87" s="35"/>
@@ -7039,7 +7063,7 @@
       <c r="V88" s="36"/>
       <c r="W88" s="35"/>
       <c r="X88" s="120"/>
-      <c r="Y88" s="122"/>
+      <c r="Y88" s="152"/>
       <c r="Z88" s="36"/>
       <c r="AA88" s="37"/>
       <c r="AB88" s="41"/>
@@ -7069,7 +7093,7 @@
       <c r="V89" s="36"/>
       <c r="W89" s="35"/>
       <c r="X89" s="120"/>
-      <c r="Y89" s="122"/>
+      <c r="Y89" s="152"/>
       <c r="Z89" s="36"/>
       <c r="AA89" s="37"/>
       <c r="AB89" s="41"/>
@@ -7099,7 +7123,7 @@
       <c r="V90" s="36"/>
       <c r="W90" s="35"/>
       <c r="X90" s="120"/>
-      <c r="Y90" s="122"/>
+      <c r="Y90" s="152"/>
       <c r="Z90" s="36"/>
       <c r="AA90" s="37"/>
       <c r="AB90" s="41"/>
@@ -7129,7 +7153,7 @@
       <c r="V91" s="36"/>
       <c r="W91" s="35"/>
       <c r="X91" s="120"/>
-      <c r="Y91" s="122"/>
+      <c r="Y91" s="152"/>
       <c r="Z91" s="36"/>
       <c r="AA91" s="37"/>
       <c r="AB91" s="41"/>
@@ -7253,10 +7277,10 @@
       <c r="AB94" s="41"/>
     </row>
     <row r="95" spans="1:28" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="150" t="s">
+      <c r="A95" s="137" t="s">
         <v>68</v>
       </c>
-      <c r="B95" s="150"/>
+      <c r="B95" s="137"/>
       <c r="C95" s="124">
         <f>SUM(C10:C94)</f>
         <v>130.5</v>
@@ -7267,7 +7291,7 @@
       </c>
       <c r="E95" s="124">
         <f>SUM(E10:E94)</f>
-        <v>107.75</v>
+        <v>108</v>
       </c>
       <c r="F95" s="124">
         <f>SUM(F10:F94)</f>
@@ -7278,7 +7302,7 @@
       <c r="I95" s="88"/>
       <c r="J95" s="86">
         <f>SUM(C95:F95)</f>
-        <v>454.75</v>
+        <v>455</v>
       </c>
       <c r="K95" s="89"/>
       <c r="L95" s="89"/>
@@ -7303,10 +7327,10 @@
       <c r="AB95" s="115"/>
     </row>
     <row r="96" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="145" t="s">
+      <c r="A96" s="132" t="s">
         <v>69</v>
       </c>
-      <c r="B96" s="145"/>
+      <c r="B96" s="132"/>
       <c r="C96" s="124">
         <f>117-C95</f>
         <v>-13.5</v>
@@ -7317,7 +7341,7 @@
       </c>
       <c r="E96" s="124">
         <f>117-E95</f>
-        <v>9.25</v>
+        <v>9</v>
       </c>
       <c r="F96" s="124">
         <f>117-F95</f>
@@ -7328,7 +7352,7 @@
       <c r="I96" s="86"/>
       <c r="J96" s="86">
         <f>SUM(C96:F96)</f>
-        <v>13.25</v>
+        <v>13</v>
       </c>
       <c r="K96" s="89"/>
       <c r="L96" s="89"/>
@@ -7350,10 +7374,10 @@
       <c r="AB96" s="89"/>
     </row>
     <row r="97" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="146" t="s">
+      <c r="A97" s="133" t="s">
         <v>70</v>
       </c>
-      <c r="B97" s="146"/>
+      <c r="B97" s="133"/>
       <c r="C97" s="124"/>
       <c r="D97" s="124"/>
       <c r="E97" s="124"/>
@@ -7385,10 +7409,10 @@
       <c r="AB97" s="89"/>
     </row>
     <row r="98" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="145" t="s">
+      <c r="A98" s="132" t="s">
         <v>71</v>
       </c>
-      <c r="B98" s="145"/>
+      <c r="B98" s="132"/>
       <c r="C98" s="124"/>
       <c r="D98" s="124"/>
       <c r="E98" s="128"/>
@@ -7401,7 +7425,7 @@
       </c>
       <c r="J98" s="86">
         <f>SUM(J10:J94)</f>
-        <v>454.75</v>
+        <v>455</v>
       </c>
       <c r="K98" s="89"/>
       <c r="L98" s="89"/>
@@ -7425,12 +7449,12 @@
     <row r="99" spans="1:28" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="91"/>
       <c r="B99" s="91"/>
-      <c r="D99" s="151" t="s">
+      <c r="D99" s="138" t="s">
         <v>88</v>
       </c>
-      <c r="E99" s="151"/>
-      <c r="F99" s="151"/>
-      <c r="G99" s="151"/>
+      <c r="E99" s="138"/>
+      <c r="F99" s="138"/>
+      <c r="G99" s="138"/>
       <c r="H99" s="92"/>
       <c r="I99" s="92"/>
       <c r="J99" s="92"/>
@@ -7454,10 +7478,10 @@
       <c r="AB99" s="89"/>
     </row>
     <row r="100" spans="1:28" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="146" t="s">
+      <c r="A100" s="133" t="s">
         <v>72</v>
       </c>
-      <c r="B100" s="146"/>
+      <c r="B100" s="133"/>
       <c r="C100" s="129">
         <f>135*4</f>
         <v>540</v>
@@ -7489,13 +7513,13 @@
       <c r="AB100" s="89"/>
     </row>
     <row r="101" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="147" t="s">
+      <c r="A101" s="134" t="s">
         <v>73</v>
       </c>
-      <c r="B101" s="147"/>
+      <c r="B101" s="134"/>
       <c r="C101" s="129">
         <f>C100-J98</f>
-        <v>85.25</v>
+        <v>85</v>
       </c>
       <c r="D101" s="131">
         <v>66</v>
@@ -7577,15 +7601,11 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="D99:G99"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K6:R6"/>
     <mergeCell ref="S6:V6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
@@ -7596,11 +7616,15 @@
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:Z7"/>
     <mergeCell ref="W6:Z6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D99:G99"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
     <cfRule type="containsText" dxfId="62" priority="75" operator="containsText" text="En cours">

</xml_diff>

<commit_message>
Partially fixed issue #44
</commit_message>
<xml_diff>
--- a/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
+++ b/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alxbo\Source\Repos\mrjrdg\marque-sans-nom\Semainiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE6150A-5754-4D48-B9D6-2DB214598E5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D213B1FD-1DE5-4D16-AA36-C30C8973BFD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1553,11 +1553,24 @@
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="12" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1590,24 +1603,11 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="12" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -2609,7 +2609,7 @@
   <dimension ref="A1:AMK106"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="F85" sqref="F85"/>
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2637,22 +2637,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="6" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="133" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="133"/>
+      <c r="A1" s="151" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="151"/>
       <c r="C1" s="123"/>
-      <c r="D1" s="134" t="s">
+      <c r="D1" s="152" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="134"/>
-      <c r="J1" s="134"/>
-      <c r="K1" s="134"/>
-      <c r="L1" s="134"/>
+      <c r="E1" s="152"/>
+      <c r="F1" s="152"/>
+      <c r="G1" s="152"/>
+      <c r="H1" s="152"/>
+      <c r="I1" s="152"/>
+      <c r="J1" s="152"/>
+      <c r="K1" s="152"/>
+      <c r="L1" s="152"/>
       <c r="N1" s="2"/>
       <c r="P1" s="7"/>
       <c r="Q1" s="6" t="s">
@@ -2664,20 +2664,20 @@
       <c r="AA1" s="8"/>
     </row>
     <row r="2" spans="1:28" s="6" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="133"/>
+      <c r="B2" s="151"/>
       <c r="C2" s="123"/>
       <c r="D2" s="123"/>
       <c r="E2" s="123"/>
-      <c r="F2" s="133" t="s">
+      <c r="F2" s="151" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="133"/>
-      <c r="H2" s="133"/>
-      <c r="I2" s="133"/>
-      <c r="J2" s="133"/>
+      <c r="G2" s="151"/>
+      <c r="H2" s="151"/>
+      <c r="I2" s="151"/>
+      <c r="J2" s="151"/>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
       <c r="N2" s="2"/>
@@ -2760,83 +2760,83 @@
       <c r="H6" s="2"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="135" t="s">
+      <c r="K6" s="140" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="135"/>
-      <c r="M6" s="135"/>
-      <c r="N6" s="135"/>
-      <c r="O6" s="135"/>
-      <c r="P6" s="135"/>
-      <c r="Q6" s="135"/>
-      <c r="R6" s="135"/>
-      <c r="S6" s="135" t="s">
+      <c r="L6" s="140"/>
+      <c r="M6" s="140"/>
+      <c r="N6" s="140"/>
+      <c r="O6" s="140"/>
+      <c r="P6" s="140"/>
+      <c r="Q6" s="140"/>
+      <c r="R6" s="140"/>
+      <c r="S6" s="140" t="s">
         <v>10</v>
       </c>
-      <c r="T6" s="135"/>
-      <c r="U6" s="135"/>
-      <c r="V6" s="135"/>
-      <c r="W6" s="143" t="s">
+      <c r="T6" s="140"/>
+      <c r="U6" s="140"/>
+      <c r="V6" s="140"/>
+      <c r="W6" s="148" t="s">
         <v>93</v>
       </c>
-      <c r="X6" s="144"/>
-      <c r="Y6" s="144"/>
-      <c r="Z6" s="145"/>
+      <c r="X6" s="149"/>
+      <c r="Y6" s="149"/>
+      <c r="Z6" s="150"/>
       <c r="AA6" s="8"/>
     </row>
     <row r="7" spans="1:28" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="136" t="s">
+      <c r="A7" s="141" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="137" t="s">
+      <c r="B7" s="142" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="138" t="s">
+      <c r="C7" s="143" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="138"/>
-      <c r="E7" s="138"/>
-      <c r="F7" s="138"/>
-      <c r="G7" s="139" t="s">
+      <c r="D7" s="143"/>
+      <c r="E7" s="143"/>
+      <c r="F7" s="143"/>
+      <c r="G7" s="144" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="140" t="s">
+      <c r="H7" s="145" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="141" t="s">
+      <c r="I7" s="146" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="141" t="s">
+      <c r="J7" s="146" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="142" t="s">
+      <c r="K7" s="147" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="142"/>
-      <c r="M7" s="142"/>
-      <c r="N7" s="142"/>
-      <c r="O7" s="142"/>
-      <c r="P7" s="142"/>
-      <c r="Q7" s="142"/>
-      <c r="R7" s="142"/>
-      <c r="S7" s="142"/>
-      <c r="T7" s="142"/>
-      <c r="U7" s="142"/>
-      <c r="V7" s="142"/>
-      <c r="W7" s="142"/>
-      <c r="X7" s="142"/>
-      <c r="Y7" s="142"/>
-      <c r="Z7" s="142"/>
-      <c r="AA7" s="149" t="s">
+      <c r="L7" s="147"/>
+      <c r="M7" s="147"/>
+      <c r="N7" s="147"/>
+      <c r="O7" s="147"/>
+      <c r="P7" s="147"/>
+      <c r="Q7" s="147"/>
+      <c r="R7" s="147"/>
+      <c r="S7" s="147"/>
+      <c r="T7" s="147"/>
+      <c r="U7" s="147"/>
+      <c r="V7" s="147"/>
+      <c r="W7" s="147"/>
+      <c r="X7" s="147"/>
+      <c r="Y7" s="147"/>
+      <c r="Z7" s="147"/>
+      <c r="AA7" s="136" t="s">
         <v>19</v>
       </c>
-      <c r="AB7" s="150" t="s">
+      <c r="AB7" s="137" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="136"/>
-      <c r="B8" s="137"/>
+      <c r="A8" s="141"/>
+      <c r="B8" s="142"/>
       <c r="C8" s="124" t="s">
         <v>21</v>
       </c>
@@ -2849,10 +2849,10 @@
       <c r="F8" s="124" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="139"/>
-      <c r="H8" s="140"/>
-      <c r="I8" s="141"/>
-      <c r="J8" s="141"/>
+      <c r="G8" s="144"/>
+      <c r="H8" s="145"/>
+      <c r="I8" s="146"/>
+      <c r="J8" s="146"/>
       <c r="K8" s="16">
         <v>43838</v>
       </c>
@@ -2916,8 +2916,8 @@
         <f>Y8+7</f>
         <v>43943</v>
       </c>
-      <c r="AA8" s="149"/>
-      <c r="AB8" s="150"/>
+      <c r="AA8" s="136"/>
+      <c r="AB8" s="137"/>
     </row>
     <row r="9" spans="1:28" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="18"/>
@@ -6855,7 +6855,7 @@
         <v>0</v>
       </c>
       <c r="E84" s="126">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="F84" s="126">
         <v>0</v>
@@ -6872,7 +6872,7 @@
       </c>
       <c r="J84" s="33">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="K84" s="35"/>
       <c r="L84" s="35"/>
@@ -7277,10 +7277,10 @@
       <c r="AB94" s="41"/>
     </row>
     <row r="95" spans="1:28" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="151" t="s">
+      <c r="A95" s="138" t="s">
         <v>68</v>
       </c>
-      <c r="B95" s="151"/>
+      <c r="B95" s="138"/>
       <c r="C95" s="124">
         <f>SUM(C10:C94)</f>
         <v>130.5</v>
@@ -7291,7 +7291,7 @@
       </c>
       <c r="E95" s="124">
         <f>SUM(E10:E94)</f>
-        <v>108.5</v>
+        <v>108.75</v>
       </c>
       <c r="F95" s="124">
         <f>SUM(F10:F94)</f>
@@ -7302,7 +7302,7 @@
       <c r="I95" s="88"/>
       <c r="J95" s="86">
         <f>SUM(C95:F95)</f>
-        <v>455.5</v>
+        <v>455.75</v>
       </c>
       <c r="K95" s="89"/>
       <c r="L95" s="89"/>
@@ -7327,10 +7327,10 @@
       <c r="AB95" s="115"/>
     </row>
     <row r="96" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="146" t="s">
+      <c r="A96" s="133" t="s">
         <v>69</v>
       </c>
-      <c r="B96" s="146"/>
+      <c r="B96" s="133"/>
       <c r="C96" s="124">
         <f>117-C95</f>
         <v>-13.5</v>
@@ -7341,7 +7341,7 @@
       </c>
       <c r="E96" s="124">
         <f>117-E95</f>
-        <v>8.5</v>
+        <v>8.25</v>
       </c>
       <c r="F96" s="124">
         <f>117-F95</f>
@@ -7352,7 +7352,7 @@
       <c r="I96" s="86"/>
       <c r="J96" s="86">
         <f>SUM(C96:F96)</f>
-        <v>12.5</v>
+        <v>12.25</v>
       </c>
       <c r="K96" s="89"/>
       <c r="L96" s="89"/>
@@ -7374,10 +7374,10 @@
       <c r="AB96" s="89"/>
     </row>
     <row r="97" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="147" t="s">
+      <c r="A97" s="134" t="s">
         <v>70</v>
       </c>
-      <c r="B97" s="147"/>
+      <c r="B97" s="134"/>
       <c r="C97" s="124"/>
       <c r="D97" s="124"/>
       <c r="E97" s="124"/>
@@ -7409,10 +7409,10 @@
       <c r="AB97" s="89"/>
     </row>
     <row r="98" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="146" t="s">
+      <c r="A98" s="133" t="s">
         <v>71</v>
       </c>
-      <c r="B98" s="146"/>
+      <c r="B98" s="133"/>
       <c r="C98" s="124"/>
       <c r="D98" s="124"/>
       <c r="E98" s="128"/>
@@ -7425,7 +7425,7 @@
       </c>
       <c r="J98" s="86">
         <f>SUM(J10:J94)</f>
-        <v>455.5</v>
+        <v>455.75</v>
       </c>
       <c r="K98" s="89"/>
       <c r="L98" s="89"/>
@@ -7449,12 +7449,12 @@
     <row r="99" spans="1:28" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="91"/>
       <c r="B99" s="91"/>
-      <c r="D99" s="152" t="s">
+      <c r="D99" s="139" t="s">
         <v>88</v>
       </c>
-      <c r="E99" s="152"/>
-      <c r="F99" s="152"/>
-      <c r="G99" s="152"/>
+      <c r="E99" s="139"/>
+      <c r="F99" s="139"/>
+      <c r="G99" s="139"/>
       <c r="H99" s="92"/>
       <c r="I99" s="92"/>
       <c r="J99" s="92"/>
@@ -7478,10 +7478,10 @@
       <c r="AB99" s="89"/>
     </row>
     <row r="100" spans="1:28" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="147" t="s">
+      <c r="A100" s="134" t="s">
         <v>72</v>
       </c>
-      <c r="B100" s="147"/>
+      <c r="B100" s="134"/>
       <c r="C100" s="129">
         <f>135*4</f>
         <v>540</v>
@@ -7513,13 +7513,13 @@
       <c r="AB100" s="89"/>
     </row>
     <row r="101" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="148" t="s">
+      <c r="A101" s="135" t="s">
         <v>73</v>
       </c>
-      <c r="B101" s="148"/>
+      <c r="B101" s="135"/>
       <c r="C101" s="129">
         <f>C100-J98</f>
-        <v>84.5</v>
+        <v>84.25</v>
       </c>
       <c r="D101" s="131">
         <v>66</v>
@@ -7601,15 +7601,11 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="D99:G99"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K6:R6"/>
     <mergeCell ref="S6:V6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
@@ -7620,11 +7616,15 @@
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:Z7"/>
     <mergeCell ref="W6:Z6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D99:G99"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
     <cfRule type="containsText" dxfId="62" priority="75" operator="containsText" text="En cours">

</xml_diff>

<commit_message>
Partially fixed issue #39
</commit_message>
<xml_diff>
--- a/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
+++ b/Semainiers/Semainiers_EquipeLaMarqueSansNom_Hebdomadaire.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alxbo\Source\Repos\mrjrdg\marque-sans-nom\Semainiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D213B1FD-1DE5-4D16-AA36-C30C8973BFD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F3932B-37CA-48EC-A502-7C59AFA8C723}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="116">
   <si>
     <t>UQÀM - Hiver 2020</t>
   </si>
@@ -442,6 +442,12 @@
   </si>
   <si>
     <t>Améliorer le visuel (user-create)</t>
+  </si>
+  <si>
+    <t>Televersement back-end</t>
+  </si>
+  <si>
+    <t>Améliorer le visuel (messagerie)</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1178,7 @@
     <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyAlignment="1">
@@ -1553,6 +1559,43 @@
       <alignment horizontal="justify" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1572,42 +1615,9 @@
     <xf numFmtId="164" fontId="2" fillId="12" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="20" fillId="10" borderId="16" xfId="9" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -2307,7 +2317,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2349,7 +2359,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2401,7 +2411,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2606,10 +2616,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AMK106"/>
+  <dimension ref="A1:AMK105"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2637,22 +2647,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="6" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="151" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="151"/>
+      <c r="A1" s="133" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="133"/>
       <c r="C1" s="123"/>
-      <c r="D1" s="152" t="s">
+      <c r="D1" s="134" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
-      <c r="G1" s="152"/>
-      <c r="H1" s="152"/>
-      <c r="I1" s="152"/>
-      <c r="J1" s="152"/>
-      <c r="K1" s="152"/>
-      <c r="L1" s="152"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="134"/>
+      <c r="I1" s="134"/>
+      <c r="J1" s="134"/>
+      <c r="K1" s="134"/>
+      <c r="L1" s="134"/>
       <c r="N1" s="2"/>
       <c r="P1" s="7"/>
       <c r="Q1" s="6" t="s">
@@ -2664,20 +2674,20 @@
       <c r="AA1" s="8"/>
     </row>
     <row r="2" spans="1:28" s="6" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="151" t="s">
+      <c r="A2" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="151"/>
+      <c r="B2" s="133"/>
       <c r="C2" s="123"/>
       <c r="D2" s="123"/>
       <c r="E2" s="123"/>
-      <c r="F2" s="151" t="s">
+      <c r="F2" s="133" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="151"/>
-      <c r="H2" s="151"/>
-      <c r="I2" s="151"/>
-      <c r="J2" s="151"/>
+      <c r="G2" s="133"/>
+      <c r="H2" s="133"/>
+      <c r="I2" s="133"/>
+      <c r="J2" s="133"/>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
       <c r="N2" s="2"/>
@@ -2760,83 +2770,83 @@
       <c r="H6" s="2"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="140" t="s">
+      <c r="K6" s="135" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="140"/>
-      <c r="M6" s="140"/>
-      <c r="N6" s="140"/>
-      <c r="O6" s="140"/>
-      <c r="P6" s="140"/>
-      <c r="Q6" s="140"/>
-      <c r="R6" s="140"/>
-      <c r="S6" s="140" t="s">
+      <c r="L6" s="135"/>
+      <c r="M6" s="135"/>
+      <c r="N6" s="135"/>
+      <c r="O6" s="135"/>
+      <c r="P6" s="135"/>
+      <c r="Q6" s="135"/>
+      <c r="R6" s="135"/>
+      <c r="S6" s="135" t="s">
         <v>10</v>
       </c>
-      <c r="T6" s="140"/>
-      <c r="U6" s="140"/>
-      <c r="V6" s="140"/>
-      <c r="W6" s="148" t="s">
+      <c r="T6" s="135"/>
+      <c r="U6" s="135"/>
+      <c r="V6" s="135"/>
+      <c r="W6" s="143" t="s">
         <v>93</v>
       </c>
-      <c r="X6" s="149"/>
-      <c r="Y6" s="149"/>
-      <c r="Z6" s="150"/>
+      <c r="X6" s="144"/>
+      <c r="Y6" s="144"/>
+      <c r="Z6" s="145"/>
       <c r="AA6" s="8"/>
     </row>
     <row r="7" spans="1:28" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="141" t="s">
+      <c r="A7" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="142" t="s">
+      <c r="B7" s="137" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="143" t="s">
+      <c r="C7" s="138" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="143"/>
-      <c r="E7" s="143"/>
-      <c r="F7" s="143"/>
-      <c r="G7" s="144" t="s">
+      <c r="D7" s="138"/>
+      <c r="E7" s="138"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="139" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="145" t="s">
+      <c r="H7" s="140" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="146" t="s">
+      <c r="I7" s="141" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="146" t="s">
+      <c r="J7" s="141" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="147" t="s">
+      <c r="K7" s="142" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="147"/>
-      <c r="M7" s="147"/>
-      <c r="N7" s="147"/>
-      <c r="O7" s="147"/>
-      <c r="P7" s="147"/>
-      <c r="Q7" s="147"/>
-      <c r="R7" s="147"/>
-      <c r="S7" s="147"/>
-      <c r="T7" s="147"/>
-      <c r="U7" s="147"/>
-      <c r="V7" s="147"/>
-      <c r="W7" s="147"/>
-      <c r="X7" s="147"/>
-      <c r="Y7" s="147"/>
-      <c r="Z7" s="147"/>
-      <c r="AA7" s="136" t="s">
+      <c r="L7" s="142"/>
+      <c r="M7" s="142"/>
+      <c r="N7" s="142"/>
+      <c r="O7" s="142"/>
+      <c r="P7" s="142"/>
+      <c r="Q7" s="142"/>
+      <c r="R7" s="142"/>
+      <c r="S7" s="142"/>
+      <c r="T7" s="142"/>
+      <c r="U7" s="142"/>
+      <c r="V7" s="142"/>
+      <c r="W7" s="142"/>
+      <c r="X7" s="142"/>
+      <c r="Y7" s="142"/>
+      <c r="Z7" s="142"/>
+      <c r="AA7" s="149" t="s">
         <v>19</v>
       </c>
-      <c r="AB7" s="137" t="s">
+      <c r="AB7" s="150" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="141"/>
-      <c r="B8" s="142"/>
+      <c r="A8" s="136"/>
+      <c r="B8" s="137"/>
       <c r="C8" s="124" t="s">
         <v>21</v>
       </c>
@@ -2849,10 +2859,10 @@
       <c r="F8" s="124" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="144"/>
-      <c r="H8" s="145"/>
-      <c r="I8" s="146"/>
-      <c r="J8" s="146"/>
+      <c r="G8" s="139"/>
+      <c r="H8" s="140"/>
+      <c r="I8" s="141"/>
+      <c r="J8" s="141"/>
       <c r="K8" s="16">
         <v>43838</v>
       </c>
@@ -2916,8 +2926,8 @@
         <f>Y8+7</f>
         <v>43943</v>
       </c>
-      <c r="AA8" s="136"/>
-      <c r="AB8" s="137"/>
+      <c r="AA8" s="149"/>
+      <c r="AB8" s="150"/>
     </row>
     <row r="9" spans="1:28" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="18"/>
@@ -3786,7 +3796,7 @@
         <v>10</v>
       </c>
       <c r="D25" s="126">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E25" s="126">
         <v>3.5</v>
@@ -3796,17 +3806,17 @@
       </c>
       <c r="G25" s="31">
         <f>VLOOKUP(H25,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H25" s="32" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I25" s="33">
         <v>30</v>
       </c>
       <c r="J25" s="33">
         <f t="shared" si="1"/>
-        <v>46.5</v>
+        <v>48.5</v>
       </c>
       <c r="K25" s="58"/>
       <c r="L25" s="51"/>
@@ -3823,10 +3833,10 @@
       <c r="W25" s="35"/>
       <c r="X25" s="35"/>
       <c r="Y25" s="35"/>
-      <c r="Z25" s="36"/>
+      <c r="Z25" s="34"/>
       <c r="AA25" s="37">
         <f t="shared" si="2"/>
-        <v>-16.5</v>
+        <v>-18.5</v>
       </c>
       <c r="AB25" s="41"/>
     </row>
@@ -5939,7 +5949,7 @@
         <v>0</v>
       </c>
       <c r="D66" s="126">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E66" s="126">
         <v>0</v>
@@ -5949,14 +5959,14 @@
       </c>
       <c r="G66" s="63"/>
       <c r="H66" s="32" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I66" s="33">
         <v>5</v>
       </c>
       <c r="J66" s="33">
         <f t="shared" ref="J66" si="6">SUM(C66:F66)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K66" s="65"/>
       <c r="L66" s="65"/>
@@ -5973,7 +5983,7 @@
       <c r="W66" s="65"/>
       <c r="X66" s="110"/>
       <c r="Y66" s="65"/>
-      <c r="Z66" s="45"/>
+      <c r="Z66" s="119"/>
       <c r="AA66" s="85"/>
       <c r="AB66" s="68"/>
     </row>
@@ -6039,7 +6049,7 @@
         <v>12</v>
       </c>
       <c r="J68" s="33">
-        <f t="shared" ref="J68:J93" si="7">SUM(C68:F68)</f>
+        <f t="shared" ref="J68:J92" si="7">SUM(C68:F68)</f>
         <v>12</v>
       </c>
       <c r="K68" s="35"/>
@@ -6280,7 +6290,7 @@
         <v>0</v>
       </c>
       <c r="D73" s="126">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E73" s="126">
         <v>2</v>
@@ -6300,7 +6310,7 @@
       </c>
       <c r="J73" s="33">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K73" s="35"/>
       <c r="L73" s="35"/>
@@ -6317,7 +6327,7 @@
       <c r="W73" s="35"/>
       <c r="X73" s="120"/>
       <c r="Y73" s="119"/>
-      <c r="Z73" s="36"/>
+      <c r="Z73" s="119"/>
       <c r="AA73" s="37"/>
       <c r="AB73" s="41"/>
     </row>
@@ -6800,7 +6810,7 @@
         <v>0</v>
       </c>
       <c r="D83" s="126">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E83" s="126">
         <v>0</v>
@@ -6820,7 +6830,7 @@
       </c>
       <c r="J83" s="33">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K83" s="35"/>
       <c r="L83" s="35"/>
@@ -6837,7 +6847,7 @@
       <c r="W83" s="35"/>
       <c r="X83" s="120"/>
       <c r="Y83" s="110"/>
-      <c r="Z83" s="36"/>
+      <c r="Z83" s="110"/>
       <c r="AA83" s="37"/>
       <c r="AB83" s="41"/>
     </row>
@@ -6914,10 +6924,10 @@
       </c>
       <c r="G85" s="63">
         <f>VLOOKUP(H85,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H85" s="32" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I85" s="33"/>
       <c r="J85" s="33">
@@ -6962,10 +6972,10 @@
       <c r="F86" s="126"/>
       <c r="G86" s="63">
         <f>VLOOKUP(H86,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H86" s="32" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I86" s="33"/>
       <c r="J86" s="33">
@@ -7039,16 +7049,33 @@
       <c r="AB87" s="41"/>
     </row>
     <row r="88" spans="1:28" s="77" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="29"/>
-      <c r="B88" s="57"/>
-      <c r="C88" s="126"/>
-      <c r="D88" s="126"/>
-      <c r="E88" s="126"/>
-      <c r="F88" s="126"/>
+      <c r="A88" s="29">
+        <v>22</v>
+      </c>
+      <c r="B88" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="C88" s="126">
+        <v>0</v>
+      </c>
+      <c r="D88" s="126">
+        <v>0</v>
+      </c>
+      <c r="E88" s="126">
+        <v>0</v>
+      </c>
+      <c r="F88" s="126">
+        <v>6</v>
+      </c>
       <c r="G88" s="63"/>
-      <c r="H88" s="32"/>
+      <c r="H88" s="32" t="s">
+        <v>2</v>
+      </c>
       <c r="I88" s="33"/>
-      <c r="J88" s="33"/>
+      <c r="J88" s="33">
+        <f t="shared" ref="J88:J89" si="8">SUM(C88:F88)</f>
+        <v>6</v>
+      </c>
       <c r="K88" s="35"/>
       <c r="L88" s="35"/>
       <c r="M88" s="35"/>
@@ -7069,16 +7096,33 @@
       <c r="AB88" s="41"/>
     </row>
     <row r="89" spans="1:28" s="77" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="29"/>
-      <c r="B89" s="57"/>
-      <c r="C89" s="126"/>
-      <c r="D89" s="126"/>
-      <c r="E89" s="126"/>
-      <c r="F89" s="126"/>
+      <c r="A89" s="29">
+        <v>23</v>
+      </c>
+      <c r="B89" s="57" t="s">
+        <v>115</v>
+      </c>
+      <c r="C89" s="126">
+        <v>0</v>
+      </c>
+      <c r="D89" s="126">
+        <v>0</v>
+      </c>
+      <c r="E89" s="126">
+        <v>3.25</v>
+      </c>
+      <c r="F89" s="126">
+        <v>0</v>
+      </c>
       <c r="G89" s="63"/>
-      <c r="H89" s="32"/>
+      <c r="H89" s="32" t="s">
+        <v>5</v>
+      </c>
       <c r="I89" s="33"/>
-      <c r="J89" s="33"/>
+      <c r="J89" s="33">
+        <f t="shared" si="8"/>
+        <v>3.25</v>
+      </c>
       <c r="K89" s="35"/>
       <c r="L89" s="35"/>
       <c r="M89" s="35"/>
@@ -7093,8 +7137,8 @@
       <c r="V89" s="36"/>
       <c r="W89" s="35"/>
       <c r="X89" s="120"/>
-      <c r="Y89" s="132"/>
-      <c r="Z89" s="36"/>
+      <c r="Y89" s="122"/>
+      <c r="Z89" s="153"/>
       <c r="AA89" s="37"/>
       <c r="AB89" s="41"/>
     </row>
@@ -7138,7 +7182,10 @@
       <c r="G91" s="63"/>
       <c r="H91" s="32"/>
       <c r="I91" s="33"/>
-      <c r="J91" s="33"/>
+      <c r="J91" s="33">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
       <c r="K91" s="35"/>
       <c r="L91" s="35"/>
       <c r="M91" s="35"/>
@@ -7153,27 +7200,43 @@
       <c r="V91" s="36"/>
       <c r="W91" s="35"/>
       <c r="X91" s="120"/>
-      <c r="Y91" s="132"/>
+      <c r="Y91" s="35"/>
       <c r="Z91" s="36"/>
       <c r="AA91" s="37"/>
       <c r="AB91" s="41"/>
     </row>
     <row r="92" spans="1:28" s="77" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="29"/>
-      <c r="B92" s="57"/>
-      <c r="C92" s="126"/>
-      <c r="D92" s="126"/>
-      <c r="E92" s="126"/>
-      <c r="F92" s="126"/>
-      <c r="G92" s="63" t="e">
+      <c r="A92" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B92" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C92" s="126">
+        <v>2</v>
+      </c>
+      <c r="D92" s="126">
+        <v>2</v>
+      </c>
+      <c r="E92" s="126">
+        <v>0.75</v>
+      </c>
+      <c r="F92" s="126">
+        <v>0</v>
+      </c>
+      <c r="G92" s="63">
         <f>VLOOKUP(H92,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H92" s="32"/>
-      <c r="I92" s="33"/>
+        <v>100</v>
+      </c>
+      <c r="H92" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="I92" s="33">
+        <v>12</v>
+      </c>
       <c r="J92" s="33">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>4.75</v>
       </c>
       <c r="K92" s="35"/>
       <c r="L92" s="35"/>
@@ -7189,44 +7252,22 @@
       <c r="V92" s="36"/>
       <c r="W92" s="35"/>
       <c r="X92" s="120"/>
-      <c r="Y92" s="35"/>
+      <c r="Y92" s="122"/>
       <c r="Z92" s="36"/>
       <c r="AA92" s="37"/>
       <c r="AB92" s="41"/>
     </row>
-    <row r="93" spans="1:28" s="77" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="B93" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="C93" s="126">
-        <v>0</v>
-      </c>
-      <c r="D93" s="126">
-        <v>0</v>
-      </c>
-      <c r="E93" s="126">
-        <v>0.75</v>
-      </c>
-      <c r="F93" s="126">
-        <v>0</v>
-      </c>
-      <c r="G93" s="63">
-        <f>VLOOKUP(H93,Feuil2!$A$1:$B$3,2,0)</f>
-        <v>100</v>
-      </c>
-      <c r="H93" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="I93" s="33">
-        <v>12</v>
-      </c>
-      <c r="J93" s="33">
-        <f t="shared" si="7"/>
-        <v>0.75</v>
-      </c>
+    <row r="93" spans="1:28" s="77" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="29"/>
+      <c r="B93" s="57"/>
+      <c r="C93" s="126"/>
+      <c r="D93" s="126"/>
+      <c r="E93" s="126"/>
+      <c r="F93" s="126"/>
+      <c r="G93" s="63"/>
+      <c r="H93" s="32"/>
+      <c r="I93" s="33"/>
+      <c r="J93" s="33"/>
       <c r="K93" s="35"/>
       <c r="L93" s="35"/>
       <c r="M93" s="35"/>
@@ -7241,68 +7282,88 @@
       <c r="V93" s="36"/>
       <c r="W93" s="35"/>
       <c r="X93" s="120"/>
-      <c r="Y93" s="122"/>
+      <c r="Y93" s="35"/>
       <c r="Z93" s="36"/>
       <c r="AA93" s="37"/>
       <c r="AB93" s="41"/>
     </row>
-    <row r="94" spans="1:28" s="77" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="29"/>
-      <c r="B94" s="57"/>
-      <c r="C94" s="126"/>
-      <c r="D94" s="126"/>
-      <c r="E94" s="126"/>
-      <c r="F94" s="126"/>
-      <c r="G94" s="63"/>
-      <c r="H94" s="32"/>
-      <c r="I94" s="33"/>
-      <c r="J94" s="33"/>
-      <c r="K94" s="35"/>
-      <c r="L94" s="35"/>
-      <c r="M94" s="35"/>
-      <c r="N94" s="36"/>
-      <c r="O94" s="35"/>
-      <c r="P94" s="35"/>
-      <c r="Q94" s="35"/>
-      <c r="R94" s="35"/>
-      <c r="S94" s="35"/>
-      <c r="T94" s="35"/>
-      <c r="U94" s="35"/>
-      <c r="V94" s="36"/>
-      <c r="W94" s="35"/>
-      <c r="X94" s="120"/>
-      <c r="Y94" s="35"/>
-      <c r="Z94" s="36"/>
-      <c r="AA94" s="37"/>
-      <c r="AB94" s="41"/>
-    </row>
-    <row r="95" spans="1:28" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="138" t="s">
+    <row r="94" spans="1:28" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="151" t="s">
         <v>68</v>
       </c>
-      <c r="B95" s="138"/>
+      <c r="B94" s="151"/>
+      <c r="C94" s="124">
+        <f>SUM(C10:C93)</f>
+        <v>132.5</v>
+      </c>
+      <c r="D94" s="124">
+        <f>SUM(D10:D93)</f>
+        <v>112.5</v>
+      </c>
+      <c r="E94" s="124">
+        <f>SUM(E10:E93)</f>
+        <v>112</v>
+      </c>
+      <c r="F94" s="124">
+        <f>SUM(F10:F93)</f>
+        <v>120</v>
+      </c>
+      <c r="G94" s="87"/>
+      <c r="H94" s="86"/>
+      <c r="I94" s="88"/>
+      <c r="J94" s="86">
+        <f>SUM(C94:F94)</f>
+        <v>477</v>
+      </c>
+      <c r="K94" s="89"/>
+      <c r="L94" s="89"/>
+      <c r="M94" s="89"/>
+      <c r="N94" s="89"/>
+      <c r="O94" s="89"/>
+      <c r="P94" s="89"/>
+      <c r="Q94" s="89"/>
+      <c r="R94" s="89"/>
+      <c r="S94" s="89"/>
+      <c r="T94" s="89"/>
+      <c r="U94" s="89"/>
+      <c r="V94" s="89"/>
+      <c r="W94" s="89"/>
+      <c r="X94" s="89"/>
+      <c r="Y94" s="89"/>
+      <c r="Z94" s="89"/>
+      <c r="AA94" s="114">
+        <f>SUM(AA10:AA93)</f>
+        <v>-2.75</v>
+      </c>
+      <c r="AB94" s="115"/>
+    </row>
+    <row r="95" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="146" t="s">
+        <v>69</v>
+      </c>
+      <c r="B95" s="146"/>
       <c r="C95" s="124">
-        <f>SUM(C10:C94)</f>
-        <v>130.5</v>
+        <f>117-C94</f>
+        <v>-15.5</v>
       </c>
       <c r="D95" s="124">
-        <f>SUM(D10:D94)</f>
-        <v>102.5</v>
+        <f>117-D94</f>
+        <v>4.5</v>
       </c>
       <c r="E95" s="124">
-        <f>SUM(E10:E94)</f>
-        <v>108.75</v>
+        <f>117-E94</f>
+        <v>5</v>
       </c>
       <c r="F95" s="124">
-        <f>SUM(F10:F94)</f>
-        <v>114</v>
+        <f>117-F94</f>
+        <v>-3</v>
       </c>
       <c r="G95" s="87"/>
       <c r="H95" s="86"/>
-      <c r="I95" s="88"/>
+      <c r="I95" s="86"/>
       <c r="J95" s="86">
         <f>SUM(C95:F95)</f>
-        <v>455.75</v>
+        <v>-9</v>
       </c>
       <c r="K95" s="89"/>
       <c r="L95" s="89"/>
@@ -7320,39 +7381,24 @@
       <c r="X95" s="89"/>
       <c r="Y95" s="89"/>
       <c r="Z95" s="89"/>
-      <c r="AA95" s="114">
-        <f>SUM(AA10:AA94)</f>
-        <v>-0.75</v>
-      </c>
-      <c r="AB95" s="115"/>
+      <c r="AA95" s="89"/>
+      <c r="AB95" s="89"/>
     </row>
     <row r="96" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="133" t="s">
-        <v>69</v>
-      </c>
-      <c r="B96" s="133"/>
-      <c r="C96" s="124">
-        <f>117-C95</f>
-        <v>-13.5</v>
-      </c>
-      <c r="D96" s="124">
-        <f>117-D95</f>
-        <v>14.5</v>
-      </c>
-      <c r="E96" s="124">
-        <f>117-E95</f>
-        <v>8.25</v>
-      </c>
-      <c r="F96" s="124">
-        <f>117-F95</f>
-        <v>3</v>
-      </c>
-      <c r="G96" s="87"/>
+      <c r="A96" s="147" t="s">
+        <v>70</v>
+      </c>
+      <c r="B96" s="147"/>
+      <c r="C96" s="124"/>
+      <c r="D96" s="124"/>
+      <c r="E96" s="124"/>
+      <c r="F96" s="124"/>
+      <c r="G96" s="86"/>
       <c r="H96" s="86"/>
       <c r="I96" s="86"/>
       <c r="J96" s="86">
-        <f>SUM(C96:F96)</f>
-        <v>12.25</v>
+        <f>C96+D96+F96+E96</f>
+        <v>0</v>
       </c>
       <c r="K96" s="89"/>
       <c r="L96" s="89"/>
@@ -7374,20 +7420,23 @@
       <c r="AB96" s="89"/>
     </row>
     <row r="97" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="134" t="s">
-        <v>70</v>
-      </c>
-      <c r="B97" s="134"/>
+      <c r="A97" s="146" t="s">
+        <v>71</v>
+      </c>
+      <c r="B97" s="146"/>
       <c r="C97" s="124"/>
       <c r="D97" s="124"/>
-      <c r="E97" s="124"/>
+      <c r="E97" s="128"/>
       <c r="F97" s="124"/>
       <c r="G97" s="86"/>
       <c r="H97" s="86"/>
-      <c r="I97" s="86"/>
+      <c r="I97" s="90">
+        <f>SUM(I10:I93)</f>
+        <v>483.25</v>
+      </c>
       <c r="J97" s="86">
-        <f>C97+D97+F97+E97</f>
-        <v>0</v>
+        <f>SUM(J10:J93)</f>
+        <v>477</v>
       </c>
       <c r="K97" s="89"/>
       <c r="L97" s="89"/>
@@ -7408,25 +7457,18 @@
       <c r="AA97" s="89"/>
       <c r="AB97" s="89"/>
     </row>
-    <row r="98" spans="1:28" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="133" t="s">
-        <v>71</v>
-      </c>
-      <c r="B98" s="133"/>
-      <c r="C98" s="124"/>
-      <c r="D98" s="124"/>
-      <c r="E98" s="128"/>
-      <c r="F98" s="124"/>
-      <c r="G98" s="86"/>
-      <c r="H98" s="86"/>
-      <c r="I98" s="90">
-        <f>SUM(I10:I94)</f>
-        <v>483.25</v>
-      </c>
-      <c r="J98" s="86">
-        <f>SUM(J10:J94)</f>
-        <v>455.75</v>
-      </c>
+    <row r="98" spans="1:28" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="91"/>
+      <c r="B98" s="91"/>
+      <c r="D98" s="152" t="s">
+        <v>88</v>
+      </c>
+      <c r="E98" s="152"/>
+      <c r="F98" s="152"/>
+      <c r="G98" s="152"/>
+      <c r="H98" s="92"/>
+      <c r="I98" s="92"/>
+      <c r="J98" s="92"/>
       <c r="K98" s="89"/>
       <c r="L98" s="89"/>
       <c r="M98" s="89"/>
@@ -7446,15 +7488,19 @@
       <c r="AA98" s="89"/>
       <c r="AB98" s="89"/>
     </row>
-    <row r="99" spans="1:28" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="91"/>
-      <c r="B99" s="91"/>
-      <c r="D99" s="139" t="s">
-        <v>88</v>
-      </c>
-      <c r="E99" s="139"/>
-      <c r="F99" s="139"/>
-      <c r="G99" s="139"/>
+    <row r="99" spans="1:28" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="147" t="s">
+        <v>72</v>
+      </c>
+      <c r="B99" s="147"/>
+      <c r="C99" s="129">
+        <f>135*4</f>
+        <v>540</v>
+      </c>
+      <c r="D99" s="130">
+        <v>468</v>
+      </c>
+      <c r="G99" s="92"/>
       <c r="H99" s="92"/>
       <c r="I99" s="92"/>
       <c r="J99" s="92"/>
@@ -7477,17 +7523,17 @@
       <c r="AA99" s="89"/>
       <c r="AB99" s="89"/>
     </row>
-    <row r="100" spans="1:28" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="134" t="s">
-        <v>72</v>
-      </c>
-      <c r="B100" s="134"/>
+    <row r="100" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="148" t="s">
+        <v>73</v>
+      </c>
+      <c r="B100" s="148"/>
       <c r="C100" s="129">
-        <f>135*4</f>
-        <v>540</v>
-      </c>
-      <c r="D100" s="130">
-        <v>468</v>
+        <f>C99-J97</f>
+        <v>63</v>
+      </c>
+      <c r="D100" s="131">
+        <v>66</v>
       </c>
       <c r="G100" s="92"/>
       <c r="H100" s="92"/>
@@ -7512,52 +7558,31 @@
       <c r="AA100" s="89"/>
       <c r="AB100" s="89"/>
     </row>
-    <row r="101" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="135" t="s">
-        <v>73</v>
-      </c>
-      <c r="B101" s="135"/>
-      <c r="C101" s="129">
-        <f>C100-J98</f>
-        <v>84.25</v>
-      </c>
-      <c r="D101" s="131">
-        <v>66</v>
-      </c>
-      <c r="G101" s="92"/>
-      <c r="H101" s="92"/>
-      <c r="I101" s="92"/>
-      <c r="J101" s="92"/>
-      <c r="K101" s="89"/>
-      <c r="L101" s="89"/>
-      <c r="M101" s="89"/>
-      <c r="N101" s="89"/>
-      <c r="O101" s="89"/>
-      <c r="P101" s="89"/>
-      <c r="Q101" s="89"/>
-      <c r="R101" s="89"/>
-      <c r="S101" s="89"/>
-      <c r="T101" s="89"/>
-      <c r="U101" s="89"/>
-      <c r="V101" s="89"/>
-      <c r="W101" s="89"/>
-      <c r="X101" s="89"/>
-      <c r="Y101" s="89"/>
-      <c r="Z101" s="89"/>
+    <row r="101" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A101" s="93"/>
+      <c r="B101" s="91"/>
+      <c r="G101" s="91"/>
+      <c r="H101" s="94"/>
+      <c r="I101" s="95"/>
+      <c r="J101" s="95"/>
       <c r="AA101" s="89"/>
-      <c r="AB101" s="89"/>
-    </row>
-    <row r="102" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A102" s="93"/>
-      <c r="B102" s="91"/>
-      <c r="G102" s="91"/>
-      <c r="H102" s="94"/>
-      <c r="I102" s="95"/>
-      <c r="J102" s="95"/>
-      <c r="AA102" s="89"/>
+    </row>
+    <row r="103" spans="1:28" s="97" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A103" s="96"/>
+      <c r="C103" s="123"/>
+      <c r="D103" s="123"/>
+      <c r="E103" s="123"/>
+      <c r="F103" s="123"/>
+      <c r="H103" s="98"/>
+      <c r="I103" s="99"/>
+      <c r="J103" s="99"/>
+      <c r="N103" s="100"/>
+      <c r="R103" s="100"/>
+      <c r="V103" s="100"/>
+      <c r="Z103" s="100"/>
+      <c r="AA103" s="101"/>
     </row>
     <row r="104" spans="1:28" s="97" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A104" s="96"/>
       <c r="C104" s="123"/>
       <c r="D104" s="123"/>
       <c r="E104" s="123"/>
@@ -7585,27 +7610,17 @@
       <c r="Z105" s="100"/>
       <c r="AA105" s="101"/>
     </row>
-    <row r="106" spans="1:28" s="97" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="C106" s="123"/>
-      <c r="D106" s="123"/>
-      <c r="E106" s="123"/>
-      <c r="F106" s="123"/>
-      <c r="H106" s="98"/>
-      <c r="I106" s="99"/>
-      <c r="J106" s="99"/>
-      <c r="N106" s="100"/>
-      <c r="R106" s="100"/>
-      <c r="V106" s="100"/>
-      <c r="Z106" s="100"/>
-      <c r="AA106" s="101"/>
-    </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="D98:G98"/>
     <mergeCell ref="S6:V6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
@@ -7616,22 +7631,18 @@
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:Z7"/>
     <mergeCell ref="W6:Z6"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="D99:G99"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K6:R6"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
     <cfRule type="containsText" dxfId="62" priority="75" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",H19)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H9:H68 H70:H80 H82:H94">
+  <conditionalFormatting sqref="H9:H68 H70:H80 H82:H93">
     <cfRule type="containsText" dxfId="61" priority="76" operator="containsText" text="En attente">
       <formula>NOT(ISERROR(SEARCH("En attente",H9)))</formula>
     </cfRule>
@@ -7642,7 +7653,7 @@
       <formula>NOT(ISERROR(SEARCH("Terminé",H9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9:F45 C47:F47 C56:F64 C49:F54 C66:F68 C70:F80 C82:F94">
+  <conditionalFormatting sqref="C9:F45 C47:F47 C56:F64 C49:F54 C66:F68 C70:F80 C82:F93">
     <cfRule type="cellIs" dxfId="58" priority="79" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -7650,7 +7661,7 @@
       <formula>$H9="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9:F45 C47:F47 C56:F64 C49:F54 C66:F68 C70:F80 C82:F94">
+  <conditionalFormatting sqref="C9:F45 C47:F47 C56:F64 C49:F54 C66:F68 C70:F80 C82:F93">
     <cfRule type="expression" dxfId="56" priority="81">
       <formula>$H9="En cours"</formula>
     </cfRule>
@@ -7738,31 +7749,31 @@
       <formula>$H66="En attente"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C94:F94">
+  <conditionalFormatting sqref="C93:F93">
     <cfRule type="expression" dxfId="34" priority="36">
-      <formula>$H94="En cours"</formula>
+      <formula>$H93="En cours"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="33" priority="37">
-      <formula>$H94="En attente"</formula>
+      <formula>$H93="En attente"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H94">
+  <conditionalFormatting sqref="H93">
     <cfRule type="containsText" dxfId="32" priority="40" operator="containsText" text="En attente">
-      <formula>NOT(ISERROR(SEARCH("En attente",H94)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En attente",H93)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="31" priority="41" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",H94)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",H93)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="30" priority="42" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",H94)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",H93)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C94:F94">
+  <conditionalFormatting sqref="C93:F93">
     <cfRule type="cellIs" dxfId="29" priority="38" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="28" priority="39">
-      <formula>$H94="Terminé"</formula>
+      <formula>$H93="Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69">
@@ -7874,7 +7885,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H9:H94" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H9:H93" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"En attente,En cours,Terminé"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>